<commit_message>
US1352 (Implement action methods for Driver view page for data-driven testing) & US1316 (Provide ability to perform keywords + data-driven testing in Automation Framework + Verify data-driven support using either Compliance Report or Driver View test cases)
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,11 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User Test Data" sheetId="5" r:id="rId1"/>
-    <sheet name="Report Test Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Driver View Test Data" sheetId="8" r:id="rId2"/>
+    <sheet name="Report Test Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Roles" sheetId="6" r:id="rId4"/>
+    <sheet name="General" sheetId="7" r:id="rId5"/>
+    <sheet name="Survey" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>Enabled</t>
   </si>
@@ -37,6 +41,123 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>sqacusua@email.com</t>
+  </si>
+  <si>
+    <t>Customer Utility Admin</t>
+  </si>
+  <si>
+    <t>sqacussu@email.com</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Customer Driver</t>
+  </si>
+  <si>
+    <t>Customer Supervisor</t>
+  </si>
+  <si>
+    <t>Picarro Admin</t>
+  </si>
+  <si>
+    <t>Picarro Support</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>sqacusdr1@email.com</t>
+  </si>
+  <si>
+    <t>sqapicad@picarro.com</t>
+  </si>
+  <si>
+    <t>sqapicsu1@picarro.com</t>
+  </si>
+  <si>
+    <t>sqa#Picarro$0</t>
+  </si>
+  <si>
+    <t>sqa#Picarro$1</t>
+  </si>
+  <si>
+    <t>sqa#Picarro$2</t>
+  </si>
+  <si>
+    <t>sqa#Picarro$3</t>
+  </si>
+  <si>
+    <t>sqa#Picarro$4</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>FastLane!911</t>
+  </si>
+  <si>
+    <t>RowID</t>
+  </si>
+  <si>
+    <t>Survey Tag</t>
+  </si>
+  <si>
+    <t>Survey Time</t>
+  </si>
+  <si>
+    <t>Solar Radiation</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Survey Type</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Overcast</t>
+  </si>
+  <si>
+    <t>Strong</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Night</t>
+  </si>
+  <si>
+    <t>Radiation</t>
+  </si>
+  <si>
+    <t>GenerateRandomString(6)</t>
+  </si>
+  <si>
+    <t>Replay Script DB3 File</t>
+  </si>
+  <si>
+    <t>replay-db3.defn</t>
+  </si>
+  <si>
+    <t>Surveyor.db3</t>
+  </si>
+  <si>
+    <t>GenerateRandomString(Integer size)</t>
+  </si>
+  <si>
+    <t>GenerateRandomNumber(Integer size)</t>
+  </si>
+  <si>
+    <t>Replay Script Defn File</t>
   </si>
 </sst>
 </file>
@@ -363,39 +484,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Roles!$A$2:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>General!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="24.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Survey!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Survey!$B$2:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Survey!$C$2:$C$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Survey!$D$2:$D$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>F1:F1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -411,4 +762,144 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="32.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Checking-in changes made for testing (unit-level) the major Actions in Driver View Page
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>Enabled</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Radiation</t>
   </si>
   <si>
-    <t>GenerateRandomString(6)</t>
-  </si>
-  <si>
     <t>Replay Script DB3 File</t>
   </si>
   <si>
@@ -158,6 +155,45 @@
   </si>
   <si>
     <t>Replay Script Defn File</t>
+  </si>
+  <si>
+    <t>instr_ready.defn</t>
+  </si>
+  <si>
+    <t>instr_warming.defn</t>
+  </si>
+  <si>
+    <t>Cloud Cover</t>
+  </si>
+  <si>
+    <t>LessThan50</t>
+  </si>
+  <si>
+    <t>GreaterThan50</t>
+  </si>
+  <si>
+    <t>RapidResponse</t>
+  </si>
+  <si>
+    <t>Operator</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Calm</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>Assessment</t>
+  </si>
+  <si>
+    <t>SurveyTag001</t>
   </si>
 </sst>
 </file>
@@ -642,10 +678,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,13 +689,14 @@
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" customWidth="1"/>
     <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" customWidth="1"/>
-    <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -676,46 +713,68 @@
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="I2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
         <v>33</v>
       </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="H4" t="s">
         <v>38</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$A$2:$A$5</xm:f>
@@ -726,17 +785,23 @@
           <x14:formula1>
             <xm:f>Survey!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D1048576</xm:sqref>
+          <xm:sqref>D1:D1048576 E5:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E1048576</xm:sqref>
+          <xm:sqref>E1:E4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$D$2:$D$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>G1:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Survey!$E$2:$E$3</xm:f>
           </x14:formula1>
           <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
@@ -834,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -842,7 +907,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -852,10 +917,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,7 +931,7 @@
     <col min="4" max="4" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -879,8 +944,11 @@
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -888,15 +956,51 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding the datareader classes + Made some fixes in ActionFunctionExecutor + Fixed a bug in RegexUtility
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="143">
   <si>
     <t>Enabled</t>
   </si>
@@ -414,12 +414,6 @@
     <t>All boundaries selected, assets unselected</t>
   </si>
   <si>
-    <t>All options selected, BaseMap=MAP</t>
-  </si>
-  <si>
-    <t>All options selected, BaseMap=SATELLITE</t>
-  </si>
-  <si>
     <t>GenerateRandomString(10)</t>
   </si>
   <si>
@@ -432,9 +426,6 @@
     <t>PG&amp;E</t>
   </si>
   <si>
-    <t>All options selected, BaseMap=NONE</t>
-  </si>
-  <si>
     <t>Number of Surveys to Include</t>
   </si>
   <si>
@@ -444,12 +435,6 @@
     <t>Annotation</t>
   </si>
   <si>
-    <t>1:3</t>
-  </si>
-  <si>
-    <t>RANDOMREPORTNAME1</t>
-  </si>
-  <si>
     <t>stnd-sqacudr</t>
   </si>
   <si>
@@ -457,6 +442,27 @@
   </si>
   <si>
     <t>sqacus</t>
+  </si>
+  <si>
+    <t>All boundaries and assets unselected</t>
+  </si>
+  <si>
+    <t>Indication, Isotopic Analysis, Gap and Percent Coverage Report Area = TRUE. All other FALSE</t>
+  </si>
+  <si>
+    <t>All options selected (except IsoCap and Annotation), BaseMap=MAP</t>
+  </si>
+  <si>
+    <t>All options selected (except IsoCap and Annotation), BaseMap=SATELLITE</t>
+  </si>
+  <si>
+    <t>All options selected (except IsoCap and Annotation), BaseMap=NONE</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>All options selected (except Gaps, Asset, Boundaries, IsoCap and Annotation), BaseMap=SATELLITE</t>
   </si>
 </sst>
 </file>
@@ -810,7 +816,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1173,9 +1179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1200,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -1211,7 +1215,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -1222,7 +1226,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -1233,7 +1237,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -1278,7 +1282,7 @@
   <dimension ref="A1:I1073"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2482,7 +2486,7 @@
   <dimension ref="A1:AA1138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2575,7 +2579,7 @@
         <v>82</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>83</v>
@@ -2604,7 +2608,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
@@ -2631,13 +2635,13 @@
         <v>-122.04883575439401</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -2663,13 +2667,13 @@
         <v>11</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="Z2" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AA2" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -3853,8 +3857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3904,10 +3908,10 @@
         <v>96</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>97</v>
@@ -3921,7 +3925,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -3957,7 +3961,7 @@
         <v>99</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3965,7 +3969,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -4001,7 +4005,7 @@
         <v>100</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -4009,7 +4013,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -4045,10 +4049,53 @@
         <v>101</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
     <row r="6" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -4871,8 +4918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J736"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="A1:I1"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5017,7 +5064,38 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -5771,7 +5849,7 @@
   <dimension ref="A1:H579"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5916,7 +5994,32 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -6511,7 +6614,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>

<commit_message>
US1377- Fixed some of the actions from ComplianceReportActions
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -33,6 +33,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Shirish Pulikkal</author>
+  </authors>
+  <commentList>
+    <comment ref="P1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Input date in "MM/dd/yyyy HH:mm:ss a" format.
+For eg. 06/17/2015 12:00:01 PM</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Input date in "MM/dd/yyyy HH:mm:ss a" format.
+For eg. 06/17/2015 12:00:01 PM</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="143">
   <si>
@@ -469,7 +529,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -503,6 +563,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2482,11 +2555,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2506,8 +2579,8 @@
     <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.5546875" customWidth="1"/>
+    <col min="17" max="17" width="23.88671875" customWidth="1"/>
     <col min="18" max="18" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="26.44140625" bestFit="1" customWidth="1"/>
@@ -2643,8 +2716,12 @@
       <c r="O2" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
+      <c r="P2" s="4">
+        <v>42294.500011574077</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>42010.500011574077</v>
+      </c>
       <c r="R2" s="2" t="s">
         <v>33</v>
       </c>
@@ -3814,6 +3891,7 @@
     <row r="1138" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
@@ -3857,8 +3935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
US1377- Fixed some actions from ComplianceReportActions
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\surveyor-qa\selenium-wd\data\"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="146">
   <si>
     <t>Enabled</t>
   </si>
@@ -519,10 +519,19 @@
     <t>All options selected (except IsoCap and Annotation), BaseMap=NONE</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>All options selected (except Gaps, Asset, Boundaries, IsoCap and Annotation), BaseMap=SATELLITE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>&lt;SPECIFY_BOUNDARY_NAME&gt;</t>
+  </si>
+  <si>
+    <t>6,7,8</t>
   </si>
 </sst>
 </file>
@@ -886,10 +895,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1062,6 +1072,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1155,6 +1166,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -1250,6 +1262,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1352,10 +1365,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I1073"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2556,10 +2570,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA1138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2684,7 +2699,7 @@
         <v>126</v>
       </c>
       <c r="C2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>60</v>
@@ -2692,9 +2707,6 @@
       <c r="E2" s="2">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="G2" s="2">
         <v>37.435339792682498</v>
       </c>
@@ -2726,16 +2738,16 @@
         <v>33</v>
       </c>
       <c r="S2" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2" s="2">
         <v>1</v>
       </c>
-      <c r="U2" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="V2" s="2">
-        <v>0.5</v>
+      <c r="U2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="W2" s="2">
         <v>8.5</v>
@@ -2744,17 +2756,129 @@
         <v>11</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="Z2" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AA2" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="P3" s="4">
+        <v>42344.500011574077</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>42010.500011574077</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="W3" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="X3" s="2">
+        <v>11</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>5</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="2">
+        <v>37.435339792682498</v>
+      </c>
+      <c r="H4" s="2">
+        <v>-121.846961975097</v>
+      </c>
+      <c r="I4" s="2">
+        <v>37.330583620739603</v>
+      </c>
+      <c r="J4" s="2">
+        <v>-122.04883575439401</v>
+      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="P4" s="4">
+        <v>42294.500011574077</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>42010.500011574077</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>2</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="W4" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="X4" s="2">
+        <v>11</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>4</v>
+      </c>
+    </row>
     <row r="5" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -3933,10 +4057,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4171,13 +4296,173 @@
         <v>100</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -4994,10 +5279,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J736"/>
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:J735"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5174,7 +5460,35 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="7" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -5770,7 +6084,7 @@
     <row r="599" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="600" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="601" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="602" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="602" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="603" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="604" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="605" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -5904,7 +6218,6 @@
     <row r="733" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="734" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="735" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="736" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -5924,10 +6237,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H579"/>
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:H578"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6670,7 +6984,6 @@
     <row r="576" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="577" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="578" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="579" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -6690,6 +7003,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6736,6 +7050,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Added additional rows for TestEnvironment data
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -1375,7 +1375,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1478,7 +1478,7 @@
   <dimension ref="A1:E1073"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9111,7 +9111,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G1073"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes to get the multiple driver view tests working
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,6 @@
     <sheet name="Report" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -137,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="150">
   <si>
     <t>Enabled</t>
   </si>
@@ -188,18 +187,6 @@
   </si>
   <si>
     <t>sqa#Picarro$0</t>
-  </si>
-  <si>
-    <t>sqa#Picarro$1</t>
-  </si>
-  <si>
-    <t>sqa#Picarro$2</t>
-  </si>
-  <si>
-    <t>sqa#Picarro$3</t>
-  </si>
-  <si>
-    <t>sqa#Picarro$4</t>
   </si>
   <si>
     <t>Administrator</t>
@@ -966,7 +953,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -979,7 +966,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1019,7 +1006,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>1</v>
@@ -1036,7 +1023,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>1</v>
@@ -1053,7 +1040,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>1</v>
@@ -1070,7 +1057,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>1</v>
@@ -1084,10 +1071,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
@@ -1156,7 +1143,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1164,7 +1151,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1172,7 +1159,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1199,74 +1186,74 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1294,75 +1281,75 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1375,7 +1362,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1386,10 +1373,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1400,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -1411,7 +1398,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -1422,7 +1409,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -1433,7 +1420,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -1478,7 +1465,7 @@
   <dimension ref="A1:E1073"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1491,19 +1478,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1511,16 +1498,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1528,16 +1515,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1545,16 +1532,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1562,16 +1549,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1579,16 +1566,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1596,16 +1583,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1613,16 +1600,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1630,16 +1617,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1647,16 +1634,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -9111,8 +9098,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G1073"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9127,25 +9114,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -9163,22 +9150,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -9186,19 +9173,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -9206,19 +9193,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -9226,19 +9213,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -10390,85 +10377,85 @@
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="Y1" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -10476,13 +10463,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E2" s="2">
         <v>3</v>
@@ -10500,13 +10487,13 @@
         <v>-122.04883575439401</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="P2" s="4">
         <v>42294.500011574077</v>
@@ -10515,7 +10502,7 @@
         <v>42010.500011574077</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="S2" s="2" t="b">
         <v>0</v>
@@ -10524,10 +10511,10 @@
         <v>1</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="W2" s="2">
         <v>8.5</v>
@@ -10536,7 +10523,7 @@
         <v>11</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="Z2" s="2">
         <v>1</v>
@@ -10550,22 +10537,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="P3" s="4">
         <v>42344.500011574077</v>
@@ -10574,7 +10561,7 @@
         <v>42010.500011574077</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="W3" s="2">
         <v>8.5</v>
@@ -10583,7 +10570,7 @@
         <v>11</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="Z3" s="2">
         <v>5</v>
@@ -10597,13 +10584,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2">
         <v>37.435339792682498</v>
@@ -10620,7 +10607,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="P4" s="4">
         <v>42294.500011574077</v>
@@ -10629,7 +10616,7 @@
         <v>42010.500011574077</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="S4" s="2" t="b">
         <v>0</v>
@@ -10638,10 +10625,10 @@
         <v>2</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="W4" s="2">
         <v>8.5</v>
@@ -10650,7 +10637,7 @@
         <v>11</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="Z4" s="2">
         <v>1</v>
@@ -11861,46 +11848,46 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -11908,7 +11895,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -11941,10 +11928,10 @@
         <v>0</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -11952,7 +11939,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -11985,10 +11972,10 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -11996,7 +11983,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -12029,10 +12016,10 @@
         <v>0</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12040,7 +12027,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -12073,10 +12060,10 @@
         <v>0</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12084,7 +12071,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -12117,7 +12104,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12125,7 +12112,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
@@ -12158,7 +12145,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12166,7 +12153,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
@@ -12199,7 +12186,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12207,7 +12194,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
@@ -12240,7 +12227,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -13082,34 +13069,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -13141,7 +13128,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -13173,7 +13160,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -13205,7 +13192,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -13237,7 +13224,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14038,28 +14025,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14085,7 +14072,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14111,7 +14098,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14137,7 +14124,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14163,7 +14150,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14189,7 +14176,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed bugs in action framework. Added exception callstack printing on error.
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="150">
   <si>
     <t>Enabled</t>
   </si>
@@ -953,7 +953,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9098,12 +9098,13 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G1073"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" customWidth="1"/>
     <col min="4" max="4" width="20.109375" customWidth="1"/>
@@ -9228,7 +9229,26 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="9" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
US1502 - Added 4 driver view test cases
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="153">
   <si>
     <t>Enabled</t>
   </si>
@@ -586,6 +586,15 @@
   </si>
   <si>
     <t>SimAuto-AnalyzerKey3</t>
+  </si>
+  <si>
+    <t>sqapgeua@email.com</t>
+  </si>
+  <si>
+    <t>sqapgesu@email.com</t>
+  </si>
+  <si>
+    <t>sqapgedr1@email.com</t>
   </si>
 </sst>
 </file>
@@ -953,7 +962,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1083,9 +1092,57 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="11" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1103,6 +1160,7 @@
     <row r="25" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -9096,10 +9154,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:G1073"/>
+  <dimension ref="A1:G1072"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9162,9 +9220,6 @@
       <c r="E4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="G4" s="2" t="s">
         <v>29</v>
       </c>
@@ -9249,7 +9304,26 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="10" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -10308,17 +10382,22 @@
     <row r="1065" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="1066" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="1067" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1068" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1068" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="1069" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="1070" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="1071" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="1072" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1073" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Survey!$B$2:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1013:E1048576 D1:D1048576</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$A$2:$A$5</xm:f>
@@ -10327,15 +10406,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Survey!$B$2:$B$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>E1014:E1048576 D1:D1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
             <xm:f>Survey!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E1013</xm:sqref>
+          <xm:sqref>E1:E1012</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
US1360 - Add additional features to Driver view page
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -952,8 +952,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9098,7 +9098,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G1073"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Made some idle time setting changes. Cleaned up code
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="153">
   <si>
     <t>Enabled</t>
   </si>
@@ -9157,7 +9157,7 @@
   <dimension ref="A1:G1072"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9324,8 +9324,46 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="12" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixes some issues and added 2 more tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="155">
   <si>
     <t>Enabled</t>
   </si>
@@ -595,6 +595,12 @@
   </si>
   <si>
     <t>sqapgedr1@email.com</t>
+  </si>
+  <si>
+    <t>TC1133_survey</t>
+  </si>
+  <si>
+    <t>TC1134_survey</t>
   </si>
 </sst>
 </file>
@@ -962,7 +968,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9157,7 +9163,7 @@
   <dimension ref="A1:G1072"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9364,8 +9370,46 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="14" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Merged test cases from excel authoring
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="155">
   <si>
     <t>Enabled</t>
   </si>
@@ -676,7 +676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -684,6 +684,7 @@
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9163,7 +9164,7 @@
   <dimension ref="A1:G1072"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9331,104 +9332,264 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G14" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
+    <row r="19" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
+    <row r="21" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="17" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="18" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="19" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="20" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="21" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="23" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="24" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="25" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="26" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="28" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="30" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="31" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="32" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="33" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="34" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="35" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -10478,31 +10639,31 @@
           <x14:formula1>
             <xm:f>Survey!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1013:E1048576 D1:D1048576</xm:sqref>
+          <xm:sqref>E1013:E1048576 D1:D9 D14:D25 D30:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C1048576</xm:sqref>
+          <xm:sqref>C1:C9 C14:C25 C30:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E1012</xm:sqref>
+          <xm:sqref>E1:E9 E14:E25 E30:E1012</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$D$2:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
+          <xm:sqref>G1:G9 G14:G25 G30:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F1048576</xm:sqref>
+          <xm:sqref>F1:F9 F14:F25 F30:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
test cases for US1570
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="158">
   <si>
     <t>Enabled</t>
   </si>
@@ -601,6 +601,15 @@
   </si>
   <si>
     <t>TC1134_survey</t>
+  </si>
+  <si>
+    <t>Surveyor_rr-pic.db3</t>
+  </si>
+  <si>
+    <t>Surveyor_rr-sqacudr.db3</t>
+  </si>
+  <si>
+    <t>Surveyor_rr.db3</t>
   </si>
 </sst>
 </file>
@@ -969,7 +978,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1052,7 +1061,7 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1529,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1073"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1712,25 +1721,55 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
@@ -9163,8 +9202,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G1072"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9579,33 +9618,213 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="33" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="34" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="35" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="36" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="37" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="38" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="39" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="40" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="41" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="42" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="43" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="44" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="45" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="46" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="47" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="48" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="49" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="50" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="51" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -10614,22 +10833,46 @@
     <row r="1054" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="1055" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="1056" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1057" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1058" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1059" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1060" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1061" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1062" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1063" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1064" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1065" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1066" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1067" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1068" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1069" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1070" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1071" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1072" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1057" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1058" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1059" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1060" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1061" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1062" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1063" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1064" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1065" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1066" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="C1066" s="5"/>
+      <c r="D1066" s="5"/>
+      <c r="E1066" s="5"/>
+      <c r="F1066" s="5"/>
+      <c r="G1066" s="5"/>
+    </row>
+    <row r="1067" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="C1067" s="5"/>
+      <c r="D1067" s="5"/>
+      <c r="E1067" s="5"/>
+      <c r="F1067" s="5"/>
+      <c r="G1067" s="5"/>
+    </row>
+    <row r="1068" spans="3:7" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1069" spans="3:7" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1070" spans="3:7" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1071" spans="3:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C1071"/>
+      <c r="D1071"/>
+      <c r="E1071"/>
+      <c r="F1071"/>
+      <c r="G1071"/>
+    </row>
+    <row r="1072" spans="3:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C1072"/>
+      <c r="D1072"/>
+      <c r="E1072"/>
+      <c r="F1072"/>
+      <c r="G1072"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -10639,31 +10882,31 @@
           <x14:formula1>
             <xm:f>Survey!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1013:E1048576 D1:D9 D14:D25 D30:D1048576</xm:sqref>
+          <xm:sqref>E1011:E1048576 D1:D9 D28:D1048576 D14:D23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C9 C14:C25 C30:C1048576</xm:sqref>
+          <xm:sqref>C1:C9 C28:C1048576 C14:C23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E9 E14:E25 E30:E1012</xm:sqref>
+          <xm:sqref>E1:E9 E28:E1010 E14:E23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$D$2:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G9 G14:G25 G30:G1048576</xm:sqref>
+          <xm:sqref>G1:G9 G28:G1048576 G14:G23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F9 F14:F25 F30:F1048576</xm:sqref>
+          <xm:sqref>F1:F9 F28:F1048576 F14:F23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add missing files in merge conflict
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="158">
   <si>
     <t>Enabled</t>
   </si>
@@ -601,6 +601,15 @@
   </si>
   <si>
     <t>TC1134_survey</t>
+  </si>
+  <si>
+    <t>Surveyor_rr-pic.db3</t>
+  </si>
+  <si>
+    <t>Surveyor_rr-sqacudr.db3</t>
+  </si>
+  <si>
+    <t>Surveyor_rr.db3</t>
   </si>
 </sst>
 </file>
@@ -969,7 +978,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1052,7 +1061,7 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1529,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1073"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1712,25 +1721,55 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
@@ -9163,8 +9202,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G1072"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9579,33 +9618,213 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="33" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="34" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="35" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="36" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="37" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="38" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="39" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="40" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="41" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="42" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="43" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="44" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="45" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="46" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="47" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="48" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="49" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="50" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="51" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -10614,22 +10833,46 @@
     <row r="1054" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="1055" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="1056" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1057" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1058" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1059" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1060" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1061" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1062" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1063" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1064" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1065" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1066" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1067" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1068" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1069" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1070" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1071" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="1072" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1057" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1058" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1059" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1060" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1061" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1062" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1063" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1064" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1065" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1066" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="C1066" s="5"/>
+      <c r="D1066" s="5"/>
+      <c r="E1066" s="5"/>
+      <c r="F1066" s="5"/>
+      <c r="G1066" s="5"/>
+    </row>
+    <row r="1067" spans="3:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="C1067" s="5"/>
+      <c r="D1067" s="5"/>
+      <c r="E1067" s="5"/>
+      <c r="F1067" s="5"/>
+      <c r="G1067" s="5"/>
+    </row>
+    <row r="1068" spans="3:7" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1069" spans="3:7" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1070" spans="3:7" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="1071" spans="3:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C1071"/>
+      <c r="D1071"/>
+      <c r="E1071"/>
+      <c r="F1071"/>
+      <c r="G1071"/>
+    </row>
+    <row r="1072" spans="3:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C1072"/>
+      <c r="D1072"/>
+      <c r="E1072"/>
+      <c r="F1072"/>
+      <c r="G1072"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -10639,31 +10882,31 @@
           <x14:formula1>
             <xm:f>Survey!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1013:E1048576 D1:D9 D14:D25 D30:D1048576</xm:sqref>
+          <xm:sqref>E1011:E1048576 D1:D9 D28:D1048576 D14:D23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C9 C14:C25 C30:C1048576</xm:sqref>
+          <xm:sqref>C1:C9 C28:C1048576 C14:C23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E9 E14:E25 E30:E1012</xm:sqref>
+          <xm:sqref>E1:E9 E28:E1010 E14:E23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$D$2:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G9 G14:G25 G30:G1048576</xm:sqref>
+          <xm:sqref>G1:G9 G28:G1048576 G14:G23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F9 F14:F25 F30:F1048576</xm:sqref>
+          <xm:sqref>F1:F9 F28:F1048576 F14:F23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Test Cases for US1743
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="159">
   <si>
     <t>Enabled</t>
   </si>
@@ -610,6 +610,9 @@
   </si>
   <si>
     <t>Surveyor_rr.db3</t>
+  </si>
+  <si>
+    <t>Surveyor_Assessment.db3</t>
   </si>
 </sst>
 </file>
@@ -1538,8 +1541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1073"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1772,11 +1775,21 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
@@ -9202,8 +9215,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G1072"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9799,8 +9812,24 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
+      <c r="A31" s="7">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
@@ -10888,7 +10917,7 @@
           <x14:formula1>
             <xm:f>Survey!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C9 C28:C1048576 C14:C23</xm:sqref>
+          <xm:sqref>C1:C9 C14:C23 C28:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Updates to execute the Observer view test cases in CI with local feature branch
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="160">
   <si>
     <t>Enabled</t>
   </si>
@@ -613,6 +613,9 @@
   </si>
   <si>
     <t>Surveyor_Assessment.db3</t>
+  </si>
+  <si>
+    <t>Min Amplitude</t>
   </si>
 </sst>
 </file>
@@ -981,7 +984,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1542,7 +1545,7 @@
   <dimension ref="A1:E1073"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9213,10 +9216,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:G1072"/>
+  <dimension ref="A1:H1072"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9228,9 +9231,10 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="14.21875" customWidth="1"/>
     <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -9252,18 +9256,23 @@
       <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -9282,8 +9291,9 @@
       <c r="G4" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -9302,8 +9312,9 @@
       <c r="G5" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -9322,8 +9333,9 @@
       <c r="G6" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -9342,8 +9354,9 @@
       <c r="G7" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -9362,8 +9375,9 @@
       <c r="G8" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -9382,8 +9396,9 @@
       <c r="G9" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -9403,8 +9418,9 @@
       <c r="G10" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -9424,8 +9440,9 @@
       <c r="G11" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -9445,8 +9462,9 @@
       <c r="G12" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -9466,8 +9484,9 @@
       <c r="G13" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -9487,8 +9506,9 @@
       <c r="G14" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -9508,8 +9528,9 @@
       <c r="G15" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -9529,8 +9550,9 @@
       <c r="G16" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -9550,8 +9572,9 @@
       <c r="G17" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -9570,8 +9593,9 @@
       <c r="G18" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -9590,8 +9614,9 @@
       <c r="G19" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -9610,8 +9635,9 @@
       <c r="G20" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -9630,8 +9656,9 @@
       <c r="G21" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -9650,8 +9677,9 @@
       <c r="G22" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -9670,8 +9698,9 @@
       <c r="G23" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -9690,8 +9719,9 @@
       <c r="G24" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -9710,8 +9740,9 @@
       <c r="G25" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -9730,8 +9761,9 @@
       <c r="G26" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -9750,8 +9782,9 @@
       <c r="G27" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -9770,8 +9803,9 @@
       <c r="G28" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -9790,8 +9824,9 @@
       <c r="G29" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -9810,8 +9845,9 @@
       <c r="G30" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -9830,10 +9866,31 @@
       <c r="G31" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" s="7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="33" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
@@ -10911,7 +10968,7 @@
           <x14:formula1>
             <xm:f>Survey!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1011:E1048576 D1:D9 D28:D1048576 D14:D23</xm:sqref>
+          <xm:sqref>E1011:E1048576 D1:D9 D14:D23 D28:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -10923,19 +10980,19 @@
           <x14:formula1>
             <xm:f>Survey!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E9 E28:E1010 E14:E23</xm:sqref>
+          <xm:sqref>E1:E9 E14:E23 E28:E1010</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$D$2:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G9 G28:G1048576 G14:G23</xm:sqref>
+          <xm:sqref>G14:G23 G28:G1048576 G1:G9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F9 F28:F1048576 F14:F23</xm:sqref>
+          <xm:sqref>F1:F9 F14:F23 F28:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updated admin username/passed in excelsheet
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="159">
   <si>
     <t>Enabled</t>
   </si>
@@ -189,12 +189,6 @@
     <t>sqa#Picarro$0</t>
   </si>
   <si>
-    <t>Administrator</t>
-  </si>
-  <si>
-    <t>FastLane!911</t>
-  </si>
-  <si>
     <t>RowID</t>
   </si>
   <si>
@@ -613,6 +607,12 @@
   </si>
   <si>
     <t>Surveyor_Assessment.db3</t>
+  </si>
+  <si>
+    <t>Min Amplitude</t>
+  </si>
+  <si>
+    <t>AutomationAdmin</t>
   </si>
 </sst>
 </file>
@@ -980,8 +980,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,7 +994,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1099,10 +1099,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>158</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
@@ -1116,7 +1116,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
@@ -1133,7 +1133,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
@@ -1150,7 +1150,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
@@ -1220,7 +1220,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1228,7 +1228,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1236,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1263,74 +1263,74 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1358,75 +1358,75 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1450,10 +1450,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1464,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -1475,7 +1475,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -1486,7 +1486,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -1497,7 +1497,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -1542,7 +1542,7 @@
   <dimension ref="A1:E1073"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1555,19 +1555,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1575,16 +1575,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1592,16 +1592,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1609,16 +1609,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1626,16 +1626,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1643,16 +1643,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1660,16 +1660,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1677,16 +1677,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1694,16 +1694,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1711,16 +1711,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1728,16 +1728,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1745,16 +1745,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>148</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1762,16 +1762,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1779,16 +1779,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>148</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -9213,10 +9213,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:G1072"/>
+  <dimension ref="A1:H1072"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9228,612 +9228,666 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="14.21875" customWidth="1"/>
     <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32" s="7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="33" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
@@ -10911,7 +10965,7 @@
           <x14:formula1>
             <xm:f>Survey!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1011:E1048576 D1:D9 D28:D1048576 D14:D23</xm:sqref>
+          <xm:sqref>E1011:E1048576 D1:D9 D14:D23 D28:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -10923,19 +10977,19 @@
           <x14:formula1>
             <xm:f>Survey!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E9 E28:E1010 E14:E23</xm:sqref>
+          <xm:sqref>E1:E9 E14:E23 E28:E1010</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$D$2:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G9 G28:G1048576 G14:G23</xm:sqref>
+          <xm:sqref>G14:G23 G28:G1048576 G1:G9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F9 F28:F1048576 F14:F23</xm:sqref>
+          <xm:sqref>F1:F9 F14:F23 F28:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10985,85 +11039,85 @@
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="S1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="Y1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -11071,13 +11125,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E2" s="2">
         <v>3</v>
@@ -11095,13 +11149,13 @@
         <v>-122.04883575439401</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P2" s="4">
         <v>42294.500011574077</v>
@@ -11110,7 +11164,7 @@
         <v>42010.500011574077</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="S2" s="2" t="b">
         <v>0</v>
@@ -11119,10 +11173,10 @@
         <v>1</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="W2" s="2">
         <v>8.5</v>
@@ -11131,7 +11185,7 @@
         <v>11</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Z2" s="2">
         <v>1</v>
@@ -11145,22 +11199,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="P3" s="4">
         <v>42344.500011574077</v>
@@ -11169,7 +11223,7 @@
         <v>42010.500011574077</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="W3" s="2">
         <v>8.5</v>
@@ -11178,7 +11232,7 @@
         <v>11</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Z3" s="2">
         <v>5</v>
@@ -11192,13 +11246,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G4" s="2">
         <v>37.435339792682498</v>
@@ -11215,7 +11269,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P4" s="4">
         <v>42294.500011574077</v>
@@ -11224,7 +11278,7 @@
         <v>42010.500011574077</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="S4" s="2" t="b">
         <v>0</v>
@@ -11233,10 +11287,10 @@
         <v>2</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="W4" s="2">
         <v>8.5</v>
@@ -11245,7 +11299,7 @@
         <v>11</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Z4" s="2">
         <v>1</v>
@@ -12456,46 +12510,46 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12503,7 +12557,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -12536,10 +12590,10 @@
         <v>0</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12547,7 +12601,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -12580,10 +12634,10 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12591,7 +12645,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -12624,10 +12678,10 @@
         <v>0</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12635,7 +12689,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -12668,10 +12722,10 @@
         <v>0</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12679,7 +12733,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -12712,7 +12766,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12720,7 +12774,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
@@ -12753,7 +12807,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12761,7 +12815,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
@@ -12794,7 +12848,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12802,7 +12856,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
@@ -12835,7 +12889,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -13677,34 +13731,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -13736,7 +13790,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -13768,7 +13822,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -13800,7 +13854,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -13832,7 +13886,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14633,28 +14687,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14680,7 +14734,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14706,7 +14760,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14732,7 +14786,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14758,7 +14812,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14784,7 +14838,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
US2079 - Test cases for Observer view
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="161">
   <si>
     <t>Enabled</t>
   </si>
@@ -189,12 +189,6 @@
     <t>sqa#Picarro$0</t>
   </si>
   <si>
-    <t>Administrator</t>
-  </si>
-  <si>
-    <t>FastLane!911</t>
-  </si>
-  <si>
     <t>RowID</t>
   </si>
   <si>
@@ -616,6 +610,15 @@
   </si>
   <si>
     <t>Min Amplitude</t>
+  </si>
+  <si>
+    <t>AutomationAdmin</t>
+  </si>
+  <si>
+    <t>Surveyor-operator-1.db3</t>
+  </si>
+  <si>
+    <t>Surveyor-operator-2.db3</t>
   </si>
 </sst>
 </file>
@@ -984,7 +987,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,7 +1000,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1102,10 +1105,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>158</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
@@ -1119,7 +1122,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
@@ -1136,7 +1139,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
@@ -1153,7 +1156,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
@@ -1223,7 +1226,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1231,7 +1234,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1239,7 +1242,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1266,74 +1269,74 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1361,75 +1364,75 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1453,10 +1456,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1467,7 +1470,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -1478,7 +1481,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -1489,7 +1492,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -1500,7 +1503,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -1542,10 +1545,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1073"/>
+  <dimension ref="A1:E1069"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1558,19 +1561,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1578,16 +1581,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1595,16 +1598,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1612,16 +1615,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1629,16 +1632,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1646,16 +1649,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1663,16 +1666,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1680,16 +1683,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1697,16 +1700,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1714,16 +1717,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1731,16 +1734,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1748,16 +1751,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>148</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1765,16 +1768,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1782,66 +1785,136 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>148</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
@@ -9145,32 +9218,32 @@
       <c r="E1064" s="2"/>
     </row>
     <row r="1065" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1065" s="2"/>
-      <c r="B1065" s="2"/>
-      <c r="C1065" s="2"/>
-      <c r="D1065" s="2"/>
-      <c r="E1065" s="2"/>
+      <c r="A1065" s="5"/>
+      <c r="B1065" s="5"/>
+      <c r="C1065" s="5"/>
+      <c r="D1065" s="5"/>
+      <c r="E1065" s="5"/>
     </row>
     <row r="1066" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1066" s="2"/>
-      <c r="B1066" s="2"/>
-      <c r="C1066" s="2"/>
-      <c r="D1066" s="2"/>
-      <c r="E1066" s="2"/>
+      <c r="A1066" s="5"/>
+      <c r="B1066" s="5"/>
+      <c r="C1066" s="5"/>
+      <c r="D1066" s="5"/>
+      <c r="E1066" s="5"/>
     </row>
     <row r="1067" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1067" s="2"/>
-      <c r="B1067" s="2"/>
-      <c r="C1067" s="2"/>
-      <c r="D1067" s="2"/>
-      <c r="E1067" s="2"/>
+      <c r="A1067" s="5"/>
+      <c r="B1067" s="5"/>
+      <c r="C1067" s="5"/>
+      <c r="D1067" s="5"/>
+      <c r="E1067" s="5"/>
     </row>
     <row r="1068" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1068" s="2"/>
-      <c r="B1068" s="2"/>
-      <c r="C1068" s="2"/>
-      <c r="D1068" s="2"/>
-      <c r="E1068" s="2"/>
+      <c r="A1068" s="5"/>
+      <c r="B1068" s="5"/>
+      <c r="C1068" s="5"/>
+      <c r="D1068" s="5"/>
+      <c r="E1068" s="5"/>
     </row>
     <row r="1069" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1069" s="5"/>
@@ -9178,34 +9251,6 @@
       <c r="C1069" s="5"/>
       <c r="D1069" s="5"/>
       <c r="E1069" s="5"/>
-    </row>
-    <row r="1070" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1070" s="5"/>
-      <c r="B1070" s="5"/>
-      <c r="C1070" s="5"/>
-      <c r="D1070" s="5"/>
-      <c r="E1070" s="5"/>
-    </row>
-    <row r="1071" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1071" s="5"/>
-      <c r="B1071" s="5"/>
-      <c r="C1071" s="5"/>
-      <c r="D1071" s="5"/>
-      <c r="E1071" s="5"/>
-    </row>
-    <row r="1072" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1072" s="5"/>
-      <c r="B1072" s="5"/>
-      <c r="C1072" s="5"/>
-      <c r="D1072" s="5"/>
-      <c r="E1072" s="5"/>
-    </row>
-    <row r="1073" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1073" s="5"/>
-      <c r="B1073" s="5"/>
-      <c r="C1073" s="5"/>
-      <c r="D1073" s="5"/>
-      <c r="E1073" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9219,7 +9264,7 @@
   <dimension ref="A1:H1072"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9236,28 +9281,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -9277,19 +9322,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H4" s="7"/>
     </row>
@@ -9298,19 +9343,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H5" s="7"/>
     </row>
@@ -9319,19 +9364,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -9340,19 +9385,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="H7" s="7"/>
     </row>
@@ -9361,19 +9406,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H8" s="7"/>
     </row>
@@ -9382,19 +9427,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H9" s="7"/>
     </row>
@@ -9403,20 +9448,20 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H10" s="7"/>
     </row>
@@ -9425,20 +9470,20 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H11" s="7"/>
     </row>
@@ -9447,20 +9492,20 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H12" s="7"/>
     </row>
@@ -9469,20 +9514,20 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H13" s="7"/>
     </row>
@@ -9491,20 +9536,20 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="H14" s="7"/>
     </row>
@@ -9513,20 +9558,20 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="H15" s="7"/>
     </row>
@@ -9535,20 +9580,20 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="H16" s="7"/>
     </row>
@@ -9557,20 +9602,20 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H17" s="7"/>
     </row>
@@ -9579,19 +9624,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="H18" s="7"/>
     </row>
@@ -9600,19 +9645,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H19" s="7"/>
     </row>
@@ -9621,19 +9666,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="H20" s="7"/>
     </row>
@@ -9642,19 +9687,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="H21" s="7"/>
     </row>
@@ -9663,19 +9708,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="H22" s="7"/>
     </row>
@@ -9684,19 +9729,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H23" s="7"/>
     </row>
@@ -9705,19 +9750,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H24" s="7"/>
     </row>
@@ -9726,19 +9771,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H25" s="7"/>
     </row>
@@ -9747,19 +9792,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H26" s="7"/>
     </row>
@@ -9768,19 +9813,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H27" s="7"/>
     </row>
@@ -9789,19 +9834,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H28" s="7"/>
     </row>
@@ -9810,19 +9855,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H29" s="7"/>
     </row>
@@ -9831,19 +9876,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H30" s="7"/>
     </row>
@@ -9852,19 +9897,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="H31" s="7"/>
     </row>
@@ -9873,23 +9918,23 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H32" s="7">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -11042,85 +11087,85 @@
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="S1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="Y1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -11128,13 +11173,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E2" s="2">
         <v>3</v>
@@ -11152,13 +11197,13 @@
         <v>-122.04883575439401</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P2" s="4">
         <v>42294.500011574077</v>
@@ -11167,7 +11212,7 @@
         <v>42010.500011574077</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="S2" s="2" t="b">
         <v>0</v>
@@ -11176,10 +11221,10 @@
         <v>1</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="W2" s="2">
         <v>8.5</v>
@@ -11188,7 +11233,7 @@
         <v>11</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Z2" s="2">
         <v>1</v>
@@ -11202,22 +11247,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="P3" s="4">
         <v>42344.500011574077</v>
@@ -11226,7 +11271,7 @@
         <v>42010.500011574077</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="W3" s="2">
         <v>8.5</v>
@@ -11235,7 +11280,7 @@
         <v>11</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Z3" s="2">
         <v>5</v>
@@ -11249,13 +11294,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G4" s="2">
         <v>37.435339792682498</v>
@@ -11272,7 +11317,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P4" s="4">
         <v>42294.500011574077</v>
@@ -11281,7 +11326,7 @@
         <v>42010.500011574077</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="S4" s="2" t="b">
         <v>0</v>
@@ -11290,10 +11335,10 @@
         <v>2</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="W4" s="2">
         <v>8.5</v>
@@ -11302,7 +11347,7 @@
         <v>11</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Z4" s="2">
         <v>1</v>
@@ -12513,46 +12558,46 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12560,7 +12605,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -12593,10 +12638,10 @@
         <v>0</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12604,7 +12649,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -12637,10 +12682,10 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12648,7 +12693,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -12681,10 +12726,10 @@
         <v>0</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12692,7 +12737,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -12725,10 +12770,10 @@
         <v>0</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12736,7 +12781,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -12769,7 +12814,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12777,7 +12822,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
@@ -12810,7 +12855,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12818,7 +12863,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
@@ -12851,7 +12896,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12859,7 +12904,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
@@ -12892,7 +12937,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -13734,34 +13779,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -13793,7 +13838,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -13825,7 +13870,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -13857,7 +13902,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -13889,7 +13934,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14690,28 +14735,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14737,7 +14782,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14763,7 +14808,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14789,7 +14834,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14815,7 +14860,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14841,7 +14886,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added Driver View Test Cases
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="161">
   <si>
     <t>Enabled</t>
   </si>
@@ -986,7 +986,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -9263,8 +9263,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H1072"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9937,25 +9937,82 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-    </row>
-    <row r="34" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:2" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="49" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="50" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="51" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -11008,36 +11065,66 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1011:E1048576 D1:D9 D14:D23 D28:D1048576</xm:sqref>
+          <xm:sqref>E1011:E1048576 D1:D9 D14:D23 D28:D32 D36:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C9 C14:C23 C28:C1048576</xm:sqref>
+          <xm:sqref>C1:C9 C14:C23 C28:C32 C36:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$C$2:$C$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E9 E14:E23 E28:E1010</xm:sqref>
+          <xm:sqref>E1:E9 E14:E23 E28:E32 E36:E1010</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$D$2:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G14:G23 G28:G1048576 G1:G9</xm:sqref>
+          <xm:sqref>G14:G23 G1:G9 G28:G32 G36:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Survey!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F9 F14:F23 F28:F1048576</xm:sqref>
+          <xm:sqref>F1:F9 F14:F23 F28:F32 F36:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Survey!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>F33:F35</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Survey!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>G33:G35</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Survey!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E33:E35</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Survey!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>C33:C35</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Survey!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D33:D35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Converted copy compliance reports to take input data externally. Added method for perf metric comparison
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -104,7 +104,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Change customer
+          <t xml:space="preserve">Actual values need to be changed once test has access to ProdSTG Scale environment
 </t>
         </r>
         <r>
@@ -139,7 +139,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Change customer</t>
+Actual values need to be changed once test has access to ProdSTG Scale environment</t>
         </r>
       </text>
     </comment>
@@ -163,7 +163,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Change customer</t>
+Actual values need to be changed once test has access to ProdSTG Scale environment</t>
         </r>
       </text>
     </comment>
@@ -187,7 +187,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Change customer</t>
+Actual values need to be changed once test has access to ProdSTG Scale environment</t>
         </r>
       </text>
     </comment>
@@ -855,16 +855,7 @@
     <t>GenerateRandomString(20)</t>
   </si>
   <si>
-    <t>PerfTest1</t>
-  </si>
-  <si>
-    <t>PerfTest2</t>
-  </si>
-  <si>
     <t>PerfTest3</t>
-  </si>
-  <si>
-    <t>PerfTest4</t>
   </si>
   <si>
     <t>TC180</t>
@@ -877,6 +868,15 @@
   </si>
   <si>
     <t>Indication, Isotopic Analysis=TRUE. All other FALSE</t>
+  </si>
+  <si>
+    <t>PerfTest6</t>
+  </si>
+  <si>
+    <t>PerfTest8</t>
+  </si>
+  <si>
+    <t>PerfTest10</t>
   </si>
 </sst>
 </file>
@@ -2854,7 +2854,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -13549,8 +13549,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2828"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13915,7 +13915,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>198</v>
@@ -13971,7 +13971,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>198</v>
@@ -14030,7 +14030,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>198</v>
@@ -14086,7 +14086,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>198</v>
@@ -14202,7 +14202,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>198</v>
@@ -14262,7 +14262,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>198</v>
@@ -14322,7 +14322,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>198</v>
@@ -35478,7 +35478,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Add placeholder test case data and baselines for perf tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -855,9 +855,6 @@
     <t>GenerateRandomString(20)</t>
   </si>
   <si>
-    <t>PerfTest3</t>
-  </si>
-  <si>
     <t>TC180</t>
   </si>
   <si>
@@ -870,13 +867,16 @@
     <t>Indication, Isotopic Analysis=TRUE. All other FALSE</t>
   </si>
   <si>
-    <t>PerfTest6</t>
+    <t>TC1841</t>
   </si>
   <si>
-    <t>PerfTest8</t>
+    <t>TC1842</t>
   </si>
   <si>
-    <t>PerfTest10</t>
+    <t>TC1843</t>
+  </si>
+  <si>
+    <t>TC1844</t>
   </si>
 </sst>
 </file>
@@ -2854,7 +2854,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -11742,7 +11742,7 @@
   <dimension ref="A1:H1072"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="G296" sqref="G296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11793,6 +11793,7 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
+      <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -11811,7 +11812,7 @@
       <c r="E4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H4" s="7"/>
@@ -11832,7 +11833,7 @@
       <c r="E5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H5" s="7"/>
@@ -11853,7 +11854,7 @@
       <c r="E6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="7" t="s">
         <v>42</v>
       </c>
       <c r="H6" s="7"/>
@@ -11874,7 +11875,7 @@
       <c r="E7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H7" s="7"/>
@@ -11895,7 +11896,7 @@
       <c r="F8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H8" s="7"/>
@@ -11916,7 +11917,7 @@
       <c r="E9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="7" t="s">
         <v>41</v>
       </c>
       <c r="H9" s="7"/>
@@ -12113,7 +12114,7 @@
       <c r="E18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H18" s="7"/>
@@ -12134,7 +12135,7 @@
       <c r="F19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H19" s="7"/>
@@ -12155,7 +12156,7 @@
       <c r="E20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H20" s="7"/>
@@ -12176,7 +12177,7 @@
       <c r="E21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H21" s="7"/>
@@ -12197,7 +12198,7 @@
       <c r="E22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H22" s="7"/>
@@ -12218,7 +12219,7 @@
       <c r="F23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H23" s="7"/>
@@ -12239,7 +12240,7 @@
       <c r="E24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H24" s="7"/>
@@ -12260,7 +12261,7 @@
       <c r="E25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H25" s="7"/>
@@ -12281,7 +12282,7 @@
       <c r="E26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="7" t="s">
         <v>41</v>
       </c>
       <c r="H26" s="7"/>
@@ -12302,7 +12303,7 @@
       <c r="F27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" s="7" t="s">
         <v>41</v>
       </c>
       <c r="H27" s="7"/>
@@ -12323,7 +12324,7 @@
       <c r="E28" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="7" t="s">
         <v>41</v>
       </c>
       <c r="H28" s="7"/>
@@ -12344,7 +12345,7 @@
       <c r="E29" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="7" t="s">
         <v>41</v>
       </c>
       <c r="H29" s="7"/>
@@ -12365,7 +12366,7 @@
       <c r="E30" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="7" t="s">
         <v>41</v>
       </c>
       <c r="H30" s="7"/>
@@ -12386,7 +12387,7 @@
       <c r="E31" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H31" s="7"/>
@@ -13541,6 +13542,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Survey!$D$2:$D$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G41</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -13550,13 +13563,13 @@
   <dimension ref="A1:V2828"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.44140625" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
@@ -13915,7 +13928,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>198</v>
@@ -13971,7 +13984,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>198</v>
@@ -14030,7 +14043,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>198</v>
@@ -14086,7 +14099,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>198</v>
@@ -14142,7 +14155,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>198</v>
@@ -35478,7 +35491,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Added checks for report job status. Used encrypted passwords in test case data sheet
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -43,6 +43,67 @@
     <author>Shirish Pulikkal</author>
   </authors>
   <commentList>
+    <comment ref="B7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This user is the Picarro admin user for automation tests.
+For performance tests we have another Picarro admin user (rowId=10)
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Shirish Pulikkal:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">This user is used in Performance test (Do NOT use for normal automation test)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Shirish Pulikkal</author>
+  </authors>
+  <commentList>
     <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
@@ -78,7 +139,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Shirish Pulikkal</author>
@@ -205,7 +266,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Shirish Pulikkal</author>
@@ -266,7 +327,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="238">
   <si>
     <t>Enabled</t>
   </si>
@@ -314,9 +375,6 @@
   </si>
   <si>
     <t>sqapicsu1@picarro.com</t>
-  </si>
-  <si>
-    <t>sqa#Picarro$0</t>
   </si>
   <si>
     <t>RowID</t>
@@ -978,6 +1036,12 @@
   <si>
     <t>Centerpoint</t>
   </si>
+  <si>
+    <t>sB9eb3LaNTshd69vgXEaJw==</t>
+  </si>
+  <si>
+    <t>oeHwHqmv621dZ1MRE2BSdw==</t>
+  </si>
 </sst>
 </file>
 
@@ -1508,19 +1572,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
     <col min="5" max="5" width="18.88671875" customWidth="1"/>
     <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
@@ -1534,7 +1598,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1549,25 +1613,25 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -1578,7 +1642,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>237</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
@@ -1587,16 +1651,16 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="K2" s="2">
         <v>2</v>
@@ -1612,8 +1676,8 @@
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
+      <c r="C3" s="7" t="s">
+        <v>237</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>1</v>
@@ -1622,17 +1686,17 @@
         <v>9</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="K3" s="2">
         <v>2</v>
@@ -1648,8 +1712,8 @@
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
+      <c r="C4" s="7" t="s">
+        <v>237</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>1</v>
@@ -1658,17 +1722,17 @@
         <v>8</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="K4" s="2">
         <v>2</v>
@@ -1684,8 +1748,8 @@
       <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
+      <c r="C5" s="7" t="s">
+        <v>237</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>1</v>
@@ -1694,17 +1758,17 @@
         <v>10</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="K5" s="2">
         <v>1</v>
@@ -1720,8 +1784,8 @@
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
+      <c r="C6" s="7" t="s">
+        <v>237</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>1</v>
@@ -1733,10 +1797,10 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
@@ -1750,10 +1814,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>16</v>
+        <v>237</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
@@ -1762,17 +1826,17 @@
         <v>10</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
@@ -1786,10 +1850,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>237</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>1</v>
@@ -1801,10 +1865,10 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="K8" s="2">
         <v>4</v>
@@ -1818,10 +1882,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>148</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>237</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>1</v>
@@ -1833,10 +1897,10 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="K9" s="2">
         <v>4</v>
@@ -1850,10 +1914,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>149</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>237</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>1</v>
@@ -1865,10 +1929,10 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="K10" s="2">
         <v>4</v>
@@ -1877,7 +1941,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:12" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="D11" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="K11" s="7">
+        <v>1</v>
+      </c>
+      <c r="L11" s="7">
+        <v>1</v>
+      </c>
+    </row>
     <row r="12" spans="1:12" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:12" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:12" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1895,6 +1994,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1941,34 +2041,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -2000,7 +2100,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -2032,7 +2132,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -2064,7 +2164,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -2096,7 +2196,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -2157,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -2928,28 +3028,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -2975,7 +3075,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3001,7 +3101,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3027,7 +3127,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3053,7 +3153,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3079,7 +3179,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3105,7 +3205,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3131,7 +3231,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3157,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -3812,7 +3912,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3820,7 +3920,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -3828,7 +3928,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3855,74 +3955,74 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -3950,78 +4050,78 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
         <v>56</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -4046,16 +4146,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4063,7 +4163,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C2" s="7">
         <v>37.402092570550302</v>
@@ -4077,7 +4177,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" s="7">
         <v>37.402092570550302</v>
@@ -4091,7 +4191,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C4" s="7">
         <v>37.402092570550302</v>
@@ -4137,19 +4237,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -4157,13 +4257,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -4171,13 +4271,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -4185,13 +4285,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -4199,13 +4299,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -4213,13 +4313,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -4272,10 +4372,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -4283,7 +4383,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -4291,7 +4391,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4299,7 +4399,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4307,7 +4407,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4315,7 +4415,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4323,7 +4423,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -4331,7 +4431,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -4357,19 +4457,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -4377,16 +4477,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -4394,16 +4494,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -4411,16 +4511,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -4428,16 +4528,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -4445,16 +4545,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -4462,16 +4562,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -4479,16 +4579,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -4496,16 +4596,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -4513,16 +4613,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -4530,16 +4630,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>143</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -4547,16 +4647,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -4564,16 +4664,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>143</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -4581,16 +4681,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -4598,16 +4698,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -4615,16 +4715,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -4632,16 +4732,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -4649,16 +4749,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -4666,16 +4766,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -4683,16 +4783,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -4700,16 +4800,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -12077,28 +12177,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12119,19 +12219,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="7"/>
     </row>
@@ -12140,19 +12240,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="H5" s="7"/>
     </row>
@@ -12161,19 +12261,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -12182,19 +12282,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="7"/>
     </row>
@@ -12203,19 +12303,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="H8" s="7"/>
     </row>
@@ -12224,19 +12324,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H9" s="7"/>
     </row>
@@ -12245,20 +12345,20 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" s="7"/>
     </row>
@@ -12267,20 +12367,20 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" s="7"/>
     </row>
@@ -12289,20 +12389,20 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12" s="7"/>
     </row>
@@ -12311,20 +12411,20 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" s="7"/>
     </row>
@@ -12333,20 +12433,20 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H14" s="7"/>
     </row>
@@ -12355,20 +12455,20 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H15" s="7"/>
     </row>
@@ -12377,20 +12477,20 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H16" s="7"/>
     </row>
@@ -12399,20 +12499,20 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="H17" s="7"/>
     </row>
@@ -12421,19 +12521,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="G18" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="H18" s="7"/>
     </row>
@@ -12442,19 +12542,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H19" s="7"/>
     </row>
@@ -12463,19 +12563,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H20" s="7"/>
     </row>
@@ -12484,19 +12584,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H21" s="7"/>
     </row>
@@ -12505,19 +12605,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H22" s="7"/>
     </row>
@@ -12526,19 +12626,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H23" s="7"/>
     </row>
@@ -12547,19 +12647,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="H24" s="7"/>
     </row>
@@ -12568,19 +12668,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H25" s="7"/>
     </row>
@@ -12589,19 +12689,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H26" s="7"/>
     </row>
@@ -12610,19 +12710,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="H27" s="7"/>
     </row>
@@ -12631,19 +12731,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H28" s="7"/>
     </row>
@@ -12652,19 +12752,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H29" s="7"/>
     </row>
@@ -12673,19 +12773,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H30" s="7"/>
     </row>
@@ -12694,19 +12794,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>47</v>
       </c>
       <c r="H31" s="7"/>
     </row>
@@ -12715,20 +12815,20 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H32" s="7">
         <v>0.1</v>
@@ -12739,20 +12839,20 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C33" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12760,20 +12860,20 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12781,20 +12881,20 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -13912,70 +14012,70 @@
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="O1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="S1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -13984,13 +14084,13 @@
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" s="2">
         <v>3</v>
@@ -14009,10 +14109,10 @@
         <v>-122.04883575439401</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q2" s="2">
         <v>8.5</v>
@@ -14021,7 +14121,7 @@
         <v>11</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T2" s="2">
         <v>1</v>
@@ -14030,7 +14130,7 @@
         <v>4</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14039,23 +14139,23 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="H3" s="7"/>
       <c r="M3" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q3" s="2">
         <v>8.5</v>
@@ -14064,7 +14164,7 @@
         <v>11</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="T3" s="2">
         <v>5</v>
@@ -14073,7 +14173,7 @@
         <v>2</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14082,13 +14182,13 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="2">
@@ -14105,10 +14205,10 @@
       </c>
       <c r="M4" s="7"/>
       <c r="O4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q4" s="2">
         <v>8.5</v>
@@ -14117,7 +14217,7 @@
         <v>11</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="T4" s="2">
         <v>1</v>
@@ -14126,7 +14226,7 @@
         <v>4</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14134,22 +14234,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="2">
@@ -14165,7 +14265,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q5" s="7">
         <v>8.5</v>
@@ -14191,22 +14291,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="7">
         <v>0</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I6" s="7">
         <v>37.4206</v>
@@ -14221,7 +14321,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q6" s="7">
         <v>8.5</v>
@@ -14247,22 +14347,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" s="7">
         <v>0</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7" s="7">
         <v>37.4206</v>
@@ -14277,7 +14377,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q7" s="7">
         <v>8.5</v>
@@ -14303,22 +14403,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F8" s="7">
         <v>0</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H8" s="7">
         <v>0.1</v>
@@ -14336,7 +14436,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q8" s="7">
         <v>8.5</v>
@@ -14362,22 +14462,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" s="7">
         <v>0</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I9" s="7">
         <v>37.4206</v>
@@ -14392,7 +14492,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q9" s="7">
         <v>8.5</v>
@@ -14418,22 +14518,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" s="7">
         <v>0</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I10" s="7">
         <v>37.4206</v>
@@ -14448,7 +14548,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q10" s="7">
         <v>8.5</v>
@@ -14474,22 +14574,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D11" s="7">
         <v>5</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="7">
         <v>0</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7">
@@ -14532,22 +14632,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D12" s="7">
         <v>5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" s="7">
         <v>0</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7">
@@ -14582,7 +14682,7 @@
         <v>8</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14590,22 +14690,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" s="7">
         <v>5</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" s="7">
         <v>0</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -14613,10 +14713,10 @@
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="N13" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>208</v>
       </c>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
@@ -14627,7 +14727,7 @@
         <v>11</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="T13" s="7">
         <v>6</v>
@@ -14636,7 +14736,7 @@
         <v>1</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14644,22 +14744,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D14" s="7">
         <v>5</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" s="7">
         <v>0</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -14667,10 +14767,10 @@
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="N14" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>208</v>
       </c>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
@@ -24691,31 +24791,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -24723,13 +24823,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E2" s="4">
         <v>42294.500011574077</v>
@@ -24738,7 +24838,7 @@
         <v>42010.500011574077</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="7" t="b">
         <v>0</v>
@@ -24761,7 +24861,7 @@
         <v>42010.500011574077</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -24773,7 +24873,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E4" s="4">
         <v>42294.500011574077</v>
@@ -24782,7 +24882,7 @@
         <v>42010.500011574077</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="7" t="b">
         <v>0</v>
@@ -24798,12 +24898,12 @@
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7">
@@ -24817,7 +24917,7 @@
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -24834,7 +24934,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -24851,7 +24951,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -24868,7 +24968,7 @@
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -24885,7 +24985,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -24902,7 +25002,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -24919,7 +25019,7 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -24936,7 +25036,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -24953,7 +25053,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -24970,7 +25070,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -24987,7 +25087,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -25004,7 +25104,7 @@
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -25021,7 +25121,7 @@
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -25038,7 +25138,7 @@
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -25055,7 +25155,7 @@
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -25072,7 +25172,7 @@
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -25089,7 +25189,7 @@
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -25106,7 +25206,7 @@
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -36317,46 +36417,46 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36364,7 +36464,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -36397,10 +36497,10 @@
         <v>0</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36408,7 +36508,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -36441,10 +36541,10 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36452,7 +36552,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -36485,10 +36585,10 @@
         <v>0</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36496,7 +36596,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -36529,10 +36629,10 @@
         <v>0</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36540,7 +36640,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -36573,7 +36673,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36581,7 +36681,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
@@ -36614,7 +36714,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36622,7 +36722,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
@@ -36655,7 +36755,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36663,7 +36763,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
@@ -36696,7 +36796,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36704,7 +36804,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>
@@ -36737,10 +36837,10 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36748,7 +36848,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>1</v>
@@ -36781,10 +36881,10 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36792,7 +36892,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>1</v>
@@ -36825,10 +36925,10 @@
         <v>0</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36836,7 +36936,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>1</v>
@@ -36869,10 +36969,10 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36880,7 +36980,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>1</v>
@@ -36913,10 +37013,10 @@
         <v>0</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add support for assets/boundaries specific to customer
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -21,12 +21,14 @@
     <sheet name="Compliance Report Test Data" sheetId="2" r:id="rId7"/>
     <sheet name="Report Survey Data" sheetId="16" r:id="rId8"/>
     <sheet name="Report Views Data" sheetId="11" r:id="rId9"/>
-    <sheet name="Report Opt View Layers" sheetId="13" r:id="rId10"/>
-    <sheet name="Report Opt Tabular PDF Content" sheetId="12" r:id="rId11"/>
-    <sheet name="Roles" sheetId="6" r:id="rId12"/>
-    <sheet name="General" sheetId="7" r:id="rId13"/>
-    <sheet name="Survey" sheetId="9" r:id="rId14"/>
-    <sheet name="Report" sheetId="10" r:id="rId15"/>
+    <sheet name="Report Opt View Layers" sheetId="21" r:id="rId10"/>
+    <sheet name="Report Opt View Layers Assets" sheetId="19" r:id="rId11"/>
+    <sheet name="Report Opt View Layers Boundary" sheetId="20" r:id="rId12"/>
+    <sheet name="Report Opt Tabular PDF Content" sheetId="12" r:id="rId13"/>
+    <sheet name="Roles" sheetId="6" r:id="rId14"/>
+    <sheet name="General" sheetId="7" r:id="rId15"/>
+    <sheet name="Survey" sheetId="9" r:id="rId16"/>
+    <sheet name="Report" sheetId="10" r:id="rId17"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -327,7 +329,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="287">
   <si>
     <t>Enabled</t>
   </si>
@@ -620,34 +622,7 @@
     <t>Report Opt Tabular PDF Content RowID</t>
   </si>
   <si>
-    <t>Asset - Copper</t>
-  </si>
-  <si>
-    <t>Asset - Unprotected Steel</t>
-  </si>
-  <si>
-    <t>Asset - Protected Steel</t>
-  </si>
-  <si>
-    <t>Asset - Cast Iron</t>
-  </si>
-  <si>
-    <t>Asset - Other Plastic</t>
-  </si>
-  <si>
-    <t>Asset - PE Plastic</t>
-  </si>
-  <si>
-    <t>Boundary - District Plat</t>
-  </si>
-  <si>
-    <t>Boundary - District</t>
-  </si>
-  <si>
     <t>NOTES</t>
-  </si>
-  <si>
-    <t>All assets and all boundaries selected</t>
   </si>
   <si>
     <t>Indication Table</t>
@@ -675,12 +650,6 @@
   </si>
   <si>
     <t>All fields selected (except Percent Coverage Forecast, Percent Coverage Report Area, Percent Coverage Assets)</t>
-  </si>
-  <si>
-    <t>All assets selected, boundaries unselected.</t>
-  </si>
-  <si>
-    <t>All boundaries selected, assets unselected</t>
   </si>
   <si>
     <t>GenerateRandomString(10)</t>
@@ -711,9 +680,6 @@
   </si>
   <si>
     <t>sqacus</t>
-  </si>
-  <si>
-    <t>All boundaries and assets unselected</t>
   </si>
   <si>
     <t>Indication, Isotopic Analysis, Gap and Percent Coverage Report Area = TRUE. All other FALSE</t>
@@ -962,63 +928,6 @@
     <t>All TRUE</t>
   </si>
   <si>
-    <t>All FALSE</t>
-  </si>
-  <si>
-    <t>perf-17</t>
-  </si>
-  <si>
-    <t>perf-1</t>
-  </si>
-  <si>
-    <t>perf-2</t>
-  </si>
-  <si>
-    <t>perf-3</t>
-  </si>
-  <si>
-    <t>perf-4</t>
-  </si>
-  <si>
-    <t>perf-5</t>
-  </si>
-  <si>
-    <t>perf-6</t>
-  </si>
-  <si>
-    <t>perf-7</t>
-  </si>
-  <si>
-    <t>perf-8</t>
-  </si>
-  <si>
-    <t>perf-9</t>
-  </si>
-  <si>
-    <t>perf-10</t>
-  </si>
-  <si>
-    <t>perf-11</t>
-  </si>
-  <si>
-    <t>perf-12</t>
-  </si>
-  <si>
-    <t>perf-13</t>
-  </si>
-  <si>
-    <t>perf-14</t>
-  </si>
-  <si>
-    <t>perf-15</t>
-  </si>
-  <si>
-    <t>perf-16</t>
-  </si>
-  <si>
-    <t>perf-18</t>
-  </si>
-  <si>
     <t>Indication, Isotopic Analysis, PCA, PCRA = TRUE</t>
   </si>
   <si>
@@ -1041,6 +950,246 @@
   </si>
   <si>
     <t>oeHwHqmv621dZ1MRE2BSdw==</t>
+  </si>
+  <si>
+    <t>perf1</t>
+  </si>
+  <si>
+    <t>perf2</t>
+  </si>
+  <si>
+    <t>perf3</t>
+  </si>
+  <si>
+    <t>perf4</t>
+  </si>
+  <si>
+    <t>perf5</t>
+  </si>
+  <si>
+    <t>perf6</t>
+  </si>
+  <si>
+    <t>perf7</t>
+  </si>
+  <si>
+    <t>perf8</t>
+  </si>
+  <si>
+    <t>perf9</t>
+  </si>
+  <si>
+    <t>perf10</t>
+  </si>
+  <si>
+    <t>perf11</t>
+  </si>
+  <si>
+    <t>perf12</t>
+  </si>
+  <si>
+    <t>perf13</t>
+  </si>
+  <si>
+    <t>perf14</t>
+  </si>
+  <si>
+    <t>perf15</t>
+  </si>
+  <si>
+    <t>perf16</t>
+  </si>
+  <si>
+    <t>perf17</t>
+  </si>
+  <si>
+    <t>perf18</t>
+  </si>
+  <si>
+    <t>Asset Name</t>
+  </si>
+  <si>
+    <t>Asset ID</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>Copper</t>
+  </si>
+  <si>
+    <t>Cast Iron</t>
+  </si>
+  <si>
+    <t>Protected Steel</t>
+  </si>
+  <si>
+    <t>PE Plastic</t>
+  </si>
+  <si>
+    <t>Other Plastic</t>
+  </si>
+  <si>
+    <t>Plastic</t>
+  </si>
+  <si>
+    <t>Wrought Iron</t>
+  </si>
+  <si>
+    <t>Un-protected Steel</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Tenite</t>
+  </si>
+  <si>
+    <t>5FB149DC-0318-4E53-8E55-252C96634CE9</t>
+  </si>
+  <si>
+    <t>C37AA3CC-F41F-42B9-8C7D-3BEA58F6F495</t>
+  </si>
+  <si>
+    <t>D08FC87F-F979-4131-92A9-3D82F37F4BBA</t>
+  </si>
+  <si>
+    <t>F3955E82-DD13-4842-84F7-502BCDA6B57A</t>
+  </si>
+  <si>
+    <t>9119E94C-B7CB-4E1D-AE92-57DD72CB41F7</t>
+  </si>
+  <si>
+    <t>44353E68-0694-4F05-85CB-84D753EA278C</t>
+  </si>
+  <si>
+    <t>69CEAB1E-77FC-47A2-A774-AE3554939C95</t>
+  </si>
+  <si>
+    <t>50987927-5724-4D0A-BD7E-BD770EBB911C</t>
+  </si>
+  <si>
+    <t>6FC8F1CF-614C-4107-8209-C40569D53100</t>
+  </si>
+  <si>
+    <t>6FC8F1CF-614C-4107-8209-C40569D53193</t>
+  </si>
+  <si>
+    <t>96CAF1F5-D5C5-461D-9CE3-D210C20A1BB0</t>
+  </si>
+  <si>
+    <t>AD701312-C470-482A-BE45-EF37770E2CE6</t>
+  </si>
+  <si>
+    <t>F14735DE-6C9B-4423-8533-F243A7FE4E90</t>
+  </si>
+  <si>
+    <t>1B5BEFF8-2754-44A9-BE1A-0675B6BE4FD1</t>
+  </si>
+  <si>
+    <t>3869C45B-DA8F-4594-A358-301EA70BC0F1</t>
+  </si>
+  <si>
+    <t>FAB1C61C-392F-451A-BB5A-45002DD6AE25</t>
+  </si>
+  <si>
+    <t>8E20654F-CA8A-4041-9DB4-46E8AF369E93</t>
+  </si>
+  <si>
+    <t>ACEF3C6D-49C3-42F0-BD2F-790963571BED</t>
+  </si>
+  <si>
+    <t>980095B1-B316-4357-9179-9A76D4C848FA</t>
+  </si>
+  <si>
+    <t>5CD4D93C-0154-4A4B-A4E8-BE69F5B80D40</t>
+  </si>
+  <si>
+    <t>9DA23FD0-9A41-46D1-9902-F204261005AB</t>
+  </si>
+  <si>
+    <t>Wrought Steel</t>
+  </si>
+  <si>
+    <t>Unset</t>
+  </si>
+  <si>
+    <t>PERF</t>
+  </si>
+  <si>
+    <t>Boundary ID</t>
+  </si>
+  <si>
+    <t>Boundary Name</t>
+  </si>
+  <si>
+    <t>a1a629ba-2003-43d0-9392-b43239f7bf54</t>
+  </si>
+  <si>
+    <t>Small Boundary</t>
+  </si>
+  <si>
+    <t>Big Boundary</t>
+  </si>
+  <si>
+    <t>3BB4B2AE-9591-4607-9CAD-FD2EB377760A</t>
+  </si>
+  <si>
+    <t>B9E69B56-E43E-4F6C-AFB1-24C01C1DD9DC</t>
+  </si>
+  <si>
+    <t>024249AE-374B-4F6F-BD87-E8FDCACB48E1</t>
+  </si>
+  <si>
+    <t>551CB7C0-005B-4E3E-BFAE-D19DA0ED7EFE</t>
+  </si>
+  <si>
+    <t>Boundaries Row IDs</t>
+  </si>
+  <si>
+    <t>Asset Row IDs</t>
+  </si>
+  <si>
+    <t>PICARRO - All assets and all boundaries selected</t>
+  </si>
+  <si>
+    <t>PICARRO - All assets selected, boundaries unselected.</t>
+  </si>
+  <si>
+    <t>PICARRO - All boundaries selected, assets unselected</t>
+  </si>
+  <si>
+    <t>PICARRO - All boundaries and assets unselected</t>
+  </si>
+  <si>
+    <t>PICARRO - All assets and boundaries FALSE</t>
+  </si>
+  <si>
+    <t>8,9,10,11,12,13</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>PICARRO - Asset (Copper, Cast Iron, Protected, Unprotected Steel)</t>
+  </si>
+  <si>
+    <t>8,9,12,13</t>
+  </si>
+  <si>
+    <t>CENTERPOINT - All assets and all boundaries selected</t>
+  </si>
+  <si>
+    <t>14,15,16,17,18,19,20,21</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1414,7 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1282,6 +1431,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1576,8 +1743,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1613,22 +1780,22 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>48</v>
@@ -1642,7 +1809,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
@@ -1651,16 +1818,16 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="K2" s="2">
         <v>2</v>
@@ -1677,7 +1844,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>1</v>
@@ -1686,17 +1853,17 @@
         <v>9</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="K3" s="2">
         <v>2</v>
@@ -1713,7 +1880,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>1</v>
@@ -1722,17 +1889,17 @@
         <v>8</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="K4" s="2">
         <v>2</v>
@@ -1749,7 +1916,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>1</v>
@@ -1758,17 +1925,17 @@
         <v>10</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="K5" s="2">
         <v>1</v>
@@ -1785,7 +1952,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>1</v>
@@ -1797,10 +1964,10 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
@@ -1814,10 +1981,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
@@ -1826,17 +1993,17 @@
         <v>10</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
@@ -1850,10 +2017,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>1</v>
@@ -1865,10 +2032,10 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="K8" s="2">
         <v>4</v>
@@ -1882,10 +2049,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>1</v>
@@ -1897,10 +2064,10 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="K9" s="2">
         <v>4</v>
@@ -1914,10 +2081,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>1</v>
@@ -1929,10 +2096,10 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="K10" s="2">
         <v>4</v>
@@ -1946,10 +2113,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="D11" s="7" t="b">
         <v>1</v>
@@ -1958,17 +2125,17 @@
         <v>10</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="K11" s="7">
         <v>1</v>
@@ -2018,994 +2185,648 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:J735"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>274</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>273</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="B2" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="B3" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="7" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="B4" s="7"/>
+      <c r="C4" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="B5" s="7"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="B6" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:10" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="17" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="18" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="19" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="20" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="21" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="23" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="24" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="25" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="26" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="28" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="30" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="31" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="32" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="33" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="34" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="35" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="36" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="37" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="38" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="39" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="40" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="41" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="42" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="43" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="44" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="45" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="46" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="47" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="48" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="49" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="50" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="51" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="52" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="53" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="54" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="55" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="56" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="57" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="58" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="59" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="60" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="61" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="62" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="63" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="64" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="65" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="66" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="67" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="68" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="69" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="70" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="71" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="72" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="73" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="74" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="75" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="76" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="77" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="78" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="79" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="80" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="81" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="82" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="83" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="84" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="85" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="86" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="87" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="88" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="89" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="90" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="91" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="92" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="93" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="94" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="95" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="96" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="97" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="98" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="99" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="100" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="101" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="102" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="103" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="104" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="105" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="106" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="107" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="108" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="109" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="110" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="111" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="112" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="113" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="114" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="115" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="116" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="117" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="118" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="119" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="120" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="121" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="122" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="123" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="124" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="125" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="126" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="127" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="128" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="129" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="130" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="131" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="132" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="133" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="134" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="135" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="136" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="137" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="138" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="139" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="140" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="141" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="142" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="143" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="144" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="145" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="146" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="147" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="148" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="149" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="150" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="151" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="152" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="153" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="154" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="155" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="156" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="157" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="158" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="159" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="160" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="161" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="162" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="163" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="164" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="165" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="166" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="167" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="168" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="169" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="170" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="171" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="172" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="173" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="174" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="175" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="176" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="177" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="178" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="179" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="180" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="181" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="182" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="183" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="184" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="185" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="186" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="187" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="188" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="189" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="190" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="191" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="192" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="193" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="194" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="195" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="196" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="197" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="198" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="199" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="200" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="201" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="202" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="203" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="204" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="205" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="206" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="207" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="208" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="209" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="210" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="211" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="212" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="213" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="214" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="215" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="216" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="217" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="218" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="219" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="220" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="221" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="222" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="223" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="224" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="225" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="226" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="227" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="228" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="229" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="230" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="231" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="232" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="233" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="234" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="235" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="236" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="237" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="238" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="239" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="240" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="241" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="242" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="243" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="244" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="245" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="246" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="247" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="248" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="249" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="250" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="251" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="252" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="253" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="254" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="255" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="256" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="257" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="258" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="259" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="260" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="261" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="262" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="263" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="264" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="265" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="266" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="267" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="268" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="269" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="270" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="271" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="272" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="273" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="274" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="275" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="276" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="277" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="278" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="279" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="280" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="281" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="282" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="283" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="284" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="285" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="286" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="287" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="288" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="289" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="290" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="291" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="292" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="293" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="294" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="295" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="296" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="297" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="298" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="299" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="300" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="301" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="302" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="303" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="304" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="305" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="306" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="307" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="308" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="309" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="310" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="311" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="312" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="313" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="314" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="315" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="316" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="317" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="318" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="319" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="320" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="321" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="322" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="323" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="324" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="325" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="326" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="327" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="328" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="329" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="330" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="331" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="332" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="333" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="334" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="335" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="336" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="337" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="338" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="339" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="340" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="341" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="342" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="343" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="344" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="345" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="346" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="347" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="348" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="349" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="350" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="351" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="352" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="353" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="354" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="355" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="356" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="357" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="358" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="359" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="360" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="361" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="362" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="363" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="364" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="365" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="366" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="367" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="368" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="369" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="370" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="371" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="372" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="373" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="374" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="375" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="376" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="377" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="378" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="379" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="380" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="381" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="382" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="383" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="384" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="385" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="386" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="387" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="388" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="389" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="390" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="391" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="392" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="393" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="394" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="395" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="396" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="397" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="398" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="399" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="400" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="401" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="402" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="403" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="404" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="405" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="406" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="407" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="408" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="409" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="410" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="411" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="412" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="413" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="414" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="415" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="416" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="417" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="418" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="419" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="420" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="421" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="422" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="423" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="424" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="425" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="426" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="427" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="428" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="429" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="430" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="431" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="432" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="433" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="434" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="435" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="436" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="437" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="438" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="439" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="440" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="441" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="442" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="443" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="444" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="445" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="446" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="447" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="448" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="449" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="450" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="451" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="452" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="453" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="454" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="455" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="456" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="457" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="458" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="459" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="460" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="461" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="462" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="463" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="464" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="465" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="466" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="467" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="468" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="469" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="470" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="471" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="472" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="473" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="474" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="475" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="476" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="477" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="478" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="479" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="480" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="481" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="482" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="483" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="484" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="485" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="486" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="487" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="488" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="489" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="490" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="491" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="492" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="493" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="494" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="495" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="496" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="497" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="498" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="499" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="500" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="501" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="502" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="503" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="504" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="505" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="506" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="507" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="508" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="509" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="510" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="511" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="512" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="513" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="514" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="515" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="516" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="517" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="518" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="519" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="520" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="521" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="522" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="523" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="524" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="525" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="526" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="527" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="528" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="529" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="530" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="531" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="532" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="533" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="534" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="535" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="536" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="537" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="538" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="539" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="540" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="541" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="542" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="543" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="544" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="545" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="546" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="547" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="548" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="549" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="550" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="551" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="552" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="553" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="554" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="555" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="556" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="557" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="558" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="559" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="560" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="561" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="562" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="563" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="564" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="565" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="566" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="567" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="568" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="569" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="570" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="571" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="572" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="573" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="574" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="575" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="576" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="577" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="578" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="579" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="580" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="581" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="582" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="583" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="584" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="585" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="586" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="587" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="588" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="589" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="590" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="591" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="592" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="593" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="594" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="595" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="596" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="597" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="598" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="599" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="600" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="601" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="602" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="603" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="604" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="605" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="606" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="607" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="608" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="609" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="610" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="611" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="612" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="613" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="614" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="615" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="616" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="617" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="618" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="619" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="620" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="621" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="622" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="623" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="624" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="625" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="626" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="627" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="628" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="629" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="630" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="631" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="632" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="633" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="634" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="635" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="636" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="637" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="638" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="639" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="640" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="641" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="642" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="643" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="644" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="645" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="646" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="647" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="648" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="649" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="650" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="651" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="652" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="653" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="654" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="655" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="656" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="657" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="658" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="659" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="660" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="661" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="662" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="663" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="664" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="665" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="666" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="667" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="668" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="669" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="670" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="671" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="672" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="673" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="674" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="675" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="676" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="677" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="678" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="679" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="680" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="681" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="682" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="683" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="684" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="685" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="686" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="687" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="688" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="689" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="690" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="691" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="692" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="693" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="694" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="695" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="696" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="697" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="698" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="699" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="700" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="701" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="702" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="703" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="704" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="705" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="706" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="707" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="708" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="709" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="710" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="711" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="712" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="713" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="714" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="715" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="716" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="717" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="718" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="719" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="720" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="721" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="722" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="723" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="724" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="725" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="726" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="727" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="728" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="729" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="730" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="731" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="732" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="733" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="734" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="735" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="C8" s="15">
+        <v>5</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>General!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:I1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D2" s="12">
+        <v>4</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" s="12">
+        <v>4</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" s="12">
+        <v>4</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D5" s="12">
+        <v>4</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D6" s="12">
+        <v>4</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" s="12">
+        <v>4</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" s="12">
+        <v>4</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D13" s="12">
+        <v>1</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="D14" s="12">
+        <v>1</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D15" s="12">
+        <v>5</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D16" s="12">
+        <v>5</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D17" s="12">
+        <v>5</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D18" s="12">
+        <v>5</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D19" s="12">
+        <v>5</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D20" s="12">
+        <v>5</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="D21" s="12">
+        <v>5</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D22" s="12">
+        <v>5</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="12">
+        <v>4</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="12">
+        <v>4</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" s="12">
+        <v>5</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H578"/>
@@ -3031,25 +2852,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3075,7 +2896,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3101,7 +2922,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3127,7 +2948,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3153,7 +2974,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3179,7 +3000,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3205,7 +3026,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3231,7 +3052,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3257,7 +3078,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -3846,12 +3667,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -3893,7 +3714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:B3"/>
@@ -3936,7 +3757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:E6"/>
@@ -4030,7 +3851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:E5"/>
@@ -4107,7 +3928,7 @@
         <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="D4" t="s">
         <v>41</v>
@@ -4152,10 +3973,10 @@
         <v>79</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4163,7 +3984,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C2" s="7">
         <v>37.402092570550302</v>
@@ -4177,7 +3998,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C3" s="7">
         <v>37.402092570550302</v>
@@ -4191,7 +4012,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="C4" s="7">
         <v>37.402092570550302</v>
@@ -4246,10 +4067,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -4257,13 +4078,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -4271,13 +4092,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -4285,13 +4106,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -4299,13 +4120,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -4313,13 +4134,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -4383,7 +4204,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -4391,7 +4212,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4407,7 +4228,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4415,7 +4236,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4423,7 +4244,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -4431,7 +4252,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -4460,10 +4281,10 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>29</v>
@@ -4477,10 +4298,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>31</v>
@@ -4494,10 +4315,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>31</v>
@@ -4511,10 +4332,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>31</v>
@@ -4528,10 +4349,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>31</v>
@@ -4545,10 +4366,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>31</v>
@@ -4562,10 +4383,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>31</v>
@@ -4579,10 +4400,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>31</v>
@@ -4596,10 +4417,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>31</v>
@@ -4613,10 +4434,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>31</v>
@@ -4630,13 +4451,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>30</v>
@@ -4647,13 +4468,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>30</v>
@@ -4664,13 +4485,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>30</v>
@@ -4681,13 +4502,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>30</v>
@@ -4698,13 +4519,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>30</v>
@@ -4715,13 +4536,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>30</v>
@@ -4732,13 +4553,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>30</v>
@@ -4749,13 +4570,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>30</v>
@@ -4766,13 +4587,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>30</v>
@@ -4783,13 +4604,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>30</v>
@@ -4800,13 +4621,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>30</v>
@@ -12198,7 +12019,7 @@
         <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -12219,7 +12040,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>23</v>
@@ -12240,7 +12061,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -12261,7 +12082,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -12282,7 +12103,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
@@ -12303,7 +12124,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>27</v>
@@ -12324,7 +12145,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>23</v>
@@ -12345,7 +12166,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>23</v>
@@ -12367,7 +12188,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>23</v>
@@ -12389,7 +12210,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>27</v>
@@ -12411,7 +12232,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>27</v>
@@ -12433,7 +12254,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>27</v>
@@ -12455,7 +12276,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>27</v>
@@ -12477,7 +12298,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>27</v>
@@ -12499,7 +12320,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>27</v>
@@ -12521,7 +12342,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>23</v>
@@ -12542,7 +12363,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>27</v>
@@ -12563,7 +12384,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>23</v>
@@ -12584,7 +12405,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>23</v>
@@ -12605,7 +12426,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>23</v>
@@ -12626,7 +12447,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>27</v>
@@ -12647,7 +12468,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>23</v>
@@ -12668,7 +12489,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>23</v>
@@ -12689,7 +12510,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>23</v>
@@ -12710,7 +12531,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>27</v>
@@ -12731,7 +12552,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>23</v>
@@ -12752,7 +12573,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>23</v>
@@ -12773,7 +12594,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>23</v>
@@ -12794,7 +12615,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>23</v>
@@ -12815,7 +12636,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>23</v>
@@ -12839,7 +12660,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>23</v>
@@ -12860,7 +12681,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>23</v>
@@ -12881,7 +12702,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>23</v>
@@ -13980,8 +13801,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2828"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14015,7 +13836,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>47</v>
@@ -14033,7 +13854,7 @@
         <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>57</v>
@@ -14075,7 +13896,7 @@
         <v>96</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14084,7 +13905,7 @@
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -14109,10 +13930,10 @@
         <v>-122.04883575439401</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="Q2" s="2">
         <v>8.5</v>
@@ -14121,7 +13942,7 @@
         <v>11</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="T2" s="2">
         <v>1</v>
@@ -14130,7 +13951,7 @@
         <v>4</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14139,7 +13960,7 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -14155,7 +13976,7 @@
         <v>65</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="Q3" s="2">
         <v>8.5</v>
@@ -14164,7 +13985,7 @@
         <v>11</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="T3" s="2">
         <v>5</v>
@@ -14173,7 +13994,7 @@
         <v>2</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14182,7 +14003,7 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -14205,10 +14026,10 @@
       </c>
       <c r="M4" s="7"/>
       <c r="O4" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="Q4" s="2">
         <v>8.5</v>
@@ -14217,7 +14038,7 @@
         <v>11</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="T4" s="2">
         <v>1</v>
@@ -14226,7 +14047,7 @@
         <v>4</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14234,10 +14055,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -14291,10 +14112,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
@@ -14347,10 +14168,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
@@ -14403,10 +14224,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
@@ -14462,10 +14283,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
@@ -14518,10 +14339,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
@@ -14574,10 +14395,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D11" s="7">
         <v>5</v>
@@ -14618,7 +14439,7 @@
         <v>11</v>
       </c>
       <c r="T11" s="7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="U11" s="7">
         <v>8</v>
@@ -14632,10 +14453,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D12" s="7">
         <v>5</v>
@@ -14676,13 +14497,13 @@
         <v>11</v>
       </c>
       <c r="T12" s="7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="U12" s="7">
         <v>8</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>232</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14690,10 +14511,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D13" s="7">
         <v>5</v>
@@ -14713,10 +14534,10 @@
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
@@ -14727,16 +14548,16 @@
         <v>11</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="T13" s="7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="U13" s="7">
         <v>1</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14744,10 +14565,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D14" s="7">
         <v>5</v>
@@ -14767,10 +14588,10 @@
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
@@ -14784,7 +14605,7 @@
         <v>11</v>
       </c>
       <c r="T14" s="7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="U14" s="7">
         <v>8</v>
@@ -24774,7 +24595,7 @@
   <dimension ref="A1:I1138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24815,7 +24636,7 @@
         <v>74</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -24823,13 +24644,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E2" s="4">
         <v>42294.500011574077</v>
@@ -24873,7 +24694,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="7" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E4" s="4">
         <v>42294.500011574077</v>
@@ -24898,7 +24719,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -24917,7 +24738,7 @@
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -24934,7 +24755,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -24951,7 +24772,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -24968,7 +24789,7 @@
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -24985,7 +24806,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -25002,7 +24823,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -25019,7 +24840,7 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -25036,7 +24857,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -25053,7 +24874,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -25070,7 +24891,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -25087,7 +24908,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -25104,7 +24925,7 @@
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -25121,7 +24942,7 @@
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -25138,7 +24959,7 @@
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -25155,7 +24976,7 @@
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -25172,7 +24993,7 @@
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -25189,7 +25010,7 @@
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -25206,7 +25027,7 @@
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -36447,16 +36268,16 @@
         <v>88</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>89</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36464,7 +36285,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -36500,7 +36321,7 @@
         <v>91</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36508,7 +36329,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -36544,7 +36365,7 @@
         <v>92</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36552,7 +36373,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -36588,7 +36409,7 @@
         <v>93</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36596,7 +36417,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -36632,7 +36453,7 @@
         <v>92</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36640,7 +36461,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -36681,7 +36502,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
@@ -36722,7 +36543,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
@@ -36763,7 +36584,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
@@ -36804,7 +36625,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>
@@ -36840,7 +36661,7 @@
         <v>91</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36848,7 +36669,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>1</v>
@@ -36884,7 +36705,7 @@
         <v>91</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36892,7 +36713,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>1</v>
@@ -36928,7 +36749,7 @@
         <v>91</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36936,7 +36757,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>1</v>
@@ -36972,7 +36793,7 @@
         <v>91</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36980,7 +36801,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>1</v>
@@ -37016,7 +36837,7 @@
         <v>91</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>233</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix for assets/boundaries dynamic checkboxes click
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" firstSheet="11" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -1051,69 +1051,6 @@
     <t>Tenite</t>
   </si>
   <si>
-    <t>5FB149DC-0318-4E53-8E55-252C96634CE9</t>
-  </si>
-  <si>
-    <t>C37AA3CC-F41F-42B9-8C7D-3BEA58F6F495</t>
-  </si>
-  <si>
-    <t>D08FC87F-F979-4131-92A9-3D82F37F4BBA</t>
-  </si>
-  <si>
-    <t>F3955E82-DD13-4842-84F7-502BCDA6B57A</t>
-  </si>
-  <si>
-    <t>9119E94C-B7CB-4E1D-AE92-57DD72CB41F7</t>
-  </si>
-  <si>
-    <t>44353E68-0694-4F05-85CB-84D753EA278C</t>
-  </si>
-  <si>
-    <t>69CEAB1E-77FC-47A2-A774-AE3554939C95</t>
-  </si>
-  <si>
-    <t>50987927-5724-4D0A-BD7E-BD770EBB911C</t>
-  </si>
-  <si>
-    <t>6FC8F1CF-614C-4107-8209-C40569D53100</t>
-  </si>
-  <si>
-    <t>6FC8F1CF-614C-4107-8209-C40569D53193</t>
-  </si>
-  <si>
-    <t>96CAF1F5-D5C5-461D-9CE3-D210C20A1BB0</t>
-  </si>
-  <si>
-    <t>AD701312-C470-482A-BE45-EF37770E2CE6</t>
-  </si>
-  <si>
-    <t>F14735DE-6C9B-4423-8533-F243A7FE4E90</t>
-  </si>
-  <si>
-    <t>1B5BEFF8-2754-44A9-BE1A-0675B6BE4FD1</t>
-  </si>
-  <si>
-    <t>3869C45B-DA8F-4594-A358-301EA70BC0F1</t>
-  </si>
-  <si>
-    <t>FAB1C61C-392F-451A-BB5A-45002DD6AE25</t>
-  </si>
-  <si>
-    <t>8E20654F-CA8A-4041-9DB4-46E8AF369E93</t>
-  </si>
-  <si>
-    <t>ACEF3C6D-49C3-42F0-BD2F-790963571BED</t>
-  </si>
-  <si>
-    <t>980095B1-B316-4357-9179-9A76D4C848FA</t>
-  </si>
-  <si>
-    <t>5CD4D93C-0154-4A4B-A4E8-BE69F5B80D40</t>
-  </si>
-  <si>
-    <t>9DA23FD0-9A41-46D1-9902-F204261005AB</t>
-  </si>
-  <si>
     <t>Wrought Steel</t>
   </si>
   <si>
@@ -1136,18 +1073,6 @@
   </si>
   <si>
     <t>Big Boundary</t>
-  </si>
-  <si>
-    <t>3BB4B2AE-9591-4607-9CAD-FD2EB377760A</t>
-  </si>
-  <si>
-    <t>B9E69B56-E43E-4F6C-AFB1-24C01C1DD9DC</t>
-  </si>
-  <si>
-    <t>024249AE-374B-4F6F-BD87-E8FDCACB48E1</t>
-  </si>
-  <si>
-    <t>551CB7C0-005B-4E3E-BFAE-D19DA0ED7EFE</t>
   </si>
   <si>
     <t>Boundaries Row IDs</t>
@@ -1190,6 +1115,81 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>3bb4b2ae-9591-4607-9cad-fd2eb377760a</t>
+  </si>
+  <si>
+    <t>b9e69b56-e43e-4f6c-afb1-24c01c1dd9dc</t>
+  </si>
+  <si>
+    <t>024249ae-374b-4f6f-bd87-e8fdcacb48e1</t>
+  </si>
+  <si>
+    <t>551cb7c0-005b-4e3e-bfae-d19da0ed7efe</t>
+  </si>
+  <si>
+    <t>50987927-5724-4d0a-bd7e-bd770ebb911c</t>
+  </si>
+  <si>
+    <t>9119e94c-b7cb-4e1d-ae92-57dd72cb41f7</t>
+  </si>
+  <si>
+    <t>5fb149dc-0318-4e53-8e55-252c96634ce9</t>
+  </si>
+  <si>
+    <t>69ceab1e-77fc-47a2-a774-ae3554939c95</t>
+  </si>
+  <si>
+    <t>6fc8f1cf-614c-4107-8209-c40569d53193</t>
+  </si>
+  <si>
+    <t>6fc8f1cf-614c-4107-8209-c40569d53100</t>
+  </si>
+  <si>
+    <t>c37aa3cc-f41f-42b9-8c7d-3bea58f6f495</t>
+  </si>
+  <si>
+    <t>96caf1f5-d5c5-461d-9ce3-d210c20a1bb0</t>
+  </si>
+  <si>
+    <t>d08fc87f-f979-4131-92a9-3d82f37f4bba</t>
+  </si>
+  <si>
+    <t>ad701312-c470-482a-be45-ef37770e2ce6</t>
+  </si>
+  <si>
+    <t>f14735de-6c9b-4423-8533-f243a7fe4e90</t>
+  </si>
+  <si>
+    <t>44353e68-0694-4f05-85cb-84d753ea278c</t>
+  </si>
+  <si>
+    <t>f3955e82-dd13-4842-84f7-502bcda6b57a</t>
+  </si>
+  <si>
+    <t>1b5beff8-2754-44a9-be1a-0675b6be4fd1</t>
+  </si>
+  <si>
+    <t>3869c45b-da8f-4594-a358-301ea70bc0f1</t>
+  </si>
+  <si>
+    <t>fab1c61c-392f-451a-bb5a-45002dd6ae25</t>
+  </si>
+  <si>
+    <t>8e20654f-ca8a-4041-9db4-46e8af369e93</t>
+  </si>
+  <si>
+    <t>acef3c6d-49c3-42f0-bd2f-790963571bed</t>
+  </si>
+  <si>
+    <t>980095b1-b316-4357-9179-9a76d4c848fa</t>
+  </si>
+  <si>
+    <t>5cd4d93c-0154-4a4b-a4e8-be69f5b80d40</t>
+  </si>
+  <si>
+    <t>9da23fd0-9a41-46d1-9902-f204261005ab</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1414,7 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1450,6 +1450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1 2" xfId="7"/>
@@ -2204,13 +2205,13 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2218,13 +2219,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2232,11 +2233,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="7" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2245,10 +2246,10 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="15" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2258,7 +2259,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="15"/>
       <c r="D5" s="7" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2266,11 +2267,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="7" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2280,7 +2281,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="15"/>
       <c r="D7" s="7" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2288,13 +2289,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
       <c r="C8" s="15">
         <v>5</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2310,7 +2311,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2344,7 +2345,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>230</v>
@@ -2361,7 +2362,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>244</v>
+        <v>267</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>229</v>
@@ -2378,7 +2379,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>240</v>
+        <v>268</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>234</v>
@@ -2395,7 +2396,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>246</v>
+        <v>269</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>237</v>
@@ -2412,7 +2413,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>249</v>
+        <v>270</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>239</v>
@@ -2429,7 +2430,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>248</v>
+        <v>271</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>238</v>
@@ -2446,7 +2447,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>241</v>
+        <v>272</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>235</v>
@@ -2463,7 +2464,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>250</v>
+        <v>273</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>230</v>
@@ -2480,7 +2481,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>242</v>
+        <v>274</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>229</v>
@@ -2497,7 +2498,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>251</v>
+        <v>275</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>233</v>
@@ -2514,7 +2515,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>232</v>
@@ -2531,7 +2532,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>245</v>
+        <v>277</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>231</v>
@@ -2548,7 +2549,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>243</v>
+        <v>278</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>236</v>
@@ -2565,7 +2566,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>230</v>
@@ -2574,7 +2575,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2582,7 +2583,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>254</v>
+        <v>280</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>237</v>
@@ -2591,7 +2592,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -2599,7 +2600,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>255</v>
+        <v>281</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>234</v>
@@ -2608,24 +2609,24 @@
         <v>5</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>256</v>
+      <c r="B18" s="17" t="s">
+        <v>282</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="D18" s="12">
         <v>5</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -2633,7 +2634,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>229</v>
@@ -2642,7 +2643,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -2650,7 +2651,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>258</v>
+        <v>284</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>235</v>
@@ -2659,7 +2660,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2667,16 +2668,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>259</v>
+        <v>285</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
       <c r="D21" s="12">
         <v>5</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -2684,7 +2685,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>260</v>
+        <v>286</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>238</v>
@@ -2693,7 +2694,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -2706,7 +2707,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2723,10 +2724,10 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>48</v>
@@ -2740,7 +2741,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>65</v>
@@ -2757,7 +2758,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>64</v>
@@ -2774,10 +2775,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
@@ -2791,10 +2792,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="D5" s="12">
         <v>1</v>
@@ -2808,7 +2809,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>194</v>
@@ -2817,7 +2818,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3672,7 +3673,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -13801,8 +13802,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2828"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14439,7 +14440,7 @@
         <v>11</v>
       </c>
       <c r="T11" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U11" s="7">
         <v>8</v>
@@ -14497,7 +14498,7 @@
         <v>11</v>
       </c>
       <c r="T12" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U12" s="7">
         <v>8</v>
@@ -14551,7 +14552,7 @@
         <v>203</v>
       </c>
       <c r="T13" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U13" s="7">
         <v>1</v>
@@ -14605,7 +14606,7 @@
         <v>11</v>
       </c>
       <c r="T14" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="U14" s="7">
         <v>8</v>

</xml_diff>

<commit_message>
update test case data for TC180 and TC182
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -892,9 +892,6 @@
     <t>TC180</t>
   </si>
   <si>
-    <t>TC181</t>
-  </si>
-  <si>
     <t>First View</t>
   </si>
   <si>
@@ -1190,6 +1187,9 @@
   </si>
   <si>
     <t>9da23fd0-9a41-46d1-9902-f204261005ab</t>
+  </si>
+  <si>
+    <t>TC182</t>
   </si>
 </sst>
 </file>
@@ -1810,7 +1810,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
@@ -1845,7 +1845,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>1</v>
@@ -1881,7 +1881,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>1</v>
@@ -1917,7 +1917,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>1</v>
@@ -1953,7 +1953,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>1</v>
@@ -1985,7 +1985,7 @@
         <v>145</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
@@ -2021,7 +2021,7 @@
         <v>135</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>1</v>
@@ -2053,7 +2053,7 @@
         <v>136</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>1</v>
@@ -2085,7 +2085,7 @@
         <v>137</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>1</v>
@@ -2117,7 +2117,7 @@
         <v>145</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D11" s="7" t="b">
         <v>1</v>
@@ -2205,13 +2205,13 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2219,13 +2219,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>256</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2233,11 +2233,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2246,10 +2246,10 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2259,7 +2259,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="15"/>
       <c r="D5" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2267,11 +2267,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2281,7 +2281,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="15"/>
       <c r="D7" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2289,13 +2289,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C8" s="15">
         <v>5</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2311,7 +2311,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2328,16 +2328,16 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2345,16 +2345,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D2" s="12">
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2362,16 +2362,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D3" s="12">
         <v>4</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2379,16 +2379,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D4" s="12">
         <v>4</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2396,16 +2396,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D5" s="12">
         <v>4</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -2413,16 +2413,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D6" s="12">
         <v>4</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2430,16 +2430,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D7" s="12">
         <v>4</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -2447,16 +2447,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D8" s="12">
         <v>4</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2464,16 +2464,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D9" s="12">
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -2481,16 +2481,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D10" s="12">
         <v>1</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -2498,16 +2498,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D11" s="12">
         <v>1</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -2515,16 +2515,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D12" s="12">
         <v>1</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -2532,16 +2532,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D13" s="12">
         <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -2549,16 +2549,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D14" s="12">
         <v>1</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -2566,16 +2566,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D15" s="12">
         <v>5</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -2583,16 +2583,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D16" s="12">
         <v>5</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -2600,16 +2600,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D17" s="12">
         <v>5</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -2617,16 +2617,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D18" s="12">
         <v>5</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -2634,16 +2634,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D19" s="12">
         <v>5</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -2651,16 +2651,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D20" s="12">
         <v>5</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -2668,16 +2668,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D21" s="12">
         <v>5</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -2685,16 +2685,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D22" s="12">
         <v>5</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -2724,16 +2724,16 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2741,7 +2741,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>65</v>
@@ -2750,7 +2750,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2758,7 +2758,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>64</v>
@@ -2767,7 +2767,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2775,16 +2775,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2792,16 +2792,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D5" s="12">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -2809,16 +2809,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D6" s="12">
         <v>5</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3053,7 +3053,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -3079,7 +3079,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -3929,7 +3929,7 @@
         <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D4" t="s">
         <v>41</v>
@@ -4135,7 +4135,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
@@ -13802,8 +13802,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2828"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14217,7 +14217,7 @@
         <v>7</v>
       </c>
       <c r="V7" s="7">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14276,7 +14276,7 @@
         <v>7</v>
       </c>
       <c r="V8" s="7">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14284,7 +14284,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>187</v>
+        <v>286</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>185</v>
@@ -14332,7 +14332,7 @@
         <v>7</v>
       </c>
       <c r="V9" s="7">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14340,7 +14340,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>187</v>
+        <v>286</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>185</v>
@@ -14388,7 +14388,7 @@
         <v>7</v>
       </c>
       <c r="V10" s="7">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14396,7 +14396,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>185</v>
@@ -14454,7 +14454,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>185</v>
@@ -14504,7 +14504,7 @@
         <v>8</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14512,7 +14512,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>185</v>
@@ -14535,10 +14535,10 @@
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="N13" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
@@ -14549,7 +14549,7 @@
         <v>11</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T13" s="7">
         <v>7</v>
@@ -14558,7 +14558,7 @@
         <v>1</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -14566,7 +14566,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>185</v>
@@ -14589,10 +14589,10 @@
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="N14" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
@@ -24596,7 +24596,7 @@
   <dimension ref="A1:I1138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24739,7 +24739,7 @@
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -24756,7 +24756,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -24773,7 +24773,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -24790,7 +24790,7 @@
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -24807,7 +24807,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -24824,7 +24824,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -24841,7 +24841,7 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -24858,7 +24858,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -24875,7 +24875,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -24892,7 +24892,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -24909,7 +24909,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -24926,7 +24926,7 @@
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -24943,7 +24943,7 @@
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -24960,7 +24960,7 @@
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -24977,7 +24977,7 @@
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -24994,7 +24994,7 @@
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -25011,7 +25011,7 @@
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -25028,7 +25028,7 @@
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -36670,7 +36670,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>1</v>
@@ -36706,7 +36706,7 @@
         <v>91</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36750,7 +36750,7 @@
         <v>91</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36794,7 +36794,7 @@
         <v>91</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -36838,7 +36838,7 @@
         <v>91</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Test Cases for US2087
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -329,7 +329,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="288">
   <si>
     <t>Enabled</t>
   </si>
@@ -1191,6 +1191,9 @@
   <si>
     <t>TC182</t>
   </si>
+  <si>
+    <t>Surveyor_man-pic.db3</t>
+  </si>
 </sst>
 </file>
 
@@ -1744,7 +1747,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -4266,7 +4269,7 @@
   <dimension ref="A1:E1069"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4635,11 +4638,21 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
@@ -11981,8 +11994,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H1072"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G296" sqref="G296"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12656,7 +12669,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -12677,7 +12690,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -12698,7 +12711,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -12719,19 +12732,158 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:7" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:8" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A37" s="7">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H37" s="7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A38" s="7">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A40" s="7">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A41" s="7">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A42" s="7">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H42" s="7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="49" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="50" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="51" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -13802,7 +13954,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2828"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added methods for verifications related to SSRS table + test data additions
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -264,6 +264,50 @@
         </r>
       </text>
     </comment>
+    <comment ref="B20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <u/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NOTE:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> 2 entries for the same test case are for Copy Compliance scenario.
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -324,12 +368,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="E24" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Add this value, post DE1540 is fixed - "6/28/2015  12:00:00 AM"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F24" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Add this value, post DE1540 is fixed - "6/30/2015  12:00:00 AM"</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="310">
   <si>
     <t>Enabled</t>
   </si>
@@ -1197,6 +1289,69 @@
   <si>
     <t>Select All Surveys</t>
   </si>
+  <si>
+    <t>TC231</t>
+  </si>
+  <si>
+    <t>TC235</t>
+  </si>
+  <si>
+    <t>Isotopic Analysis, Indications, Field Notes TRUE</t>
+  </si>
+  <si>
+    <t>9,11</t>
+  </si>
+  <si>
+    <t>PICARRO - Asset (Copper, Plastic)</t>
+  </si>
+  <si>
+    <t>11,15</t>
+  </si>
+  <si>
+    <t>All TRUE except Gap, Assets and Boundaries (Map=Satellite)</t>
+  </si>
+  <si>
+    <t>TC237</t>
+  </si>
+  <si>
+    <t>Level 2-AB</t>
+  </si>
+  <si>
+    <t>Level 2-A</t>
+  </si>
+  <si>
+    <t>TC509</t>
+  </si>
+  <si>
+    <t>Indication, Isotopic Analysis, Field Notes=TRUE. All other FALSE</t>
+  </si>
+  <si>
+    <t>All FALSE. Map=Map</t>
+  </si>
+  <si>
+    <t>All FALSE. Map=Satellite</t>
+  </si>
+  <si>
+    <t>16,17</t>
+  </si>
+  <si>
+    <t>TC510</t>
+  </si>
+  <si>
+    <t>TC514</t>
+  </si>
+  <si>
+    <t>TC520</t>
+  </si>
+  <si>
+    <t>LISA, FOV, Breadcrumbs, Indications TRUE, (BaseMap=Map)</t>
+  </si>
+  <si>
+    <t>2,18</t>
+  </si>
+  <si>
+    <t>TC521</t>
+  </si>
 </sst>
 </file>
 
@@ -1751,7 +1906,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2195,7 +2350,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2305,7 +2460,18 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C9" s="15">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>293</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2317,7 +2483,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2713,7 +2879,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2839,7 +3005,7 @@
   <dimension ref="A1:H578"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3088,7 +3254,32 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>300</v>
+      </c>
+    </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -3861,10 +4052,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3948,8 +4139,16 @@
       <c r="A5" t="s">
         <v>55</v>
       </c>
+      <c r="C5" t="s">
+        <v>245</v>
+      </c>
       <c r="D5" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -13957,8 +14156,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2828"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14770,92 +14969,533 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="M15" s="7"/>
-    </row>
-    <row r="16" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="M16" s="7"/>
-    </row>
-    <row r="17" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="M17" s="7"/>
-    </row>
-    <row r="18" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="M18" s="7"/>
-    </row>
-    <row r="19" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="M19" s="7"/>
-    </row>
-    <row r="20" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="M20" s="7"/>
-    </row>
-    <row r="21" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B21" s="7"/>
+    <row r="15" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J15" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K15" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L15" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q15" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R15" s="7">
+        <v>11</v>
+      </c>
+      <c r="S15" s="7">
+        <v>9</v>
+      </c>
+      <c r="T15" s="7">
+        <v>2</v>
+      </c>
+      <c r="U15" s="7">
+        <v>6</v>
+      </c>
+      <c r="V15" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J16" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K16" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L16" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q16" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R16" s="7">
+        <v>11</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="T16" s="7">
+        <v>8</v>
+      </c>
+      <c r="U16" s="7">
+        <v>8</v>
+      </c>
+      <c r="V16" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R17" s="7">
+        <v>11</v>
+      </c>
+      <c r="S17" s="7">
+        <v>9</v>
+      </c>
+      <c r="T17" s="7">
+        <v>2</v>
+      </c>
+      <c r="U17" s="7">
+        <v>6</v>
+      </c>
+      <c r="V17" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="7">
+        <v>3</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J18" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K18" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L18" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R18" s="7">
+        <v>11</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="T18" s="7">
+        <v>1</v>
+      </c>
+      <c r="U18" s="7">
+        <v>7</v>
+      </c>
+      <c r="V18" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J19" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K19" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L19" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R19" s="7">
+        <v>11</v>
+      </c>
+      <c r="S19" s="7">
+        <v>9</v>
+      </c>
+      <c r="T19" s="7">
+        <v>2</v>
+      </c>
+      <c r="U19" s="7">
+        <v>6</v>
+      </c>
+      <c r="V19" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J20" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K20" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L20" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R20" s="7">
+        <v>11</v>
+      </c>
+      <c r="S20" s="7">
+        <v>9</v>
+      </c>
+      <c r="T20" s="7">
+        <v>2</v>
+      </c>
+      <c r="U20" s="7">
+        <v>6</v>
+      </c>
+      <c r="V20" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H21" s="7"/>
+      <c r="I21" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J21" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K21" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L21" s="7">
+        <v>-121.98390000000001</v>
+      </c>
       <c r="M21" s="7"/>
-    </row>
-    <row r="22" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B22" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R21" s="7">
+        <v>11</v>
+      </c>
+      <c r="S21" s="7">
+        <v>9</v>
+      </c>
+      <c r="T21" s="7">
+        <v>2</v>
+      </c>
+      <c r="U21" s="7">
+        <v>6</v>
+      </c>
+      <c r="V21" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H22" s="7"/>
-      <c r="M22" s="7"/>
-    </row>
-    <row r="23" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B23" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R22" s="7">
+        <v>11</v>
+      </c>
+      <c r="S22" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="T22" s="7">
+        <v>4</v>
+      </c>
+      <c r="U22" s="7">
+        <v>6</v>
+      </c>
+      <c r="V22" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" s="7">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H23" s="7"/>
+      <c r="I23" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J23" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K23" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L23" s="7">
+        <v>-121.98390000000001</v>
+      </c>
       <c r="M23" s="7"/>
-    </row>
-    <row r="24" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R23" s="7">
+        <v>11</v>
+      </c>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7">
+        <v>8</v>
+      </c>
+      <c r="U23" s="7">
+        <v>6</v>
+      </c>
+      <c r="V23" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B24" s="7"/>
       <c r="H24" s="7"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B25" s="7"/>
       <c r="H25" s="7"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B26" s="7"/>
       <c r="H26" s="7"/>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B27" s="7"/>
       <c r="H27" s="7"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
       <c r="H28" s="7"/>
       <c r="M28" s="7"/>
     </row>
-    <row r="29" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
       <c r="H29" s="7"/>
       <c r="M29" s="7"/>
     </row>
-    <row r="30" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B30" s="7"/>
       <c r="H30" s="7"/>
       <c r="M30" s="7"/>
     </row>
-    <row r="31" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
       <c r="H31" s="7"/>
       <c r="M31" s="7"/>
     </row>
-    <row r="32" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
       <c r="H32" s="7"/>
       <c r="M32" s="7"/>
@@ -24726,19 +25366,19 @@
           <x14:formula1>
             <xm:f>Report!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G1048576 H2829:H1048576</xm:sqref>
+          <xm:sqref>H2829:H1048576 G1:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Report!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>M1 M836:M1048576</xm:sqref>
+          <xm:sqref>M1 M2826:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Report!$C$2:$C$4</xm:f>
+            <xm:f>Report!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M835</xm:sqref>
+          <xm:sqref>M2:M2825</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -24750,8 +25390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25256,16 +25896,26 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
+      <c r="D24" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
+      <c r="I24" s="7">
+        <v>1</v>
+      </c>
+      <c r="J24" s="7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B25" s="7"/>
@@ -37523,7 +38173,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -37531,7 +38182,7 @@
           <x14:formula1>
             <xm:f>General!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576 J2:J1048576</xm:sqref>
+          <xm:sqref>J2:J1048576 H1:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -37551,7 +38202,7 @@
   <dimension ref="A1:N800"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38173,24 +38824,239 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="17" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="18" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="19" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="20" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="21" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="23" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="24" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="25" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="26" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="28" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="30" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="31" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="32" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="33" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="34" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="35" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added some test steps to tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -421,7 +421,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="320">
   <si>
     <t>Enabled</t>
   </si>
@@ -1323,9 +1323,6 @@
     <t>TC509</t>
   </si>
   <si>
-    <t>Indication, Isotopic Analysis, Field Notes=TRUE. All other FALSE</t>
-  </si>
-  <si>
     <t>All FALSE. Map=Map</t>
   </si>
   <si>
@@ -1351,6 +1348,39 @@
   </si>
   <si>
     <t>TC521</t>
+  </si>
+  <si>
+    <t>Indication, Isotopic Analysis. All other FALSE</t>
+  </si>
+  <si>
+    <t>All TRUE except Assets and Boundaries (Map=Satellite)</t>
+  </si>
+  <si>
+    <t>LISA, FOV, Breadcrumbs TRUE, (BaseMap=Map)</t>
+  </si>
+  <si>
+    <t>Breadcrumbs, Indications, Isotopic Analysis TRUE, (BaseMap=Map)</t>
+  </si>
+  <si>
+    <t>Indications, Field Notes, Gaps, Assets, Boundaries = TRUE, (BaseMap = Map)</t>
+  </si>
+  <si>
+    <t>FOV, Gaps = TRUE, (BaseMap = Satellite)</t>
+  </si>
+  <si>
+    <t>Breadcrumbs, Indications, Assets, Boundaries = TRUE, (BaseMap=Map)</t>
+  </si>
+  <si>
+    <t>LISA, FOV, Indications, Assets, Boundaries = TRUE (BaseMap = Satellite)</t>
+  </si>
+  <si>
+    <t>Isotopic Analysis, Field Notes, Assets = TRUE, (BaseMap=Map)</t>
+  </si>
+  <si>
+    <t>Field Notes, Assets, Boundaries = TRUE, (BaseMap=Map)</t>
+  </si>
+  <si>
+    <t>12,19,20,21,14,22,23</t>
   </si>
 </sst>
 </file>
@@ -2350,7 +2380,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3005,7 +3035,7 @@
   <dimension ref="A1:H578"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3277,7 +3307,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -14157,7 +14187,7 @@
   <dimension ref="A1:V2828"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15169,7 +15199,7 @@
         <v>11</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="T18" s="7">
         <v>1</v>
@@ -15186,7 +15216,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>185</v>
@@ -15239,7 +15269,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>185</v>
@@ -15292,7 +15322,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>185</v>
@@ -15350,7 +15380,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>185</v>
@@ -15387,7 +15417,7 @@
         <v>11</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="T22" s="7">
         <v>4</v>
@@ -15404,7 +15434,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>185</v>
@@ -15444,12 +15474,14 @@
       <c r="R23" s="7">
         <v>11</v>
       </c>
-      <c r="S23" s="7"/>
+      <c r="S23" s="7" t="s">
+        <v>319</v>
+      </c>
       <c r="T23" s="7">
         <v>8</v>
       </c>
       <c r="U23" s="7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="V23" s="7">
         <v>4</v>
@@ -25390,8 +25422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1138"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38202,7 +38234,7 @@
   <dimension ref="A1:N800"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38480,6 +38512,9 @@
       <c r="M6" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="N6" s="2" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
@@ -38521,6 +38556,9 @@
       <c r="M7" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="N7" s="2" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -38562,6 +38600,9 @@
       <c r="M8" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="N8" s="2" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="9" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -38603,6 +38644,9 @@
       <c r="M9" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="N9" s="2" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -38953,7 +38997,7 @@
         <v>91</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -38997,7 +39041,7 @@
         <v>92</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -39041,14 +39085,229 @@
         <v>91</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+        <v>306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
     <row r="25" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
test cases cleaned up + added customer page action methods
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -421,7 +421,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="332">
   <si>
     <t>Enabled</t>
   </si>
@@ -1382,6 +1382,42 @@
   <si>
     <t>12,19,20,21,14,22,23</t>
   </si>
+  <si>
+    <t>TC526</t>
+  </si>
+  <si>
+    <t>TC678</t>
+  </si>
+  <si>
+    <t>TC680</t>
+  </si>
+  <si>
+    <t>TC681</t>
+  </si>
+  <si>
+    <t>ONLY LISA TRUE</t>
+  </si>
+  <si>
+    <t>ONLY FOV TRUE</t>
+  </si>
+  <si>
+    <t>ONLY Breadcrumbs TRUE</t>
+  </si>
+  <si>
+    <t>ONLY Gaps TRUE</t>
+  </si>
+  <si>
+    <t>ONLY Assets TRUE</t>
+  </si>
+  <si>
+    <t>LISA, FOV, Breadcrumbs, Gaps, Assets TRUE</t>
+  </si>
+  <si>
+    <t>24,25</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6</t>
+  </si>
 </sst>
 </file>
 
@@ -4280,13 +4316,13 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.77734375" bestFit="1" customWidth="1"/>
@@ -4379,7 +4415,23 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -4418,7 +4470,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12227,7 +12279,7 @@
   <dimension ref="A1:H1072"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14184,10 +14236,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:V2828"/>
+  <dimension ref="A1:V2827"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15488,126 +15540,790 @@
       </c>
     </row>
     <row r="24" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B24" s="7"/>
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>320</v>
+      </c>
       <c r="H24" s="7"/>
       <c r="M24" s="7"/>
     </row>
     <row r="25" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B25" s="7"/>
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H25" s="7"/>
+      <c r="I25" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J25" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K25" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L25" s="7">
+        <v>-121.98390000000001</v>
+      </c>
       <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R25" s="7">
+        <v>11</v>
+      </c>
+      <c r="S25" s="7">
+        <v>24</v>
+      </c>
+      <c r="T25" s="7">
+        <v>1</v>
+      </c>
+      <c r="U25" s="7">
+        <v>1</v>
+      </c>
+      <c r="V25" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="26" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B26" s="7"/>
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H26" s="7"/>
+      <c r="I26" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J26" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K26" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L26" s="7">
+        <v>-121.98390000000001</v>
+      </c>
       <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R26" s="7">
+        <v>11</v>
+      </c>
+      <c r="S26" s="7">
+        <v>25</v>
+      </c>
+      <c r="T26" s="7">
+        <v>1</v>
+      </c>
+      <c r="U26" s="7">
+        <v>1</v>
+      </c>
+      <c r="V26" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B27" s="7"/>
+      <c r="A27" s="7">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H27" s="7"/>
+      <c r="I27" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J27" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K27" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L27" s="7">
+        <v>-121.98390000000001</v>
+      </c>
       <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R27" s="7">
+        <v>11</v>
+      </c>
+      <c r="S27" s="7">
+        <v>26</v>
+      </c>
+      <c r="T27" s="7">
+        <v>1</v>
+      </c>
+      <c r="U27" s="7">
+        <v>1</v>
+      </c>
+      <c r="V27" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B28" s="7"/>
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H28" s="7"/>
+      <c r="I28" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J28" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K28" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L28" s="7">
+        <v>-121.98390000000001</v>
+      </c>
       <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R28" s="7">
+        <v>11</v>
+      </c>
+      <c r="S28" s="7">
+        <v>27</v>
+      </c>
+      <c r="T28" s="7">
+        <v>1</v>
+      </c>
+      <c r="U28" s="7">
+        <v>1</v>
+      </c>
+      <c r="V28" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B29" s="7"/>
+      <c r="A29" s="7">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H29" s="7"/>
+      <c r="I29" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J29" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K29" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L29" s="7">
+        <v>-121.98390000000001</v>
+      </c>
       <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R29" s="7">
+        <v>11</v>
+      </c>
+      <c r="S29" s="7">
+        <v>28</v>
+      </c>
+      <c r="T29" s="7">
+        <v>1</v>
+      </c>
+      <c r="U29" s="7">
+        <v>1</v>
+      </c>
+      <c r="V29" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B30" s="7"/>
+      <c r="A30" s="7">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D30" s="7">
+        <v>1</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H30" s="7"/>
+      <c r="I30" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J30" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K30" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L30" s="7">
+        <v>-121.98390000000001</v>
+      </c>
       <c r="M30" s="7"/>
-    </row>
-    <row r="31" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="M31" s="7"/>
-    </row>
-    <row r="32" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="M32" s="7"/>
-    </row>
-    <row r="33" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="M33" s="7"/>
-    </row>
-    <row r="34" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="M34" s="7"/>
-    </row>
-    <row r="35" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="M35" s="7"/>
-    </row>
-    <row r="36" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="M36" s="7"/>
-    </row>
-    <row r="37" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B37" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R30" s="7">
+        <v>11</v>
+      </c>
+      <c r="S30" s="7">
+        <v>29</v>
+      </c>
+      <c r="T30" s="7">
+        <v>1</v>
+      </c>
+      <c r="U30" s="7">
+        <v>1</v>
+      </c>
+      <c r="V30" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D31" s="7">
+        <v>1</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I31" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J31" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K31" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L31" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q31" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R31" s="7">
+        <v>11</v>
+      </c>
+      <c r="S31" s="7">
+        <v>24</v>
+      </c>
+      <c r="T31" s="7">
+        <v>1</v>
+      </c>
+      <c r="U31" s="7">
+        <v>1</v>
+      </c>
+      <c r="V31" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D32" s="7">
+        <v>1</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="7">
+        <v>0</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I32" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J32" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K32" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L32" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R32" s="7">
+        <v>11</v>
+      </c>
+      <c r="S32" s="7">
+        <v>25</v>
+      </c>
+      <c r="T32" s="7">
+        <v>1</v>
+      </c>
+      <c r="U32" s="7">
+        <v>1</v>
+      </c>
+      <c r="V32" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D33" s="7">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I33" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J33" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K33" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L33" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q33" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R33" s="7">
+        <v>11</v>
+      </c>
+      <c r="S33" s="7">
+        <v>26</v>
+      </c>
+      <c r="T33" s="7">
+        <v>1</v>
+      </c>
+      <c r="U33" s="7">
+        <v>1</v>
+      </c>
+      <c r="V33" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D34" s="7">
+        <v>1</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" s="7">
+        <v>0</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I34" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J34" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K34" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L34" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q34" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R34" s="7">
+        <v>11</v>
+      </c>
+      <c r="S34" s="7">
+        <v>27</v>
+      </c>
+      <c r="T34" s="7">
+        <v>1</v>
+      </c>
+      <c r="U34" s="7">
+        <v>1</v>
+      </c>
+      <c r="V34" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D35" s="7">
+        <v>1</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I35" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J35" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K35" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L35" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q35" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R35" s="7">
+        <v>11</v>
+      </c>
+      <c r="S35" s="7">
+        <v>28</v>
+      </c>
+      <c r="T35" s="7">
+        <v>1</v>
+      </c>
+      <c r="U35" s="7">
+        <v>1</v>
+      </c>
+      <c r="V35" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I36" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J36" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K36" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L36" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q36" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R36" s="7">
+        <v>11</v>
+      </c>
+      <c r="S36" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="T36" s="7">
+        <v>1</v>
+      </c>
+      <c r="U36" s="7">
+        <v>1</v>
+      </c>
+      <c r="V36" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A37" s="7">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D37" s="2">
+        <v>6</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="H37" s="7"/>
+      <c r="I37" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J37" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K37" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L37" s="7">
+        <v>-121.98390000000001</v>
+      </c>
       <c r="M37" s="7"/>
-    </row>
-    <row r="38" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R37" s="7">
+        <v>11</v>
+      </c>
+      <c r="S37" s="7">
+        <v>29</v>
+      </c>
+      <c r="T37" s="7">
+        <v>1</v>
+      </c>
+      <c r="U37" s="7">
+        <v>1</v>
+      </c>
+      <c r="V37" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B38" s="7"/>
       <c r="H38" s="7"/>
       <c r="M38" s="7"/>
     </row>
-    <row r="39" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B39" s="7"/>
       <c r="H39" s="7"/>
       <c r="M39" s="7"/>
     </row>
-    <row r="40" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B40" s="7"/>
       <c r="H40" s="7"/>
       <c r="M40" s="7"/>
     </row>
-    <row r="41" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B41" s="7"/>
       <c r="H41" s="7"/>
       <c r="M41" s="7"/>
     </row>
-    <row r="42" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B42" s="7"/>
       <c r="H42" s="7"/>
       <c r="M42" s="7"/>
     </row>
-    <row r="43" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B43" s="7"/>
       <c r="H43" s="7"/>
       <c r="M43" s="7"/>
     </row>
-    <row r="44" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B44" s="7"/>
       <c r="H44" s="7"/>
       <c r="M44" s="7"/>
     </row>
-    <row r="45" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B45" s="7"/>
       <c r="H45" s="7"/>
       <c r="M45" s="7"/>
     </row>
-    <row r="46" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B46" s="7"/>
       <c r="H46" s="7"/>
       <c r="M46" s="7"/>
     </row>
-    <row r="47" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B47" s="7"/>
       <c r="H47" s="7"/>
       <c r="M47" s="7"/>
     </row>
-    <row r="48" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B48" s="7"/>
       <c r="H48" s="7"/>
       <c r="M48" s="7"/>
@@ -18817,8 +19533,7 @@
       <c r="H689" s="7"/>
       <c r="M689" s="7"/>
     </row>
-    <row r="690" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B690" s="7"/>
+    <row r="690" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H690" s="7"/>
       <c r="M690" s="7"/>
     </row>
@@ -19400,7 +20115,6 @@
     </row>
     <row r="835" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H835" s="7"/>
-      <c r="M835" s="7"/>
     </row>
     <row r="836" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H836" s="7"/>
@@ -20320,7 +21034,7 @@
     <row r="1141" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1141" s="7"/>
     </row>
-    <row r="1142" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="1142" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H1142" s="7"/>
     </row>
     <row r="1143" spans="8:8" x14ac:dyDescent="0.3">
@@ -25377,9 +26091,6 @@
     </row>
     <row r="2827" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H2827" s="7"/>
-    </row>
-    <row r="2828" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H2828" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25390,27 +26101,27 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
+            <xm:f>Report!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2828:H1048576 G1:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Report!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>M1 M2825:M1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
             <xm:f>Report!$A$2:$A$5</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Report!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2829:H1048576 G1:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Report!$C$2:$C$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>M1 M2826:M1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
             <xm:f>Report!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M2825</xm:sqref>
+          <xm:sqref>M2:M2824</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -38234,7 +38945,7 @@
   <dimension ref="A1:N800"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39308,12 +40019,270 @@
         <v>318</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L25" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J27" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L27" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L28" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L29" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L30" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
     <row r="31" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="33" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
filled test steps and test case data
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -421,7 +421,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="352">
   <si>
     <t>Enabled</t>
   </si>
@@ -1421,6 +1421,63 @@
   <si>
     <t>1,2,3,4,5,6,7</t>
   </si>
+  <si>
+    <t>TC689</t>
+  </si>
+  <si>
+    <t>All TRUE (except GAP)</t>
+  </si>
+  <si>
+    <t>TC690</t>
+  </si>
+  <si>
+    <t>TC698</t>
+  </si>
+  <si>
+    <t>LISA, FOV, Gaps = TRUE, (BaseMap = Satellite)</t>
+  </si>
+  <si>
+    <t>TC700</t>
+  </si>
+  <si>
+    <t>TC699</t>
+  </si>
+  <si>
+    <t>TC701</t>
+  </si>
+  <si>
+    <t>LISA, Gaps = TRUE, (BaseMap = Satellite)</t>
+  </si>
+  <si>
+    <t>TC706</t>
+  </si>
+  <si>
+    <t>2,7</t>
+  </si>
+  <si>
+    <t>TC719</t>
+  </si>
+  <si>
+    <t>LISA, FOV, Breadcrumbs, Indications, GAP, Asset = TRUE, (BaseMap=Map)</t>
+  </si>
+  <si>
+    <t>TC722</t>
+  </si>
+  <si>
+    <t>TC736</t>
+  </si>
+  <si>
+    <t>LISA, Assets = TRUE</t>
+  </si>
+  <si>
+    <t>TC737</t>
+  </si>
+  <si>
+    <t>Gaps, Assets = TRUE</t>
+  </si>
+  <si>
+    <t>TC786</t>
+  </si>
 </sst>
 </file>
 
@@ -3074,7 +3131,7 @@
   <dimension ref="A1:H578"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3349,7 +3406,32 @@
         <v>309</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
     <row r="12" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -4318,8 +4400,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4452,7 +4534,23 @@
         <v>332</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>343</v>
+      </c>
+    </row>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -14257,8 +14355,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16245,7 +16343,7 @@
         <v>185</v>
       </c>
       <c r="D37" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>52</v>
@@ -16293,136 +16391,714 @@
       </c>
     </row>
     <row r="38" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B38" s="7"/>
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D38" s="2">
+        <v>6</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="H38" s="7"/>
+      <c r="I38" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J38" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K38" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L38" s="7">
+        <v>-121.98390000000001</v>
+      </c>
       <c r="M38" s="7"/>
-    </row>
-    <row r="39" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="M39" s="7"/>
-    </row>
-    <row r="40" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="M40" s="7"/>
-    </row>
-    <row r="41" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="M41" s="7"/>
-    </row>
-    <row r="42" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="M42" s="7"/>
-    </row>
-    <row r="43" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="M43" s="7"/>
-    </row>
-    <row r="44" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="M44" s="7"/>
-    </row>
-    <row r="45" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="M45" s="7"/>
-    </row>
-    <row r="46" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="M46" s="7"/>
-    </row>
-    <row r="47" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="M47" s="7"/>
-    </row>
-    <row r="48" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="M48" s="7"/>
-    </row>
-    <row r="49" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="M49" s="7"/>
-    </row>
-    <row r="50" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="Q38" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R38" s="7">
+        <v>11</v>
+      </c>
+      <c r="S38" s="7">
+        <v>29</v>
+      </c>
+      <c r="T38" s="2">
+        <v>1</v>
+      </c>
+      <c r="U38" s="2">
+        <v>10</v>
+      </c>
+      <c r="V38" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D39" s="7">
+        <v>7</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" s="7">
+        <v>0</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I39" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J39" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K39" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L39" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q39" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R39" s="7">
+        <v>11</v>
+      </c>
+      <c r="S39" s="7">
+        <v>29</v>
+      </c>
+      <c r="T39" s="7">
+        <v>1</v>
+      </c>
+      <c r="U39" s="7">
+        <v>10</v>
+      </c>
+      <c r="V39" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A40" s="7">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D40" s="7">
+        <v>1</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I40" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J40" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K40" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L40" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q40" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R40" s="7">
+        <v>11</v>
+      </c>
+      <c r="S40" s="7">
+        <v>24</v>
+      </c>
+      <c r="T40" s="7">
+        <v>1</v>
+      </c>
+      <c r="U40" s="7">
+        <v>10</v>
+      </c>
+      <c r="V40" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A41" s="7">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D41" s="7">
+        <v>1</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I41" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J41" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K41" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L41" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q41" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R41" s="7">
+        <v>11</v>
+      </c>
+      <c r="S41" s="7">
+        <v>27</v>
+      </c>
+      <c r="T41" s="7">
+        <v>1</v>
+      </c>
+      <c r="U41" s="7">
+        <v>10</v>
+      </c>
+      <c r="V41" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A42" s="7">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D42" s="7">
+        <v>1</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I42" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J42" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K42" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L42" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q42" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R42" s="7">
+        <v>11</v>
+      </c>
+      <c r="S42" s="7">
+        <v>30</v>
+      </c>
+      <c r="T42" s="7">
+        <v>1</v>
+      </c>
+      <c r="U42" s="7">
+        <v>10</v>
+      </c>
+      <c r="V42" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A43" s="7">
+        <v>42</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D43" s="7">
+        <v>1</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I43" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J43" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K43" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L43" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q43" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R43" s="7">
+        <v>11</v>
+      </c>
+      <c r="S43" s="7">
+        <v>24</v>
+      </c>
+      <c r="T43" s="7">
+        <v>1</v>
+      </c>
+      <c r="U43" s="7">
+        <v>10</v>
+      </c>
+      <c r="V43" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A44" s="7">
+        <v>43</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D44" s="7">
+        <v>1</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F44" s="7">
+        <v>0</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I44" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J44" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K44" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L44" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q44" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R44" s="7">
+        <v>11</v>
+      </c>
+      <c r="S44" s="7">
+        <v>31</v>
+      </c>
+      <c r="T44" s="7">
+        <v>1</v>
+      </c>
+      <c r="U44" s="7">
+        <v>10</v>
+      </c>
+      <c r="V44" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A45" s="7">
+        <v>44</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D45" s="7">
+        <v>8</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F45" s="7">
+        <v>0</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I45" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J45" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K45" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L45" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q45" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R45" s="7">
+        <v>11</v>
+      </c>
+      <c r="S45" s="7">
+        <v>32</v>
+      </c>
+      <c r="T45" s="7">
+        <v>1</v>
+      </c>
+      <c r="U45" s="7">
+        <v>10</v>
+      </c>
+      <c r="V45" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A46" s="7">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D46" s="7">
+        <v>1</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F46" s="7">
+        <v>0</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I46" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J46" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K46" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L46" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q46" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R46" s="7">
+        <v>11</v>
+      </c>
+      <c r="S46" s="7">
+        <v>24</v>
+      </c>
+      <c r="T46" s="7">
+        <v>1</v>
+      </c>
+      <c r="U46" s="7">
+        <v>10</v>
+      </c>
+      <c r="V46" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A47" s="7">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D47" s="7">
+        <v>1</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" s="7">
+        <v>0</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I47" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J47" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K47" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L47" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q47" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R47" s="7">
+        <v>11</v>
+      </c>
+      <c r="S47" s="7">
+        <v>33</v>
+      </c>
+      <c r="T47" s="7">
+        <v>1</v>
+      </c>
+      <c r="U47" s="7">
+        <v>10</v>
+      </c>
+      <c r="V47" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A48" s="7">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D48" s="7">
+        <v>1</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F48" s="7">
+        <v>0</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I48" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J48" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K48" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L48" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q48" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R48" s="7">
+        <v>11</v>
+      </c>
+      <c r="S48" s="7">
+        <v>34</v>
+      </c>
+      <c r="T48" s="7">
+        <v>1</v>
+      </c>
+      <c r="U48" s="7">
+        <v>10</v>
+      </c>
+      <c r="V48" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A49" s="7">
+        <v>48</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" s="7">
+        <v>6</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F49" s="7">
+        <v>0</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I49" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J49" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K49" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L49" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="Q49" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R49" s="7">
+        <v>11</v>
+      </c>
+      <c r="S49" s="7">
+        <v>29</v>
+      </c>
+      <c r="T49" s="7">
+        <v>1</v>
+      </c>
+      <c r="U49" s="7">
+        <v>10</v>
+      </c>
+      <c r="V49" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B50" s="7"/>
       <c r="H50" s="7"/>
       <c r="M50" s="7"/>
     </row>
-    <row r="51" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B51" s="7"/>
       <c r="H51" s="7"/>
       <c r="M51" s="7"/>
     </row>
-    <row r="52" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B52" s="7"/>
       <c r="H52" s="7"/>
       <c r="M52" s="7"/>
     </row>
-    <row r="53" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B53" s="7"/>
       <c r="H53" s="7"/>
       <c r="M53" s="7"/>
     </row>
-    <row r="54" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B54" s="7"/>
       <c r="H54" s="7"/>
       <c r="M54" s="7"/>
     </row>
-    <row r="55" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B55" s="7"/>
       <c r="H55" s="7"/>
       <c r="M55" s="7"/>
     </row>
-    <row r="56" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B56" s="7"/>
       <c r="H56" s="7"/>
       <c r="M56" s="7"/>
     </row>
-    <row r="57" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B57" s="7"/>
       <c r="H57" s="7"/>
       <c r="M57" s="7"/>
     </row>
-    <row r="58" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B58" s="7"/>
       <c r="H58" s="7"/>
       <c r="M58" s="7"/>
     </row>
-    <row r="59" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B59" s="7"/>
       <c r="H59" s="7"/>
       <c r="M59" s="7"/>
     </row>
-    <row r="60" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B60" s="7"/>
       <c r="H60" s="7"/>
       <c r="M60" s="7"/>
     </row>
-    <row r="61" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B61" s="7"/>
       <c r="H61" s="7"/>
       <c r="M61" s="7"/>
     </row>
-    <row r="62" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B62" s="7"/>
       <c r="H62" s="7"/>
       <c r="M62" s="7"/>
     </row>
-    <row r="63" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B63" s="7"/>
       <c r="H63" s="7"/>
       <c r="M63" s="7"/>
     </row>
-    <row r="64" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B64" s="7"/>
       <c r="H64" s="7"/>
       <c r="M64" s="7"/>
@@ -26153,7 +26829,7 @@
   <dimension ref="A1:J1138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26680,14 +27356,23 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="D25" s="7" t="s">
+        <v>184</v>
+      </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
+      <c r="G25" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="I25" s="7">
+        <v>2</v>
+      </c>
       <c r="J25" s="7"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -38944,7 +39629,7 @@
           <x14:formula1>
             <xm:f>General!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J1048576 H1:H1048576</xm:sqref>
+          <xm:sqref>H1:H1048576 J2:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -38964,7 +39649,7 @@
   <dimension ref="A1:N800"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40302,24 +40987,239 @@
         <v>329</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="33" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="34" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="35" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="36" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="37" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="38" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="39" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="40" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="41" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="42" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="43" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="44" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="45" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="46" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="47" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="48" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J31" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L31" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J32" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L32" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L33" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L34" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N34" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L35" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="49" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="50" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="51" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
changes for tests + bug fixes in page actions
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="383">
   <si>
     <t>Enabled</t>
   </si>
@@ -579,18 +579,6 @@
   </si>
   <si>
     <t>Report Mode</t>
-  </si>
-  <si>
-    <t>Pacific Time (US and Canada)</t>
-  </si>
-  <si>
-    <t>Mountain Time (US and Canada)</t>
-  </si>
-  <si>
-    <t>Central Time (US and Canada)</t>
-  </si>
-  <si>
-    <t>Eastern Time (US and Canada)</t>
   </si>
   <si>
     <t>Rapid Response</t>
@@ -1568,10 +1556,22 @@
     <t>sqapicsup@picarro.com</t>
   </si>
   <si>
-    <t>TC517 Report793428</t>
+    <t>TC148 Report364651</t>
   </si>
   <si>
-    <t>23,24,25</t>
+    <t>23,24</t>
+  </si>
+  <si>
+    <t>Mountain Standard Time</t>
+  </si>
+  <si>
+    <t>Central Standard Time</t>
+  </si>
+  <si>
+    <t>Eastern Standard Time</t>
+  </si>
+  <si>
+    <t>China Standard Time</t>
   </si>
 </sst>
 </file>
@@ -2150,19 +2150,19 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>359</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2170,10 +2170,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>353</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>357</v>
       </c>
       <c r="D2" s="9">
         <v>1</v>
@@ -2182,7 +2182,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2190,10 +2190,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D3" s="7">
         <v>2</v>
@@ -2202,7 +2202,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -2215,9 +2215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2238,34 +2236,34 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -2273,13 +2271,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E2" s="4">
         <v>42294.500011574077</v>
@@ -2315,7 +2313,7 @@
         <v>42010.500011574077</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -2331,7 +2329,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E4" s="4">
         <v>42294.500011574077</v>
@@ -2360,7 +2358,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -2383,7 +2381,7 @@
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -2406,7 +2404,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -2429,7 +2427,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -2452,7 +2450,7 @@
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -2475,7 +2473,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -2498,7 +2496,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -2521,7 +2519,7 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -2544,7 +2542,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -2567,7 +2565,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -2590,7 +2588,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -2613,7 +2611,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -2636,7 +2634,7 @@
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -2659,7 +2657,7 @@
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -2682,7 +2680,7 @@
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -2705,7 +2703,7 @@
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -2728,7 +2726,7 @@
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -2751,7 +2749,7 @@
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -2774,7 +2772,7 @@
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -2797,7 +2795,7 @@
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -2822,7 +2820,7 @@
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -15111,8 +15109,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15135,43 +15133,43 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15179,7 +15177,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -15212,10 +15210,10 @@
         <v>0</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15223,7 +15221,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -15256,10 +15254,10 @@
         <v>0</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15267,7 +15265,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -15300,10 +15298,10 @@
         <v>0</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15311,7 +15309,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -15344,10 +15342,10 @@
         <v>0</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15355,7 +15353,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -15388,10 +15386,10 @@
         <v>0</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15399,7 +15397,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
@@ -15432,10 +15430,10 @@
         <v>0</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15443,7 +15441,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
@@ -15476,10 +15474,10 @@
         <v>0</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15487,7 +15485,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
@@ -15520,10 +15518,10 @@
         <v>0</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15531,7 +15529,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>
@@ -15564,10 +15562,10 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15575,7 +15573,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>1</v>
@@ -15608,10 +15606,10 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15619,7 +15617,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>1</v>
@@ -15652,10 +15650,10 @@
         <v>0</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15663,7 +15661,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>1</v>
@@ -15696,10 +15694,10 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15707,7 +15705,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>1</v>
@@ -15740,10 +15738,10 @@
         <v>0</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15751,7 +15749,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C15" s="7" t="b">
         <v>0</v>
@@ -15784,10 +15782,10 @@
         <v>0</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15795,7 +15793,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C16" s="7" t="b">
         <v>1</v>
@@ -15828,10 +15826,10 @@
         <v>0</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15839,7 +15837,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C17" s="7" t="b">
         <v>0</v>
@@ -15872,10 +15870,10 @@
         <v>0</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15883,7 +15881,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C18" s="7" t="b">
         <v>0</v>
@@ -15916,10 +15914,10 @@
         <v>0</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15927,7 +15925,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C19" s="7" t="b">
         <v>1</v>
@@ -15960,10 +15958,10 @@
         <v>0</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15971,7 +15969,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C20" s="7" t="b">
         <v>1</v>
@@ -16004,10 +16002,10 @@
         <v>0</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16015,7 +16013,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C21" s="7" t="b">
         <v>1</v>
@@ -16048,10 +16046,10 @@
         <v>0</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16059,7 +16057,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C22" s="7" t="b">
         <v>0</v>
@@ -16092,10 +16090,10 @@
         <v>0</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16103,7 +16101,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C23" s="7" t="b">
         <v>0</v>
@@ -16136,10 +16134,10 @@
         <v>0</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16147,7 +16145,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C24" s="7" t="b">
         <v>0</v>
@@ -16180,10 +16178,10 @@
         <v>0</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16191,7 +16189,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C25" s="2" t="b">
         <v>1</v>
@@ -16224,10 +16222,10 @@
         <v>0</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16235,7 +16233,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C26" s="7" t="b">
         <v>0</v>
@@ -16268,10 +16266,10 @@
         <v>0</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16279,7 +16277,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C27" s="7" t="b">
         <v>0</v>
@@ -16312,10 +16310,10 @@
         <v>0</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="28" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16323,7 +16321,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C28" s="7" t="b">
         <v>0</v>
@@ -16356,10 +16354,10 @@
         <v>0</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16367,7 +16365,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C29" s="7" t="b">
         <v>0</v>
@@ -16400,10 +16398,10 @@
         <v>0</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16411,7 +16409,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C30" s="7" t="b">
         <v>1</v>
@@ -16444,10 +16442,10 @@
         <v>0</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="31" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16455,7 +16453,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C31" s="7" t="b">
         <v>1</v>
@@ -16488,10 +16486,10 @@
         <v>0</v>
       </c>
       <c r="M31" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16499,7 +16497,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C32" s="7" t="b">
         <v>1</v>
@@ -16532,10 +16530,10 @@
         <v>0</v>
       </c>
       <c r="M32" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="33" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16543,7 +16541,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C33" s="7" t="b">
         <v>1</v>
@@ -16576,10 +16574,10 @@
         <v>0</v>
       </c>
       <c r="M33" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="34" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16587,7 +16585,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C34" s="7" t="b">
         <v>1</v>
@@ -16620,10 +16618,10 @@
         <v>0</v>
       </c>
       <c r="M34" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16631,7 +16629,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C35" s="7" t="b">
         <v>0</v>
@@ -16664,10 +16662,10 @@
         <v>0</v>
       </c>
       <c r="M35" s="7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="36" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -17463,7 +17461,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17479,13 +17477,13 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -17493,13 +17491,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -17507,11 +17505,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="7" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -17520,10 +17518,10 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -17533,7 +17531,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="15"/>
       <c r="D5" s="7" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -17541,11 +17539,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="7" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -17555,7 +17553,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="15"/>
       <c r="D7" s="7" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -17563,13 +17561,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C8" s="15">
         <v>5</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -17577,13 +17575,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C9" s="15">
         <v>4</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -17613,16 +17611,16 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -17630,16 +17628,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D2" s="12">
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -17647,16 +17645,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D3" s="12">
         <v>4</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -17664,16 +17662,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D4" s="12">
         <v>4</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -17681,16 +17679,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D5" s="12">
         <v>4</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -17698,16 +17696,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D6" s="12">
         <v>4</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -17715,16 +17713,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D7" s="12">
         <v>4</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -17732,16 +17730,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D8" s="12">
         <v>4</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -17749,16 +17747,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D9" s="12">
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -17766,16 +17764,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D10" s="12">
         <v>1</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -17783,16 +17781,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D11" s="12">
         <v>1</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -17800,16 +17798,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D12" s="12">
         <v>1</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -17817,16 +17815,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D13" s="12">
         <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -17834,16 +17832,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D14" s="12">
         <v>1</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -17851,16 +17849,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D15" s="12">
         <v>5</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -17868,16 +17866,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D16" s="12">
         <v>5</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -17885,16 +17883,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D17" s="12">
         <v>5</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -17902,16 +17900,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D18" s="12">
         <v>5</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -17919,16 +17917,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D19" s="12">
         <v>5</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -17936,16 +17934,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D20" s="12">
         <v>5</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -17953,16 +17951,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D21" s="12">
         <v>5</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -17970,16 +17968,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D22" s="12">
         <v>5</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -18009,16 +18007,16 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -18026,16 +18024,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D2" s="12">
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -18043,16 +18041,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D3" s="12">
         <v>4</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -18060,16 +18058,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -18077,16 +18075,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D5" s="12">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -18094,16 +18092,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D6" s="12">
         <v>5</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -18138,25 +18136,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18182,7 +18180,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18208,7 +18206,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18234,7 +18232,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18260,7 +18258,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18286,7 +18284,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18312,7 +18310,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18338,7 +18336,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18364,7 +18362,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18390,7 +18388,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18416,7 +18414,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -19184,7 +19182,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -19197,8 +19195,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19218,80 +19216,83 @@
         <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>380</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D4" t="s">
         <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>381</v>
       </c>
       <c r="C5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>382</v>
+      </c>
       <c r="C6" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
@@ -19299,7 +19300,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -19327,13 +19328,13 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -19341,7 +19342,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
@@ -19355,7 +19356,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
@@ -19411,22 +19412,22 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>48</v>
@@ -19440,7 +19441,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
@@ -19449,16 +19450,16 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K2" s="2">
         <v>2</v>
@@ -19475,7 +19476,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>1</v>
@@ -19484,17 +19485,17 @@
         <v>9</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K3" s="2">
         <v>2</v>
@@ -19511,7 +19512,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>1</v>
@@ -19520,17 +19521,17 @@
         <v>8</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K4" s="2">
         <v>2</v>
@@ -19547,7 +19548,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>1</v>
@@ -19556,17 +19557,17 @@
         <v>10</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K5" s="2">
         <v>1</v>
@@ -19583,7 +19584,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>1</v>
@@ -19595,10 +19596,10 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
@@ -19612,10 +19613,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
@@ -19624,17 +19625,17 @@
         <v>10</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
@@ -19648,10 +19649,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>1</v>
@@ -19663,10 +19664,10 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K8" s="2">
         <v>4</v>
@@ -19680,10 +19681,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>1</v>
@@ -19695,10 +19696,10 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K9" s="2">
         <v>4</v>
@@ -19712,10 +19713,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>1</v>
@@ -19727,10 +19728,10 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K10" s="2">
         <v>4</v>
@@ -19744,10 +19745,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D11" s="7" t="b">
         <v>1</v>
@@ -19756,17 +19757,17 @@
         <v>10</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K11" s="7">
         <v>1</v>
@@ -19780,10 +19781,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D12" s="7" t="b">
         <v>1</v>
@@ -19792,10 +19793,10 @@
         <v>11</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K12" s="7">
         <v>1</v>
@@ -19873,46 +19874,46 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -19920,7 +19921,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C2" s="7">
         <v>37.402092570550302</v>
@@ -19967,7 +19968,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C3" s="7">
         <v>37.402092570550302</v>
@@ -20014,7 +20015,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C4" s="7">
         <v>37.402092570550302</v>
@@ -20096,16 +20097,16 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20113,13 +20114,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20127,13 +20128,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20141,13 +20142,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20155,13 +20156,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20169,13 +20170,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20183,16 +20184,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20200,16 +20201,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C8" s="7" t="b">
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20217,16 +20218,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C9" s="7" t="b">
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -20279,7 +20280,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -20287,7 +20288,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -20295,7 +20296,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -20311,7 +20312,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -20319,7 +20320,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -20327,7 +20328,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -20335,7 +20336,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -20364,10 +20365,10 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>29</v>
@@ -20381,10 +20382,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>31</v>
@@ -20398,10 +20399,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>31</v>
@@ -20415,10 +20416,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>31</v>
@@ -20432,10 +20433,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>31</v>
@@ -20449,10 +20450,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>31</v>
@@ -20466,10 +20467,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>31</v>
@@ -20483,10 +20484,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>31</v>
@@ -20500,10 +20501,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>31</v>
@@ -20517,10 +20518,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>31</v>
@@ -20534,13 +20535,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>30</v>
@@ -20551,13 +20552,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>30</v>
@@ -20568,13 +20569,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>30</v>
@@ -20585,13 +20586,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>30</v>
@@ -20602,13 +20603,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>30</v>
@@ -20619,13 +20620,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>30</v>
@@ -20636,13 +20637,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>30</v>
@@ -20653,13 +20654,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>30</v>
@@ -20670,13 +20671,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>30</v>
@@ -20687,13 +20688,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>30</v>
@@ -20704,13 +20705,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>30</v>
@@ -20721,13 +20722,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>30</v>
@@ -28112,7 +28113,7 @@
         <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -28133,7 +28134,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>23</v>
@@ -28154,7 +28155,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -28175,7 +28176,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -28196,7 +28197,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>23</v>
@@ -28217,7 +28218,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>27</v>
@@ -28238,7 +28239,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>23</v>
@@ -28259,7 +28260,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>23</v>
@@ -28281,7 +28282,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>23</v>
@@ -28303,7 +28304,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>27</v>
@@ -28325,7 +28326,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>27</v>
@@ -28347,7 +28348,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>27</v>
@@ -28369,7 +28370,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>27</v>
@@ -28391,7 +28392,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>27</v>
@@ -28413,7 +28414,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>27</v>
@@ -28435,7 +28436,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>23</v>
@@ -28456,7 +28457,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>27</v>
@@ -28477,7 +28478,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>23</v>
@@ -28498,7 +28499,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>23</v>
@@ -28519,7 +28520,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>23</v>
@@ -28540,7 +28541,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>27</v>
@@ -28561,7 +28562,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>23</v>
@@ -28582,7 +28583,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>23</v>
@@ -28603,7 +28604,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>23</v>
@@ -28624,7 +28625,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>27</v>
@@ -28645,7 +28646,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>23</v>
@@ -28666,7 +28667,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>23</v>
@@ -28687,7 +28688,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>23</v>
@@ -28708,7 +28709,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>23</v>
@@ -28729,7 +28730,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>23</v>
@@ -28753,7 +28754,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>23</v>
@@ -28774,7 +28775,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>23</v>
@@ -28795,7 +28796,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>23</v>
@@ -28816,7 +28817,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>23</v>
@@ -28836,7 +28837,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>23</v>
@@ -28859,7 +28860,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>27</v>
@@ -28879,7 +28880,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>27</v>
@@ -28899,7 +28900,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>27</v>
@@ -28919,7 +28920,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>27</v>
@@ -28939,7 +28940,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>27</v>
@@ -30033,8 +30034,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P19" workbookViewId="0">
-      <selection activeCell="S51" sqref="S51"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30043,7 +30044,7 @@
     <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.44140625" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.109375" customWidth="1"/>
@@ -30068,7 +30069,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>47</v>
@@ -30086,49 +30087,49 @@
         <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -30137,13 +30138,13 @@
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F2" s="2">
         <v>3</v>
@@ -30162,10 +30163,10 @@
         <v>-122.04883575439401</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="Q2" s="2">
         <v>8.5</v>
@@ -30174,7 +30175,7 @@
         <v>11</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="T2" s="2">
         <v>1</v>
@@ -30183,7 +30184,7 @@
         <v>4</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -30192,23 +30193,23 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>55</v>
+        <v>381</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="H3" s="7"/>
       <c r="M3" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="Q3" s="2">
         <v>8.5</v>
@@ -30217,7 +30218,7 @@
         <v>11</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="T3" s="2">
         <v>5</v>
@@ -30226,7 +30227,7 @@
         <v>2</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -30235,13 +30236,13 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="2">
@@ -30258,10 +30259,10 @@
       </c>
       <c r="M4" s="7"/>
       <c r="O4" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="Q4" s="2">
         <v>8.5</v>
@@ -30270,7 +30271,7 @@
         <v>11</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="T4" s="2">
         <v>1</v>
@@ -30279,7 +30280,7 @@
         <v>4</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -30287,16 +30288,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>185</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -30318,7 +30319,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q5" s="7">
         <v>8.5</v>
@@ -30344,16 +30345,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>185</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F6" s="7">
         <v>0</v>
@@ -30374,7 +30375,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q6" s="7">
         <v>8.5</v>
@@ -30400,16 +30401,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F7" s="7">
         <v>0</v>
@@ -30430,7 +30431,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q7" s="7">
         <v>8.5</v>
@@ -30456,16 +30457,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F8" s="7">
         <v>0</v>
@@ -30489,7 +30490,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q8" s="7">
         <v>8.5</v>
@@ -30515,22 +30516,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F9" s="7">
         <v>0</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I9" s="7">
         <v>37.4206</v>
@@ -30545,7 +30546,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q9" s="7">
         <v>8.5</v>
@@ -30571,16 +30572,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F10" s="7">
         <v>0</v>
@@ -30601,7 +30602,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q10" s="7">
         <v>8.5</v>
@@ -30627,16 +30628,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D11" s="7">
         <v>5</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F11" s="7">
         <v>0</v>
@@ -30685,16 +30686,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D12" s="7">
         <v>5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F12" s="7">
         <v>0</v>
@@ -30735,7 +30736,7 @@
         <v>8</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -30743,16 +30744,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D13" s="7">
         <v>5</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F13" s="7">
         <v>0</v>
@@ -30766,10 +30767,10 @@
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
@@ -30780,7 +30781,7 @@
         <v>11</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="T13" s="7">
         <v>7</v>
@@ -30789,7 +30790,7 @@
         <v>1</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -30797,16 +30798,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D14" s="7">
         <v>5</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F14" s="7">
         <v>0</v>
@@ -30820,10 +30821,10 @@
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
@@ -30851,16 +30852,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D15" s="7">
         <v>1</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F15" s="7">
         <v>0</v>
@@ -30881,7 +30882,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q15" s="7">
         <v>8.5</v>
@@ -30907,16 +30908,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D16" s="7">
         <v>1</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>54</v>
+        <v>380</v>
       </c>
       <c r="F16" s="7">
         <v>0</v>
@@ -30937,7 +30938,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q16" s="7">
         <v>8.5</v>
@@ -30946,7 +30947,7 @@
         <v>11</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="T16" s="7">
         <v>8</v>
@@ -30963,16 +30964,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D17" s="7">
         <v>1</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F17" s="7">
         <v>0</v>
@@ -30981,10 +30982,10 @@
         <v>26</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="Q17" s="7">
         <v>8.5</v>
@@ -31010,16 +31011,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D18" s="7">
         <v>1</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F18" s="7">
         <v>3</v>
@@ -31046,7 +31047,7 @@
         <v>11</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="T18" s="7">
         <v>1</v>
@@ -31063,16 +31064,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D19" s="7">
         <v>1</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F19" s="7">
         <v>0</v>
@@ -31116,16 +31117,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D20" s="7">
         <v>1</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F20" s="7">
         <v>0</v>
@@ -31169,16 +31170,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D21" s="7">
         <v>1</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F21" s="7">
         <v>0</v>
@@ -31227,16 +31228,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D22" s="7">
         <v>1</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F22" s="7">
         <v>0</v>
@@ -31250,10 +31251,10 @@
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
@@ -31264,7 +31265,7 @@
         <v>11</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="T22" s="7">
         <v>4</v>
@@ -31281,16 +31282,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D23" s="7">
         <v>1</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F23" s="7">
         <v>0</v>
@@ -31322,7 +31323,7 @@
         <v>11</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="T23" s="7">
         <v>8</v>
@@ -31339,7 +31340,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="H24" s="7"/>
       <c r="M24" s="7"/>
@@ -31349,16 +31350,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D25" s="7">
         <v>1</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F25" s="7">
         <v>0</v>
@@ -31407,16 +31408,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D26" s="7">
         <v>1</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F26" s="7">
         <v>0</v>
@@ -31465,16 +31466,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D27" s="7">
         <v>1</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F27" s="7">
         <v>0</v>
@@ -31523,16 +31524,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D28" s="7">
         <v>1</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F28" s="7">
         <v>0</v>
@@ -31581,16 +31582,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D29" s="7">
         <v>1</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F29" s="7">
         <v>0</v>
@@ -31639,16 +31640,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D30" s="7">
         <v>1</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F30" s="7">
         <v>0</v>
@@ -31697,16 +31698,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D31" s="7">
         <v>1</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F31" s="7">
         <v>0</v>
@@ -31750,16 +31751,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D32" s="7">
         <v>1</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F32" s="7">
         <v>0</v>
@@ -31803,16 +31804,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D33" s="7">
         <v>1</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F33" s="7">
         <v>0</v>
@@ -31856,16 +31857,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D34" s="7">
         <v>1</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F34" s="7">
         <v>0</v>
@@ -31909,16 +31910,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D35" s="7">
         <v>1</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F35" s="7">
         <v>0</v>
@@ -31962,16 +31963,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D36" s="7">
         <v>1</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F36" s="7">
         <v>0</v>
@@ -31998,7 +31999,7 @@
         <v>11</v>
       </c>
       <c r="S36" s="7" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="T36" s="7">
         <v>1</v>
@@ -32015,16 +32016,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D37" s="2">
         <v>2</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F37" s="2">
         <v>0</v>
@@ -32073,16 +32074,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D38" s="2">
         <v>6</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F38" s="2">
         <v>0</v>
@@ -32128,16 +32129,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D39" s="7">
         <v>7</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="F39" s="7">
         <v>0</v>
@@ -32181,16 +32182,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D40" s="7">
         <v>1</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F40" s="7">
         <v>0</v>
@@ -32234,16 +32235,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D41" s="7">
         <v>1</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F41" s="7">
         <v>0</v>
@@ -32287,16 +32288,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D42" s="7">
         <v>1</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F42" s="7">
         <v>0</v>
@@ -32340,16 +32341,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D43" s="7">
         <v>1</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F43" s="7">
         <v>0</v>
@@ -32393,16 +32394,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D44" s="7">
         <v>1</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F44" s="7">
         <v>0</v>
@@ -32446,16 +32447,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D45" s="7">
         <v>8</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F45" s="7">
         <v>0</v>
@@ -32499,16 +32500,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D46" s="7">
         <v>1</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F46" s="7">
         <v>0</v>
@@ -32552,16 +32553,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D47" s="7">
         <v>1</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F47" s="7">
         <v>0</v>
@@ -32605,16 +32606,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D48" s="7">
         <v>1</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F48" s="7">
         <v>0</v>
@@ -32658,16 +32659,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D49" s="7">
         <v>6</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>53</v>
+        <v>379</v>
       </c>
       <c r="F49" s="7">
         <v>0</v>
@@ -32711,16 +32712,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D50" s="7">
         <v>1</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>53</v>
+        <v>166</v>
       </c>
       <c r="F50" s="7">
         <v>0</v>
@@ -32742,7 +32743,7 @@
         <v>-121.98390000000001</v>
       </c>
       <c r="M50" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N50" s="7"/>
       <c r="O50" s="7"/>
@@ -32754,7 +32755,7 @@
         <v>11</v>
       </c>
       <c r="S50" s="7" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="T50" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
add support for new report job type=ZIP
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -1013,9 +1013,6 @@
     <t>6,8,13,14,15</t>
   </si>
   <si>
-    <t>5,11,16,17,18,21</t>
-  </si>
-  <si>
     <t>LISA, Breadcrumbs and Assets TRUE</t>
   </si>
   <si>
@@ -1572,6 +1569,9 @@
   </si>
   <si>
     <t>China Standard Time</t>
+  </si>
+  <si>
+    <t>11,16,17,18,21</t>
   </si>
 </sst>
 </file>
@@ -2150,19 +2150,19 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2170,10 +2170,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D2" s="9">
         <v>1</v>
@@ -2182,7 +2182,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2190,10 +2190,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>361</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>362</v>
       </c>
       <c r="D3" s="7">
         <v>2</v>
@@ -2202,7 +2202,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -2260,10 +2260,10 @@
         <v>107</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -2381,7 +2381,7 @@
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -2404,7 +2404,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -2427,7 +2427,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -2450,7 +2450,7 @@
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -2473,7 +2473,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -2496,7 +2496,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -2519,7 +2519,7 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -2542,7 +2542,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -2565,7 +2565,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -2588,7 +2588,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -2611,7 +2611,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -2634,7 +2634,7 @@
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -2657,7 +2657,7 @@
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -2680,7 +2680,7 @@
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -2703,7 +2703,7 @@
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -2726,7 +2726,7 @@
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -2749,7 +2749,7 @@
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -2772,7 +2772,7 @@
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -15109,8 +15109,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15389,7 +15389,7 @@
         <v>87</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15433,7 +15433,7 @@
         <v>88</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15477,7 +15477,7 @@
         <v>87</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15521,7 +15521,7 @@
         <v>88</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15741,7 +15741,7 @@
         <v>87</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15785,7 +15785,7 @@
         <v>87</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15829,7 +15829,7 @@
         <v>88</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15873,7 +15873,7 @@
         <v>87</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15917,7 +15917,7 @@
         <v>88</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15961,7 +15961,7 @@
         <v>87</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16005,7 +16005,7 @@
         <v>88</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16049,7 +16049,7 @@
         <v>87</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16093,7 +16093,7 @@
         <v>87</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16137,7 +16137,7 @@
         <v>87</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16181,7 +16181,7 @@
         <v>87</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16225,7 +16225,7 @@
         <v>87</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16269,7 +16269,7 @@
         <v>87</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16313,7 +16313,7 @@
         <v>87</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="28" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16357,7 +16357,7 @@
         <v>87</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="29" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16401,7 +16401,7 @@
         <v>87</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16445,7 +16445,7 @@
         <v>87</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="31" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16489,7 +16489,7 @@
         <v>88</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16533,7 +16533,7 @@
         <v>88</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="33" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16577,7 +16577,7 @@
         <v>87</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="34" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16621,7 +16621,7 @@
         <v>87</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16665,7 +16665,7 @@
         <v>87</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="36" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -17477,13 +17477,13 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -17491,13 +17491,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>251</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -17505,11 +17505,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -17518,10 +17518,10 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -17531,7 +17531,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="15"/>
       <c r="D5" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -17539,11 +17539,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -17553,7 +17553,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="15"/>
       <c r="D7" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -17561,13 +17561,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C8" s="15">
         <v>5</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -17575,13 +17575,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C9" s="15">
         <v>4</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -17611,16 +17611,16 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -17628,16 +17628,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D2" s="12">
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -17645,16 +17645,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D3" s="12">
         <v>4</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -17662,16 +17662,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D4" s="12">
         <v>4</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -17679,16 +17679,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D5" s="12">
         <v>4</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -17696,16 +17696,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D6" s="12">
         <v>4</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -17713,16 +17713,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D7" s="12">
         <v>4</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -17730,16 +17730,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D8" s="12">
         <v>4</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -17747,16 +17747,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D9" s="12">
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -17764,16 +17764,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D10" s="12">
         <v>1</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -17781,16 +17781,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D11" s="12">
         <v>1</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -17798,16 +17798,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D12" s="12">
         <v>1</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -17815,16 +17815,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D13" s="12">
         <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -17832,16 +17832,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D14" s="12">
         <v>1</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -17849,16 +17849,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D15" s="12">
         <v>5</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -17866,16 +17866,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D16" s="12">
         <v>5</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -17883,16 +17883,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D17" s="12">
         <v>5</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -17900,16 +17900,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D18" s="12">
         <v>5</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -17917,16 +17917,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D19" s="12">
         <v>5</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -17934,16 +17934,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D20" s="12">
         <v>5</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -17951,16 +17951,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D21" s="12">
         <v>5</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -17968,16 +17968,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D22" s="12">
         <v>5</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -18007,16 +18007,16 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -18024,7 +18024,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>61</v>
@@ -18033,7 +18033,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -18041,7 +18041,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>60</v>
@@ -18050,7 +18050,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -18058,16 +18058,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -18075,16 +18075,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D5" s="12">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -18092,7 +18092,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>189</v>
@@ -18101,7 +18101,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -18388,7 +18388,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18414,7 +18414,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -19244,7 +19244,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B3" t="s">
         <v>52</v>
@@ -19261,7 +19261,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
@@ -19278,10 +19278,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D5" t="s">
         <v>52</v>
@@ -19289,10 +19289,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
@@ -19328,13 +19328,13 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -19342,7 +19342,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
@@ -19356,7 +19356,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
@@ -19441,7 +19441,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
@@ -19476,7 +19476,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>1</v>
@@ -19512,7 +19512,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>1</v>
@@ -19548,7 +19548,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>1</v>
@@ -19584,7 +19584,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>1</v>
@@ -19616,7 +19616,7 @@
         <v>141</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
@@ -19652,7 +19652,7 @@
         <v>131</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>1</v>
@@ -19684,7 +19684,7 @@
         <v>132</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>1</v>
@@ -19716,7 +19716,7 @@
         <v>133</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>1</v>
@@ -19748,7 +19748,7 @@
         <v>141</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D11" s="7" t="b">
         <v>1</v>
@@ -19781,10 +19781,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D12" s="7" t="b">
         <v>1</v>
@@ -19883,37 +19883,37 @@
         <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>373</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -20170,7 +20170,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
@@ -20193,7 +20193,7 @@
         <v>149</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20210,7 +20210,7 @@
         <v>149</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20227,7 +20227,7 @@
         <v>149</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -20728,7 +20728,7 @@
         <v>130</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>30</v>
@@ -30034,8 +30034,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30199,7 +30199,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -30242,7 +30242,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="2">
@@ -30297,7 +30297,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -30354,7 +30354,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F6" s="7">
         <v>0</v>
@@ -30410,7 +30410,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F7" s="7">
         <v>0</v>
@@ -30466,7 +30466,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F8" s="7">
         <v>0</v>
@@ -30516,7 +30516,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>181</v>
@@ -30525,7 +30525,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F9" s="7">
         <v>0</v>
@@ -30572,7 +30572,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>181</v>
@@ -30581,7 +30581,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F10" s="7">
         <v>0</v>
@@ -30736,7 +30736,7 @@
         <v>8</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>196</v>
+        <v>382</v>
       </c>
     </row>
     <row r="13" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -30781,7 +30781,7 @@
         <v>11</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T13" s="7">
         <v>7</v>
@@ -30852,7 +30852,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>181</v>
@@ -30861,7 +30861,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F15" s="7">
         <v>0</v>
@@ -30908,7 +30908,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>181</v>
@@ -30917,7 +30917,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F16" s="7">
         <v>0</v>
@@ -30947,7 +30947,7 @@
         <v>11</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="T16" s="7">
         <v>8</v>
@@ -30964,7 +30964,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>181</v>
@@ -30973,7 +30973,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F17" s="7">
         <v>0</v>
@@ -30982,10 +30982,10 @@
         <v>26</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q17" s="7">
         <v>8.5</v>
@@ -31011,7 +31011,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>181</v>
@@ -31047,7 +31047,7 @@
         <v>11</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="T18" s="7">
         <v>1</v>
@@ -31064,7 +31064,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>181</v>
@@ -31073,7 +31073,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F19" s="7">
         <v>0</v>
@@ -31117,7 +31117,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>181</v>
@@ -31126,7 +31126,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F20" s="7">
         <v>0</v>
@@ -31170,7 +31170,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>181</v>
@@ -31179,7 +31179,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F21" s="7">
         <v>0</v>
@@ -31228,7 +31228,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>181</v>
@@ -31237,7 +31237,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F22" s="7">
         <v>0</v>
@@ -31251,10 +31251,10 @@
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
@@ -31265,7 +31265,7 @@
         <v>11</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="T22" s="7">
         <v>4</v>
@@ -31282,7 +31282,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>181</v>
@@ -31323,7 +31323,7 @@
         <v>11</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="T23" s="7">
         <v>8</v>
@@ -31340,7 +31340,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H24" s="7"/>
       <c r="M24" s="7"/>
@@ -31350,7 +31350,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>181</v>
@@ -31408,7 +31408,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>181</v>
@@ -31466,7 +31466,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>181</v>
@@ -31524,7 +31524,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>181</v>
@@ -31582,7 +31582,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>181</v>
@@ -31640,7 +31640,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>181</v>
@@ -31698,7 +31698,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>181</v>
@@ -31751,7 +31751,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>181</v>
@@ -31804,7 +31804,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>181</v>
@@ -31857,7 +31857,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>181</v>
@@ -31910,7 +31910,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>181</v>
@@ -31963,7 +31963,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>181</v>
@@ -31999,7 +31999,7 @@
         <v>11</v>
       </c>
       <c r="S36" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="T36" s="7">
         <v>1</v>
@@ -32016,7 +32016,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>181</v>
@@ -32074,7 +32074,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>181</v>
@@ -32129,7 +32129,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>181</v>
@@ -32182,7 +32182,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>181</v>
@@ -32191,7 +32191,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F40" s="7">
         <v>0</v>
@@ -32235,7 +32235,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>181</v>
@@ -32244,7 +32244,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F41" s="7">
         <v>0</v>
@@ -32288,7 +32288,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>181</v>
@@ -32297,7 +32297,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F42" s="7">
         <v>0</v>
@@ -32341,7 +32341,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>181</v>
@@ -32350,7 +32350,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F43" s="7">
         <v>0</v>
@@ -32394,7 +32394,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>181</v>
@@ -32403,7 +32403,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F44" s="7">
         <v>0</v>
@@ -32447,7 +32447,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>181</v>
@@ -32456,7 +32456,7 @@
         <v>8</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F45" s="7">
         <v>0</v>
@@ -32500,7 +32500,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>181</v>
@@ -32509,7 +32509,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F46" s="7">
         <v>0</v>
@@ -32553,7 +32553,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>181</v>
@@ -32562,7 +32562,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F47" s="7">
         <v>0</v>
@@ -32606,7 +32606,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>181</v>
@@ -32615,7 +32615,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F48" s="7">
         <v>0</v>
@@ -32659,7 +32659,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>181</v>
@@ -32668,7 +32668,7 @@
         <v>6</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F49" s="7">
         <v>0</v>
@@ -32712,10 +32712,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D50" s="7">
         <v>1</v>
@@ -32755,7 +32755,7 @@
         <v>11</v>
       </c>
       <c r="S50" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="T50" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
perf test case fixes
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -81,7 +81,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Shirish Pulikkal:
 </t>
@@ -157,7 +157,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Shirish Pulikkal:</t>
         </r>
@@ -166,7 +166,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -186,7 +186,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> 2 entries for the same test case are for Copy Compliance scenario.
 </t>
@@ -241,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V14" authorId="0" shapeId="0">
+    <comment ref="B20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -249,7 +249,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Shirish Pulikkal:</t>
         </r>
@@ -258,32 +258,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Over 700 survey tags in this test case. Don't have the tags in TC. Using first perf survey tag for now.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B20" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Shirish Pulikkal:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -303,7 +278,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> 2 entries for the same test case are for Copy Compliance scenario.
 </t>
@@ -423,7 +398,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="384">
   <si>
     <t>Enabled</t>
   </si>
@@ -1016,9 +991,6 @@
     <t>LISA, Breadcrumbs and Assets TRUE</t>
   </si>
   <si>
-    <t>12,13</t>
-  </si>
-  <si>
     <t>Centerpoint</t>
   </si>
   <si>
@@ -1026,33 +998,6 @@
   </si>
   <si>
     <t>oeHwHqmv621dZ1MRE2BSdw==</t>
-  </si>
-  <si>
-    <t>perf1</t>
-  </si>
-  <si>
-    <t>perf2</t>
-  </si>
-  <si>
-    <t>perf3</t>
-  </si>
-  <si>
-    <t>perf4</t>
-  </si>
-  <si>
-    <t>perf5</t>
-  </si>
-  <si>
-    <t>perf6</t>
-  </si>
-  <si>
-    <t>perf7</t>
-  </si>
-  <si>
-    <t>perf8</t>
-  </si>
-  <si>
-    <t>perf9</t>
   </si>
   <si>
     <t>perf10</t>
@@ -1571,7 +1516,40 @@
     <t>China Standard Time</t>
   </si>
   <si>
-    <t>11,16,17,18,21</t>
+    <t>perf01</t>
+  </si>
+  <si>
+    <t>perf02</t>
+  </si>
+  <si>
+    <t>perf03</t>
+  </si>
+  <si>
+    <t>perf04</t>
+  </si>
+  <si>
+    <t>perf05</t>
+  </si>
+  <si>
+    <t>perf06</t>
+  </si>
+  <si>
+    <t>perf07</t>
+  </si>
+  <si>
+    <t>perf08</t>
+  </si>
+  <si>
+    <t>perf09</t>
+  </si>
+  <si>
+    <t>5,11,16,17,18,21</t>
+  </si>
+  <si>
+    <t>Over700</t>
+  </si>
+  <si>
+    <t>11,13</t>
   </si>
 </sst>
 </file>
@@ -1581,7 +1559,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1628,19 +1606,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1791,16 +1756,16 @@
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1839,7 +1804,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1 2" xfId="7"/>
@@ -2150,19 +2115,19 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2170,10 +2135,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="D2" s="9">
         <v>1</v>
@@ -2182,7 +2147,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2190,10 +2155,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="D3" s="7">
         <v>2</v>
@@ -2202,7 +2167,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -2215,7 +2180,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1138"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2260,10 +2227,10 @@
         <v>107</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -2381,12 +2348,14 @@
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>201</v>
+        <v>372</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="H6" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I6" s="7">
         <v>-1</v>
       </c>
@@ -2404,12 +2373,14 @@
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>202</v>
+        <v>373</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I7" s="7">
         <v>-1</v>
       </c>
@@ -2427,12 +2398,14 @@
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>203</v>
+        <v>374</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I8" s="7">
         <v>-1</v>
       </c>
@@ -2450,12 +2423,14 @@
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>204</v>
+        <v>375</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="H9" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I9" s="7">
         <v>-1</v>
       </c>
@@ -2473,12 +2448,14 @@
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>205</v>
+        <v>376</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I10" s="7">
         <v>-1</v>
       </c>
@@ -2496,12 +2473,14 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>206</v>
+        <v>377</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I11" s="7">
         <v>-1</v>
       </c>
@@ -2519,12 +2498,14 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>207</v>
+        <v>378</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I12" s="7">
         <v>-1</v>
       </c>
@@ -2542,12 +2523,14 @@
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>208</v>
+        <v>379</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I13" s="7">
         <v>-1</v>
       </c>
@@ -2565,12 +2548,14 @@
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>209</v>
+        <v>380</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="H14" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I14" s="7">
         <v>-1</v>
       </c>
@@ -2588,12 +2573,14 @@
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="H15" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I15" s="7">
         <v>-1</v>
       </c>
@@ -2611,12 +2598,14 @@
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="H16" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I16" s="7">
         <v>-1</v>
       </c>
@@ -2634,12 +2623,14 @@
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I17" s="7">
         <v>-1</v>
       </c>
@@ -2657,12 +2648,14 @@
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="H18" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I18" s="7">
         <v>-1</v>
       </c>
@@ -2680,12 +2673,14 @@
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="H19" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I19" s="7">
         <v>-1</v>
       </c>
@@ -2703,12 +2698,14 @@
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="H20" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I20" s="7">
         <v>-1</v>
       </c>
@@ -2726,12 +2723,14 @@
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="H21" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I21" s="7">
         <v>-1</v>
       </c>
@@ -2749,12 +2748,14 @@
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="H22" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I22" s="7">
         <v>-1</v>
       </c>
@@ -2772,12 +2773,14 @@
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
+      <c r="H23" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="I23" s="7">
         <v>-1</v>
       </c>
@@ -2837,15 +2840,29 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="D26" s="7" t="s">
+        <v>382</v>
+      </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
+      <c r="H26" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="7">
+        <v>-1</v>
+      </c>
+      <c r="J26" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
@@ -15110,7 +15127,7 @@
   <dimension ref="A1:N800"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15389,7 +15406,7 @@
         <v>87</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15433,7 +15450,7 @@
         <v>88</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15477,7 +15494,7 @@
         <v>87</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15521,7 +15538,7 @@
         <v>88</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15785,7 +15802,7 @@
         <v>87</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15829,7 +15846,7 @@
         <v>88</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15873,7 +15890,7 @@
         <v>87</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15917,7 +15934,7 @@
         <v>88</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15961,7 +15978,7 @@
         <v>87</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16005,7 +16022,7 @@
         <v>88</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16049,7 +16066,7 @@
         <v>87</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16093,7 +16110,7 @@
         <v>87</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16137,7 +16154,7 @@
         <v>87</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16181,7 +16198,7 @@
         <v>87</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16225,7 +16242,7 @@
         <v>87</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="26" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16269,7 +16286,7 @@
         <v>87</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16313,7 +16330,7 @@
         <v>87</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16357,7 +16374,7 @@
         <v>87</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="29" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16401,7 +16418,7 @@
         <v>87</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16445,7 +16462,7 @@
         <v>87</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="31" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16489,7 +16506,7 @@
         <v>88</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16533,7 +16550,7 @@
         <v>88</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16577,7 +16594,7 @@
         <v>87</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
     </row>
     <row r="34" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16621,7 +16638,7 @@
         <v>87</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16665,7 +16682,7 @@
         <v>87</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="36" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -17477,13 +17494,13 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -17491,13 +17508,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -17505,11 +17522,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="7" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -17518,10 +17535,10 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="15" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -17531,7 +17548,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="15"/>
       <c r="D5" s="7" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -17539,11 +17556,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="7" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -17553,7 +17570,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="15"/>
       <c r="D7" s="7" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -17561,13 +17578,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C8" s="15">
         <v>5</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -17575,13 +17592,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C9" s="15">
         <v>4</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -17611,16 +17628,16 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -17628,16 +17645,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="D2" s="12">
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -17645,16 +17662,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D3" s="12">
         <v>4</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -17662,16 +17679,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D4" s="12">
         <v>4</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -17679,16 +17696,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="D5" s="12">
         <v>4</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -17696,16 +17713,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="D6" s="12">
         <v>4</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -17713,16 +17730,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="D7" s="12">
         <v>4</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -17730,16 +17747,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D8" s="12">
         <v>4</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -17747,16 +17764,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="D9" s="12">
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -17764,16 +17781,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D10" s="12">
         <v>1</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -17781,16 +17798,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D11" s="12">
         <v>1</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -17798,16 +17815,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="D12" s="12">
         <v>1</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -17815,16 +17832,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D13" s="12">
         <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -17832,16 +17849,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="D14" s="12">
         <v>1</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -17849,16 +17866,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="D15" s="12">
         <v>5</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -17866,16 +17883,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="D16" s="12">
         <v>5</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -17883,16 +17900,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D17" s="12">
         <v>5</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -17900,16 +17917,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="D18" s="12">
         <v>5</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -17917,16 +17934,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D19" s="12">
         <v>5</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -17934,16 +17951,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D20" s="12">
         <v>5</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -17951,16 +17968,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="D21" s="12">
         <v>5</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -17968,16 +17985,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="D22" s="12">
         <v>5</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -18007,16 +18024,16 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -18024,7 +18041,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>61</v>
@@ -18033,7 +18050,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -18041,7 +18058,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>60</v>
@@ -18050,7 +18067,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -18058,16 +18075,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -18075,16 +18092,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D5" s="12">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -18092,7 +18109,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>189</v>
@@ -18101,7 +18118,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -18116,7 +18133,7 @@
   <dimension ref="A1:H578"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18388,7 +18405,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18414,7 +18431,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -19244,7 +19261,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="B3" t="s">
         <v>52</v>
@@ -19261,7 +19278,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
@@ -19278,10 +19295,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C5" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D5" t="s">
         <v>52</v>
@@ -19289,10 +19306,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="C6" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
@@ -19328,13 +19345,13 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -19342,7 +19359,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
@@ -19356,7 +19373,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
@@ -19376,7 +19393,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19441,7 +19458,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
@@ -19476,7 +19493,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>1</v>
@@ -19512,7 +19529,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>1</v>
@@ -19548,7 +19565,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>1</v>
@@ -19584,7 +19601,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>1</v>
@@ -19616,7 +19633,7 @@
         <v>141</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
@@ -19652,7 +19669,7 @@
         <v>131</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>1</v>
@@ -19684,7 +19701,7 @@
         <v>132</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>1</v>
@@ -19716,7 +19733,7 @@
         <v>133</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>1</v>
@@ -19748,7 +19765,7 @@
         <v>141</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D11" s="7" t="b">
         <v>1</v>
@@ -19781,10 +19798,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D12" s="7" t="b">
         <v>1</v>
@@ -19883,37 +19900,37 @@
         <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -20170,7 +20187,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
@@ -20193,7 +20210,7 @@
         <v>149</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20210,7 +20227,7 @@
         <v>149</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20227,7 +20244,7 @@
         <v>149</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -20728,7 +20745,7 @@
         <v>130</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>30</v>
@@ -28074,8 +28091,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H1072"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30034,8 +30051,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N14" sqref="M14:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30199,7 +30216,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -30242,7 +30259,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="2">
@@ -30297,7 +30314,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -30354,7 +30371,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F6" s="7">
         <v>0</v>
@@ -30410,7 +30427,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F7" s="7">
         <v>0</v>
@@ -30466,7 +30483,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F8" s="7">
         <v>0</v>
@@ -30516,7 +30533,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>181</v>
@@ -30525,7 +30542,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F9" s="7">
         <v>0</v>
@@ -30572,7 +30589,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>181</v>
@@ -30581,7 +30598,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F10" s="7">
         <v>0</v>
@@ -30714,7 +30731,7 @@
         <v>29.7362085557276</v>
       </c>
       <c r="L12" s="7">
-        <v>95.381543693542397</v>
+        <v>-95.381543693542397</v>
       </c>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
@@ -30736,7 +30753,7 @@
         <v>8</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -30781,13 +30798,13 @@
         <v>11</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>197</v>
+        <v>383</v>
       </c>
       <c r="T13" s="7">
         <v>7</v>
       </c>
       <c r="U13" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="V13" s="7" t="s">
         <v>195</v>
@@ -30816,16 +30833,20 @@
         <v>26</v>
       </c>
       <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>190</v>
-      </c>
+      <c r="I14" s="7">
+        <v>29.757819448754098</v>
+      </c>
+      <c r="J14" s="7">
+        <v>-95.353906211853001</v>
+      </c>
+      <c r="K14" s="7">
+        <v>29.7362085557276</v>
+      </c>
+      <c r="L14" s="7">
+        <v>-95.381543693542397</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="7">
@@ -30844,7 +30865,7 @@
         <v>8</v>
       </c>
       <c r="V14" s="7">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:22" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -30852,7 +30873,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>181</v>
@@ -30861,7 +30882,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F15" s="7">
         <v>0</v>
@@ -30908,7 +30929,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>181</v>
@@ -30917,7 +30938,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="F16" s="7">
         <v>0</v>
@@ -30947,7 +30968,7 @@
         <v>11</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="T16" s="7">
         <v>8</v>
@@ -30964,7 +30985,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>181</v>
@@ -30973,7 +30994,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F17" s="7">
         <v>0</v>
@@ -30982,10 +31003,10 @@
         <v>26</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="Q17" s="7">
         <v>8.5</v>
@@ -31011,7 +31032,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>181</v>
@@ -31047,7 +31068,7 @@
         <v>11</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="T18" s="7">
         <v>1</v>
@@ -31064,7 +31085,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>181</v>
@@ -31073,7 +31094,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F19" s="7">
         <v>0</v>
@@ -31117,7 +31138,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>181</v>
@@ -31126,7 +31147,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F20" s="7">
         <v>0</v>
@@ -31170,7 +31191,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>181</v>
@@ -31179,7 +31200,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F21" s="7">
         <v>0</v>
@@ -31228,7 +31249,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>181</v>
@@ -31237,7 +31258,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F22" s="7">
         <v>0</v>
@@ -31251,10 +31272,10 @@
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
@@ -31265,7 +31286,7 @@
         <v>11</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="T22" s="7">
         <v>4</v>
@@ -31282,7 +31303,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>181</v>
@@ -31323,7 +31344,7 @@
         <v>11</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="T23" s="7">
         <v>8</v>
@@ -31340,7 +31361,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="H24" s="7"/>
       <c r="M24" s="7"/>
@@ -31350,7 +31371,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>181</v>
@@ -31408,7 +31429,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>181</v>
@@ -31466,7 +31487,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>181</v>
@@ -31524,7 +31545,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>181</v>
@@ -31582,7 +31603,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>181</v>
@@ -31640,7 +31661,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>181</v>
@@ -31698,7 +31719,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>181</v>
@@ -31751,7 +31772,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>181</v>
@@ -31804,7 +31825,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>181</v>
@@ -31857,7 +31878,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>181</v>
@@ -31910,7 +31931,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>181</v>
@@ -31963,7 +31984,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>181</v>
@@ -31999,7 +32020,7 @@
         <v>11</v>
       </c>
       <c r="S36" s="7" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="T36" s="7">
         <v>1</v>
@@ -32016,7 +32037,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>181</v>
@@ -32074,7 +32095,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>181</v>
@@ -32129,7 +32150,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>181</v>
@@ -32182,7 +32203,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>181</v>
@@ -32191,7 +32212,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F40" s="7">
         <v>0</v>
@@ -32235,7 +32256,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>181</v>
@@ -32244,7 +32265,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F41" s="7">
         <v>0</v>
@@ -32288,7 +32309,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>181</v>
@@ -32297,7 +32318,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F42" s="7">
         <v>0</v>
@@ -32341,7 +32362,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>181</v>
@@ -32350,7 +32371,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F43" s="7">
         <v>0</v>
@@ -32394,7 +32415,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>181</v>
@@ -32403,7 +32424,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F44" s="7">
         <v>0</v>
@@ -32447,7 +32468,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>181</v>
@@ -32456,7 +32477,7 @@
         <v>8</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F45" s="7">
         <v>0</v>
@@ -32500,7 +32521,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>181</v>
@@ -32509,7 +32530,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F46" s="7">
         <v>0</v>
@@ -32553,7 +32574,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>181</v>
@@ -32562,7 +32583,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F47" s="7">
         <v>0</v>
@@ -32606,7 +32627,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>181</v>
@@ -32615,7 +32636,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F48" s="7">
         <v>0</v>
@@ -32659,7 +32680,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>181</v>
@@ -32668,7 +32689,7 @@
         <v>6</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="F49" s="7">
         <v>0</v>
@@ -32712,10 +32733,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="D50" s="7">
         <v>1</v>
@@ -32755,7 +32776,7 @@
         <v>11</v>
       </c>
       <c r="S50" s="7" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="T50" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
Added tests for compliance reports on test page 3
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="390">
   <si>
     <t>Enabled</t>
   </si>
@@ -1574,22 +1574,25 @@
     <t>China Standard Time</t>
   </si>
   <si>
-    <t>TC1319</t>
-  </si>
-  <si>
-    <t>TC1319 Report</t>
-  </si>
-  <si>
     <t>TESTPlat-Auto-1.5km</t>
-  </si>
-  <si>
-    <t>24,25,26</t>
   </si>
   <si>
     <t>stnd-pic</t>
   </si>
   <si>
     <t>iso-cap</t>
+  </si>
+  <si>
+    <t>TC1319TC1320</t>
+  </si>
+  <si>
+    <t>23,25,26</t>
+  </si>
+  <si>
+    <t>29,26</t>
+  </si>
+  <si>
+    <t>23,26,25,29</t>
   </si>
 </sst>
 </file>
@@ -2236,8 +2239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25:K27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2866,7 +2869,7 @@
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -2881,10 +2884,13 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="20">
+        <v>26</v>
+      </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -2898,38 +2904,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
+    <row r="28" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="20">
+        <v>27</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20">
+        <v>3</v>
+      </c>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="20">
+        <v>28</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20">
+        <v>2</v>
+      </c>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="20">
+        <v>29</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20">
+        <v>1</v>
+      </c>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
@@ -15130,7 +15172,7 @@
           <x14:formula1>
             <xm:f>General!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576 J2:J1048576</xm:sqref>
+          <xm:sqref>J2:J1048576 H1:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -19416,7 +19458,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28114,7 +28156,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H1072"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A62" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -30074,14 +30116,14 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView topLeftCell="D73" workbookViewId="0">
-      <selection activeCell="I104" sqref="I104"/>
+    <sheetView topLeftCell="O79" workbookViewId="0">
+      <selection activeCell="V106" sqref="V106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="30.44140625" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
@@ -30101,7 +30143,7 @@
     <col min="19" max="19" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -33062,10 +33104,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="21" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C101" s="20" t="s">
-        <v>384</v>
+        <v>103</v>
       </c>
       <c r="D101" s="21">
         <v>1</v>
@@ -33088,7 +33130,7 @@
         <v>241</v>
       </c>
       <c r="N101" s="19" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="O101" s="21">
         <v>0.5</v>
@@ -33112,46 +33154,308 @@
         <v>1</v>
       </c>
       <c r="V101" s="21" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="102" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B102" s="7"/>
-      <c r="H102" s="7"/>
-      <c r="M102" s="7"/>
-    </row>
-    <row r="103" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B103" s="7"/>
-      <c r="H103" s="7"/>
-      <c r="M103" s="7"/>
-    </row>
-    <row r="104" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B104" s="7"/>
-      <c r="H104" s="7"/>
-      <c r="M104" s="7"/>
-    </row>
-    <row r="105" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B105" s="7"/>
-      <c r="H105" s="7"/>
-      <c r="M105" s="7"/>
-    </row>
-    <row r="106" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B106" s="7"/>
-      <c r="H106" s="7"/>
-      <c r="M106" s="7"/>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="102" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="21">
+        <v>101</v>
+      </c>
+      <c r="B102" s="21"/>
+      <c r="C102" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D102" s="21">
+        <v>1</v>
+      </c>
+      <c r="E102" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="F102" s="21">
+        <v>0</v>
+      </c>
+      <c r="G102" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H102" s="21"/>
+      <c r="I102" s="21"/>
+      <c r="J102" s="21"/>
+      <c r="K102" s="21"/>
+      <c r="L102" s="21"/>
+      <c r="M102" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="N102" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="O102" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="P102" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="Q102" s="21">
+        <v>8.5</v>
+      </c>
+      <c r="R102" s="21">
+        <v>11</v>
+      </c>
+      <c r="S102" s="21">
+        <v>12</v>
+      </c>
+      <c r="T102" s="21">
+        <v>1</v>
+      </c>
+      <c r="U102" s="21">
+        <v>1</v>
+      </c>
+      <c r="V102" s="21"/>
+    </row>
+    <row r="103" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="21">
+        <v>102</v>
+      </c>
+      <c r="B103" s="21"/>
+      <c r="C103" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D103" s="21">
+        <v>1</v>
+      </c>
+      <c r="E103" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="F103" s="21">
+        <v>0</v>
+      </c>
+      <c r="G103" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H103" s="21"/>
+      <c r="I103" s="21"/>
+      <c r="J103" s="21"/>
+      <c r="K103" s="21"/>
+      <c r="L103" s="21"/>
+      <c r="M103" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="N103" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="O103" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="P103" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="Q103" s="21">
+        <v>8.5</v>
+      </c>
+      <c r="R103" s="21">
+        <v>11</v>
+      </c>
+      <c r="S103" s="21">
+        <v>12</v>
+      </c>
+      <c r="T103" s="21">
+        <v>1</v>
+      </c>
+      <c r="U103" s="21">
+        <v>1</v>
+      </c>
+      <c r="V103" s="21" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="104" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="21">
+        <v>103</v>
+      </c>
+      <c r="B104" s="21"/>
+      <c r="C104" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D104" s="21">
+        <v>1</v>
+      </c>
+      <c r="E104" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="F104" s="21">
+        <v>0</v>
+      </c>
+      <c r="G104" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H104" s="21"/>
+      <c r="I104" s="21"/>
+      <c r="J104" s="21"/>
+      <c r="K104" s="21"/>
+      <c r="L104" s="21"/>
+      <c r="M104" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="N104" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="O104" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="P104" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="Q104" s="21">
+        <v>8.5</v>
+      </c>
+      <c r="R104" s="21">
+        <v>11</v>
+      </c>
+      <c r="S104" s="21">
+        <v>12</v>
+      </c>
+      <c r="T104" s="21">
+        <v>1</v>
+      </c>
+      <c r="U104" s="21">
+        <v>1</v>
+      </c>
+      <c r="V104" s="21">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="21">
+        <v>104</v>
+      </c>
+      <c r="B105" s="21"/>
+      <c r="C105" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D105" s="21">
+        <v>1</v>
+      </c>
+      <c r="E105" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="F105" s="21">
+        <v>0</v>
+      </c>
+      <c r="G105" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H105" s="21"/>
+      <c r="I105" s="21"/>
+      <c r="J105" s="21"/>
+      <c r="K105" s="21"/>
+      <c r="L105" s="21"/>
+      <c r="M105" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="N105" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="O105" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="P105" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="Q105" s="21">
+        <v>8.5</v>
+      </c>
+      <c r="R105" s="21">
+        <v>11</v>
+      </c>
+      <c r="S105" s="21">
+        <v>12</v>
+      </c>
+      <c r="T105" s="21">
+        <v>1</v>
+      </c>
+      <c r="U105" s="21">
+        <v>1</v>
+      </c>
+      <c r="V105" s="21">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="106" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="21">
+        <v>105</v>
+      </c>
+      <c r="B106" s="21"/>
+      <c r="C106" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D106" s="21">
+        <v>1</v>
+      </c>
+      <c r="E106" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="F106" s="21">
+        <v>0</v>
+      </c>
+      <c r="G106" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H106" s="21"/>
+      <c r="I106" s="21"/>
+      <c r="J106" s="21"/>
+      <c r="K106" s="21"/>
+      <c r="L106" s="21"/>
+      <c r="M106" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="N106" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="O106" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="P106" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="Q106" s="21">
+        <v>8.5</v>
+      </c>
+      <c r="R106" s="21">
+        <v>11</v>
+      </c>
+      <c r="S106" s="21">
+        <v>12</v>
+      </c>
+      <c r="T106" s="21">
+        <v>1</v>
+      </c>
+      <c r="U106" s="21">
+        <v>1</v>
+      </c>
+      <c r="V106" s="21" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="107" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B107" s="7"/>
+      <c r="C107" s="20" t="s">
+        <v>103</v>
+      </c>
       <c r="H107" s="7"/>
       <c r="M107" s="7"/>
     </row>
     <row r="108" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B108" s="7"/>
+      <c r="C108" s="20" t="s">
+        <v>103</v>
+      </c>
       <c r="H108" s="7"/>
       <c r="M108" s="7"/>
     </row>
     <row r="109" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B109" s="7"/>
+      <c r="C109" s="20" t="s">
+        <v>103</v>
+      </c>
       <c r="H109" s="7"/>
       <c r="M109" s="7"/>
     </row>

</xml_diff>

<commit_message>
fixes to compliance report tests - set V
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="384">
   <si>
     <t>Enabled</t>
   </si>
@@ -1573,6 +1573,9 @@
   <si>
     <t>Administrator</t>
   </si>
+  <si>
+    <t>Customer DataRow ID</t>
+  </si>
 </sst>
 </file>
 
@@ -19376,7 +19379,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19831,13 +19834,41 @@
         <v>163</v>
       </c>
       <c r="K13" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L13" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:12" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="K14" s="7">
+        <v>5</v>
+      </c>
+      <c r="L14" s="7">
+        <v>8</v>
+      </c>
+    </row>
     <row r="15" spans="1:12" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:12" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="17" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -19876,16 +19907,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.88671875" bestFit="1" customWidth="1"/>
@@ -19897,10 +19928,10 @@
     <col min="12" max="12" width="31.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -19946,8 +19977,11 @@
       <c r="O1" s="1" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -19993,8 +20027,11 @@
       <c r="O2" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -20040,8 +20077,11 @@
       <c r="O3" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -20087,18 +20127,109 @@
       <c r="O4" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="P4" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="7">
+        <v>37.402092570550302</v>
+      </c>
+      <c r="D5" s="7">
+        <v>-121.98482039739901</v>
+      </c>
+      <c r="E5" s="7">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F5" s="7">
+        <v>5</v>
+      </c>
+      <c r="G5" s="7">
+        <v>5</v>
+      </c>
+      <c r="H5" s="7">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="I5" s="7">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="J5" s="7">
+        <v>-43</v>
+      </c>
+      <c r="K5" s="7">
+        <v>-40</v>
+      </c>
+      <c r="L5" s="7">
+        <v>-30</v>
+      </c>
+      <c r="M5" s="7">
+        <v>-25</v>
+      </c>
+      <c r="N5" s="7">
+        <v>2</v>
+      </c>
+      <c r="O5" s="7">
+        <v>10</v>
+      </c>
+      <c r="P5" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="7">
+        <v>37.402092570550302</v>
+      </c>
+      <c r="D6" s="7">
+        <v>-121.98482039739901</v>
+      </c>
+      <c r="E6" s="7">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F6" s="7">
+        <v>5</v>
+      </c>
+      <c r="G6" s="7">
+        <v>5</v>
+      </c>
+      <c r="H6" s="7">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="I6" s="7">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="J6" s="7">
+        <v>-43</v>
+      </c>
+      <c r="K6" s="7">
+        <v>-40</v>
+      </c>
+      <c r="L6" s="7">
+        <v>-30</v>
+      </c>
+      <c r="M6" s="7">
+        <v>-25</v>
+      </c>
+      <c r="N6" s="7">
+        <v>2</v>
+      </c>
+      <c r="O6" s="7">
+        <v>10</v>
+      </c>
+      <c r="P6" s="7">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20111,7 +20242,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
implemented few more test cases
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="387">
   <si>
     <t>Enabled</t>
   </si>
@@ -1573,6 +1573,18 @@
   <si>
     <t>China Standard Time</t>
   </si>
+  <si>
+    <t>TC204</t>
+  </si>
+  <si>
+    <t>TC204 #%&lt;&gt;$&amp;*Report</t>
+  </si>
+  <si>
+    <t>7473314aca15403</t>
+  </si>
+  <si>
+    <t>TC210</t>
+  </si>
 </sst>
 </file>
 
@@ -2215,7 +2227,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1138"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2837,15 +2851,25 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="D26" s="18" t="s">
+        <v>385</v>
+      </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
+      <c r="I26" s="7">
+        <v>1</v>
+      </c>
       <c r="J26" s="7"/>
+      <c r="K26" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
@@ -15109,7 +15133,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -19376,7 +19400,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30034,8 +30058,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32768,14 +32792,121 @@
       </c>
     </row>
     <row r="51" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B51" s="7"/>
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="D51" s="2">
+        <v>6</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="H51" s="7"/>
-      <c r="M51" s="7"/>
+      <c r="I51" s="2">
+        <v>37.4206</v>
+      </c>
+      <c r="J51" s="2">
+        <v>-121.9725</v>
+      </c>
+      <c r="K51" s="2">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L51" s="2">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="M51" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q51" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R51" s="7">
+        <v>11</v>
+      </c>
+      <c r="S51" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="T51" s="7">
+        <v>1</v>
+      </c>
+      <c r="U51" s="7">
+        <v>8</v>
+      </c>
+      <c r="V51" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="52" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B52" s="7"/>
+      <c r="A52" s="7">
+        <v>51</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D52" s="7">
+        <v>6</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="F52" s="7">
+        <v>0</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H52" s="7"/>
-      <c r="M52" s="7"/>
+      <c r="I52" s="7">
+        <v>37.4206</v>
+      </c>
+      <c r="J52" s="7">
+        <v>-121.9725</v>
+      </c>
+      <c r="K52" s="7">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L52" s="7">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N52" s="7"/>
+      <c r="O52" s="7"/>
+      <c r="P52" s="7"/>
+      <c r="Q52" s="7">
+        <v>8.5</v>
+      </c>
+      <c r="R52" s="7">
+        <v>11</v>
+      </c>
+      <c r="S52" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="T52" s="7">
+        <v>1</v>
+      </c>
+      <c r="U52" s="7">
+        <v>8</v>
+      </c>
+      <c r="V52" s="7">
+        <v>25</v>
+      </c>
     </row>
     <row r="53" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B53" s="7"/>

</xml_diff>

<commit_message>
fixes in page actions/page class + test case data update + added pagetest6 target in build.xml for local verification
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -992,9 +992,6 @@
     <t>All TRUE except Gaps</t>
   </si>
   <si>
-    <t>All TRUE</t>
-  </si>
-  <si>
     <t>Indication, Isotopic Analysis, PCA, PCRA = TRUE</t>
   </si>
   <si>
@@ -1301,15 +1298,6 @@
     <t>TC509</t>
   </si>
   <si>
-    <t>All FALSE. Map=Map</t>
-  </si>
-  <si>
-    <t>All FALSE. Map=Satellite</t>
-  </si>
-  <si>
-    <t>16,17</t>
-  </si>
-  <si>
     <t>TC510</t>
   </si>
   <si>
@@ -1575,6 +1563,18 @@
   </si>
   <si>
     <t>Customer DataRow ID</t>
+  </si>
+  <si>
+    <t>All TRUE. Map=Satellite</t>
+  </si>
+  <si>
+    <t>All TRUE. Map=None</t>
+  </si>
+  <si>
+    <t>All TRUE. Map=Map</t>
+  </si>
+  <si>
+    <t>12,16,17</t>
   </si>
 </sst>
 </file>
@@ -2153,19 +2153,19 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2173,10 +2173,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>345</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>349</v>
       </c>
       <c r="D2" s="9">
         <v>1</v>
@@ -2185,7 +2185,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2193,10 +2193,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D3" s="7">
         <v>2</v>
@@ -2205,7 +2205,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -2218,7 +2218,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1138"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2263,10 +2265,10 @@
         <v>103</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -2384,7 +2386,7 @@
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -2407,7 +2409,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -2430,7 +2432,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -2453,7 +2455,7 @@
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -2476,7 +2478,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -2499,7 +2501,7 @@
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -2522,7 +2524,7 @@
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -2545,7 +2547,7 @@
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -2568,7 +2570,7 @@
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -2591,7 +2593,7 @@
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -2614,7 +2616,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -2637,7 +2639,7 @@
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -2660,7 +2662,7 @@
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -2683,7 +2685,7 @@
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -2706,7 +2708,7 @@
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -2729,7 +2731,7 @@
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -2752,7 +2754,7 @@
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -2775,7 +2777,7 @@
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -15113,7 +15115,7 @@
   <dimension ref="A1:N800"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15392,7 +15394,7 @@
         <v>83</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15436,7 +15438,7 @@
         <v>84</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15480,7 +15482,7 @@
         <v>83</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15524,7 +15526,7 @@
         <v>84</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15700,7 +15702,7 @@
         <v>83</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>189</v>
+        <v>382</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15744,7 +15746,7 @@
         <v>83</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15788,7 +15790,7 @@
         <v>83</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15832,7 +15834,7 @@
         <v>84</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15843,40 +15845,40 @@
         <v>99</v>
       </c>
       <c r="C17" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="7" t="b">
         <v>0</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>292</v>
+        <v>380</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15887,40 +15889,40 @@
         <v>99</v>
       </c>
       <c r="C18" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" s="7" t="b">
         <v>0</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>293</v>
+        <v>381</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15964,7 +15966,7 @@
         <v>83</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16008,7 +16010,7 @@
         <v>84</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16052,7 +16054,7 @@
         <v>83</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16096,7 +16098,7 @@
         <v>83</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16140,7 +16142,7 @@
         <v>83</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16184,7 +16186,7 @@
         <v>83</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16228,7 +16230,7 @@
         <v>83</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16272,7 +16274,7 @@
         <v>83</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16316,7 +16318,7 @@
         <v>83</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16360,7 +16362,7 @@
         <v>83</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16404,7 +16406,7 @@
         <v>83</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16448,7 +16450,7 @@
         <v>83</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16492,7 +16494,7 @@
         <v>84</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16536,7 +16538,7 @@
         <v>84</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="33" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16580,7 +16582,7 @@
         <v>83</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="34" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16624,7 +16626,7 @@
         <v>83</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16668,7 +16670,7 @@
         <v>83</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="36" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -17464,7 +17466,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17480,13 +17482,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -17494,13 +17496,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>247</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -17508,11 +17510,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -17521,10 +17523,10 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -17534,7 +17536,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="15"/>
       <c r="D5" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -17542,11 +17544,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -17556,7 +17558,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="15"/>
       <c r="D7" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -17564,13 +17566,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C8" s="15">
         <v>5</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -17578,13 +17580,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C9" s="15">
         <v>4</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -17614,16 +17616,16 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>44</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -17631,16 +17633,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D2" s="12">
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -17648,16 +17650,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D3" s="12">
         <v>4</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -17665,16 +17667,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D4" s="12">
         <v>4</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -17682,16 +17684,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D5" s="12">
         <v>4</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -17699,16 +17701,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D6" s="12">
         <v>4</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -17716,16 +17718,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D7" s="12">
         <v>4</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -17733,16 +17735,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D8" s="12">
         <v>4</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -17750,16 +17752,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D9" s="12">
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -17767,16 +17769,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D10" s="12">
         <v>1</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -17784,16 +17786,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D11" s="12">
         <v>1</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -17801,16 +17803,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D12" s="12">
         <v>1</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -17818,16 +17820,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D13" s="12">
         <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -17835,16 +17837,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D14" s="12">
         <v>1</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -17852,16 +17854,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D15" s="12">
         <v>5</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -17869,16 +17871,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D16" s="12">
         <v>5</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -17886,16 +17888,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D17" s="12">
         <v>5</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -17903,16 +17905,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D18" s="12">
         <v>5</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -17920,16 +17922,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D19" s="12">
         <v>5</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -17937,16 +17939,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D20" s="12">
         <v>5</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -17954,16 +17956,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D21" s="12">
         <v>5</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -17971,16 +17973,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D22" s="12">
         <v>5</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -18010,16 +18012,16 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>44</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -18027,7 +18029,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>57</v>
@@ -18036,7 +18038,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -18044,7 +18046,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>56</v>
@@ -18053,7 +18055,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -18061,16 +18063,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -18078,16 +18080,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D5" s="12">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -18095,7 +18097,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>185</v>
@@ -18104,7 +18106,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -18119,7 +18121,7 @@
   <dimension ref="A1:H578"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18365,7 +18367,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18391,7 +18393,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -18417,7 +18419,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -19022,22 +19024,22 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -19247,7 +19249,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B3" t="s">
         <v>48</v>
@@ -19264,7 +19266,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -19281,10 +19283,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D5" t="s">
         <v>48</v>
@@ -19292,10 +19294,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D6" t="s">
         <v>42</v>
@@ -19331,13 +19333,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -19345,7 +19347,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
@@ -19359,7 +19361,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
@@ -19378,7 +19380,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -19444,13 +19446,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>160</v>
@@ -19479,13 +19481,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>164</v>
@@ -19515,13 +19517,13 @@
         <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>165</v>
@@ -19551,13 +19553,13 @@
         <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>166</v>
@@ -19587,7 +19589,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>1</v>
@@ -19619,13 +19621,13 @@
         <v>137</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>167</v>
@@ -19655,13 +19657,13 @@
         <v>127</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -19687,13 +19689,13 @@
         <v>128</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -19719,13 +19721,13 @@
         <v>129</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -19751,13 +19753,13 @@
         <v>137</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D11" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>167</v>
@@ -19784,10 +19786,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D12" s="7" t="b">
         <v>1</v>
@@ -19813,16 +19815,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D13" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -19845,16 +19847,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D14" s="7" t="b">
         <v>1</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>162</v>
@@ -19945,40 +19947,40 @@
         <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>370</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -20332,7 +20334,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
@@ -20355,7 +20357,7 @@
         <v>145</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20372,7 +20374,7 @@
         <v>145</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20389,7 +20391,7 @@
         <v>145</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -20890,7 +20892,7 @@
         <v>126</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>26</v>
@@ -30196,8 +30198,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="M13" workbookViewId="0">
+      <selection activeCell="T50" sqref="T50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30361,7 +30363,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -30404,7 +30406,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="2">
@@ -30459,7 +30461,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -30516,7 +30518,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F6" s="7">
         <v>0</v>
@@ -30572,7 +30574,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F7" s="7">
         <v>0</v>
@@ -30628,7 +30630,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F8" s="7">
         <v>0</v>
@@ -30678,7 +30680,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>177</v>
@@ -30687,7 +30689,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F9" s="7">
         <v>0</v>
@@ -30734,7 +30736,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>177</v>
@@ -30743,7 +30745,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F10" s="7">
         <v>0</v>
@@ -30898,7 +30900,7 @@
         <v>8</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -30943,16 +30945,16 @@
         <v>11</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T13" s="7">
         <v>7</v>
       </c>
       <c r="U13" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -31014,7 +31016,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>177</v>
@@ -31023,7 +31025,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F15" s="7">
         <v>0</v>
@@ -31059,7 +31061,7 @@
         <v>2</v>
       </c>
       <c r="U15" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="V15" s="7">
         <v>4</v>
@@ -31070,7 +31072,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>177</v>
@@ -31079,7 +31081,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F16" s="7">
         <v>0</v>
@@ -31109,7 +31111,7 @@
         <v>11</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T16" s="7">
         <v>8</v>
@@ -31126,7 +31128,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>177</v>
@@ -31135,7 +31137,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F17" s="7">
         <v>0</v>
@@ -31144,10 +31146,10 @@
         <v>22</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q17" s="7">
         <v>8.5</v>
@@ -31162,7 +31164,7 @@
         <v>2</v>
       </c>
       <c r="U17" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="V17" s="7">
         <v>4</v>
@@ -31173,7 +31175,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>177</v>
@@ -31209,7 +31211,7 @@
         <v>11</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>294</v>
+        <v>383</v>
       </c>
       <c r="T18" s="7">
         <v>1</v>
@@ -31226,7 +31228,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>177</v>
@@ -31235,7 +31237,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F19" s="7">
         <v>0</v>
@@ -31268,7 +31270,7 @@
         <v>2</v>
       </c>
       <c r="U19" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="V19" s="7">
         <v>4</v>
@@ -31279,7 +31281,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>177</v>
@@ -31288,7 +31290,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F20" s="7">
         <v>0</v>
@@ -31321,7 +31323,7 @@
         <v>2</v>
       </c>
       <c r="U20" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="V20" s="7">
         <v>4</v>
@@ -31332,7 +31334,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>177</v>
@@ -31341,7 +31343,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F21" s="7">
         <v>0</v>
@@ -31379,7 +31381,7 @@
         <v>2</v>
       </c>
       <c r="U21" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="V21" s="7">
         <v>4</v>
@@ -31390,7 +31392,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>177</v>
@@ -31399,7 +31401,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F22" s="7">
         <v>0</v>
@@ -31413,10 +31415,10 @@
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
@@ -31427,13 +31429,13 @@
         <v>11</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="T22" s="7">
         <v>4</v>
       </c>
       <c r="U22" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="V22" s="7">
         <v>4</v>
@@ -31444,7 +31446,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>177</v>
@@ -31485,7 +31487,7 @@
         <v>11</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="T23" s="7">
         <v>8</v>
@@ -31502,7 +31504,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H24" s="7"/>
       <c r="M24" s="7"/>
@@ -31512,7 +31514,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>177</v>
@@ -31556,10 +31558,10 @@
         <v>24</v>
       </c>
       <c r="T25" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U25" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V25" s="7">
         <v>4</v>
@@ -31570,7 +31572,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>177</v>
@@ -31614,10 +31616,10 @@
         <v>25</v>
       </c>
       <c r="T26" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U26" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V26" s="7">
         <v>4</v>
@@ -31628,7 +31630,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>177</v>
@@ -31672,10 +31674,10 @@
         <v>26</v>
       </c>
       <c r="T27" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U27" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V27" s="7">
         <v>4</v>
@@ -31686,7 +31688,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>177</v>
@@ -31730,10 +31732,10 @@
         <v>27</v>
       </c>
       <c r="T28" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U28" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V28" s="7">
         <v>4</v>
@@ -31744,7 +31746,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>177</v>
@@ -31788,10 +31790,10 @@
         <v>28</v>
       </c>
       <c r="T29" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U29" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V29" s="7">
         <v>4</v>
@@ -31802,7 +31804,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>177</v>
@@ -31849,7 +31851,7 @@
         <v>1</v>
       </c>
       <c r="U30" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V30" s="7">
         <v>4</v>
@@ -31860,7 +31862,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>177</v>
@@ -31899,10 +31901,10 @@
         <v>24</v>
       </c>
       <c r="T31" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U31" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V31" s="7">
         <v>4</v>
@@ -31913,7 +31915,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>177</v>
@@ -31952,10 +31954,10 @@
         <v>25</v>
       </c>
       <c r="T32" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U32" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V32" s="7">
         <v>4</v>
@@ -31966,7 +31968,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>177</v>
@@ -32005,10 +32007,10 @@
         <v>26</v>
       </c>
       <c r="T33" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U33" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V33" s="7">
         <v>4</v>
@@ -32019,7 +32021,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>177</v>
@@ -32058,10 +32060,10 @@
         <v>27</v>
       </c>
       <c r="T34" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U34" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V34" s="7">
         <v>4</v>
@@ -32072,7 +32074,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>177</v>
@@ -32111,10 +32113,10 @@
         <v>28</v>
       </c>
       <c r="T35" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U35" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V35" s="7">
         <v>4</v>
@@ -32125,7 +32127,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>177</v>
@@ -32161,13 +32163,13 @@
         <v>11</v>
       </c>
       <c r="S36" s="7" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="T36" s="7">
         <v>1</v>
       </c>
       <c r="U36" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V36" s="7">
         <v>4</v>
@@ -32178,7 +32180,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>177</v>
@@ -32222,10 +32224,10 @@
         <v>29</v>
       </c>
       <c r="T37" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U37" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V37" s="7">
         <v>4</v>
@@ -32236,7 +32238,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>177</v>
@@ -32277,7 +32279,7 @@
         <v>29</v>
       </c>
       <c r="T38" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U38" s="2">
         <v>10</v>
@@ -32291,7 +32293,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>177</v>
@@ -32330,7 +32332,7 @@
         <v>29</v>
       </c>
       <c r="T39" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U39" s="7">
         <v>10</v>
@@ -32344,7 +32346,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>177</v>
@@ -32353,7 +32355,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F40" s="7">
         <v>0</v>
@@ -32383,7 +32385,7 @@
         <v>24</v>
       </c>
       <c r="T40" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U40" s="7">
         <v>10</v>
@@ -32397,7 +32399,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>177</v>
@@ -32406,7 +32408,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F41" s="7">
         <v>0</v>
@@ -32436,7 +32438,7 @@
         <v>27</v>
       </c>
       <c r="T41" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U41" s="7">
         <v>10</v>
@@ -32450,7 +32452,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>177</v>
@@ -32459,7 +32461,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F42" s="7">
         <v>0</v>
@@ -32489,7 +32491,7 @@
         <v>30</v>
       </c>
       <c r="T42" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U42" s="7">
         <v>10</v>
@@ -32503,7 +32505,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>177</v>
@@ -32512,7 +32514,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F43" s="7">
         <v>0</v>
@@ -32542,7 +32544,7 @@
         <v>24</v>
       </c>
       <c r="T43" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U43" s="7">
         <v>10</v>
@@ -32556,7 +32558,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>177</v>
@@ -32565,7 +32567,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F44" s="7">
         <v>0</v>
@@ -32595,7 +32597,7 @@
         <v>31</v>
       </c>
       <c r="T44" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U44" s="7">
         <v>10</v>
@@ -32609,7 +32611,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>177</v>
@@ -32618,7 +32620,7 @@
         <v>8</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F45" s="7">
         <v>0</v>
@@ -32648,7 +32650,7 @@
         <v>32</v>
       </c>
       <c r="T45" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U45" s="7">
         <v>10</v>
@@ -32662,7 +32664,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>177</v>
@@ -32671,7 +32673,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F46" s="7">
         <v>0</v>
@@ -32701,7 +32703,7 @@
         <v>24</v>
       </c>
       <c r="T46" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U46" s="7">
         <v>10</v>
@@ -32715,7 +32717,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>177</v>
@@ -32724,7 +32726,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F47" s="7">
         <v>0</v>
@@ -32754,7 +32756,7 @@
         <v>33</v>
       </c>
       <c r="T47" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U47" s="7">
         <v>10</v>
@@ -32768,7 +32770,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>177</v>
@@ -32777,7 +32779,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F48" s="7">
         <v>0</v>
@@ -32807,7 +32809,7 @@
         <v>34</v>
       </c>
       <c r="T48" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U48" s="7">
         <v>10</v>
@@ -32821,7 +32823,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>177</v>
@@ -32830,7 +32832,7 @@
         <v>6</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F49" s="7">
         <v>0</v>
@@ -32860,7 +32862,7 @@
         <v>29</v>
       </c>
       <c r="T49" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U49" s="7">
         <v>10</v>
@@ -32874,10 +32876,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D50" s="7">
         <v>7</v>

</xml_diff>

<commit_message>
opt tabular pdf content update
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="385">
   <si>
     <t>Enabled</t>
   </si>
@@ -1576,6 +1576,9 @@
   <si>
     <t>12,16,17</t>
   </si>
+  <si>
+    <t>All TRUE (except GAP and PCF)</t>
+  </si>
 </sst>
 </file>
 
@@ -18120,8 +18123,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H578"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18422,7 +18425,32 @@
         <v>322</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:8" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>384</v>
+      </c>
+    </row>
     <row r="13" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -30198,8 +30226,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M13" workbookViewId="0">
-      <selection activeCell="T50" sqref="T50"/>
+    <sheetView tabSelected="1" topLeftCell="T19" workbookViewId="0">
+      <selection activeCell="U49" sqref="U49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32282,7 +32310,7 @@
         <v>2</v>
       </c>
       <c r="U38" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="V38" s="2">
         <v>4</v>
@@ -32335,7 +32363,7 @@
         <v>2</v>
       </c>
       <c r="U39" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="V39" s="7">
         <v>4</v>
@@ -32388,7 +32416,7 @@
         <v>4</v>
       </c>
       <c r="U40" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="V40" s="7">
         <v>4</v>
@@ -32441,7 +32469,7 @@
         <v>4</v>
       </c>
       <c r="U41" s="7">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="V41" s="7">
         <v>4</v>
@@ -32494,7 +32522,7 @@
         <v>4</v>
       </c>
       <c r="U42" s="7">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="V42" s="7">
         <v>4</v>
@@ -32547,7 +32575,7 @@
         <v>4</v>
       </c>
       <c r="U43" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="V43" s="7">
         <v>4</v>
@@ -32600,7 +32628,7 @@
         <v>4</v>
       </c>
       <c r="U44" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="V44" s="7">
         <v>4</v>
@@ -32653,7 +32681,7 @@
         <v>2</v>
       </c>
       <c r="U45" s="7">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="V45" s="7">
         <v>4</v>
@@ -32706,7 +32734,7 @@
         <v>4</v>
       </c>
       <c r="U46" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="V46" s="7">
         <v>24</v>
@@ -32759,7 +32787,7 @@
         <v>2</v>
       </c>
       <c r="U47" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="V47" s="7">
         <v>24</v>
@@ -32812,7 +32840,7 @@
         <v>2</v>
       </c>
       <c r="U48" s="7">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="V48" s="7">
         <v>24</v>
@@ -32865,7 +32893,7 @@
         <v>2</v>
       </c>
       <c r="U49" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="V49" s="7">
         <v>4</v>
@@ -32925,7 +32953,7 @@
         <v>1</v>
       </c>
       <c r="U50" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="V50" s="7">
         <v>4</v>

</xml_diff>

<commit_message>
test case data excel
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -15118,7 +15118,7 @@
   <dimension ref="A1:N800"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30226,8 +30226,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O4" workbookViewId="0">
-      <selection activeCell="T36" sqref="T36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fixed problems of compliance report tests on framework level
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="417">
   <si>
     <t>Enabled</t>
   </si>
@@ -1583,9 +1583,6 @@
     <t>iso-cap</t>
   </si>
   <si>
-    <t>TC1319TC1320</t>
-  </si>
-  <si>
     <t>23,25,26</t>
   </si>
   <si>
@@ -1593,6 +1590,90 @@
   </si>
   <si>
     <t>23,26,25,29</t>
+  </si>
+  <si>
+    <t>26,25,28</t>
+  </si>
+  <si>
+    <t>26,25</t>
+  </si>
+  <si>
+    <t>Annotations, Isotopic, Assets, Boundaries = TRUE, (BaseMap=Map)</t>
+  </si>
+  <si>
+    <t>Breadcrumbs, Indications, Annotations = TRUE, (BaseMap=Map)</t>
+  </si>
+  <si>
+    <t>35,36,37</t>
+  </si>
+  <si>
+    <t>TC1339,TC1340</t>
+  </si>
+  <si>
+    <t>TC1340</t>
+  </si>
+  <si>
+    <t>TC1352</t>
+  </si>
+  <si>
+    <t>TC1339,TC1340,TC1363</t>
+  </si>
+  <si>
+    <t>TC1370,TC1371</t>
+  </si>
+  <si>
+    <t>TC1373,TC1389</t>
+  </si>
+  <si>
+    <t>TC1394,TC1395</t>
+  </si>
+  <si>
+    <t>TC14</t>
+  </si>
+  <si>
+    <t>TC149</t>
+  </si>
+  <si>
+    <t>TC1319,TC1320,TC1364-TC1367,TC1491,TC1496,TC1497</t>
+  </si>
+  <si>
+    <t>RandomString50</t>
+  </si>
+  <si>
+    <t>RandomString51</t>
+  </si>
+  <si>
+    <t>RandomString52</t>
+  </si>
+  <si>
+    <t>RandomString53</t>
+  </si>
+  <si>
+    <t>RandomString54</t>
+  </si>
+  <si>
+    <t>RandomString55</t>
+  </si>
+  <si>
+    <t>RandomString56</t>
+  </si>
+  <si>
+    <t>RandomString57</t>
+  </si>
+  <si>
+    <t>RandomString58</t>
+  </si>
+  <si>
+    <t>RandomString59</t>
+  </si>
+  <si>
+    <t>RandomString60</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Indication, Analysis, PCRA = TRUE. All other FALSE</t>
   </si>
 </sst>
 </file>
@@ -1823,7 +1904,7 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1862,6 +1943,11 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -2237,10 +2323,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1138"/>
+  <dimension ref="A1:K1137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2873,7 +2959,9 @@
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
+      <c r="G26" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7">
         <v>1</v>
@@ -2894,7 +2982,9 @@
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
+      <c r="G27" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="H27" s="7"/>
       <c r="I27" s="7">
         <v>1</v>
@@ -10179,15 +10269,15 @@
       <c r="J685" s="7"/>
     </row>
     <row r="686" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B686" s="7"/>
-      <c r="C686" s="7"/>
-      <c r="D686" s="7"/>
-      <c r="E686" s="7"/>
-      <c r="F686" s="7"/>
-      <c r="G686" s="7"/>
-      <c r="H686" s="7"/>
-      <c r="I686" s="7"/>
-      <c r="J686" s="7"/>
+      <c r="B686" s="5"/>
+      <c r="C686" s="5"/>
+      <c r="D686" s="5"/>
+      <c r="E686" s="5"/>
+      <c r="F686" s="5"/>
+      <c r="G686" s="5"/>
+      <c r="H686" s="5"/>
+      <c r="I686" s="5"/>
+      <c r="J686" s="5"/>
     </row>
     <row r="687" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B687" s="5"/>
@@ -15149,17 +15239,6 @@
       <c r="H1137" s="5"/>
       <c r="I1137" s="5"/>
       <c r="J1137" s="5"/>
-    </row>
-    <row r="1138" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B1138" s="5"/>
-      <c r="C1138" s="5"/>
-      <c r="D1138" s="5"/>
-      <c r="E1138" s="5"/>
-      <c r="F1138" s="5"/>
-      <c r="G1138" s="5"/>
-      <c r="H1138" s="5"/>
-      <c r="I1138" s="5"/>
-      <c r="J1138" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15191,8 +15270,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16750,9 +16829,138 @@
         <v>346</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A36" s="21">
+        <v>35</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H36" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K36" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L36" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M36" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="N36" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" s="21" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A37" s="22">
+        <v>36</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J37" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L37" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M37" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="N37" s="21" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A38" s="22">
+        <v>37</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="L38" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M38" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="N38" s="22" t="s">
+        <v>392</v>
+      </c>
+    </row>
     <row r="39" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -17517,6 +17725,7 @@
     <row r="800" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -17542,9 +17751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -18195,10 +18402,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:H578"/>
+  <dimension ref="A1:I578"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18210,10 +18417,11 @@
     <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="92.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" style="23" customWidth="1"/>
+    <col min="9" max="9" width="92.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -18235,11 +18443,14 @@
       <c r="G1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="24" t="s">
+        <v>415</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -18261,11 +18472,14 @@
       <c r="G2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -18287,11 +18501,14 @@
       <c r="G3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -18313,11 +18530,14 @@
       <c r="G4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -18339,11 +18559,14 @@
       <c r="G5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -18365,11 +18588,14 @@
       <c r="G6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -18391,11 +18617,14 @@
       <c r="G7" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -18417,11 +18646,14 @@
       <c r="G8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -18443,11 +18675,14 @@
       <c r="G9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -18469,11 +18704,14 @@
       <c r="G10" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -18495,577 +18733,1740 @@
       <c r="G11" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="17" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="18" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="19" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="20" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="21" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="23" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="24" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="25" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="26" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="28" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="30" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="31" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="32" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="33" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="34" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="35" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="36" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="37" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="38" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="39" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="40" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="41" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="42" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="43" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="44" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="45" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="46" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="47" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="48" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="49" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="50" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="51" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="52" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="53" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="54" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="55" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="56" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="57" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="58" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="59" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="60" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="61" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="62" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="63" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="64" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="65" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="66" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="67" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="68" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="69" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="70" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="71" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="72" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="73" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="74" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="75" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="76" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="77" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="78" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="79" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="80" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="81" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="82" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="83" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="84" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="85" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="86" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="87" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="88" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="89" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="90" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="91" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="92" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="93" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="94" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="95" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="96" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="97" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="98" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="99" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="100" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="101" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="102" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="103" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="104" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="105" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="106" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="107" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="108" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="109" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="110" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="111" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="112" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="113" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="114" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="115" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="116" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="117" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="118" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="119" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="120" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="121" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="122" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="123" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="124" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="125" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="126" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="127" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="128" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="129" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="130" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="131" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="132" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="133" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="134" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="135" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="136" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="137" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="138" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="139" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="140" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="141" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="142" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="143" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="144" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="145" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="146" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="147" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="148" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="149" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="150" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="151" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="152" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="153" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="154" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="155" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="156" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="157" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="158" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="159" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="160" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="161" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="162" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="163" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="164" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="165" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="166" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="167" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="168" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="169" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="170" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="171" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="172" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="173" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="174" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="175" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="176" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="177" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="178" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="179" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="180" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="181" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="182" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="183" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="184" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="185" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="186" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="187" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="188" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="189" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="190" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="191" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="192" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="193" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="194" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="195" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="196" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="197" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="198" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="199" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="200" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="201" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="202" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="203" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="204" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="205" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="206" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="207" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="208" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="209" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="210" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="211" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="212" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="213" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="214" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="215" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="216" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="217" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="218" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="219" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="220" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="221" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="222" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="223" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="224" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="225" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="226" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="227" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="228" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="229" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="230" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="231" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="232" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="233" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="234" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="235" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="236" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="237" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="238" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="239" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="240" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="241" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="242" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="243" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="244" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="245" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="246" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="247" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="248" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="249" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="250" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="251" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="252" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="253" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="254" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="255" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="256" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="257" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="258" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="259" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="260" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="261" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="262" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="263" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="264" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="265" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="266" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="267" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="268" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="269" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="270" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="271" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="272" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="273" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="274" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="275" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="276" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="277" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="278" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="279" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="280" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="281" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="282" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="283" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="284" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="285" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="286" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="287" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="288" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="289" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="290" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="291" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="292" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="293" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="294" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="295" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="296" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="297" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="298" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="299" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="300" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="301" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="302" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="303" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="304" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="305" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="306" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="307" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="308" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="309" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="310" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="311" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="312" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="313" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="314" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="315" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="316" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="317" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="318" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="319" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="320" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="321" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="322" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="323" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="324" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="325" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="326" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="327" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="328" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="329" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="330" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="331" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="332" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="333" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="334" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="335" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="336" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="337" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="338" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="339" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="340" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="341" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="342" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="343" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="344" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="345" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="346" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="347" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="348" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="349" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="350" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="351" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="352" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="353" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="354" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="355" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="356" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="357" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="358" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="359" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="360" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="361" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="362" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="363" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="364" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="365" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="366" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="367" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="368" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="369" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="370" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="371" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="372" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="373" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="374" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="375" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="376" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="377" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="378" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="379" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="380" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="381" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="382" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="383" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="384" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="385" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="386" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="387" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="388" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="389" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="390" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="391" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="392" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="393" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="394" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="395" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="396" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="397" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="398" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="399" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="400" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="401" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="402" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="403" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="404" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="405" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="406" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="407" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="408" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="409" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="410" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="411" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="412" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="413" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="414" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="415" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="416" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="417" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="418" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="419" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="420" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="421" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="422" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="423" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="424" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="425" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="426" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="427" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="428" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="429" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="430" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="431" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="432" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="433" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="434" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="435" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="436" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="437" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="438" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="439" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="440" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="441" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="442" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="443" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="444" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="445" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="446" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="447" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="448" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="449" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="450" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="451" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="452" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="453" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="454" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="455" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="456" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="457" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="458" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="459" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="460" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="461" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="462" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="463" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="464" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="465" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="466" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="467" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="468" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="469" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="470" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="471" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="472" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="473" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="474" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="475" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="476" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="477" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="478" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="479" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="480" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="481" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="482" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="483" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="484" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="485" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="486" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="487" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="488" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="489" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="490" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="491" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="492" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="493" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="494" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="495" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="496" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="497" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="498" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="499" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="500" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="501" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="502" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="503" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="504" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="505" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="506" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="507" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="508" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="509" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="510" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="511" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="512" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="513" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="514" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="515" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="516" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="517" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="518" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="519" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="520" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="521" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="522" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="523" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="524" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="525" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="526" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="527" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="528" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="529" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="530" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="531" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="532" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="533" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="534" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="535" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="536" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="537" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="538" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="539" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="540" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="541" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="542" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="543" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="544" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="545" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="546" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="547" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="548" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="549" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="550" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="551" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="552" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="553" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="554" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="555" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="556" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="557" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="558" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="559" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="560" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="561" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="562" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="563" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="564" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="565" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="566" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="567" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="568" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="569" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="570" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="571" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="572" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="573" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="574" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="575" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="576" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="577" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="578" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" s="25" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A12" s="25">
+        <v>11</v>
+      </c>
+      <c r="B12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="1:9" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H17" s="25"/>
+    </row>
+    <row r="18" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H18" s="25"/>
+    </row>
+    <row r="19" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H19" s="25"/>
+    </row>
+    <row r="20" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H20" s="25"/>
+    </row>
+    <row r="21" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H21" s="25"/>
+    </row>
+    <row r="22" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H22" s="25"/>
+    </row>
+    <row r="23" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H23" s="25"/>
+    </row>
+    <row r="24" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H24" s="25"/>
+    </row>
+    <row r="25" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H25" s="25"/>
+    </row>
+    <row r="26" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H26" s="25"/>
+    </row>
+    <row r="27" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H27" s="25"/>
+    </row>
+    <row r="28" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H28" s="25"/>
+    </row>
+    <row r="29" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H29" s="25"/>
+    </row>
+    <row r="30" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H30" s="25"/>
+    </row>
+    <row r="31" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H31" s="25"/>
+    </row>
+    <row r="32" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H32" s="25"/>
+    </row>
+    <row r="33" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H33" s="25"/>
+    </row>
+    <row r="34" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H34" s="25"/>
+    </row>
+    <row r="35" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H35" s="25"/>
+    </row>
+    <row r="36" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H36" s="25"/>
+    </row>
+    <row r="37" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H37" s="25"/>
+    </row>
+    <row r="38" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H38" s="25"/>
+    </row>
+    <row r="39" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H39" s="25"/>
+    </row>
+    <row r="40" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H40" s="25"/>
+    </row>
+    <row r="41" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H41" s="25"/>
+    </row>
+    <row r="42" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H42" s="25"/>
+    </row>
+    <row r="43" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H43" s="25"/>
+    </row>
+    <row r="44" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H44" s="25"/>
+    </row>
+    <row r="45" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H45" s="25"/>
+    </row>
+    <row r="46" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H46" s="25"/>
+    </row>
+    <row r="47" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H47" s="25"/>
+    </row>
+    <row r="48" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H48" s="25"/>
+    </row>
+    <row r="49" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H49" s="25"/>
+    </row>
+    <row r="50" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H50" s="25"/>
+    </row>
+    <row r="51" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H51" s="25"/>
+    </row>
+    <row r="52" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H52" s="25"/>
+    </row>
+    <row r="53" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H53" s="25"/>
+    </row>
+    <row r="54" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H54" s="25"/>
+    </row>
+    <row r="55" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H55" s="25"/>
+    </row>
+    <row r="56" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H56" s="25"/>
+    </row>
+    <row r="57" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H57" s="25"/>
+    </row>
+    <row r="58" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H58" s="25"/>
+    </row>
+    <row r="59" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H59" s="25"/>
+    </row>
+    <row r="60" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H60" s="25"/>
+    </row>
+    <row r="61" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H61" s="25"/>
+    </row>
+    <row r="62" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H62" s="25"/>
+    </row>
+    <row r="63" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H63" s="25"/>
+    </row>
+    <row r="64" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H64" s="25"/>
+    </row>
+    <row r="65" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H65" s="25"/>
+    </row>
+    <row r="66" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H66" s="25"/>
+    </row>
+    <row r="67" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H67" s="25"/>
+    </row>
+    <row r="68" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H68" s="25"/>
+    </row>
+    <row r="69" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H69" s="25"/>
+    </row>
+    <row r="70" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H70" s="25"/>
+    </row>
+    <row r="71" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H71" s="25"/>
+    </row>
+    <row r="72" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H72" s="25"/>
+    </row>
+    <row r="73" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H73" s="25"/>
+    </row>
+    <row r="74" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H74" s="25"/>
+    </row>
+    <row r="75" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H75" s="25"/>
+    </row>
+    <row r="76" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H76" s="25"/>
+    </row>
+    <row r="77" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H77" s="25"/>
+    </row>
+    <row r="78" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H78" s="25"/>
+    </row>
+    <row r="79" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H79" s="25"/>
+    </row>
+    <row r="80" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H80" s="25"/>
+    </row>
+    <row r="81" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H81" s="25"/>
+    </row>
+    <row r="82" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H82" s="25"/>
+    </row>
+    <row r="83" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H83" s="25"/>
+    </row>
+    <row r="84" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H84" s="25"/>
+    </row>
+    <row r="85" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H85" s="25"/>
+    </row>
+    <row r="86" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H86" s="25"/>
+    </row>
+    <row r="87" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H87" s="25"/>
+    </row>
+    <row r="88" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H88" s="25"/>
+    </row>
+    <row r="89" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H89" s="25"/>
+    </row>
+    <row r="90" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H90" s="25"/>
+    </row>
+    <row r="91" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H91" s="25"/>
+    </row>
+    <row r="92" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H92" s="25"/>
+    </row>
+    <row r="93" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H93" s="25"/>
+    </row>
+    <row r="94" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H94" s="25"/>
+    </row>
+    <row r="95" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H95" s="25"/>
+    </row>
+    <row r="96" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H96" s="25"/>
+    </row>
+    <row r="97" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H97" s="25"/>
+    </row>
+    <row r="98" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H98" s="25"/>
+    </row>
+    <row r="99" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H99" s="25"/>
+    </row>
+    <row r="100" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H100" s="25"/>
+    </row>
+    <row r="101" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H101" s="25"/>
+    </row>
+    <row r="102" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H102" s="25"/>
+    </row>
+    <row r="103" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H103" s="25"/>
+    </row>
+    <row r="104" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H104" s="25"/>
+    </row>
+    <row r="105" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H105" s="25"/>
+    </row>
+    <row r="106" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H106" s="25"/>
+    </row>
+    <row r="107" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H107" s="25"/>
+    </row>
+    <row r="108" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H108" s="25"/>
+    </row>
+    <row r="109" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H109" s="25"/>
+    </row>
+    <row r="110" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H110" s="25"/>
+    </row>
+    <row r="111" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H111" s="25"/>
+    </row>
+    <row r="112" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H112" s="25"/>
+    </row>
+    <row r="113" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H113" s="25"/>
+    </row>
+    <row r="114" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H114" s="25"/>
+    </row>
+    <row r="115" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H115" s="25"/>
+    </row>
+    <row r="116" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H116" s="25"/>
+    </row>
+    <row r="117" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H117" s="25"/>
+    </row>
+    <row r="118" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H118" s="25"/>
+    </row>
+    <row r="119" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H119" s="25"/>
+    </row>
+    <row r="120" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H120" s="25"/>
+    </row>
+    <row r="121" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H121" s="25"/>
+    </row>
+    <row r="122" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H122" s="25"/>
+    </row>
+    <row r="123" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H123" s="25"/>
+    </row>
+    <row r="124" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H124" s="25"/>
+    </row>
+    <row r="125" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H125" s="25"/>
+    </row>
+    <row r="126" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H126" s="25"/>
+    </row>
+    <row r="127" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H127" s="25"/>
+    </row>
+    <row r="128" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H128" s="25"/>
+    </row>
+    <row r="129" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H129" s="25"/>
+    </row>
+    <row r="130" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H130" s="25"/>
+    </row>
+    <row r="131" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H131" s="25"/>
+    </row>
+    <row r="132" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H132" s="25"/>
+    </row>
+    <row r="133" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H133" s="25"/>
+    </row>
+    <row r="134" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H134" s="25"/>
+    </row>
+    <row r="135" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H135" s="25"/>
+    </row>
+    <row r="136" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H136" s="25"/>
+    </row>
+    <row r="137" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H137" s="25"/>
+    </row>
+    <row r="138" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H138" s="25"/>
+    </row>
+    <row r="139" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H139" s="25"/>
+    </row>
+    <row r="140" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H140" s="25"/>
+    </row>
+    <row r="141" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H141" s="25"/>
+    </row>
+    <row r="142" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H142" s="25"/>
+    </row>
+    <row r="143" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H143" s="25"/>
+    </row>
+    <row r="144" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H144" s="25"/>
+    </row>
+    <row r="145" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H145" s="25"/>
+    </row>
+    <row r="146" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H146" s="25"/>
+    </row>
+    <row r="147" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H147" s="25"/>
+    </row>
+    <row r="148" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H148" s="25"/>
+    </row>
+    <row r="149" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H149" s="25"/>
+    </row>
+    <row r="150" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H150" s="25"/>
+    </row>
+    <row r="151" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H151" s="25"/>
+    </row>
+    <row r="152" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H152" s="25"/>
+    </row>
+    <row r="153" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H153" s="25"/>
+    </row>
+    <row r="154" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H154" s="25"/>
+    </row>
+    <row r="155" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H155" s="25"/>
+    </row>
+    <row r="156" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H156" s="25"/>
+    </row>
+    <row r="157" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H157" s="25"/>
+    </row>
+    <row r="158" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H158" s="25"/>
+    </row>
+    <row r="159" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H159" s="25"/>
+    </row>
+    <row r="160" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H160" s="25"/>
+    </row>
+    <row r="161" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H161" s="25"/>
+    </row>
+    <row r="162" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H162" s="25"/>
+    </row>
+    <row r="163" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H163" s="25"/>
+    </row>
+    <row r="164" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H164" s="25"/>
+    </row>
+    <row r="165" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H165" s="25"/>
+    </row>
+    <row r="166" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H166" s="25"/>
+    </row>
+    <row r="167" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H167" s="25"/>
+    </row>
+    <row r="168" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H168" s="25"/>
+    </row>
+    <row r="169" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H169" s="25"/>
+    </row>
+    <row r="170" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H170" s="25"/>
+    </row>
+    <row r="171" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H171" s="25"/>
+    </row>
+    <row r="172" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H172" s="25"/>
+    </row>
+    <row r="173" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H173" s="25"/>
+    </row>
+    <row r="174" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H174" s="25"/>
+    </row>
+    <row r="175" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H175" s="25"/>
+    </row>
+    <row r="176" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H176" s="25"/>
+    </row>
+    <row r="177" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H177" s="25"/>
+    </row>
+    <row r="178" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H178" s="25"/>
+    </row>
+    <row r="179" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H179" s="25"/>
+    </row>
+    <row r="180" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H180" s="25"/>
+    </row>
+    <row r="181" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H181" s="25"/>
+    </row>
+    <row r="182" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H182" s="25"/>
+    </row>
+    <row r="183" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H183" s="25"/>
+    </row>
+    <row r="184" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H184" s="25"/>
+    </row>
+    <row r="185" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H185" s="25"/>
+    </row>
+    <row r="186" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H186" s="25"/>
+    </row>
+    <row r="187" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H187" s="25"/>
+    </row>
+    <row r="188" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H188" s="25"/>
+    </row>
+    <row r="189" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H189" s="25"/>
+    </row>
+    <row r="190" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H190" s="25"/>
+    </row>
+    <row r="191" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H191" s="25"/>
+    </row>
+    <row r="192" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H192" s="25"/>
+    </row>
+    <row r="193" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H193" s="25"/>
+    </row>
+    <row r="194" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H194" s="25"/>
+    </row>
+    <row r="195" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H195" s="25"/>
+    </row>
+    <row r="196" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H196" s="25"/>
+    </row>
+    <row r="197" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H197" s="25"/>
+    </row>
+    <row r="198" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H198" s="25"/>
+    </row>
+    <row r="199" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H199" s="25"/>
+    </row>
+    <row r="200" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H200" s="25"/>
+    </row>
+    <row r="201" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H201" s="25"/>
+    </row>
+    <row r="202" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H202" s="25"/>
+    </row>
+    <row r="203" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H203" s="25"/>
+    </row>
+    <row r="204" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H204" s="25"/>
+    </row>
+    <row r="205" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H205" s="25"/>
+    </row>
+    <row r="206" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H206" s="25"/>
+    </row>
+    <row r="207" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H207" s="25"/>
+    </row>
+    <row r="208" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H208" s="25"/>
+    </row>
+    <row r="209" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H209" s="25"/>
+    </row>
+    <row r="210" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H210" s="25"/>
+    </row>
+    <row r="211" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H211" s="25"/>
+    </row>
+    <row r="212" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H212" s="25"/>
+    </row>
+    <row r="213" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H213" s="25"/>
+    </row>
+    <row r="214" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H214" s="25"/>
+    </row>
+    <row r="215" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H215" s="25"/>
+    </row>
+    <row r="216" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H216" s="25"/>
+    </row>
+    <row r="217" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H217" s="25"/>
+    </row>
+    <row r="218" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H218" s="25"/>
+    </row>
+    <row r="219" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H219" s="25"/>
+    </row>
+    <row r="220" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H220" s="25"/>
+    </row>
+    <row r="221" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H221" s="25"/>
+    </row>
+    <row r="222" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H222" s="25"/>
+    </row>
+    <row r="223" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H223" s="25"/>
+    </row>
+    <row r="224" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H224" s="25"/>
+    </row>
+    <row r="225" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H225" s="25"/>
+    </row>
+    <row r="226" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H226" s="25"/>
+    </row>
+    <row r="227" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H227" s="25"/>
+    </row>
+    <row r="228" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H228" s="25"/>
+    </row>
+    <row r="229" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H229" s="25"/>
+    </row>
+    <row r="230" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H230" s="25"/>
+    </row>
+    <row r="231" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H231" s="25"/>
+    </row>
+    <row r="232" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H232" s="25"/>
+    </row>
+    <row r="233" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H233" s="25"/>
+    </row>
+    <row r="234" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H234" s="25"/>
+    </row>
+    <row r="235" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H235" s="25"/>
+    </row>
+    <row r="236" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H236" s="25"/>
+    </row>
+    <row r="237" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H237" s="25"/>
+    </row>
+    <row r="238" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H238" s="25"/>
+    </row>
+    <row r="239" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H239" s="25"/>
+    </row>
+    <row r="240" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H240" s="25"/>
+    </row>
+    <row r="241" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H241" s="25"/>
+    </row>
+    <row r="242" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H242" s="25"/>
+    </row>
+    <row r="243" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H243" s="25"/>
+    </row>
+    <row r="244" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H244" s="25"/>
+    </row>
+    <row r="245" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H245" s="25"/>
+    </row>
+    <row r="246" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H246" s="25"/>
+    </row>
+    <row r="247" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H247" s="25"/>
+    </row>
+    <row r="248" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H248" s="25"/>
+    </row>
+    <row r="249" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H249" s="25"/>
+    </row>
+    <row r="250" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H250" s="25"/>
+    </row>
+    <row r="251" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H251" s="25"/>
+    </row>
+    <row r="252" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H252" s="25"/>
+    </row>
+    <row r="253" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H253" s="25"/>
+    </row>
+    <row r="254" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H254" s="25"/>
+    </row>
+    <row r="255" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H255" s="25"/>
+    </row>
+    <row r="256" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H256" s="25"/>
+    </row>
+    <row r="257" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H257" s="25"/>
+    </row>
+    <row r="258" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H258" s="25"/>
+    </row>
+    <row r="259" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H259" s="25"/>
+    </row>
+    <row r="260" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H260" s="25"/>
+    </row>
+    <row r="261" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H261" s="25"/>
+    </row>
+    <row r="262" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H262" s="25"/>
+    </row>
+    <row r="263" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H263" s="25"/>
+    </row>
+    <row r="264" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H264" s="25"/>
+    </row>
+    <row r="265" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H265" s="25"/>
+    </row>
+    <row r="266" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H266" s="25"/>
+    </row>
+    <row r="267" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H267" s="25"/>
+    </row>
+    <row r="268" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H268" s="25"/>
+    </row>
+    <row r="269" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H269" s="25"/>
+    </row>
+    <row r="270" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H270" s="25"/>
+    </row>
+    <row r="271" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H271" s="25"/>
+    </row>
+    <row r="272" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H272" s="25"/>
+    </row>
+    <row r="273" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H273" s="25"/>
+    </row>
+    <row r="274" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H274" s="25"/>
+    </row>
+    <row r="275" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H275" s="25"/>
+    </row>
+    <row r="276" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H276" s="25"/>
+    </row>
+    <row r="277" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H277" s="25"/>
+    </row>
+    <row r="278" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H278" s="25"/>
+    </row>
+    <row r="279" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H279" s="25"/>
+    </row>
+    <row r="280" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H280" s="25"/>
+    </row>
+    <row r="281" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H281" s="25"/>
+    </row>
+    <row r="282" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H282" s="25"/>
+    </row>
+    <row r="283" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H283" s="25"/>
+    </row>
+    <row r="284" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H284" s="25"/>
+    </row>
+    <row r="285" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H285" s="25"/>
+    </row>
+    <row r="286" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H286" s="25"/>
+    </row>
+    <row r="287" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H287" s="25"/>
+    </row>
+    <row r="288" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H288" s="25"/>
+    </row>
+    <row r="289" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H289" s="25"/>
+    </row>
+    <row r="290" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H290" s="25"/>
+    </row>
+    <row r="291" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H291" s="25"/>
+    </row>
+    <row r="292" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H292" s="25"/>
+    </row>
+    <row r="293" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H293" s="25"/>
+    </row>
+    <row r="294" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H294" s="25"/>
+    </row>
+    <row r="295" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H295" s="25"/>
+    </row>
+    <row r="296" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H296" s="25"/>
+    </row>
+    <row r="297" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H297" s="25"/>
+    </row>
+    <row r="298" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H298" s="25"/>
+    </row>
+    <row r="299" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H299" s="25"/>
+    </row>
+    <row r="300" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H300" s="25"/>
+    </row>
+    <row r="301" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H301" s="25"/>
+    </row>
+    <row r="302" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H302" s="25"/>
+    </row>
+    <row r="303" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H303" s="25"/>
+    </row>
+    <row r="304" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H304" s="25"/>
+    </row>
+    <row r="305" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H305" s="25"/>
+    </row>
+    <row r="306" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H306" s="25"/>
+    </row>
+    <row r="307" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H307" s="25"/>
+    </row>
+    <row r="308" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H308" s="25"/>
+    </row>
+    <row r="309" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H309" s="25"/>
+    </row>
+    <row r="310" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H310" s="25"/>
+    </row>
+    <row r="311" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H311" s="25"/>
+    </row>
+    <row r="312" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H312" s="25"/>
+    </row>
+    <row r="313" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H313" s="25"/>
+    </row>
+    <row r="314" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H314" s="25"/>
+    </row>
+    <row r="315" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H315" s="25"/>
+    </row>
+    <row r="316" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H316" s="25"/>
+    </row>
+    <row r="317" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H317" s="25"/>
+    </row>
+    <row r="318" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H318" s="25"/>
+    </row>
+    <row r="319" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H319" s="25"/>
+    </row>
+    <row r="320" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H320" s="25"/>
+    </row>
+    <row r="321" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H321" s="25"/>
+    </row>
+    <row r="322" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H322" s="25"/>
+    </row>
+    <row r="323" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H323" s="25"/>
+    </row>
+    <row r="324" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H324" s="25"/>
+    </row>
+    <row r="325" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H325" s="25"/>
+    </row>
+    <row r="326" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H326" s="25"/>
+    </row>
+    <row r="327" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H327" s="25"/>
+    </row>
+    <row r="328" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H328" s="25"/>
+    </row>
+    <row r="329" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H329" s="25"/>
+    </row>
+    <row r="330" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H330" s="25"/>
+    </row>
+    <row r="331" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H331" s="25"/>
+    </row>
+    <row r="332" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H332" s="25"/>
+    </row>
+    <row r="333" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H333" s="25"/>
+    </row>
+    <row r="334" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H334" s="25"/>
+    </row>
+    <row r="335" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H335" s="25"/>
+    </row>
+    <row r="336" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H336" s="25"/>
+    </row>
+    <row r="337" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H337" s="25"/>
+    </row>
+    <row r="338" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H338" s="25"/>
+    </row>
+    <row r="339" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H339" s="25"/>
+    </row>
+    <row r="340" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H340" s="25"/>
+    </row>
+    <row r="341" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H341" s="25"/>
+    </row>
+    <row r="342" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H342" s="25"/>
+    </row>
+    <row r="343" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H343" s="25"/>
+    </row>
+    <row r="344" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H344" s="25"/>
+    </row>
+    <row r="345" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H345" s="25"/>
+    </row>
+    <row r="346" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H346" s="25"/>
+    </row>
+    <row r="347" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H347" s="25"/>
+    </row>
+    <row r="348" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H348" s="25"/>
+    </row>
+    <row r="349" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H349" s="25"/>
+    </row>
+    <row r="350" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H350" s="25"/>
+    </row>
+    <row r="351" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H351" s="25"/>
+    </row>
+    <row r="352" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H352" s="25"/>
+    </row>
+    <row r="353" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H353" s="25"/>
+    </row>
+    <row r="354" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H354" s="25"/>
+    </row>
+    <row r="355" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H355" s="25"/>
+    </row>
+    <row r="356" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H356" s="25"/>
+    </row>
+    <row r="357" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H357" s="25"/>
+    </row>
+    <row r="358" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H358" s="25"/>
+    </row>
+    <row r="359" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H359" s="25"/>
+    </row>
+    <row r="360" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H360" s="25"/>
+    </row>
+    <row r="361" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H361" s="25"/>
+    </row>
+    <row r="362" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H362" s="25"/>
+    </row>
+    <row r="363" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H363" s="25"/>
+    </row>
+    <row r="364" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H364" s="25"/>
+    </row>
+    <row r="365" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H365" s="25"/>
+    </row>
+    <row r="366" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H366" s="25"/>
+    </row>
+    <row r="367" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H367" s="25"/>
+    </row>
+    <row r="368" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H368" s="25"/>
+    </row>
+    <row r="369" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H369" s="25"/>
+    </row>
+    <row r="370" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H370" s="25"/>
+    </row>
+    <row r="371" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H371" s="25"/>
+    </row>
+    <row r="372" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H372" s="25"/>
+    </row>
+    <row r="373" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H373" s="25"/>
+    </row>
+    <row r="374" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H374" s="25"/>
+    </row>
+    <row r="375" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H375" s="25"/>
+    </row>
+    <row r="376" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H376" s="25"/>
+    </row>
+    <row r="377" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H377" s="25"/>
+    </row>
+    <row r="378" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H378" s="25"/>
+    </row>
+    <row r="379" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H379" s="25"/>
+    </row>
+    <row r="380" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H380" s="25"/>
+    </row>
+    <row r="381" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H381" s="25"/>
+    </row>
+    <row r="382" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H382" s="25"/>
+    </row>
+    <row r="383" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H383" s="25"/>
+    </row>
+    <row r="384" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H384" s="25"/>
+    </row>
+    <row r="385" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H385" s="25"/>
+    </row>
+    <row r="386" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H386" s="25"/>
+    </row>
+    <row r="387" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H387" s="25"/>
+    </row>
+    <row r="388" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H388" s="25"/>
+    </row>
+    <row r="389" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H389" s="25"/>
+    </row>
+    <row r="390" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H390" s="25"/>
+    </row>
+    <row r="391" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H391" s="25"/>
+    </row>
+    <row r="392" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H392" s="25"/>
+    </row>
+    <row r="393" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H393" s="25"/>
+    </row>
+    <row r="394" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H394" s="25"/>
+    </row>
+    <row r="395" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H395" s="25"/>
+    </row>
+    <row r="396" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H396" s="25"/>
+    </row>
+    <row r="397" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H397" s="25"/>
+    </row>
+    <row r="398" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H398" s="25"/>
+    </row>
+    <row r="399" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H399" s="25"/>
+    </row>
+    <row r="400" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H400" s="25"/>
+    </row>
+    <row r="401" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H401" s="25"/>
+    </row>
+    <row r="402" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H402" s="25"/>
+    </row>
+    <row r="403" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H403" s="25"/>
+    </row>
+    <row r="404" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H404" s="25"/>
+    </row>
+    <row r="405" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H405" s="25"/>
+    </row>
+    <row r="406" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H406" s="25"/>
+    </row>
+    <row r="407" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H407" s="25"/>
+    </row>
+    <row r="408" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H408" s="25"/>
+    </row>
+    <row r="409" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H409" s="25"/>
+    </row>
+    <row r="410" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H410" s="25"/>
+    </row>
+    <row r="411" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H411" s="25"/>
+    </row>
+    <row r="412" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H412" s="25"/>
+    </row>
+    <row r="413" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H413" s="25"/>
+    </row>
+    <row r="414" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H414" s="25"/>
+    </row>
+    <row r="415" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H415" s="25"/>
+    </row>
+    <row r="416" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H416" s="25"/>
+    </row>
+    <row r="417" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H417" s="25"/>
+    </row>
+    <row r="418" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H418" s="25"/>
+    </row>
+    <row r="419" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H419" s="25"/>
+    </row>
+    <row r="420" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H420" s="25"/>
+    </row>
+    <row r="421" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H421" s="25"/>
+    </row>
+    <row r="422" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H422" s="25"/>
+    </row>
+    <row r="423" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H423" s="25"/>
+    </row>
+    <row r="424" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H424" s="25"/>
+    </row>
+    <row r="425" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H425" s="25"/>
+    </row>
+    <row r="426" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H426" s="25"/>
+    </row>
+    <row r="427" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H427" s="25"/>
+    </row>
+    <row r="428" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H428" s="25"/>
+    </row>
+    <row r="429" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H429" s="25"/>
+    </row>
+    <row r="430" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H430" s="25"/>
+    </row>
+    <row r="431" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H431" s="25"/>
+    </row>
+    <row r="432" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H432" s="25"/>
+    </row>
+    <row r="433" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H433" s="25"/>
+    </row>
+    <row r="434" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H434" s="25"/>
+    </row>
+    <row r="435" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H435" s="25"/>
+    </row>
+    <row r="436" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H436" s="25"/>
+    </row>
+    <row r="437" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H437" s="25"/>
+    </row>
+    <row r="438" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H438" s="25"/>
+    </row>
+    <row r="439" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H439" s="25"/>
+    </row>
+    <row r="440" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H440" s="25"/>
+    </row>
+    <row r="441" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H441" s="25"/>
+    </row>
+    <row r="442" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H442" s="25"/>
+    </row>
+    <row r="443" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H443" s="25"/>
+    </row>
+    <row r="444" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H444" s="25"/>
+    </row>
+    <row r="445" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H445" s="25"/>
+    </row>
+    <row r="446" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H446" s="25"/>
+    </row>
+    <row r="447" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H447" s="25"/>
+    </row>
+    <row r="448" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H448" s="25"/>
+    </row>
+    <row r="449" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H449" s="25"/>
+    </row>
+    <row r="450" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H450" s="25"/>
+    </row>
+    <row r="451" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H451" s="25"/>
+    </row>
+    <row r="452" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H452" s="25"/>
+    </row>
+    <row r="453" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H453" s="25"/>
+    </row>
+    <row r="454" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H454" s="25"/>
+    </row>
+    <row r="455" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H455" s="25"/>
+    </row>
+    <row r="456" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H456" s="25"/>
+    </row>
+    <row r="457" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H457" s="25"/>
+    </row>
+    <row r="458" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H458" s="25"/>
+    </row>
+    <row r="459" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H459" s="25"/>
+    </row>
+    <row r="460" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H460" s="25"/>
+    </row>
+    <row r="461" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H461" s="25"/>
+    </row>
+    <row r="462" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H462" s="25"/>
+    </row>
+    <row r="463" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H463" s="25"/>
+    </row>
+    <row r="464" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H464" s="25"/>
+    </row>
+    <row r="465" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H465" s="25"/>
+    </row>
+    <row r="466" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H466" s="25"/>
+    </row>
+    <row r="467" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H467" s="25"/>
+    </row>
+    <row r="468" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H468" s="25"/>
+    </row>
+    <row r="469" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H469" s="25"/>
+    </row>
+    <row r="470" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H470" s="25"/>
+    </row>
+    <row r="471" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H471" s="25"/>
+    </row>
+    <row r="472" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H472" s="25"/>
+    </row>
+    <row r="473" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H473" s="25"/>
+    </row>
+    <row r="474" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H474" s="25"/>
+    </row>
+    <row r="475" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H475" s="25"/>
+    </row>
+    <row r="476" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H476" s="25"/>
+    </row>
+    <row r="477" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H477" s="25"/>
+    </row>
+    <row r="478" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H478" s="25"/>
+    </row>
+    <row r="479" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H479" s="25"/>
+    </row>
+    <row r="480" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H480" s="25"/>
+    </row>
+    <row r="481" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H481" s="25"/>
+    </row>
+    <row r="482" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H482" s="25"/>
+    </row>
+    <row r="483" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H483" s="25"/>
+    </row>
+    <row r="484" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H484" s="25"/>
+    </row>
+    <row r="485" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H485" s="25"/>
+    </row>
+    <row r="486" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H486" s="25"/>
+    </row>
+    <row r="487" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H487" s="25"/>
+    </row>
+    <row r="488" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H488" s="25"/>
+    </row>
+    <row r="489" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H489" s="25"/>
+    </row>
+    <row r="490" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H490" s="25"/>
+    </row>
+    <row r="491" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H491" s="25"/>
+    </row>
+    <row r="492" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H492" s="25"/>
+    </row>
+    <row r="493" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H493" s="25"/>
+    </row>
+    <row r="494" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H494" s="25"/>
+    </row>
+    <row r="495" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H495" s="25"/>
+    </row>
+    <row r="496" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H496" s="25"/>
+    </row>
+    <row r="497" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H497" s="25"/>
+    </row>
+    <row r="498" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H498" s="25"/>
+    </row>
+    <row r="499" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H499" s="25"/>
+    </row>
+    <row r="500" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H500" s="25"/>
+    </row>
+    <row r="501" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H501" s="25"/>
+    </row>
+    <row r="502" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H502" s="25"/>
+    </row>
+    <row r="503" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H503" s="25"/>
+    </row>
+    <row r="504" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H504" s="25"/>
+    </row>
+    <row r="505" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H505" s="25"/>
+    </row>
+    <row r="506" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H506" s="25"/>
+    </row>
+    <row r="507" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H507" s="25"/>
+    </row>
+    <row r="508" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H508" s="25"/>
+    </row>
+    <row r="509" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H509" s="25"/>
+    </row>
+    <row r="510" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H510" s="25"/>
+    </row>
+    <row r="511" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H511" s="25"/>
+    </row>
+    <row r="512" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H512" s="25"/>
+    </row>
+    <row r="513" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H513" s="25"/>
+    </row>
+    <row r="514" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H514" s="25"/>
+    </row>
+    <row r="515" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H515" s="25"/>
+    </row>
+    <row r="516" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H516" s="25"/>
+    </row>
+    <row r="517" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H517" s="25"/>
+    </row>
+    <row r="518" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H518" s="25"/>
+    </row>
+    <row r="519" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H519" s="25"/>
+    </row>
+    <row r="520" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H520" s="25"/>
+    </row>
+    <row r="521" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H521" s="25"/>
+    </row>
+    <row r="522" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H522" s="25"/>
+    </row>
+    <row r="523" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H523" s="25"/>
+    </row>
+    <row r="524" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H524" s="25"/>
+    </row>
+    <row r="525" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H525" s="25"/>
+    </row>
+    <row r="526" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H526" s="25"/>
+    </row>
+    <row r="527" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H527" s="25"/>
+    </row>
+    <row r="528" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H528" s="25"/>
+    </row>
+    <row r="529" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H529" s="25"/>
+    </row>
+    <row r="530" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H530" s="25"/>
+    </row>
+    <row r="531" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H531" s="25"/>
+    </row>
+    <row r="532" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H532" s="25"/>
+    </row>
+    <row r="533" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H533" s="25"/>
+    </row>
+    <row r="534" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H534" s="25"/>
+    </row>
+    <row r="535" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H535" s="25"/>
+    </row>
+    <row r="536" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H536" s="25"/>
+    </row>
+    <row r="537" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H537" s="25"/>
+    </row>
+    <row r="538" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H538" s="25"/>
+    </row>
+    <row r="539" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H539" s="25"/>
+    </row>
+    <row r="540" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H540" s="25"/>
+    </row>
+    <row r="541" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H541" s="25"/>
+    </row>
+    <row r="542" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H542" s="25"/>
+    </row>
+    <row r="543" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H543" s="25"/>
+    </row>
+    <row r="544" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H544" s="25"/>
+    </row>
+    <row r="545" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H545" s="25"/>
+    </row>
+    <row r="546" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H546" s="25"/>
+    </row>
+    <row r="547" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H547" s="25"/>
+    </row>
+    <row r="548" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H548" s="25"/>
+    </row>
+    <row r="549" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H549" s="25"/>
+    </row>
+    <row r="550" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H550" s="25"/>
+    </row>
+    <row r="551" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H551" s="25"/>
+    </row>
+    <row r="552" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H552" s="25"/>
+    </row>
+    <row r="553" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H553" s="25"/>
+    </row>
+    <row r="554" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H554" s="25"/>
+    </row>
+    <row r="555" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H555" s="25"/>
+    </row>
+    <row r="556" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H556" s="25"/>
+    </row>
+    <row r="557" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H557" s="25"/>
+    </row>
+    <row r="558" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H558" s="25"/>
+    </row>
+    <row r="559" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H559" s="25"/>
+    </row>
+    <row r="560" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H560" s="25"/>
+    </row>
+    <row r="561" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H561" s="25"/>
+    </row>
+    <row r="562" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H562" s="25"/>
+    </row>
+    <row r="563" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H563" s="25"/>
+    </row>
+    <row r="564" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H564" s="25"/>
+    </row>
+    <row r="565" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H565" s="25"/>
+    </row>
+    <row r="566" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H566" s="25"/>
+    </row>
+    <row r="567" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H567" s="25"/>
+    </row>
+    <row r="568" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H568" s="25"/>
+    </row>
+    <row r="569" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H569" s="25"/>
+    </row>
+    <row r="570" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H570" s="25"/>
+    </row>
+    <row r="571" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H571" s="25"/>
+    </row>
+    <row r="572" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H572" s="25"/>
+    </row>
+    <row r="573" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H573" s="25"/>
+    </row>
+    <row r="574" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H574" s="25"/>
+    </row>
+    <row r="575" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H575" s="25"/>
+    </row>
+    <row r="576" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H576" s="25"/>
+    </row>
+    <row r="577" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H577" s="25"/>
+    </row>
+    <row r="578" spans="8:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="H578" s="25"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -19075,7 +20476,7 @@
           <x14:formula1>
             <xm:f>General!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:G1048576</xm:sqref>
+          <xm:sqref>B2:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -20162,7 +21563,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28156,8 +29557,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H1072"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30114,17 +31515,17 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:V2827"/>
+  <dimension ref="A1:V2816"/>
   <sheetViews>
-    <sheetView topLeftCell="O79" workbookViewId="0">
-      <selection activeCell="V106" sqref="V106"/>
+    <sheetView topLeftCell="R46" workbookViewId="0">
+      <selection activeCell="V60" sqref="V60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
@@ -32849,60 +34250,649 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="M51" s="7"/>
-    </row>
-    <row r="52" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="M52" s="7"/>
-    </row>
-    <row r="53" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="M53" s="7"/>
-    </row>
-    <row r="54" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="M54" s="7"/>
-    </row>
-    <row r="55" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B55" s="7"/>
-      <c r="H55" s="7"/>
-      <c r="M55" s="7"/>
-    </row>
-    <row r="56" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="M56" s="7"/>
-    </row>
-    <row r="57" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="M57" s="7"/>
-    </row>
-    <row r="58" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="M58" s="7"/>
-    </row>
-    <row r="59" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B59" s="7"/>
-      <c r="H59" s="7"/>
-      <c r="M59" s="7"/>
-    </row>
-    <row r="60" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B60" s="7"/>
-      <c r="H60" s="7"/>
-      <c r="M60" s="7"/>
-    </row>
-    <row r="61" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B61" s="7"/>
-      <c r="H61" s="7"/>
-      <c r="M61" s="7"/>
+    <row r="51" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="25">
+        <v>50</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>404</v>
+      </c>
+      <c r="D51" s="26">
+        <v>1</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F51" s="26">
+        <v>0</v>
+      </c>
+      <c r="G51" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="N51" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="O51" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="P51" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="Q51" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="R51" s="26">
+        <v>11</v>
+      </c>
+      <c r="S51" s="26">
+        <v>11</v>
+      </c>
+      <c r="T51" s="26">
+        <v>1</v>
+      </c>
+      <c r="U51" s="26">
+        <v>1</v>
+      </c>
+      <c r="V51" s="26" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="25">
+        <v>51</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>405</v>
+      </c>
+      <c r="D52" s="26">
+        <v>1</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F52" s="26">
+        <v>0</v>
+      </c>
+      <c r="G52" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="N52" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="O52" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="P52" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="Q52" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="R52" s="26">
+        <v>11</v>
+      </c>
+      <c r="S52" s="26">
+        <v>11</v>
+      </c>
+      <c r="T52" s="26">
+        <v>1</v>
+      </c>
+      <c r="U52" s="26">
+        <v>1</v>
+      </c>
+      <c r="V52" s="26"/>
+    </row>
+    <row r="53" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="25">
+        <v>52</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>397</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="D53" s="26">
+        <v>1</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F53" s="26">
+        <v>0</v>
+      </c>
+      <c r="G53" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="26"/>
+      <c r="K53" s="26"/>
+      <c r="L53" s="26"/>
+      <c r="M53" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="N53" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="O53" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="P53" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="Q53" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="R53" s="26">
+        <v>11</v>
+      </c>
+      <c r="S53" s="26">
+        <v>11</v>
+      </c>
+      <c r="T53" s="26">
+        <v>1</v>
+      </c>
+      <c r="U53" s="26">
+        <v>1</v>
+      </c>
+      <c r="V53" s="26" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="25">
+        <v>53</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>407</v>
+      </c>
+      <c r="D54" s="26">
+        <v>1</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F54" s="26">
+        <v>0</v>
+      </c>
+      <c r="G54" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="26"/>
+      <c r="M54" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="N54" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="O54" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="P54" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="Q54" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="R54" s="26">
+        <v>11</v>
+      </c>
+      <c r="S54" s="26">
+        <v>11</v>
+      </c>
+      <c r="T54" s="26">
+        <v>1</v>
+      </c>
+      <c r="U54" s="26">
+        <v>1</v>
+      </c>
+      <c r="V54" s="26">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="25">
+        <v>54</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>395</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>408</v>
+      </c>
+      <c r="D55" s="26">
+        <v>1</v>
+      </c>
+      <c r="E55" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F55" s="26">
+        <v>0</v>
+      </c>
+      <c r="G55" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="26"/>
+      <c r="K55" s="26"/>
+      <c r="L55" s="26"/>
+      <c r="M55" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="N55" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="O55" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="P55" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="Q55" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="R55" s="26">
+        <v>11</v>
+      </c>
+      <c r="S55" s="26">
+        <v>11</v>
+      </c>
+      <c r="T55" s="26">
+        <v>1</v>
+      </c>
+      <c r="U55" s="26">
+        <v>1</v>
+      </c>
+      <c r="V55" s="26">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="25">
+        <v>55</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="D56" s="26">
+        <v>1</v>
+      </c>
+      <c r="E56" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="F56" s="26">
+        <v>0</v>
+      </c>
+      <c r="G56" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="26"/>
+      <c r="L56" s="26"/>
+      <c r="M56" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="N56" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="O56" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="P56" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="Q56" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="R56" s="26">
+        <v>11</v>
+      </c>
+      <c r="S56" s="26">
+        <v>21</v>
+      </c>
+      <c r="T56" s="26">
+        <v>1</v>
+      </c>
+      <c r="U56" s="26">
+        <v>1</v>
+      </c>
+      <c r="V56" s="26" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="25">
+        <v>56</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>410</v>
+      </c>
+      <c r="D57" s="26">
+        <v>1</v>
+      </c>
+      <c r="E57" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="F57" s="26">
+        <v>0</v>
+      </c>
+      <c r="G57" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H57" s="26"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="26"/>
+      <c r="L57" s="26"/>
+      <c r="M57" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="N57" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="O57" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="P57" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="Q57" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="R57" s="26">
+        <v>11</v>
+      </c>
+      <c r="S57" s="26">
+        <v>21</v>
+      </c>
+      <c r="T57" s="26">
+        <v>1</v>
+      </c>
+      <c r="U57" s="26">
+        <v>1</v>
+      </c>
+      <c r="V57" s="26" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="25">
+        <v>57</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>399</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="D58" s="26">
+        <v>1</v>
+      </c>
+      <c r="E58" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="F58" s="26">
+        <v>0</v>
+      </c>
+      <c r="G58" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="26"/>
+      <c r="L58" s="26"/>
+      <c r="M58" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="N58" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="O58" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="P58" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="Q58" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="R58" s="26">
+        <v>11</v>
+      </c>
+      <c r="S58" s="26">
+        <v>21</v>
+      </c>
+      <c r="T58" s="26">
+        <v>1</v>
+      </c>
+      <c r="U58" s="26">
+        <v>1</v>
+      </c>
+      <c r="V58" s="26" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="25">
+        <v>58</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="C59" s="25" t="s">
+        <v>412</v>
+      </c>
+      <c r="D59" s="26">
+        <v>1</v>
+      </c>
+      <c r="E59" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="F59" s="26">
+        <v>0</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H59" s="26"/>
+      <c r="I59" s="25">
+        <v>37.4206</v>
+      </c>
+      <c r="J59" s="25">
+        <v>-121.9725</v>
+      </c>
+      <c r="K59" s="25">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L59" s="25">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="M59" s="25"/>
+      <c r="N59" s="23"/>
+      <c r="O59" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="P59" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="Q59" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="R59" s="26">
+        <v>11</v>
+      </c>
+      <c r="S59" s="26">
+        <v>21</v>
+      </c>
+      <c r="T59" s="26">
+        <v>4</v>
+      </c>
+      <c r="U59" s="26">
+        <v>11</v>
+      </c>
+      <c r="V59" s="26">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="25">
+        <v>59</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="C60" s="25" t="s">
+        <v>413</v>
+      </c>
+      <c r="D60" s="26">
+        <v>1</v>
+      </c>
+      <c r="E60" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="F60" s="26">
+        <v>0</v>
+      </c>
+      <c r="G60" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H60" s="26"/>
+      <c r="I60" s="25"/>
+      <c r="J60" s="25"/>
+      <c r="K60" s="25"/>
+      <c r="L60" s="25"/>
+      <c r="M60" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="N60" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="O60" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="P60" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="Q60" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="R60" s="26">
+        <v>11</v>
+      </c>
+      <c r="S60" s="26">
+        <v>18</v>
+      </c>
+      <c r="T60" s="26">
+        <v>4</v>
+      </c>
+      <c r="U60" s="26">
+        <v>11</v>
+      </c>
+      <c r="V60" s="26">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="25">
+        <v>60</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="C61" s="25" t="s">
+        <v>414</v>
+      </c>
+      <c r="D61" s="26">
+        <v>1</v>
+      </c>
+      <c r="E61" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="F61" s="26">
+        <v>0</v>
+      </c>
+      <c r="G61" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H61" s="26"/>
+      <c r="I61" s="25">
+        <v>37.4206</v>
+      </c>
+      <c r="J61" s="25">
+        <v>-121.9725</v>
+      </c>
+      <c r="K61" s="25">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L61" s="25">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="M61" s="25"/>
+      <c r="N61" s="23"/>
+      <c r="O61" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="P61" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="Q61" s="26">
+        <v>8.5</v>
+      </c>
+      <c r="R61" s="26">
+        <v>11</v>
+      </c>
+      <c r="S61" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="T61" s="26">
+        <v>1</v>
+      </c>
+      <c r="U61" s="26">
+        <v>7</v>
+      </c>
+      <c r="V61" s="26">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B62" s="7"/>
@@ -33079,397 +35069,82 @@
       <c r="H96" s="7"/>
       <c r="M96" s="7"/>
     </row>
-    <row r="97" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B97" s="7"/>
       <c r="H97" s="7"/>
       <c r="M97" s="7"/>
     </row>
-    <row r="98" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B98" s="7"/>
       <c r="H98" s="7"/>
       <c r="M98" s="7"/>
     </row>
-    <row r="99" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B99" s="7"/>
       <c r="H99" s="7"/>
       <c r="M99" s="7"/>
     </row>
-    <row r="100" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B100" s="7"/>
       <c r="H100" s="7"/>
       <c r="M100" s="7"/>
     </row>
-    <row r="101" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="21">
-        <v>100</v>
-      </c>
-      <c r="B101" s="21" t="s">
-        <v>386</v>
-      </c>
-      <c r="C101" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D101" s="21">
-        <v>1</v>
-      </c>
-      <c r="E101" s="21" t="s">
-        <v>381</v>
-      </c>
-      <c r="F101" s="21">
-        <v>0</v>
-      </c>
-      <c r="G101" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H101" s="21"/>
-      <c r="I101" s="21"/>
-      <c r="J101" s="21"/>
-      <c r="K101" s="21"/>
-      <c r="L101" s="21"/>
-      <c r="M101" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="N101" s="19" t="s">
-        <v>383</v>
-      </c>
-      <c r="O101" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="P101" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="Q101" s="21">
-        <v>8.5</v>
-      </c>
-      <c r="R101" s="21">
-        <v>11</v>
-      </c>
-      <c r="S101" s="21">
-        <v>12</v>
-      </c>
-      <c r="T101" s="21">
-        <v>1</v>
-      </c>
-      <c r="U101" s="21">
-        <v>1</v>
-      </c>
-      <c r="V101" s="21" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="102" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="21">
-        <v>101</v>
-      </c>
-      <c r="B102" s="21"/>
-      <c r="C102" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D102" s="21">
-        <v>1</v>
-      </c>
-      <c r="E102" s="21" t="s">
-        <v>381</v>
-      </c>
-      <c r="F102" s="21">
-        <v>0</v>
-      </c>
-      <c r="G102" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H102" s="21"/>
-      <c r="I102" s="21"/>
-      <c r="J102" s="21"/>
-      <c r="K102" s="21"/>
-      <c r="L102" s="21"/>
-      <c r="M102" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="N102" s="19" t="s">
-        <v>383</v>
-      </c>
-      <c r="O102" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="P102" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="Q102" s="21">
-        <v>8.5</v>
-      </c>
-      <c r="R102" s="21">
-        <v>11</v>
-      </c>
-      <c r="S102" s="21">
-        <v>12</v>
-      </c>
-      <c r="T102" s="21">
-        <v>1</v>
-      </c>
-      <c r="U102" s="21">
-        <v>1</v>
-      </c>
-      <c r="V102" s="21"/>
-    </row>
-    <row r="103" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="21">
-        <v>102</v>
-      </c>
-      <c r="B103" s="21"/>
-      <c r="C103" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D103" s="21">
-        <v>1</v>
-      </c>
-      <c r="E103" s="21" t="s">
-        <v>381</v>
-      </c>
-      <c r="F103" s="21">
-        <v>0</v>
-      </c>
-      <c r="G103" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H103" s="21"/>
-      <c r="I103" s="21"/>
-      <c r="J103" s="21"/>
-      <c r="K103" s="21"/>
-      <c r="L103" s="21"/>
-      <c r="M103" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="N103" s="19" t="s">
-        <v>383</v>
-      </c>
-      <c r="O103" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="P103" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="Q103" s="21">
-        <v>8.5</v>
-      </c>
-      <c r="R103" s="21">
-        <v>11</v>
-      </c>
-      <c r="S103" s="21">
-        <v>12</v>
-      </c>
-      <c r="T103" s="21">
-        <v>1</v>
-      </c>
-      <c r="U103" s="21">
-        <v>1</v>
-      </c>
-      <c r="V103" s="21" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="104" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="21">
-        <v>103</v>
-      </c>
-      <c r="B104" s="21"/>
-      <c r="C104" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D104" s="21">
-        <v>1</v>
-      </c>
-      <c r="E104" s="21" t="s">
-        <v>381</v>
-      </c>
-      <c r="F104" s="21">
-        <v>0</v>
-      </c>
-      <c r="G104" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H104" s="21"/>
-      <c r="I104" s="21"/>
-      <c r="J104" s="21"/>
-      <c r="K104" s="21"/>
-      <c r="L104" s="21"/>
-      <c r="M104" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="N104" s="19" t="s">
-        <v>383</v>
-      </c>
-      <c r="O104" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="P104" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="Q104" s="21">
-        <v>8.5</v>
-      </c>
-      <c r="R104" s="21">
-        <v>11</v>
-      </c>
-      <c r="S104" s="21">
-        <v>12</v>
-      </c>
-      <c r="T104" s="21">
-        <v>1</v>
-      </c>
-      <c r="U104" s="21">
-        <v>1</v>
-      </c>
-      <c r="V104" s="21">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="105" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="21">
-        <v>104</v>
-      </c>
-      <c r="B105" s="21"/>
-      <c r="C105" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D105" s="21">
-        <v>1</v>
-      </c>
-      <c r="E105" s="21" t="s">
-        <v>381</v>
-      </c>
-      <c r="F105" s="21">
-        <v>0</v>
-      </c>
-      <c r="G105" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H105" s="21"/>
-      <c r="I105" s="21"/>
-      <c r="J105" s="21"/>
-      <c r="K105" s="21"/>
-      <c r="L105" s="21"/>
-      <c r="M105" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="N105" s="19" t="s">
-        <v>383</v>
-      </c>
-      <c r="O105" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="P105" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="Q105" s="21">
-        <v>8.5</v>
-      </c>
-      <c r="R105" s="21">
-        <v>11</v>
-      </c>
-      <c r="S105" s="21">
-        <v>12</v>
-      </c>
-      <c r="T105" s="21">
-        <v>1</v>
-      </c>
-      <c r="U105" s="21">
-        <v>1</v>
-      </c>
-      <c r="V105" s="21">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="106" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="21">
-        <v>105</v>
-      </c>
-      <c r="B106" s="21"/>
-      <c r="C106" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D106" s="21">
-        <v>1</v>
-      </c>
-      <c r="E106" s="21" t="s">
-        <v>381</v>
-      </c>
-      <c r="F106" s="21">
-        <v>0</v>
-      </c>
-      <c r="G106" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="H106" s="21"/>
-      <c r="I106" s="21"/>
-      <c r="J106" s="21"/>
-      <c r="K106" s="21"/>
-      <c r="L106" s="21"/>
-      <c r="M106" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="N106" s="19" t="s">
-        <v>383</v>
-      </c>
-      <c r="O106" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="P106" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="Q106" s="21">
-        <v>8.5</v>
-      </c>
-      <c r="R106" s="21">
-        <v>11</v>
-      </c>
-      <c r="S106" s="21">
-        <v>12</v>
-      </c>
-      <c r="T106" s="21">
-        <v>1</v>
-      </c>
-      <c r="U106" s="21">
-        <v>1</v>
-      </c>
-      <c r="V106" s="21" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="107" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B101" s="7"/>
+      <c r="H101" s="7"/>
+      <c r="M101" s="7"/>
+    </row>
+    <row r="102" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B102" s="7"/>
+      <c r="H102" s="7"/>
+      <c r="M102" s="7"/>
+    </row>
+    <row r="103" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B103" s="7"/>
+      <c r="H103" s="7"/>
+      <c r="M103" s="7"/>
+    </row>
+    <row r="104" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B104" s="7"/>
+      <c r="H104" s="7"/>
+      <c r="M104" s="7"/>
+    </row>
+    <row r="105" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B105" s="7"/>
+      <c r="H105" s="7"/>
+      <c r="M105" s="7"/>
+    </row>
+    <row r="106" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B106" s="7"/>
+      <c r="H106" s="7"/>
+      <c r="M106" s="7"/>
+    </row>
+    <row r="107" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B107" s="7"/>
-      <c r="C107" s="20" t="s">
-        <v>103</v>
-      </c>
       <c r="H107" s="7"/>
       <c r="M107" s="7"/>
     </row>
-    <row r="108" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B108" s="7"/>
-      <c r="C108" s="20" t="s">
-        <v>103</v>
-      </c>
       <c r="H108" s="7"/>
       <c r="M108" s="7"/>
     </row>
-    <row r="109" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B109" s="7"/>
-      <c r="C109" s="20" t="s">
-        <v>103</v>
-      </c>
       <c r="H109" s="7"/>
       <c r="M109" s="7"/>
     </row>
-    <row r="110" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B110" s="7"/>
       <c r="H110" s="7"/>
       <c r="M110" s="7"/>
     </row>
-    <row r="111" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B111" s="7"/>
       <c r="H111" s="7"/>
       <c r="M111" s="7"/>
     </row>
-    <row r="112" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B112" s="7"/>
       <c r="H112" s="7"/>
       <c r="M112" s="7"/>
@@ -36304,118 +37979,107 @@
       <c r="H678" s="7"/>
       <c r="M678" s="7"/>
     </row>
-    <row r="679" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B679" s="7"/>
+    <row r="679" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H679" s="7"/>
       <c r="M679" s="7"/>
     </row>
-    <row r="680" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B680" s="7"/>
+    <row r="680" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H680" s="7"/>
       <c r="M680" s="7"/>
     </row>
-    <row r="681" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B681" s="7"/>
+    <row r="681" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H681" s="7"/>
       <c r="M681" s="7"/>
     </row>
-    <row r="682" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B682" s="7"/>
+    <row r="682" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H682" s="7"/>
       <c r="M682" s="7"/>
     </row>
-    <row r="683" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B683" s="7"/>
+    <row r="683" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H683" s="7"/>
       <c r="M683" s="7"/>
     </row>
-    <row r="684" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B684" s="7"/>
+    <row r="684" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H684" s="7"/>
       <c r="M684" s="7"/>
     </row>
-    <row r="685" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B685" s="7"/>
+    <row r="685" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H685" s="7"/>
       <c r="M685" s="7"/>
     </row>
-    <row r="686" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B686" s="7"/>
+    <row r="686" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H686" s="7"/>
       <c r="M686" s="7"/>
     </row>
-    <row r="687" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B687" s="7"/>
+    <row r="687" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H687" s="7"/>
       <c r="M687" s="7"/>
     </row>
-    <row r="688" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B688" s="7"/>
+    <row r="688" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H688" s="7"/>
       <c r="M688" s="7"/>
     </row>
-    <row r="689" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B689" s="7"/>
+    <row r="689" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H689" s="7"/>
       <c r="M689" s="7"/>
     </row>
-    <row r="690" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="690" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H690" s="7"/>
       <c r="M690" s="7"/>
     </row>
-    <row r="691" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="691" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H691" s="7"/>
       <c r="M691" s="7"/>
     </row>
-    <row r="692" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="692" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H692" s="7"/>
       <c r="M692" s="7"/>
     </row>
-    <row r="693" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="693" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H693" s="7"/>
       <c r="M693" s="7"/>
     </row>
-    <row r="694" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="694" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H694" s="7"/>
       <c r="M694" s="7"/>
     </row>
-    <row r="695" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="695" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H695" s="7"/>
       <c r="M695" s="7"/>
     </row>
-    <row r="696" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="696" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H696" s="7"/>
       <c r="M696" s="7"/>
     </row>
-    <row r="697" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="697" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H697" s="7"/>
       <c r="M697" s="7"/>
     </row>
-    <row r="698" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="698" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H698" s="7"/>
       <c r="M698" s="7"/>
     </row>
-    <row r="699" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="699" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H699" s="7"/>
       <c r="M699" s="7"/>
     </row>
-    <row r="700" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="700" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H700" s="7"/>
       <c r="M700" s="7"/>
     </row>
-    <row r="701" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="701" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H701" s="7"/>
       <c r="M701" s="7"/>
     </row>
-    <row r="702" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="702" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H702" s="7"/>
       <c r="M702" s="7"/>
     </row>
-    <row r="703" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="703" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H703" s="7"/>
       <c r="M703" s="7"/>
     </row>
-    <row r="704" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="704" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H704" s="7"/>
       <c r="M704" s="7"/>
     </row>
@@ -36897,88 +38561,77 @@
     </row>
     <row r="824" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H824" s="7"/>
-      <c r="M824" s="7"/>
     </row>
     <row r="825" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H825" s="7"/>
-      <c r="M825" s="7"/>
     </row>
     <row r="826" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H826" s="7"/>
-      <c r="M826" s="7"/>
     </row>
     <row r="827" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H827" s="7"/>
-      <c r="M827" s="7"/>
     </row>
     <row r="828" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H828" s="7"/>
-      <c r="M828" s="7"/>
     </row>
     <row r="829" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H829" s="7"/>
-      <c r="M829" s="7"/>
     </row>
     <row r="830" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H830" s="7"/>
-      <c r="M830" s="7"/>
     </row>
     <row r="831" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H831" s="7"/>
-      <c r="M831" s="7"/>
     </row>
     <row r="832" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H832" s="7"/>
-      <c r="M832" s="7"/>
-    </row>
-    <row r="833" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    </row>
+    <row r="833" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H833" s="7"/>
-      <c r="M833" s="7"/>
-    </row>
-    <row r="834" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    </row>
+    <row r="834" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H834" s="7"/>
-      <c r="M834" s="7"/>
-    </row>
-    <row r="835" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    </row>
+    <row r="835" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H835" s="7"/>
     </row>
-    <row r="836" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="836" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H836" s="7"/>
     </row>
-    <row r="837" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="837" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H837" s="7"/>
     </row>
-    <row r="838" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="838" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H838" s="7"/>
     </row>
-    <row r="839" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="839" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H839" s="7"/>
     </row>
-    <row r="840" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="840" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H840" s="7"/>
     </row>
-    <row r="841" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="841" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H841" s="7"/>
     </row>
-    <row r="842" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="842" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H842" s="7"/>
     </row>
-    <row r="843" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="843" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H843" s="7"/>
     </row>
-    <row r="844" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="844" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H844" s="7"/>
     </row>
-    <row r="845" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="845" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H845" s="7"/>
     </row>
-    <row r="846" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="846" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H846" s="7"/>
     </row>
-    <row r="847" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="847" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H847" s="7"/>
     </row>
-    <row r="848" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="848" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H848" s="7"/>
     </row>
     <row r="849" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -37827,37 +39480,37 @@
     <row r="1130" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1130" s="7"/>
     </row>
-    <row r="1131" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="1131" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H1131" s="7"/>
     </row>
-    <row r="1132" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="1132" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H1132" s="7"/>
     </row>
-    <row r="1133" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="1133" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H1133" s="7"/>
     </row>
-    <row r="1134" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="1134" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H1134" s="7"/>
     </row>
-    <row r="1135" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="1135" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H1135" s="7"/>
     </row>
-    <row r="1136" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="1136" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H1136" s="7"/>
     </row>
-    <row r="1137" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="1137" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H1137" s="7"/>
     </row>
-    <row r="1138" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="1138" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H1138" s="7"/>
     </row>
-    <row r="1139" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="1139" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H1139" s="7"/>
     </row>
-    <row r="1140" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="1140" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H1140" s="7"/>
     </row>
-    <row r="1141" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="1141" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H1141" s="7"/>
     </row>
     <row r="1142" spans="8:8" x14ac:dyDescent="0.3">
@@ -42884,39 +44537,6 @@
     </row>
     <row r="2816" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H2816" s="7"/>
-    </row>
-    <row r="2817" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H2817" s="7"/>
-    </row>
-    <row r="2818" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H2818" s="7"/>
-    </row>
-    <row r="2819" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H2819" s="7"/>
-    </row>
-    <row r="2820" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H2820" s="7"/>
-    </row>
-    <row r="2821" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H2821" s="7"/>
-    </row>
-    <row r="2822" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H2822" s="7"/>
-    </row>
-    <row r="2823" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H2823" s="7"/>
-    </row>
-    <row r="2824" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H2824" s="7"/>
-    </row>
-    <row r="2825" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H2825" s="7"/>
-    </row>
-    <row r="2826" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H2826" s="7"/>
-    </row>
-    <row r="2827" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H2827" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -42929,13 +44549,13 @@
           <x14:formula1>
             <xm:f>Report!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H2828:H1048576 G1:G1048576</xm:sqref>
+          <xm:sqref>H2817:H1048576 G1:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Report!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>M1 M2825:M1048576</xm:sqref>
+          <xm:sqref>M1 M2814:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -42947,7 +44567,7 @@
           <x14:formula1>
             <xm:f>Report!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M2824</xm:sqref>
+          <xm:sqref>M2:M2813</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Fixed comparison of list of array of strings
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="431">
   <si>
     <t>Enabled</t>
   </si>
@@ -1631,9 +1631,6 @@
     <t>Over700</t>
   </si>
   <si>
-    <t>TC1319,TC1320,TC1364-TC1367,TC1491,TC1496,TC1497</t>
-  </si>
-  <si>
     <t>RandomString50</t>
   </si>
   <si>
@@ -1644,9 +1641,6 @@
   </si>
   <si>
     <t>RandomString51</t>
-  </si>
-  <si>
-    <t>TC1339,TC1340,TC1363</t>
   </si>
   <si>
     <t>RandomString52</t>
@@ -1725,6 +1719,51 @@
   </si>
   <si>
     <t>31,26,27,30</t>
+  </si>
+  <si>
+    <t>TC1339</t>
+  </si>
+  <si>
+    <t>TC1339,TC1340,TC1363,TC1366</t>
+  </si>
+  <si>
+    <t>TC1319,TC1320,TC1364,TC1365,TC1367,TC1491,TC1496,TC1497</t>
+  </si>
+  <si>
+    <t>TC1320</t>
+  </si>
+  <si>
+    <t>TC1364</t>
+  </si>
+  <si>
+    <t>TC1365</t>
+  </si>
+  <si>
+    <t>TC1367</t>
+  </si>
+  <si>
+    <t>TC1497</t>
+  </si>
+  <si>
+    <t>TC1496</t>
+  </si>
+  <si>
+    <t>TC1491</t>
+  </si>
+  <si>
+    <t>TC1363</t>
+  </si>
+  <si>
+    <t>TC1366</t>
+  </si>
+  <si>
+    <t>TC1395</t>
+  </si>
+  <si>
+    <t>TC1371</t>
+  </si>
+  <si>
+    <t>TC1389</t>
   </si>
 </sst>
 </file>
@@ -2376,7 +2415,7 @@
   <dimension ref="A1:K1138"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3030,7 +3069,7 @@
       <c r="B27" s="25"/>
       <c r="C27" s="25"/>
       <c r="D27" s="25" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E27" s="25"/>
       <c r="F27" s="25"/>
@@ -3053,7 +3092,7 @@
       <c r="B28" s="25"/>
       <c r="C28" s="25"/>
       <c r="D28" s="25" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E28" s="25"/>
       <c r="F28" s="25"/>
@@ -15357,8 +15396,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:N38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16957,7 +16996,7 @@
         <v>83</v>
       </c>
       <c r="N36" s="24" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17045,7 +17084,7 @@
         <v>83</v>
       </c>
       <c r="N38" s="24" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -18493,7 +18532,7 @@
   <dimension ref="A1:H578"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30593,16 +30632,16 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:V2827"/>
+  <dimension ref="A1:V2841"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P34" workbookViewId="0">
-      <selection activeCell="V56" sqref="V56"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" customWidth="1"/>
     <col min="3" max="3" width="30.44140625" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
@@ -33333,10 +33372,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="C51" s="21" t="s">
         <v>386</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>387</v>
       </c>
       <c r="D51" s="23">
         <v>1</v>
@@ -33359,7 +33398,7 @@
         <v>236</v>
       </c>
       <c r="N51" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O51" s="23">
         <v>0.5</v>
@@ -33383,18 +33422,18 @@
         <v>1</v>
       </c>
       <c r="V51" s="23" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="52" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="21">
-        <v>51</v>
-      </c>
-      <c r="B52" s="21" t="s">
-        <v>389</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>390</v>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="25">
+        <v>50</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>419</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>386</v>
       </c>
       <c r="D52" s="23">
         <v>1</v>
@@ -33413,11 +33452,11 @@
       <c r="J52" s="23"/>
       <c r="K52" s="23"/>
       <c r="L52" s="23"/>
-      <c r="M52" s="21" t="s">
+      <c r="M52" s="25" t="s">
         <v>236</v>
       </c>
       <c r="N52" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O52" s="23">
         <v>0.5</v>
@@ -33440,17 +33479,19 @@
       <c r="U52" s="23">
         <v>1</v>
       </c>
-      <c r="V52" s="23"/>
-    </row>
-    <row r="53" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="21">
-        <v>52</v>
-      </c>
-      <c r="B53" s="21" t="s">
-        <v>391</v>
-      </c>
-      <c r="C53" s="21" t="s">
-        <v>392</v>
+      <c r="V52" s="23" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="25">
+        <v>50</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>420</v>
+      </c>
+      <c r="C53" s="25" t="s">
+        <v>386</v>
       </c>
       <c r="D53" s="23">
         <v>1</v>
@@ -33469,11 +33510,11 @@
       <c r="J53" s="23"/>
       <c r="K53" s="23"/>
       <c r="L53" s="23"/>
-      <c r="M53" s="21" t="s">
+      <c r="M53" s="25" t="s">
         <v>236</v>
       </c>
       <c r="N53" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O53" s="23">
         <v>0.5</v>
@@ -33497,18 +33538,18 @@
         <v>1</v>
       </c>
       <c r="V53" s="23" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="54" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="21">
-        <v>53</v>
-      </c>
-      <c r="B54" s="21" t="s">
-        <v>389</v>
-      </c>
-      <c r="C54" s="21" t="s">
-        <v>394</v>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="25">
+        <v>50</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>421</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>386</v>
       </c>
       <c r="D54" s="23">
         <v>1</v>
@@ -33527,11 +33568,11 @@
       <c r="J54" s="23"/>
       <c r="K54" s="23"/>
       <c r="L54" s="23"/>
-      <c r="M54" s="21" t="s">
+      <c r="M54" s="25" t="s">
         <v>236</v>
       </c>
       <c r="N54" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O54" s="23">
         <v>0.5</v>
@@ -33554,19 +33595,19 @@
       <c r="U54" s="23">
         <v>1</v>
       </c>
-      <c r="V54" s="23">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="55" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="21">
-        <v>54</v>
-      </c>
-      <c r="B55" s="21" t="s">
-        <v>395</v>
-      </c>
-      <c r="C55" s="21" t="s">
-        <v>396</v>
+      <c r="V54" s="23" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="25">
+        <v>50</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>422</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>386</v>
       </c>
       <c r="D55" s="23">
         <v>1</v>
@@ -33585,11 +33626,11 @@
       <c r="J55" s="23"/>
       <c r="K55" s="23"/>
       <c r="L55" s="23"/>
-      <c r="M55" s="21" t="s">
+      <c r="M55" s="25" t="s">
         <v>236</v>
       </c>
       <c r="N55" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O55" s="23">
         <v>0.5</v>
@@ -33612,19 +33653,19 @@
       <c r="U55" s="23">
         <v>1</v>
       </c>
-      <c r="V55" s="23">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="56" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="21">
-        <v>55</v>
-      </c>
-      <c r="B56" s="21" t="s">
-        <v>397</v>
-      </c>
-      <c r="C56" s="21" t="s">
-        <v>398</v>
+      <c r="V55" s="23" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="25">
+        <v>50</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>425</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>386</v>
       </c>
       <c r="D56" s="23">
         <v>1</v>
@@ -33643,11 +33684,11 @@
       <c r="J56" s="23"/>
       <c r="K56" s="23"/>
       <c r="L56" s="23"/>
-      <c r="M56" s="21" t="s">
+      <c r="M56" s="25" t="s">
         <v>236</v>
       </c>
       <c r="N56" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O56" s="23">
         <v>0.5</v>
@@ -33662,7 +33703,7 @@
         <v>11</v>
       </c>
       <c r="S56" s="23">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="T56" s="23">
         <v>1</v>
@@ -33671,24 +33712,24 @@
         <v>1</v>
       </c>
       <c r="V56" s="23" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="57" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="21">
-        <v>56</v>
-      </c>
-      <c r="B57" s="21" t="s">
-        <v>399</v>
-      </c>
-      <c r="C57" s="21" t="s">
-        <v>400</v>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="25">
+        <v>50</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>386</v>
       </c>
       <c r="D57" s="23">
         <v>1</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>162</v>
+        <v>371</v>
       </c>
       <c r="F57" s="23">
         <v>0</v>
@@ -33701,11 +33742,11 @@
       <c r="J57" s="23"/>
       <c r="K57" s="23"/>
       <c r="L57" s="23"/>
-      <c r="M57" s="21" t="s">
+      <c r="M57" s="25" t="s">
         <v>236</v>
       </c>
       <c r="N57" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O57" s="23">
         <v>0.5</v>
@@ -33720,7 +33761,7 @@
         <v>11</v>
       </c>
       <c r="S57" s="23">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="T57" s="23">
         <v>1</v>
@@ -33729,24 +33770,24 @@
         <v>1</v>
       </c>
       <c r="V57" s="23" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="58" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="21">
-        <v>57</v>
-      </c>
-      <c r="B58" s="21" t="s">
-        <v>402</v>
-      </c>
-      <c r="C58" s="21" t="s">
-        <v>403</v>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="25">
+        <v>50</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>423</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>386</v>
       </c>
       <c r="D58" s="23">
         <v>1</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>162</v>
+        <v>371</v>
       </c>
       <c r="F58" s="23">
         <v>0</v>
@@ -33759,11 +33800,11 @@
       <c r="J58" s="23"/>
       <c r="K58" s="23"/>
       <c r="L58" s="23"/>
-      <c r="M58" s="21" t="s">
+      <c r="M58" s="25" t="s">
         <v>236</v>
       </c>
       <c r="N58" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O58" s="23">
         <v>0.5</v>
@@ -33778,7 +33819,7 @@
         <v>11</v>
       </c>
       <c r="S58" s="23">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="T58" s="23">
         <v>1</v>
@@ -33787,24 +33828,24 @@
         <v>1</v>
       </c>
       <c r="V58" s="23" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
     </row>
     <row r="59" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="21">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>405</v>
+        <v>416</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="D59" s="23">
         <v>1</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>162</v>
+        <v>371</v>
       </c>
       <c r="F59" s="23">
         <v>0</v>
@@ -33813,20 +33854,16 @@
         <v>22</v>
       </c>
       <c r="H59" s="23"/>
-      <c r="I59" s="21">
-        <v>37.4206</v>
-      </c>
-      <c r="J59" s="21">
-        <v>-121.9725</v>
-      </c>
-      <c r="K59" s="21">
-        <v>37.415700000000001</v>
-      </c>
-      <c r="L59" s="21">
-        <v>-121.98390000000001</v>
-      </c>
-      <c r="M59" s="21"/>
-      <c r="N59" s="20"/>
+      <c r="I59" s="23"/>
+      <c r="J59" s="23"/>
+      <c r="K59" s="23"/>
+      <c r="L59" s="23"/>
+      <c r="M59" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="N59" s="20" t="s">
+        <v>387</v>
+      </c>
       <c r="O59" s="23">
         <v>0.5</v>
       </c>
@@ -33840,33 +33877,33 @@
         <v>11</v>
       </c>
       <c r="S59" s="23">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="T59" s="23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U59" s="23">
-        <v>11</v>
-      </c>
-      <c r="V59" s="23">
-        <v>30</v>
+        <v>1</v>
+      </c>
+      <c r="V59" s="25">
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="21">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="D60" s="23">
         <v>1</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>162</v>
+        <v>371</v>
       </c>
       <c r="F60" s="23">
         <v>0</v>
@@ -33875,15 +33912,15 @@
         <v>22</v>
       </c>
       <c r="H60" s="23"/>
-      <c r="I60" s="21"/>
-      <c r="J60" s="21"/>
-      <c r="K60" s="21"/>
-      <c r="L60" s="21"/>
+      <c r="I60" s="23"/>
+      <c r="J60" s="23"/>
+      <c r="K60" s="23"/>
+      <c r="L60" s="23"/>
       <c r="M60" s="21" t="s">
         <v>236</v>
       </c>
       <c r="N60" s="20" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O60" s="23">
         <v>0.5</v>
@@ -33898,33 +33935,33 @@
         <v>11</v>
       </c>
       <c r="S60" s="23">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="T60" s="23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U60" s="23">
-        <v>11</v>
-      </c>
-      <c r="V60" s="23">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="61" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="21">
-        <v>60</v>
-      </c>
-      <c r="B61" s="21" t="s">
-        <v>409</v>
-      </c>
-      <c r="C61" s="21" t="s">
-        <v>410</v>
+        <v>1</v>
+      </c>
+      <c r="V60" s="23" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="25">
+        <v>52</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>417</v>
+      </c>
+      <c r="C61" s="25" t="s">
+        <v>390</v>
       </c>
       <c r="D61" s="23">
         <v>1</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>162</v>
+        <v>371</v>
       </c>
       <c r="F61" s="23">
         <v>0</v>
@@ -33933,20 +33970,16 @@
         <v>22</v>
       </c>
       <c r="H61" s="23"/>
-      <c r="I61" s="21">
-        <v>37.4206</v>
-      </c>
-      <c r="J61" s="21">
-        <v>-121.9725</v>
-      </c>
-      <c r="K61" s="21">
-        <v>37.415700000000001</v>
-      </c>
-      <c r="L61" s="21">
-        <v>-121.98390000000001</v>
-      </c>
-      <c r="M61" s="21"/>
-      <c r="N61" s="20"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="23"/>
+      <c r="K61" s="23"/>
+      <c r="L61" s="23"/>
+      <c r="M61" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="N61" s="20" t="s">
+        <v>387</v>
+      </c>
       <c r="O61" s="23">
         <v>0.5</v>
       </c>
@@ -33959,110 +33992,913 @@
       <c r="R61" s="23">
         <v>11</v>
       </c>
-      <c r="S61" s="23" t="s">
-        <v>411</v>
+      <c r="S61" s="23">
+        <v>11</v>
       </c>
       <c r="T61" s="23">
         <v>1</v>
       </c>
       <c r="U61" s="23">
+        <v>1</v>
+      </c>
+      <c r="V61" s="23" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="25">
+        <v>52</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>426</v>
+      </c>
+      <c r="C62" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="D62" s="23">
+        <v>1</v>
+      </c>
+      <c r="E62" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F62" s="23">
+        <v>0</v>
+      </c>
+      <c r="G62" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H62" s="23"/>
+      <c r="I62" s="23"/>
+      <c r="J62" s="23"/>
+      <c r="K62" s="23"/>
+      <c r="L62" s="23"/>
+      <c r="M62" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="N62" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="O62" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P62" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q62" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R62" s="23">
+        <v>11</v>
+      </c>
+      <c r="S62" s="23">
+        <v>11</v>
+      </c>
+      <c r="T62" s="23">
+        <v>1</v>
+      </c>
+      <c r="U62" s="23">
+        <v>1</v>
+      </c>
+      <c r="V62" s="23" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="25">
+        <v>52</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>427</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="D63" s="23">
+        <v>1</v>
+      </c>
+      <c r="E63" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F63" s="23">
+        <v>0</v>
+      </c>
+      <c r="G63" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H63" s="23"/>
+      <c r="I63" s="23"/>
+      <c r="J63" s="23"/>
+      <c r="K63" s="23"/>
+      <c r="L63" s="23"/>
+      <c r="M63" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="N63" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="O63" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P63" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q63" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R63" s="23">
+        <v>11</v>
+      </c>
+      <c r="S63" s="23">
+        <v>11</v>
+      </c>
+      <c r="T63" s="23">
+        <v>1</v>
+      </c>
+      <c r="U63" s="23">
+        <v>1</v>
+      </c>
+      <c r="V63" s="23" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="21">
+        <v>53</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>388</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>392</v>
+      </c>
+      <c r="D64" s="23">
+        <v>1</v>
+      </c>
+      <c r="E64" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F64" s="23">
+        <v>0</v>
+      </c>
+      <c r="G64" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H64" s="23"/>
+      <c r="I64" s="23"/>
+      <c r="J64" s="23"/>
+      <c r="K64" s="23"/>
+      <c r="L64" s="23"/>
+      <c r="M64" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="N64" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="O64" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P64" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q64" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R64" s="23">
+        <v>11</v>
+      </c>
+      <c r="S64" s="23">
+        <v>11</v>
+      </c>
+      <c r="T64" s="23">
+        <v>1</v>
+      </c>
+      <c r="U64" s="23">
+        <v>1</v>
+      </c>
+      <c r="V64" s="23">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="25">
+        <v>53</v>
+      </c>
+      <c r="B65" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="C65" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="D65" s="23">
+        <v>1</v>
+      </c>
+      <c r="E65" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F65" s="23">
+        <v>0</v>
+      </c>
+      <c r="G65" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H65" s="23"/>
+      <c r="I65" s="23"/>
+      <c r="J65" s="23"/>
+      <c r="K65" s="23"/>
+      <c r="L65" s="23"/>
+      <c r="M65" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="N65" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="O65" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P65" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q65" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R65" s="23">
+        <v>11</v>
+      </c>
+      <c r="S65" s="23">
+        <v>11</v>
+      </c>
+      <c r="T65" s="23">
+        <v>1</v>
+      </c>
+      <c r="U65" s="23">
+        <v>1</v>
+      </c>
+      <c r="V65" s="23">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="21">
+        <v>54</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>393</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>394</v>
+      </c>
+      <c r="D66" s="23">
+        <v>1</v>
+      </c>
+      <c r="E66" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F66" s="23">
+        <v>0</v>
+      </c>
+      <c r="G66" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H66" s="23"/>
+      <c r="I66" s="23"/>
+      <c r="J66" s="23"/>
+      <c r="K66" s="23"/>
+      <c r="L66" s="23"/>
+      <c r="M66" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="N66" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="O66" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P66" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q66" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R66" s="23">
+        <v>11</v>
+      </c>
+      <c r="S66" s="23">
+        <v>11</v>
+      </c>
+      <c r="T66" s="23">
+        <v>1</v>
+      </c>
+      <c r="U66" s="23">
+        <v>1</v>
+      </c>
+      <c r="V66" s="23">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="21">
+        <v>55</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>395</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="D67" s="23">
+        <v>1</v>
+      </c>
+      <c r="E67" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F67" s="23">
+        <v>0</v>
+      </c>
+      <c r="G67" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H67" s="23"/>
+      <c r="I67" s="23"/>
+      <c r="J67" s="23"/>
+      <c r="K67" s="23"/>
+      <c r="L67" s="23"/>
+      <c r="M67" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="N67" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="O67" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P67" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q67" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R67" s="23">
+        <v>11</v>
+      </c>
+      <c r="S67" s="23">
+        <v>12</v>
+      </c>
+      <c r="T67" s="23">
+        <v>1</v>
+      </c>
+      <c r="U67" s="23">
+        <v>1</v>
+      </c>
+      <c r="V67" s="23" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="21">
+        <v>56</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>397</v>
+      </c>
+      <c r="C68" s="21" t="s">
+        <v>398</v>
+      </c>
+      <c r="D68" s="23">
+        <v>1</v>
+      </c>
+      <c r="E68" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="F68" s="23">
+        <v>0</v>
+      </c>
+      <c r="G68" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H68" s="23"/>
+      <c r="I68" s="23"/>
+      <c r="J68" s="23"/>
+      <c r="K68" s="23"/>
+      <c r="L68" s="23"/>
+      <c r="M68" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="N68" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="O68" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P68" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q68" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R68" s="23">
+        <v>11</v>
+      </c>
+      <c r="S68" s="23">
+        <v>21</v>
+      </c>
+      <c r="T68" s="23">
+        <v>1</v>
+      </c>
+      <c r="U68" s="23">
+        <v>1</v>
+      </c>
+      <c r="V68" s="23" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="25">
+        <v>56</v>
+      </c>
+      <c r="B69" s="25" t="s">
+        <v>429</v>
+      </c>
+      <c r="C69" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="D69" s="23">
+        <v>1</v>
+      </c>
+      <c r="E69" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="F69" s="23">
+        <v>0</v>
+      </c>
+      <c r="G69" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H69" s="23"/>
+      <c r="I69" s="23"/>
+      <c r="J69" s="23"/>
+      <c r="K69" s="23"/>
+      <c r="L69" s="23"/>
+      <c r="M69" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="N69" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="O69" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P69" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q69" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R69" s="23">
+        <v>11</v>
+      </c>
+      <c r="S69" s="23">
+        <v>21</v>
+      </c>
+      <c r="T69" s="23">
+        <v>1</v>
+      </c>
+      <c r="U69" s="23">
+        <v>1</v>
+      </c>
+      <c r="V69" s="23" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="25">
+        <v>57</v>
+      </c>
+      <c r="B70" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="C70" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="D70" s="23">
+        <v>1</v>
+      </c>
+      <c r="E70" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="F70" s="23">
+        <v>0</v>
+      </c>
+      <c r="G70" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H70" s="23"/>
+      <c r="I70" s="23"/>
+      <c r="J70" s="23"/>
+      <c r="K70" s="23"/>
+      <c r="L70" s="23"/>
+      <c r="M70" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="N70" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="O70" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P70" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q70" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R70" s="23">
+        <v>11</v>
+      </c>
+      <c r="S70" s="23">
+        <v>21</v>
+      </c>
+      <c r="T70" s="23">
+        <v>1</v>
+      </c>
+      <c r="U70" s="23">
+        <v>1</v>
+      </c>
+      <c r="V70" s="23" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="21">
+        <v>57</v>
+      </c>
+      <c r="B71" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="C71" s="21" t="s">
+        <v>401</v>
+      </c>
+      <c r="D71" s="23">
+        <v>1</v>
+      </c>
+      <c r="E71" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="F71" s="23">
+        <v>0</v>
+      </c>
+      <c r="G71" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H71" s="23"/>
+      <c r="I71" s="23"/>
+      <c r="J71" s="23"/>
+      <c r="K71" s="23"/>
+      <c r="L71" s="23"/>
+      <c r="M71" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="N71" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="O71" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P71" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q71" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R71" s="23">
+        <v>11</v>
+      </c>
+      <c r="S71" s="23">
+        <v>21</v>
+      </c>
+      <c r="T71" s="23">
+        <v>1</v>
+      </c>
+      <c r="U71" s="23">
+        <v>1</v>
+      </c>
+      <c r="V71" s="23" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="21">
+        <v>58</v>
+      </c>
+      <c r="B72" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="C72" s="21" t="s">
+        <v>404</v>
+      </c>
+      <c r="D72" s="23">
+        <v>1</v>
+      </c>
+      <c r="E72" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="F72" s="23">
+        <v>0</v>
+      </c>
+      <c r="G72" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H72" s="23"/>
+      <c r="I72" s="21">
+        <v>37.4206</v>
+      </c>
+      <c r="J72" s="21">
+        <v>-121.9725</v>
+      </c>
+      <c r="K72" s="21">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L72" s="21">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="M72" s="21"/>
+      <c r="N72" s="20"/>
+      <c r="O72" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P72" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q72" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R72" s="23">
+        <v>11</v>
+      </c>
+      <c r="S72" s="23">
+        <v>21</v>
+      </c>
+      <c r="T72" s="23">
+        <v>4</v>
+      </c>
+      <c r="U72" s="23">
         <v>7</v>
       </c>
-      <c r="V61" s="23">
+      <c r="V72" s="23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="25">
+        <v>58</v>
+      </c>
+      <c r="B73" s="25" t="s">
+        <v>428</v>
+      </c>
+      <c r="C73" s="25" t="s">
+        <v>404</v>
+      </c>
+      <c r="D73" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="M62" s="7"/>
-    </row>
-    <row r="63" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B63" s="7"/>
-      <c r="H63" s="7"/>
-      <c r="M63" s="7"/>
-    </row>
-    <row r="64" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B64" s="7"/>
-      <c r="H64" s="7"/>
-      <c r="M64" s="7"/>
-    </row>
-    <row r="65" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B65" s="7"/>
-      <c r="H65" s="7"/>
-      <c r="M65" s="7"/>
-    </row>
-    <row r="66" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B66" s="7"/>
-      <c r="H66" s="7"/>
-      <c r="M66" s="7"/>
-    </row>
-    <row r="67" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B67" s="7"/>
-      <c r="H67" s="7"/>
-      <c r="M67" s="7"/>
-    </row>
-    <row r="68" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B68" s="7"/>
-      <c r="H68" s="7"/>
-      <c r="M68" s="7"/>
-    </row>
-    <row r="69" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B69" s="7"/>
-      <c r="H69" s="7"/>
-      <c r="M69" s="7"/>
-    </row>
-    <row r="70" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B70" s="7"/>
-      <c r="H70" s="7"/>
-      <c r="M70" s="7"/>
-    </row>
-    <row r="71" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B71" s="7"/>
-      <c r="H71" s="7"/>
-      <c r="M71" s="7"/>
-    </row>
-    <row r="72" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B72" s="7"/>
-      <c r="H72" s="7"/>
-      <c r="M72" s="7"/>
-    </row>
-    <row r="73" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B73" s="7"/>
-      <c r="H73" s="7"/>
-      <c r="M73" s="7"/>
-    </row>
-    <row r="74" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B74" s="7"/>
-      <c r="H74" s="7"/>
-      <c r="M74" s="7"/>
-    </row>
-    <row r="75" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B75" s="7"/>
-      <c r="H75" s="7"/>
-      <c r="M75" s="7"/>
-    </row>
-    <row r="76" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B76" s="7"/>
-      <c r="H76" s="7"/>
-      <c r="M76" s="7"/>
-    </row>
-    <row r="77" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="E73" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="F73" s="23">
+        <v>0</v>
+      </c>
+      <c r="G73" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H73" s="23"/>
+      <c r="I73" s="25">
+        <v>37.4206</v>
+      </c>
+      <c r="J73" s="25">
+        <v>-121.9725</v>
+      </c>
+      <c r="K73" s="25">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L73" s="25">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="N73" s="20"/>
+      <c r="O73" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P73" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q73" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R73" s="23">
+        <v>11</v>
+      </c>
+      <c r="S73" s="23">
+        <v>21</v>
+      </c>
+      <c r="T73" s="23">
+        <v>4</v>
+      </c>
+      <c r="U73" s="23">
+        <v>7</v>
+      </c>
+      <c r="V73" s="23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="21">
+        <v>59</v>
+      </c>
+      <c r="B74" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="C74" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="D74" s="23">
+        <v>1</v>
+      </c>
+      <c r="E74" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="F74" s="23">
+        <v>0</v>
+      </c>
+      <c r="G74" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H74" s="23"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="21"/>
+      <c r="M74" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="N74" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="O74" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P74" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q74" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R74" s="23">
+        <v>11</v>
+      </c>
+      <c r="S74" s="23">
+        <v>18</v>
+      </c>
+      <c r="T74" s="23">
+        <v>4</v>
+      </c>
+      <c r="U74" s="23">
+        <v>11</v>
+      </c>
+      <c r="V74" s="23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="21">
+        <v>60</v>
+      </c>
+      <c r="B75" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="C75" s="21" t="s">
+        <v>408</v>
+      </c>
+      <c r="D75" s="23">
+        <v>1</v>
+      </c>
+      <c r="E75" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="F75" s="23">
+        <v>0</v>
+      </c>
+      <c r="G75" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H75" s="23"/>
+      <c r="I75" s="21">
+        <v>37.4206</v>
+      </c>
+      <c r="J75" s="21">
+        <v>-121.9725</v>
+      </c>
+      <c r="K75" s="21">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L75" s="21">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="M75" s="21"/>
+      <c r="N75" s="20"/>
+      <c r="O75" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P75" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q75" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R75" s="23">
+        <v>11</v>
+      </c>
+      <c r="S75" s="23" t="s">
+        <v>409</v>
+      </c>
+      <c r="T75" s="23">
+        <v>1</v>
+      </c>
+      <c r="U75" s="23">
+        <v>7</v>
+      </c>
+      <c r="V75" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="25">
+        <v>61</v>
+      </c>
+      <c r="B76" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="C76" s="25" t="s">
+        <v>389</v>
+      </c>
+      <c r="D76" s="23">
+        <v>1</v>
+      </c>
+      <c r="E76" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="F76" s="23">
+        <v>0</v>
+      </c>
+      <c r="G76" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H76" s="23"/>
+      <c r="I76" s="23"/>
+      <c r="J76" s="23"/>
+      <c r="K76" s="23"/>
+      <c r="L76" s="23"/>
+      <c r="M76" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="N76" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="O76" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P76" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q76" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="R76" s="23">
+        <v>11</v>
+      </c>
+      <c r="S76" s="23">
+        <v>11</v>
+      </c>
+      <c r="T76" s="23">
+        <v>1</v>
+      </c>
+      <c r="U76" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B77" s="7"/>
       <c r="H77" s="7"/>
       <c r="M77" s="7"/>
     </row>
-    <row r="78" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B78" s="7"/>
       <c r="H78" s="7"/>
       <c r="M78" s="7"/>
     </row>
-    <row r="79" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B79" s="7"/>
       <c r="H79" s="7"/>
       <c r="M79" s="7"/>
     </row>
-    <row r="80" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B80" s="7"/>
       <c r="H80" s="7"/>
       <c r="M80" s="7"/>
@@ -37112,59 +37948,73 @@
       <c r="H689" s="7"/>
       <c r="M689" s="7"/>
     </row>
-    <row r="690" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="690" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B690" s="7"/>
       <c r="H690" s="7"/>
       <c r="M690" s="7"/>
     </row>
-    <row r="691" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="691" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B691" s="7"/>
       <c r="H691" s="7"/>
       <c r="M691" s="7"/>
     </row>
-    <row r="692" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="692" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B692" s="7"/>
       <c r="H692" s="7"/>
       <c r="M692" s="7"/>
     </row>
-    <row r="693" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="693" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B693" s="7"/>
       <c r="H693" s="7"/>
       <c r="M693" s="7"/>
     </row>
-    <row r="694" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="694" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B694" s="7"/>
       <c r="H694" s="7"/>
       <c r="M694" s="7"/>
     </row>
-    <row r="695" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="695" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B695" s="7"/>
       <c r="H695" s="7"/>
       <c r="M695" s="7"/>
     </row>
-    <row r="696" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="696" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B696" s="7"/>
       <c r="H696" s="7"/>
       <c r="M696" s="7"/>
     </row>
-    <row r="697" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="697" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B697" s="7"/>
       <c r="H697" s="7"/>
       <c r="M697" s="7"/>
     </row>
-    <row r="698" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="698" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B698" s="7"/>
       <c r="H698" s="7"/>
       <c r="M698" s="7"/>
     </row>
-    <row r="699" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="699" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B699" s="7"/>
       <c r="H699" s="7"/>
       <c r="M699" s="7"/>
     </row>
-    <row r="700" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="700" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B700" s="7"/>
       <c r="H700" s="7"/>
       <c r="M700" s="7"/>
     </row>
-    <row r="701" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="701" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B701" s="7"/>
       <c r="H701" s="7"/>
       <c r="M701" s="7"/>
     </row>
-    <row r="702" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="702" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B702" s="7"/>
       <c r="H702" s="7"/>
       <c r="M702" s="7"/>
     </row>
-    <row r="703" spans="2:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="703" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="B703" s="7"/>
       <c r="H703" s="7"/>
       <c r="M703" s="7"/>
     </row>
@@ -37694,45 +38544,59 @@
     </row>
     <row r="835" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H835" s="7"/>
+      <c r="M835" s="7"/>
     </row>
     <row r="836" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H836" s="7"/>
+      <c r="M836" s="7"/>
     </row>
     <row r="837" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H837" s="7"/>
+      <c r="M837" s="7"/>
     </row>
     <row r="838" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H838" s="7"/>
+      <c r="M838" s="7"/>
     </row>
     <row r="839" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H839" s="7"/>
+      <c r="M839" s="7"/>
     </row>
     <row r="840" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H840" s="7"/>
+      <c r="M840" s="7"/>
     </row>
     <row r="841" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H841" s="7"/>
+      <c r="M841" s="7"/>
     </row>
     <row r="842" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H842" s="7"/>
+      <c r="M842" s="7"/>
     </row>
     <row r="843" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H843" s="7"/>
+      <c r="M843" s="7"/>
     </row>
     <row r="844" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H844" s="7"/>
+      <c r="M844" s="7"/>
     </row>
     <row r="845" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H845" s="7"/>
+      <c r="M845" s="7"/>
     </row>
     <row r="846" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H846" s="7"/>
+      <c r="M846" s="7"/>
     </row>
     <row r="847" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H847" s="7"/>
+      <c r="M847" s="7"/>
     </row>
     <row r="848" spans="8:13" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H848" s="7"/>
+      <c r="M848" s="7"/>
     </row>
     <row r="849" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H849" s="7"/>
@@ -38613,46 +39477,46 @@
     <row r="1141" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1141" s="7"/>
     </row>
-    <row r="1142" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1142" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1142" s="7"/>
     </row>
-    <row r="1143" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1143" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1143" s="7"/>
     </row>
-    <row r="1144" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1144" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1144" s="7"/>
     </row>
-    <row r="1145" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1145" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1145" s="7"/>
     </row>
-    <row r="1146" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1146" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1146" s="7"/>
     </row>
-    <row r="1147" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1147" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1147" s="7"/>
     </row>
-    <row r="1148" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1148" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1148" s="7"/>
     </row>
-    <row r="1149" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1149" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1149" s="7"/>
     </row>
-    <row r="1150" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1150" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1150" s="7"/>
     </row>
-    <row r="1151" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1151" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1151" s="7"/>
     </row>
-    <row r="1152" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1152" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1152" s="7"/>
     </row>
-    <row r="1153" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1153" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1153" s="7"/>
     </row>
-    <row r="1154" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1154" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1154" s="7"/>
     </row>
-    <row r="1155" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="1155" spans="8:8" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="H1155" s="7"/>
     </row>
     <row r="1156" spans="8:8" x14ac:dyDescent="0.3">
@@ -43670,6 +44534,48 @@
     </row>
     <row r="2827" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H2827" s="7"/>
+    </row>
+    <row r="2828" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2828" s="7"/>
+    </row>
+    <row r="2829" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2829" s="7"/>
+    </row>
+    <row r="2830" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2830" s="7"/>
+    </row>
+    <row r="2831" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2831" s="7"/>
+    </row>
+    <row r="2832" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2832" s="7"/>
+    </row>
+    <row r="2833" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2833" s="7"/>
+    </row>
+    <row r="2834" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2834" s="7"/>
+    </row>
+    <row r="2835" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2835" s="7"/>
+    </row>
+    <row r="2836" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2836" s="7"/>
+    </row>
+    <row r="2837" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2837" s="7"/>
+    </row>
+    <row r="2838" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2838" s="7"/>
+    </row>
+    <row r="2839" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2839" s="7"/>
+    </row>
+    <row r="2840" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2840" s="7"/>
+    </row>
+    <row r="2841" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H2841" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43682,13 +44588,13 @@
           <x14:formula1>
             <xm:f>Report!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H2828:H1048576 G1:G1048576</xm:sqref>
+          <xm:sqref>H2842:H1048576 G1:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Report!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>M1 M2825:M1048576</xm:sqref>
+          <xm:sqref>M1 M2839:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -43700,7 +44606,7 @@
           <x14:formula1>
             <xm:f>Report!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M2824</xm:sqref>
+          <xm:sqref>M2:M2838</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
fix failures in compliance report tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="15" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -81,7 +81,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Shirish Pulikkal:
 </t>
@@ -157,7 +157,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Shirish Pulikkal:</t>
         </r>
@@ -166,7 +166,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -186,7 +186,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> 2 entries for the same test case are for Copy Compliance scenario.
 </t>
@@ -249,7 +249,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Shirish Pulikkal:</t>
         </r>
@@ -258,7 +258,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Over 700 survey tags in this test case. Don't have the tags in TC. Using first perf survey tag for now.
@@ -274,7 +274,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Shirish Pulikkal:</t>
         </r>
@@ -283,7 +283,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -303,7 +303,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> 2 entries for the same test case are for Copy Compliance scenario.
 </t>
@@ -1577,10 +1577,10 @@
     <t>All TRUE (except GAP and PCF)</t>
   </si>
   <si>
-    <t>6349369ad74e475f85bd</t>
+    <t>Over700</t>
   </si>
   <si>
-    <t>Over700</t>
+    <t>TC1091 Report558596</t>
   </si>
 </sst>
 </file>
@@ -1590,7 +1590,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1637,19 +1637,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1800,16 +1787,16 @@
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1848,7 +1835,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
@@ -2225,8 +2212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:K26"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2855,7 +2842,7 @@
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
       <c r="D26" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
@@ -15136,7 +15123,7 @@
   <dimension ref="A1:N800"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18141,8 +18128,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H578"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18463,7 +18450,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>383</v>
@@ -19246,7 +19233,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -19426,8 +19413,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30244,8 +30231,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView topLeftCell="Q19" workbookViewId="0">
+      <selection activeCell="U46" sqref="U46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31894,7 +31881,7 @@
         <v>29</v>
       </c>
       <c r="T30" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U30" s="7">
         <v>2</v>
@@ -32925,7 +32912,7 @@
         <v>340</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D50" s="7">
         <v>7</v>
@@ -33003,126 +32990,144 @@
       <c r="M55" s="7"/>
     </row>
     <row r="56" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A56" s="19"/>
       <c r="B56" s="7"/>
       <c r="H56" s="7"/>
       <c r="M56" s="7"/>
     </row>
     <row r="57" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A57" s="19"/>
       <c r="B57" s="7"/>
       <c r="H57" s="7"/>
       <c r="M57" s="7"/>
     </row>
     <row r="58" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A58" s="19"/>
       <c r="B58" s="7"/>
       <c r="H58" s="7"/>
       <c r="M58" s="7"/>
     </row>
     <row r="59" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A59" s="19"/>
       <c r="B59" s="7"/>
       <c r="H59" s="7"/>
       <c r="M59" s="7"/>
     </row>
     <row r="60" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A60" s="19"/>
       <c r="B60" s="7"/>
       <c r="H60" s="7"/>
       <c r="M60" s="7"/>
     </row>
     <row r="61" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A61" s="19"/>
       <c r="B61" s="7"/>
       <c r="H61" s="7"/>
       <c r="M61" s="7"/>
     </row>
     <row r="62" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A62" s="19"/>
       <c r="B62" s="7"/>
       <c r="H62" s="7"/>
       <c r="M62" s="7"/>
     </row>
     <row r="63" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A63" s="19"/>
       <c r="B63" s="7"/>
       <c r="H63" s="7"/>
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A64" s="19"/>
       <c r="B64" s="7"/>
       <c r="H64" s="7"/>
       <c r="M64" s="7"/>
     </row>
-    <row r="65" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A65" s="19"/>
       <c r="B65" s="7"/>
       <c r="H65" s="7"/>
       <c r="M65" s="7"/>
     </row>
-    <row r="66" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A66" s="19"/>
       <c r="B66" s="7"/>
       <c r="H66" s="7"/>
       <c r="M66" s="7"/>
     </row>
-    <row r="67" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A67" s="19"/>
       <c r="B67" s="7"/>
       <c r="H67" s="7"/>
       <c r="M67" s="7"/>
     </row>
-    <row r="68" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A68" s="19"/>
       <c r="B68" s="7"/>
       <c r="H68" s="7"/>
       <c r="M68" s="7"/>
     </row>
-    <row r="69" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A69" s="19"/>
       <c r="B69" s="7"/>
       <c r="H69" s="7"/>
       <c r="M69" s="7"/>
     </row>
-    <row r="70" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A70" s="19"/>
       <c r="B70" s="7"/>
       <c r="H70" s="7"/>
       <c r="M70" s="7"/>
     </row>
-    <row r="71" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A71" s="19"/>
       <c r="B71" s="7"/>
       <c r="H71" s="7"/>
       <c r="M71" s="7"/>
     </row>
-    <row r="72" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A72" s="19"/>
       <c r="B72" s="7"/>
       <c r="H72" s="7"/>
       <c r="M72" s="7"/>
     </row>
-    <row r="73" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A73" s="19"/>
       <c r="B73" s="7"/>
       <c r="H73" s="7"/>
       <c r="M73" s="7"/>
     </row>
-    <row r="74" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B74" s="7"/>
       <c r="H74" s="7"/>
       <c r="M74" s="7"/>
     </row>
-    <row r="75" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B75" s="7"/>
       <c r="H75" s="7"/>
       <c r="M75" s="7"/>
     </row>
-    <row r="76" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B76" s="7"/>
       <c r="H76" s="7"/>
       <c r="M76" s="7"/>
     </row>
-    <row r="77" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B77" s="7"/>
       <c r="H77" s="7"/>
       <c r="M77" s="7"/>
     </row>
-    <row r="78" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B78" s="7"/>
       <c r="H78" s="7"/>
       <c r="M78" s="7"/>
     </row>
-    <row r="79" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B79" s="7"/>
       <c r="H79" s="7"/>
       <c r="M79" s="7"/>
     </row>
-    <row r="80" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B80" s="7"/>
       <c r="H80" s="7"/>
       <c r="M80" s="7"/>

</xml_diff>

<commit_message>
fix for updated TC678
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -306,6 +306,31 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve"> 2 entries for the same test case are for Copy Compliance scenario.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Invalid entry. This entry is NOT used in test case. TC678 was updated in dataprovider to ignore this entry.
 </t>
         </r>
       </text>
@@ -15123,7 +15148,7 @@
   <dimension ref="A1:N800"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18128,7 +18153,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H578"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -30231,8 +30256,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView topLeftCell="Q19" workbookViewId="0">
-      <selection activeCell="U46" sqref="U46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Modified TestCaseData.xlsx to use randomnumber for report titles
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxiang\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxiang\dev\surveyor-qa\selenium-wd\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="423">
   <si>
     <t>Enabled</t>
   </si>
@@ -1659,9 +1659,6 @@
     <t>TC1319</t>
   </si>
   <si>
-    <t>RandomString50</t>
-  </si>
-  <si>
     <t>TESTPlat-Auto-1.5km</t>
   </si>
   <si>
@@ -1692,13 +1689,7 @@
     <t>TC1339</t>
   </si>
   <si>
-    <t>RandomString51</t>
-  </si>
-  <si>
     <t>TC1363</t>
-  </si>
-  <si>
-    <t>RandomString52</t>
   </si>
   <si>
     <t>27,30</t>
@@ -1710,22 +1701,13 @@
     <t>TC1340</t>
   </si>
   <si>
-    <t>RandomString53</t>
-  </si>
-  <si>
     <t>TC1352</t>
-  </si>
-  <si>
-    <t>RandomString55</t>
   </si>
   <si>
     <t>31,26,27,30</t>
   </si>
   <si>
     <t>TC1370</t>
-  </si>
-  <si>
-    <t>RandomString56</t>
   </si>
   <si>
     <t>26,27,29</t>
@@ -1737,16 +1719,10 @@
     <t>TC1373</t>
   </si>
   <si>
-    <t>RandomString57</t>
-  </si>
-  <si>
     <t>26,27</t>
   </si>
   <si>
     <t>TC1389</t>
-  </si>
-  <si>
-    <t>RandomString58</t>
   </si>
   <si>
     <t>TC1394</t>
@@ -1758,13 +1734,7 @@
     <t>TC14</t>
   </si>
   <si>
-    <t>RandomString59</t>
-  </si>
-  <si>
     <t>TC149</t>
-  </si>
-  <si>
-    <t>RandomString60</t>
   </si>
   <si>
     <t>35,36,37</t>
@@ -3082,7 +3052,7 @@
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
       <c r="D27" s="19" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
@@ -3105,7 +3075,7 @@
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
@@ -15400,13 +15370,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]Report!#REF!</xm:f>
+            <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G27:G32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]General!#REF!</xm:f>
+            <xm:f>General!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>J27:J32 H27:H32</xm:sqref>
         </x14:dataValidation>
@@ -17021,7 +16991,7 @@
         <v>83</v>
       </c>
       <c r="N36" s="19" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17109,7 +17079,7 @@
         <v>83</v>
       </c>
       <c r="N38" s="19" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17153,7 +17123,7 @@
         <v>84</v>
       </c>
       <c r="N39" s="19" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17197,7 +17167,7 @@
         <v>83</v>
       </c>
       <c r="N40" s="19" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -17979,13 +17949,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]General!#REF!</xm:f>
+            <xm:f>General!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>C36:L40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]Report!#REF!</xm:f>
+            <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>M36:M40</xm:sqref>
         </x14:dataValidation>
@@ -30757,8 +30727,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33498,7 +33468,7 @@
         <v>386</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>387</v>
+        <v>177</v>
       </c>
       <c r="D51" s="20">
         <v>1</v>
@@ -33521,7 +33491,7 @@
         <v>236</v>
       </c>
       <c r="N51" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O51" s="20">
         <v>0.5</v>
@@ -33545,7 +33515,7 @@
         <v>1</v>
       </c>
       <c r="V51" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="52" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -33553,10 +33523,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>387</v>
+        <v>177</v>
       </c>
       <c r="D52" s="20">
         <v>1</v>
@@ -33579,7 +33549,7 @@
         <v>236</v>
       </c>
       <c r="N52" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O52" s="20">
         <v>0.5</v>
@@ -33603,7 +33573,7 @@
         <v>1</v>
       </c>
       <c r="V52" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="53" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -33611,10 +33581,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>387</v>
+        <v>177</v>
       </c>
       <c r="D53" s="20">
         <v>1</v>
@@ -33637,7 +33607,7 @@
         <v>236</v>
       </c>
       <c r="N53" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O53" s="20">
         <v>0.5</v>
@@ -33661,7 +33631,7 @@
         <v>1</v>
       </c>
       <c r="V53" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="54" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -33669,10 +33639,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>387</v>
+        <v>177</v>
       </c>
       <c r="D54" s="20">
         <v>1</v>
@@ -33695,7 +33665,7 @@
         <v>236</v>
       </c>
       <c r="N54" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O54" s="20">
         <v>0.5</v>
@@ -33719,7 +33689,7 @@
         <v>1</v>
       </c>
       <c r="V54" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="55" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -33727,10 +33697,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>387</v>
+        <v>177</v>
       </c>
       <c r="D55" s="20">
         <v>1</v>
@@ -33753,7 +33723,7 @@
         <v>236</v>
       </c>
       <c r="N55" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O55" s="20">
         <v>0.5</v>
@@ -33777,7 +33747,7 @@
         <v>1</v>
       </c>
       <c r="V55" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="56" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -33785,10 +33755,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>387</v>
+        <v>177</v>
       </c>
       <c r="D56" s="20">
         <v>1</v>
@@ -33811,7 +33781,7 @@
         <v>236</v>
       </c>
       <c r="N56" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O56" s="20">
         <v>0.5</v>
@@ -33835,7 +33805,7 @@
         <v>1</v>
       </c>
       <c r="V56" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="57" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -33843,10 +33813,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>387</v>
+        <v>177</v>
       </c>
       <c r="D57" s="20">
         <v>1</v>
@@ -33869,7 +33839,7 @@
         <v>236</v>
       </c>
       <c r="N57" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O57" s="20">
         <v>0.5</v>
@@ -33893,7 +33863,7 @@
         <v>1</v>
       </c>
       <c r="V57" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="58" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -33901,10 +33871,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>387</v>
+        <v>177</v>
       </c>
       <c r="D58" s="20">
         <v>1</v>
@@ -33927,7 +33897,7 @@
         <v>236</v>
       </c>
       <c r="N58" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O58" s="20">
         <v>0.5</v>
@@ -33951,7 +33921,7 @@
         <v>1</v>
       </c>
       <c r="V58" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="59" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -33959,10 +33929,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>398</v>
+        <v>177</v>
       </c>
       <c r="D59" s="20">
         <v>1</v>
@@ -33985,7 +33955,7 @@
         <v>236</v>
       </c>
       <c r="N59" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O59" s="20">
         <v>0.5</v>
@@ -34017,10 +33987,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>400</v>
+        <v>177</v>
       </c>
       <c r="D60" s="20">
         <v>1</v>
@@ -34043,7 +34013,7 @@
         <v>236</v>
       </c>
       <c r="N60" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O60" s="20">
         <v>0.5</v>
@@ -34067,7 +34037,7 @@
         <v>1</v>
       </c>
       <c r="V60" s="20" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="61" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -34075,10 +34045,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>400</v>
+        <v>177</v>
       </c>
       <c r="D61" s="20">
         <v>1</v>
@@ -34101,7 +34071,7 @@
         <v>236</v>
       </c>
       <c r="N61" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O61" s="20">
         <v>0.5</v>
@@ -34125,7 +34095,7 @@
         <v>1</v>
       </c>
       <c r="V61" s="20" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="62" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -34133,10 +34103,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>404</v>
+        <v>177</v>
       </c>
       <c r="D62" s="20">
         <v>1</v>
@@ -34159,7 +34129,7 @@
         <v>236</v>
       </c>
       <c r="N62" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O62" s="20">
         <v>0.5</v>
@@ -34191,10 +34161,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>406</v>
+        <v>177</v>
       </c>
       <c r="D63" s="20">
         <v>1</v>
@@ -34217,7 +34187,7 @@
         <v>236</v>
       </c>
       <c r="N63" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O63" s="20">
         <v>0.5</v>
@@ -34241,7 +34211,7 @@
         <v>1</v>
       </c>
       <c r="V63" s="20" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="64" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -34249,10 +34219,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>409</v>
+        <v>177</v>
       </c>
       <c r="D64" s="20">
         <v>1</v>
@@ -34275,7 +34245,7 @@
         <v>236</v>
       </c>
       <c r="N64" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O64" s="20">
         <v>0.5</v>
@@ -34299,7 +34269,7 @@
         <v>1</v>
       </c>
       <c r="V64" s="20" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="65" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -34307,10 +34277,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>409</v>
+        <v>177</v>
       </c>
       <c r="D65" s="20">
         <v>1</v>
@@ -34333,7 +34303,7 @@
         <v>236</v>
       </c>
       <c r="N65" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O65" s="20">
         <v>0.5</v>
@@ -34357,7 +34327,7 @@
         <v>1</v>
       </c>
       <c r="V65" s="20" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="66" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -34365,10 +34335,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>413</v>
+        <v>177</v>
       </c>
       <c r="D66" s="20">
         <v>1</v>
@@ -34391,7 +34361,7 @@
         <v>236</v>
       </c>
       <c r="N66" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O66" s="20">
         <v>0.5</v>
@@ -34415,7 +34385,7 @@
         <v>1</v>
       </c>
       <c r="V66" s="20" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="67" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -34423,10 +34393,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>416</v>
+        <v>177</v>
       </c>
       <c r="D67" s="20">
         <v>1</v>
@@ -34484,10 +34454,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>416</v>
+        <v>177</v>
       </c>
       <c r="D68" s="20">
         <v>1</v>
@@ -34545,10 +34515,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>416</v>
+        <v>177</v>
       </c>
       <c r="D69" s="20">
         <v>1</v>
@@ -34606,10 +34576,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>420</v>
+        <v>177</v>
       </c>
       <c r="D70" s="20">
         <v>1</v>
@@ -34628,7 +34598,7 @@
         <v>236</v>
       </c>
       <c r="N70" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O70" s="20">
         <v>0.5</v>
@@ -34660,10 +34630,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>422</v>
+        <v>177</v>
       </c>
       <c r="D71" s="20">
         <v>1</v>
@@ -34704,7 +34674,7 @@
         <v>11</v>
       </c>
       <c r="S71" s="20" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="T71" s="20">
         <v>1</v>
@@ -34721,10 +34691,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>398</v>
+        <v>177</v>
       </c>
       <c r="D72" s="20">
         <v>1</v>
@@ -34747,7 +34717,7 @@
         <v>236</v>
       </c>
       <c r="N72" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O72" s="20">
         <v>0.5</v>
@@ -34776,10 +34746,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>398</v>
+        <v>177</v>
       </c>
       <c r="D73" s="20">
         <v>1</v>
@@ -34837,10 +34807,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="C74" s="19" t="s">
-        <v>398</v>
+        <v>177</v>
       </c>
       <c r="D74" s="20">
         <v>1</v>
@@ -34881,7 +34851,7 @@
         <v>20</v>
       </c>
       <c r="S74" s="20" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="T74" s="20">
         <v>1</v>
@@ -44560,19 +44530,19 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]Report!#REF!</xm:f>
+            <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>M51:M74</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]Report!#REF!</xm:f>
+            <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E51:E74</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]Report!#REF!</xm:f>
+            <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G51:G74</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
added few compliance report page actions
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxiang\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\surveyor-qa\selenium-wd\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1800,7 +1800,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -2012,7 +2012,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2051,7 +2051,6 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1 2" xfId="7"/>
@@ -15400,13 +15399,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]Report!#REF!</xm:f>
+            <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G27:G32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]General!#REF!</xm:f>
+            <xm:f>General!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>J27:J32 H27:H32</xm:sqref>
         </x14:dataValidation>
@@ -17979,13 +17978,13 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]General!#REF!</xm:f>
+            <xm:f>General!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>C36:L40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]Report!#REF!</xm:f>
+            <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>M36:M40</xm:sqref>
         </x14:dataValidation>
@@ -30757,8 +30756,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33490,471 +33489,431 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A51" s="19">
         <v>50</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="19" t="s">
         <v>386</v>
       </c>
       <c r="C51" s="19" t="s">
         <v>387</v>
       </c>
-      <c r="D51" s="20">
+      <c r="D51" s="19">
         <v>1</v>
       </c>
-      <c r="E51" s="20" t="s">
+      <c r="E51" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F51" s="20">
+      <c r="F51" s="19">
         <v>0</v>
       </c>
-      <c r="G51" s="20" t="s">
+      <c r="G51" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="20"/>
       <c r="M51" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N51" t="s">
+      <c r="N51" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O51" s="20">
+      <c r="O51" s="19">
         <v>0.5</v>
       </c>
-      <c r="P51" s="20">
+      <c r="P51" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q51" s="20">
+      <c r="Q51" s="19">
         <v>8.5</v>
       </c>
-      <c r="R51" s="20">
+      <c r="R51" s="19">
         <v>11</v>
       </c>
-      <c r="S51" s="20">
+      <c r="S51" s="19">
         <v>11</v>
       </c>
-      <c r="T51" s="20">
+      <c r="T51" s="19">
         <v>1</v>
       </c>
-      <c r="U51" s="20">
+      <c r="U51" s="19">
         <v>1</v>
       </c>
-      <c r="V51" s="20" t="s">
+      <c r="V51" s="19" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="52" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A52" s="19">
         <v>51</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="19" t="s">
         <v>390</v>
       </c>
       <c r="C52" s="19" t="s">
         <v>387</v>
       </c>
-      <c r="D52" s="20">
+      <c r="D52" s="19">
         <v>1</v>
       </c>
-      <c r="E52" s="20" t="s">
+      <c r="E52" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F52" s="20">
+      <c r="F52" s="19">
         <v>0</v>
       </c>
-      <c r="G52" s="20" t="s">
+      <c r="G52" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="20"/>
       <c r="M52" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N52" t="s">
+      <c r="N52" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O52" s="20">
+      <c r="O52" s="19">
         <v>0.5</v>
       </c>
-      <c r="P52" s="20">
+      <c r="P52" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q52" s="20">
+      <c r="Q52" s="19">
         <v>8.5</v>
       </c>
-      <c r="R52" s="20">
+      <c r="R52" s="19">
         <v>11</v>
       </c>
-      <c r="S52" s="20">
+      <c r="S52" s="19">
         <v>11</v>
       </c>
-      <c r="T52" s="20">
+      <c r="T52" s="19">
         <v>1</v>
       </c>
-      <c r="U52" s="20">
+      <c r="U52" s="19">
         <v>1</v>
       </c>
-      <c r="V52" s="20" t="s">
+      <c r="V52" s="19" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="53" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A53" s="19">
         <v>52</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="19" t="s">
         <v>391</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>387</v>
       </c>
-      <c r="D53" s="20">
+      <c r="D53" s="19">
         <v>1</v>
       </c>
-      <c r="E53" s="20" t="s">
+      <c r="E53" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F53" s="20">
+      <c r="F53" s="19">
         <v>0</v>
       </c>
-      <c r="G53" s="20" t="s">
+      <c r="G53" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
-      <c r="J53" s="20"/>
-      <c r="K53" s="20"/>
-      <c r="L53" s="20"/>
       <c r="M53" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N53" t="s">
+      <c r="N53" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O53" s="20">
+      <c r="O53" s="19">
         <v>0.5</v>
       </c>
-      <c r="P53" s="20">
+      <c r="P53" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q53" s="20">
+      <c r="Q53" s="19">
         <v>8.5</v>
       </c>
-      <c r="R53" s="20">
+      <c r="R53" s="19">
         <v>11</v>
       </c>
-      <c r="S53" s="20">
+      <c r="S53" s="19">
         <v>11</v>
       </c>
-      <c r="T53" s="20">
+      <c r="T53" s="19">
         <v>1</v>
       </c>
-      <c r="U53" s="20">
+      <c r="U53" s="19">
         <v>1</v>
       </c>
-      <c r="V53" s="20" t="s">
+      <c r="V53" s="19" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="54" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A54" s="19">
         <v>53</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="19" t="s">
         <v>392</v>
       </c>
       <c r="C54" s="19" t="s">
         <v>387</v>
       </c>
-      <c r="D54" s="20">
+      <c r="D54" s="19">
         <v>1</v>
       </c>
-      <c r="E54" s="20" t="s">
+      <c r="E54" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F54" s="20">
+      <c r="F54" s="19">
         <v>0</v>
       </c>
-      <c r="G54" s="20" t="s">
+      <c r="G54" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="20"/>
-      <c r="K54" s="20"/>
-      <c r="L54" s="20"/>
       <c r="M54" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N54" t="s">
+      <c r="N54" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O54" s="20">
+      <c r="O54" s="19">
         <v>0.5</v>
       </c>
-      <c r="P54" s="20">
+      <c r="P54" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q54" s="20">
+      <c r="Q54" s="19">
         <v>8.5</v>
       </c>
-      <c r="R54" s="20">
+      <c r="R54" s="19">
         <v>11</v>
       </c>
-      <c r="S54" s="20">
+      <c r="S54" s="19">
         <v>11</v>
       </c>
-      <c r="T54" s="20">
+      <c r="T54" s="19">
         <v>1</v>
       </c>
-      <c r="U54" s="20">
+      <c r="U54" s="19">
         <v>1</v>
       </c>
-      <c r="V54" s="20" t="s">
+      <c r="V54" s="19" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="55" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A55" s="19">
         <v>54</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="19" t="s">
         <v>393</v>
       </c>
       <c r="C55" s="19" t="s">
         <v>387</v>
       </c>
-      <c r="D55" s="20">
+      <c r="D55" s="19">
         <v>1</v>
       </c>
-      <c r="E55" s="20" t="s">
+      <c r="E55" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F55" s="20">
+      <c r="F55" s="19">
         <v>0</v>
       </c>
-      <c r="G55" s="20" t="s">
+      <c r="G55" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-      <c r="K55" s="20"/>
-      <c r="L55" s="20"/>
       <c r="M55" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N55" t="s">
+      <c r="N55" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O55" s="20">
+      <c r="O55" s="19">
         <v>0.5</v>
       </c>
-      <c r="P55" s="20">
+      <c r="P55" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q55" s="20">
+      <c r="Q55" s="19">
         <v>8.5</v>
       </c>
-      <c r="R55" s="20">
+      <c r="R55" s="19">
         <v>11</v>
       </c>
-      <c r="S55" s="20">
+      <c r="S55" s="19">
         <v>11</v>
       </c>
-      <c r="T55" s="20">
+      <c r="T55" s="19">
         <v>1</v>
       </c>
-      <c r="U55" s="20">
+      <c r="U55" s="19">
         <v>1</v>
       </c>
-      <c r="V55" s="20" t="s">
+      <c r="V55" s="19" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="56" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A56" s="19">
         <v>55</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="19" t="s">
         <v>394</v>
       </c>
       <c r="C56" s="19" t="s">
         <v>387</v>
       </c>
-      <c r="D56" s="20">
+      <c r="D56" s="19">
         <v>1</v>
       </c>
-      <c r="E56" s="20" t="s">
+      <c r="E56" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F56" s="20">
+      <c r="F56" s="19">
         <v>0</v>
       </c>
-      <c r="G56" s="20" t="s">
+      <c r="G56" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H56" s="20"/>
-      <c r="I56" s="20"/>
-      <c r="J56" s="20"/>
-      <c r="K56" s="20"/>
-      <c r="L56" s="20"/>
       <c r="M56" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N56" t="s">
+      <c r="N56" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O56" s="20">
+      <c r="O56" s="19">
         <v>0.5</v>
       </c>
-      <c r="P56" s="20">
+      <c r="P56" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q56" s="20">
+      <c r="Q56" s="19">
         <v>8.5</v>
       </c>
-      <c r="R56" s="20">
+      <c r="R56" s="19">
         <v>11</v>
       </c>
-      <c r="S56" s="20">
+      <c r="S56" s="19">
         <v>11</v>
       </c>
-      <c r="T56" s="20">
+      <c r="T56" s="19">
         <v>1</v>
       </c>
-      <c r="U56" s="20">
+      <c r="U56" s="19">
         <v>1</v>
       </c>
-      <c r="V56" s="20" t="s">
+      <c r="V56" s="19" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="57" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A57" s="19">
         <v>56</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="19" t="s">
         <v>395</v>
       </c>
       <c r="C57" s="19" t="s">
         <v>387</v>
       </c>
-      <c r="D57" s="20">
+      <c r="D57" s="19">
         <v>1</v>
       </c>
-      <c r="E57" s="20" t="s">
+      <c r="E57" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F57" s="20">
+      <c r="F57" s="19">
         <v>0</v>
       </c>
-      <c r="G57" s="20" t="s">
+      <c r="G57" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H57" s="20"/>
-      <c r="I57" s="20"/>
-      <c r="J57" s="20"/>
-      <c r="K57" s="20"/>
-      <c r="L57" s="20"/>
       <c r="M57" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N57" t="s">
+      <c r="N57" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O57" s="20">
+      <c r="O57" s="19">
         <v>0.5</v>
       </c>
-      <c r="P57" s="20">
+      <c r="P57" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q57" s="20">
+      <c r="Q57" s="19">
         <v>8.5</v>
       </c>
-      <c r="R57" s="20">
+      <c r="R57" s="19">
         <v>11</v>
       </c>
-      <c r="S57" s="20">
+      <c r="S57" s="19">
         <v>11</v>
       </c>
-      <c r="T57" s="20">
+      <c r="T57" s="19">
         <v>1</v>
       </c>
-      <c r="U57" s="20">
+      <c r="U57" s="19">
         <v>1</v>
       </c>
-      <c r="V57" s="20" t="s">
+      <c r="V57" s="19" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="58" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A58" s="19">
         <v>57</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="19" t="s">
         <v>396</v>
       </c>
       <c r="C58" s="19" t="s">
         <v>387</v>
       </c>
-      <c r="D58" s="20">
+      <c r="D58" s="19">
         <v>1</v>
       </c>
-      <c r="E58" s="20" t="s">
+      <c r="E58" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F58" s="20">
+      <c r="F58" s="19">
         <v>0</v>
       </c>
-      <c r="G58" s="20" t="s">
+      <c r="G58" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H58" s="20"/>
-      <c r="I58" s="20"/>
-      <c r="J58" s="20"/>
-      <c r="K58" s="20"/>
-      <c r="L58" s="20"/>
       <c r="M58" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N58" t="s">
+      <c r="N58" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O58" s="20">
+      <c r="O58" s="19">
         <v>0.5</v>
       </c>
-      <c r="P58" s="20">
+      <c r="P58" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q58" s="20">
+      <c r="Q58" s="19">
         <v>8.5</v>
       </c>
-      <c r="R58" s="20">
+      <c r="R58" s="19">
         <v>11</v>
       </c>
-      <c r="S58" s="20">
+      <c r="S58" s="19">
         <v>11</v>
       </c>
-      <c r="T58" s="20">
+      <c r="T58" s="19">
         <v>1</v>
       </c>
-      <c r="U58" s="20">
+      <c r="U58" s="19">
         <v>1</v>
       </c>
-      <c r="V58" s="20" t="s">
+      <c r="V58" s="19" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="59" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A59" s="19">
         <v>58</v>
       </c>
@@ -33964,55 +33923,50 @@
       <c r="C59" s="19" t="s">
         <v>398</v>
       </c>
-      <c r="D59" s="20">
+      <c r="D59" s="19">
         <v>1</v>
       </c>
-      <c r="E59" s="20" t="s">
+      <c r="E59" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F59" s="20">
+      <c r="F59" s="19">
         <v>0</v>
       </c>
-      <c r="G59" s="20" t="s">
+      <c r="G59" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H59" s="20"/>
-      <c r="I59" s="20"/>
-      <c r="J59" s="20"/>
-      <c r="K59" s="20"/>
-      <c r="L59" s="20"/>
       <c r="M59" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N59" t="s">
+      <c r="N59" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O59" s="20">
+      <c r="O59" s="19">
         <v>0.5</v>
       </c>
-      <c r="P59" s="20">
+      <c r="P59" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q59" s="20">
+      <c r="Q59" s="19">
         <v>8.5</v>
       </c>
-      <c r="R59" s="20">
+      <c r="R59" s="19">
         <v>11</v>
       </c>
-      <c r="S59" s="20">
+      <c r="S59" s="19">
         <v>11</v>
       </c>
-      <c r="T59" s="20">
+      <c r="T59" s="19">
         <v>1</v>
       </c>
-      <c r="U59" s="20">
+      <c r="U59" s="19">
         <v>1</v>
       </c>
       <c r="V59" s="19">
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A60" s="19">
         <v>59</v>
       </c>
@@ -34022,55 +33976,50 @@
       <c r="C60" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="D60" s="20">
+      <c r="D60" s="19">
         <v>1</v>
       </c>
-      <c r="E60" s="20" t="s">
+      <c r="E60" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F60" s="20">
+      <c r="F60" s="19">
         <v>0</v>
       </c>
-      <c r="G60" s="20" t="s">
+      <c r="G60" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H60" s="20"/>
-      <c r="I60" s="20"/>
-      <c r="J60" s="20"/>
-      <c r="K60" s="20"/>
-      <c r="L60" s="20"/>
       <c r="M60" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N60" t="s">
+      <c r="N60" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O60" s="20">
+      <c r="O60" s="19">
         <v>0.5</v>
       </c>
-      <c r="P60" s="20">
+      <c r="P60" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q60" s="20">
+      <c r="Q60" s="19">
         <v>8.5</v>
       </c>
-      <c r="R60" s="20">
+      <c r="R60" s="19">
         <v>11</v>
       </c>
-      <c r="S60" s="20">
+      <c r="S60" s="19">
         <v>11</v>
       </c>
-      <c r="T60" s="20">
+      <c r="T60" s="19">
         <v>1</v>
       </c>
-      <c r="U60" s="20">
+      <c r="U60" s="19">
         <v>1</v>
       </c>
-      <c r="V60" s="20" t="s">
+      <c r="V60" s="19" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="61" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A61" s="19">
         <v>60</v>
       </c>
@@ -34080,55 +34029,50 @@
       <c r="C61" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="D61" s="20">
+      <c r="D61" s="19">
         <v>1</v>
       </c>
-      <c r="E61" s="20" t="s">
+      <c r="E61" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F61" s="20">
+      <c r="F61" s="19">
         <v>0</v>
       </c>
-      <c r="G61" s="20" t="s">
+      <c r="G61" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H61" s="20"/>
-      <c r="I61" s="20"/>
-      <c r="J61" s="20"/>
-      <c r="K61" s="20"/>
-      <c r="L61" s="20"/>
       <c r="M61" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N61" t="s">
+      <c r="N61" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O61" s="20">
+      <c r="O61" s="19">
         <v>0.5</v>
       </c>
-      <c r="P61" s="20">
+      <c r="P61" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q61" s="20">
+      <c r="Q61" s="19">
         <v>8.5</v>
       </c>
-      <c r="R61" s="20">
+      <c r="R61" s="19">
         <v>11</v>
       </c>
-      <c r="S61" s="20">
+      <c r="S61" s="19">
         <v>11</v>
       </c>
-      <c r="T61" s="20">
+      <c r="T61" s="19">
         <v>1</v>
       </c>
-      <c r="U61" s="20">
+      <c r="U61" s="19">
         <v>1</v>
       </c>
-      <c r="V61" s="20" t="s">
+      <c r="V61" s="19" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="62" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A62" s="19">
         <v>61</v>
       </c>
@@ -34138,55 +34082,50 @@
       <c r="C62" s="19" t="s">
         <v>404</v>
       </c>
-      <c r="D62" s="20">
+      <c r="D62" s="19">
         <v>1</v>
       </c>
-      <c r="E62" s="20" t="s">
+      <c r="E62" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F62" s="20">
+      <c r="F62" s="19">
         <v>0</v>
       </c>
-      <c r="G62" s="20" t="s">
+      <c r="G62" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H62" s="20"/>
-      <c r="I62" s="20"/>
-      <c r="J62" s="20"/>
-      <c r="K62" s="20"/>
-      <c r="L62" s="20"/>
       <c r="M62" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N62" t="s">
+      <c r="N62" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O62" s="20">
+      <c r="O62" s="19">
         <v>0.5</v>
       </c>
-      <c r="P62" s="20">
+      <c r="P62" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q62" s="20">
+      <c r="Q62" s="19">
         <v>8.5</v>
       </c>
-      <c r="R62" s="20">
+      <c r="R62" s="19">
         <v>11</v>
       </c>
-      <c r="S62" s="20">
+      <c r="S62" s="19">
         <v>11</v>
       </c>
-      <c r="T62" s="20">
+      <c r="T62" s="19">
         <v>1</v>
       </c>
-      <c r="U62" s="20">
+      <c r="U62" s="19">
         <v>1</v>
       </c>
-      <c r="V62" s="20">
+      <c r="V62" s="19">
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A63" s="19">
         <v>62</v>
       </c>
@@ -34196,55 +34135,50 @@
       <c r="C63" s="19" t="s">
         <v>406</v>
       </c>
-      <c r="D63" s="20">
+      <c r="D63" s="19">
         <v>1</v>
       </c>
-      <c r="E63" s="20" t="s">
+      <c r="E63" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F63" s="20">
+      <c r="F63" s="19">
         <v>0</v>
       </c>
-      <c r="G63" s="20" t="s">
+      <c r="G63" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H63" s="20"/>
-      <c r="I63" s="20"/>
-      <c r="J63" s="20"/>
-      <c r="K63" s="20"/>
-      <c r="L63" s="20"/>
       <c r="M63" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N63" t="s">
+      <c r="N63" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O63" s="20">
+      <c r="O63" s="19">
         <v>0.5</v>
       </c>
-      <c r="P63" s="20">
+      <c r="P63" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q63" s="20">
+      <c r="Q63" s="19">
         <v>8.5</v>
       </c>
-      <c r="R63" s="20">
+      <c r="R63" s="19">
         <v>11</v>
       </c>
-      <c r="S63" s="20">
+      <c r="S63" s="19">
         <v>12</v>
       </c>
-      <c r="T63" s="20">
+      <c r="T63" s="19">
         <v>1</v>
       </c>
-      <c r="U63" s="20">
+      <c r="U63" s="19">
         <v>1</v>
       </c>
-      <c r="V63" s="20" t="s">
+      <c r="V63" s="19" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="64" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A64" s="19">
         <v>63</v>
       </c>
@@ -34254,55 +34188,50 @@
       <c r="C64" s="19" t="s">
         <v>409</v>
       </c>
-      <c r="D64" s="20">
+      <c r="D64" s="19">
         <v>1</v>
       </c>
-      <c r="E64" s="20" t="s">
+      <c r="E64" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F64" s="20">
+      <c r="F64" s="19">
         <v>0</v>
       </c>
-      <c r="G64" s="20" t="s">
+      <c r="G64" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H64" s="20"/>
-      <c r="I64" s="20"/>
-      <c r="J64" s="20"/>
-      <c r="K64" s="20"/>
-      <c r="L64" s="20"/>
       <c r="M64" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N64" t="s">
+      <c r="N64" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O64" s="20">
+      <c r="O64" s="19">
         <v>0.5</v>
       </c>
-      <c r="P64" s="20">
+      <c r="P64" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q64" s="20">
+      <c r="Q64" s="19">
         <v>8.5</v>
       </c>
-      <c r="R64" s="20">
+      <c r="R64" s="19">
         <v>11</v>
       </c>
-      <c r="S64" s="20">
+      <c r="S64" s="19">
         <v>21</v>
       </c>
-      <c r="T64" s="20">
+      <c r="T64" s="19">
         <v>1</v>
       </c>
-      <c r="U64" s="20">
+      <c r="U64" s="19">
         <v>1</v>
       </c>
-      <c r="V64" s="20" t="s">
+      <c r="V64" s="19" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="65" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A65" s="19">
         <v>64</v>
       </c>
@@ -34312,55 +34241,50 @@
       <c r="C65" s="19" t="s">
         <v>409</v>
       </c>
-      <c r="D65" s="20">
+      <c r="D65" s="19">
         <v>1</v>
       </c>
-      <c r="E65" s="20" t="s">
+      <c r="E65" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F65" s="20">
+      <c r="F65" s="19">
         <v>0</v>
       </c>
-      <c r="G65" s="20" t="s">
+      <c r="G65" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H65" s="20"/>
-      <c r="I65" s="20"/>
-      <c r="J65" s="20"/>
-      <c r="K65" s="20"/>
-      <c r="L65" s="20"/>
       <c r="M65" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N65" t="s">
+      <c r="N65" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O65" s="20">
+      <c r="O65" s="19">
         <v>0.5</v>
       </c>
-      <c r="P65" s="20">
+      <c r="P65" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q65" s="20">
+      <c r="Q65" s="19">
         <v>8.5</v>
       </c>
-      <c r="R65" s="20">
+      <c r="R65" s="19">
         <v>11</v>
       </c>
-      <c r="S65" s="20">
+      <c r="S65" s="19">
         <v>21</v>
       </c>
-      <c r="T65" s="20">
+      <c r="T65" s="19">
         <v>1</v>
       </c>
-      <c r="U65" s="20">
+      <c r="U65" s="19">
         <v>1</v>
       </c>
-      <c r="V65" s="20" t="s">
+      <c r="V65" s="19" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="66" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A66" s="19">
         <v>65</v>
       </c>
@@ -34370,55 +34294,50 @@
       <c r="C66" s="19" t="s">
         <v>413</v>
       </c>
-      <c r="D66" s="20">
+      <c r="D66" s="19">
         <v>1</v>
       </c>
-      <c r="E66" s="20" t="s">
+      <c r="E66" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F66" s="20">
+      <c r="F66" s="19">
         <v>0</v>
       </c>
-      <c r="G66" s="20" t="s">
+      <c r="G66" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H66" s="20"/>
-      <c r="I66" s="20"/>
-      <c r="J66" s="20"/>
-      <c r="K66" s="20"/>
-      <c r="L66" s="20"/>
       <c r="M66" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N66" t="s">
+      <c r="N66" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O66" s="20">
+      <c r="O66" s="19">
         <v>0.5</v>
       </c>
-      <c r="P66" s="20">
+      <c r="P66" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q66" s="20">
+      <c r="Q66" s="19">
         <v>8.5</v>
       </c>
-      <c r="R66" s="20">
+      <c r="R66" s="19">
         <v>11</v>
       </c>
-      <c r="S66" s="20">
+      <c r="S66" s="19">
         <v>21</v>
       </c>
-      <c r="T66" s="20">
+      <c r="T66" s="19">
         <v>1</v>
       </c>
-      <c r="U66" s="20">
+      <c r="U66" s="19">
         <v>1</v>
       </c>
-      <c r="V66" s="20" t="s">
+      <c r="V66" s="19" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="67" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A67" s="19">
         <v>66</v>
       </c>
@@ -34428,19 +34347,18 @@
       <c r="C67" s="19" t="s">
         <v>416</v>
       </c>
-      <c r="D67" s="20">
+      <c r="D67" s="19">
         <v>1</v>
       </c>
-      <c r="E67" s="20" t="s">
+      <c r="E67" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F67" s="20">
+      <c r="F67" s="19">
         <v>0</v>
       </c>
-      <c r="G67" s="20" t="s">
+      <c r="G67" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H67" s="20"/>
       <c r="I67" s="19">
         <v>37.4206</v>
       </c>
@@ -34453,33 +34371,32 @@
       <c r="L67" s="19">
         <v>-121.98390000000001</v>
       </c>
-      <c r="N67"/>
-      <c r="O67" s="20">
+      <c r="O67" s="19">
         <v>0.5</v>
       </c>
-      <c r="P67" s="20">
+      <c r="P67" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q67" s="20">
+      <c r="Q67" s="19">
         <v>8.5</v>
       </c>
-      <c r="R67" s="20">
+      <c r="R67" s="19">
         <v>11</v>
       </c>
-      <c r="S67" s="20">
+      <c r="S67" s="19">
         <v>21</v>
       </c>
-      <c r="T67" s="20">
+      <c r="T67" s="19">
         <v>4</v>
       </c>
-      <c r="U67" s="20">
+      <c r="U67" s="19">
         <v>7</v>
       </c>
-      <c r="V67" s="20">
+      <c r="V67" s="19">
         <v>30</v>
       </c>
     </row>
-    <row r="68" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A68" s="19">
         <v>67</v>
       </c>
@@ -34489,19 +34406,18 @@
       <c r="C68" s="19" t="s">
         <v>416</v>
       </c>
-      <c r="D68" s="20">
+      <c r="D68" s="19">
         <v>1</v>
       </c>
-      <c r="E68" s="20" t="s">
+      <c r="E68" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F68" s="20">
+      <c r="F68" s="19">
         <v>0</v>
       </c>
-      <c r="G68" s="20" t="s">
+      <c r="G68" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H68" s="20"/>
       <c r="I68" s="19">
         <v>37.4206</v>
       </c>
@@ -34514,33 +34430,32 @@
       <c r="L68" s="19">
         <v>-121.98390000000001</v>
       </c>
-      <c r="N68"/>
-      <c r="O68" s="20">
+      <c r="O68" s="19">
         <v>0.5</v>
       </c>
-      <c r="P68" s="20">
+      <c r="P68" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q68" s="20">
+      <c r="Q68" s="19">
         <v>8.5</v>
       </c>
-      <c r="R68" s="20">
+      <c r="R68" s="19">
         <v>11</v>
       </c>
-      <c r="S68" s="20">
+      <c r="S68" s="19">
         <v>21</v>
       </c>
-      <c r="T68" s="20">
+      <c r="T68" s="19">
         <v>4</v>
       </c>
-      <c r="U68" s="20">
+      <c r="U68" s="19">
         <v>7</v>
       </c>
-      <c r="V68" s="20">
+      <c r="V68" s="19">
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A69" s="19">
         <v>68</v>
       </c>
@@ -34550,19 +34465,18 @@
       <c r="C69" s="19" t="s">
         <v>416</v>
       </c>
-      <c r="D69" s="20">
+      <c r="D69" s="19">
         <v>1</v>
       </c>
-      <c r="E69" s="20" t="s">
+      <c r="E69" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F69" s="20">
+      <c r="F69" s="19">
         <v>0</v>
       </c>
-      <c r="G69" s="20" t="s">
+      <c r="G69" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H69" s="20"/>
       <c r="I69" s="19">
         <v>37.4206</v>
       </c>
@@ -34575,33 +34489,32 @@
       <c r="L69" s="19">
         <v>-121.98390000000001</v>
       </c>
-      <c r="N69"/>
-      <c r="O69" s="20">
+      <c r="O69" s="19">
         <v>0.5</v>
       </c>
-      <c r="P69" s="20">
+      <c r="P69" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q69" s="20">
+      <c r="Q69" s="19">
         <v>8.5</v>
       </c>
-      <c r="R69" s="20">
+      <c r="R69" s="19">
         <v>11</v>
       </c>
-      <c r="S69" s="20">
+      <c r="S69" s="19">
         <v>21</v>
       </c>
-      <c r="T69" s="20">
+      <c r="T69" s="19">
         <v>4</v>
       </c>
-      <c r="U69" s="20">
+      <c r="U69" s="19">
         <v>7</v>
       </c>
-      <c r="V69" s="20">
+      <c r="V69" s="19">
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A70" s="19">
         <v>69</v>
       </c>
@@ -34611,51 +34524,50 @@
       <c r="C70" s="19" t="s">
         <v>420</v>
       </c>
-      <c r="D70" s="20">
+      <c r="D70" s="19">
         <v>1</v>
       </c>
-      <c r="E70" s="20" t="s">
+      <c r="E70" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F70" s="20">
+      <c r="F70" s="19">
         <v>0</v>
       </c>
-      <c r="G70" s="20" t="s">
+      <c r="G70" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H70" s="20"/>
       <c r="M70" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N70" t="s">
+      <c r="N70" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O70" s="20">
+      <c r="O70" s="19">
         <v>0.5</v>
       </c>
-      <c r="P70" s="20">
+      <c r="P70" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q70" s="20">
+      <c r="Q70" s="19">
         <v>8.5</v>
       </c>
-      <c r="R70" s="20">
+      <c r="R70" s="19">
         <v>11</v>
       </c>
-      <c r="S70" s="20">
+      <c r="S70" s="19">
         <v>18</v>
       </c>
-      <c r="T70" s="20">
+      <c r="T70" s="19">
         <v>4</v>
       </c>
-      <c r="U70" s="20">
+      <c r="U70" s="19">
         <v>11</v>
       </c>
-      <c r="V70" s="20">
+      <c r="V70" s="19">
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A71" s="19">
         <v>70</v>
       </c>
@@ -34665,19 +34577,18 @@
       <c r="C71" s="19" t="s">
         <v>422</v>
       </c>
-      <c r="D71" s="20">
+      <c r="D71" s="19">
         <v>1</v>
       </c>
-      <c r="E71" s="20" t="s">
+      <c r="E71" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F71" s="20">
+      <c r="F71" s="19">
         <v>0</v>
       </c>
-      <c r="G71" s="20" t="s">
+      <c r="G71" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H71" s="20"/>
       <c r="I71" s="19">
         <v>37.4206</v>
       </c>
@@ -34690,33 +34601,32 @@
       <c r="L71" s="19">
         <v>-121.98390000000001</v>
       </c>
-      <c r="N71"/>
-      <c r="O71" s="20">
+      <c r="O71" s="19">
         <v>0.5</v>
       </c>
-      <c r="P71" s="20">
+      <c r="P71" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q71" s="20">
+      <c r="Q71" s="19">
         <v>8.5</v>
       </c>
-      <c r="R71" s="20">
+      <c r="R71" s="19">
         <v>11</v>
       </c>
-      <c r="S71" s="20" t="s">
+      <c r="S71" s="19" t="s">
         <v>423</v>
       </c>
-      <c r="T71" s="20">
+      <c r="T71" s="19">
         <v>1</v>
       </c>
-      <c r="U71" s="20">
+      <c r="U71" s="19">
         <v>7</v>
       </c>
-      <c r="V71" s="20">
+      <c r="V71" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A72" s="19">
         <v>71</v>
       </c>
@@ -34726,52 +34636,47 @@
       <c r="C72" s="19" t="s">
         <v>398</v>
       </c>
-      <c r="D72" s="20">
+      <c r="D72" s="19">
         <v>1</v>
       </c>
-      <c r="E72" s="20" t="s">
+      <c r="E72" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F72" s="20">
+      <c r="F72" s="19">
         <v>0</v>
       </c>
-      <c r="G72" s="20" t="s">
+      <c r="G72" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H72" s="20"/>
-      <c r="I72" s="20"/>
-      <c r="J72" s="20"/>
-      <c r="K72" s="20"/>
-      <c r="L72" s="20"/>
       <c r="M72" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="N72" t="s">
+      <c r="N72" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="O72" s="20">
+      <c r="O72" s="19">
         <v>0.5</v>
       </c>
-      <c r="P72" s="20">
+      <c r="P72" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q72" s="20">
+      <c r="Q72" s="19">
         <v>8.5</v>
       </c>
-      <c r="R72" s="20">
+      <c r="R72" s="19">
         <v>11</v>
       </c>
-      <c r="S72" s="20">
+      <c r="S72" s="19">
         <v>11</v>
       </c>
-      <c r="T72" s="20">
+      <c r="T72" s="19">
         <v>1</v>
       </c>
-      <c r="U72" s="20">
+      <c r="U72" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A73" s="19">
         <v>72</v>
       </c>
@@ -34781,19 +34686,18 @@
       <c r="C73" s="19" t="s">
         <v>398</v>
       </c>
-      <c r="D73" s="20">
+      <c r="D73" s="19">
         <v>1</v>
       </c>
-      <c r="E73" s="20" t="s">
+      <c r="E73" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F73" s="20">
+      <c r="F73" s="19">
         <v>0</v>
       </c>
-      <c r="G73" s="20" t="s">
+      <c r="G73" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H73" s="20"/>
       <c r="I73" s="19">
         <v>37.4206</v>
       </c>
@@ -34806,33 +34710,32 @@
       <c r="L73" s="19">
         <v>-121.98390000000001</v>
       </c>
-      <c r="N73"/>
-      <c r="O73" s="20">
+      <c r="O73" s="19">
         <v>0.5</v>
       </c>
-      <c r="P73" s="20">
+      <c r="P73" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q73" s="20">
+      <c r="Q73" s="19">
         <v>8.5</v>
       </c>
-      <c r="R73" s="20">
+      <c r="R73" s="19">
         <v>11</v>
       </c>
-      <c r="S73" s="20">
+      <c r="S73" s="19">
         <v>18</v>
       </c>
-      <c r="T73" s="20">
+      <c r="T73" s="19">
         <v>1</v>
       </c>
-      <c r="U73" s="20">
+      <c r="U73" s="19">
         <v>1</v>
       </c>
       <c r="V73" s="19">
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A74" s="19">
         <v>73</v>
       </c>
@@ -34842,19 +34745,18 @@
       <c r="C74" s="19" t="s">
         <v>398</v>
       </c>
-      <c r="D74" s="20">
+      <c r="D74" s="19">
         <v>1</v>
       </c>
-      <c r="E74" s="20" t="s">
+      <c r="E74" s="19" t="s">
         <v>371</v>
       </c>
-      <c r="F74" s="20">
+      <c r="F74" s="19">
         <v>0</v>
       </c>
-      <c r="G74" s="20" t="s">
+      <c r="G74" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H74" s="20"/>
       <c r="I74" s="19">
         <v>37.4206</v>
       </c>
@@ -34867,357 +34769,96 @@
       <c r="L74" s="19">
         <v>-121.98390000000001</v>
       </c>
-      <c r="N74"/>
-      <c r="O74" s="20">
+      <c r="O74" s="19">
         <v>0.5</v>
       </c>
-      <c r="P74" s="20">
+      <c r="P74" s="19">
         <v>0.5</v>
       </c>
-      <c r="Q74" s="20">
+      <c r="Q74" s="19">
         <v>20</v>
       </c>
-      <c r="R74" s="20">
+      <c r="R74" s="19">
         <v>20</v>
       </c>
-      <c r="S74" s="20" t="s">
+      <c r="S74" s="19" t="s">
         <v>426</v>
       </c>
-      <c r="T74" s="20">
+      <c r="T74" s="19">
         <v>1</v>
       </c>
-      <c r="U74" s="20">
+      <c r="U74" s="19">
         <v>1</v>
       </c>
       <c r="V74" s="19">
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B75" s="7"/>
-      <c r="H75" s="7"/>
-      <c r="M75" s="7"/>
-    </row>
-    <row r="76" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B76" s="7"/>
-      <c r="H76" s="7"/>
-      <c r="M76" s="7"/>
-    </row>
-    <row r="77" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B77" s="7"/>
-      <c r="H77" s="7"/>
-      <c r="M77" s="7"/>
-    </row>
-    <row r="78" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B78" s="7"/>
-      <c r="H78" s="7"/>
-      <c r="M78" s="7"/>
-    </row>
-    <row r="79" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B79" s="7"/>
-      <c r="H79" s="7"/>
-      <c r="M79" s="7"/>
-    </row>
-    <row r="80" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B80" s="7"/>
-      <c r="H80" s="7"/>
-      <c r="M80" s="7"/>
-    </row>
-    <row r="81" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B81" s="7"/>
-      <c r="H81" s="7"/>
-      <c r="M81" s="7"/>
-    </row>
-    <row r="82" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B82" s="7"/>
-      <c r="H82" s="7"/>
-      <c r="M82" s="7"/>
-    </row>
-    <row r="83" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B83" s="7"/>
-      <c r="H83" s="7"/>
-      <c r="M83" s="7"/>
-    </row>
-    <row r="84" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B84" s="7"/>
-      <c r="H84" s="7"/>
-      <c r="M84" s="7"/>
-    </row>
-    <row r="85" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B85" s="7"/>
-      <c r="H85" s="7"/>
-      <c r="M85" s="7"/>
-    </row>
-    <row r="86" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B86" s="7"/>
-      <c r="H86" s="7"/>
-      <c r="M86" s="7"/>
-    </row>
-    <row r="87" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B87" s="7"/>
-      <c r="H87" s="7"/>
-      <c r="M87" s="7"/>
-    </row>
-    <row r="88" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B88" s="7"/>
-      <c r="H88" s="7"/>
-      <c r="M88" s="7"/>
-    </row>
-    <row r="89" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B89" s="7"/>
-      <c r="H89" s="7"/>
-      <c r="M89" s="7"/>
-    </row>
-    <row r="90" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B90" s="7"/>
-      <c r="H90" s="7"/>
-      <c r="M90" s="7"/>
-    </row>
-    <row r="91" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B91" s="7"/>
-      <c r="H91" s="7"/>
-      <c r="M91" s="7"/>
-    </row>
-    <row r="92" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B92" s="7"/>
-      <c r="H92" s="7"/>
-      <c r="M92" s="7"/>
-    </row>
-    <row r="93" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B93" s="7"/>
-      <c r="H93" s="7"/>
-      <c r="M93" s="7"/>
-    </row>
-    <row r="94" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B94" s="7"/>
-      <c r="H94" s="7"/>
-      <c r="M94" s="7"/>
-    </row>
-    <row r="95" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B95" s="7"/>
-      <c r="H95" s="7"/>
-      <c r="M95" s="7"/>
-    </row>
-    <row r="96" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B96" s="7"/>
-      <c r="H96" s="7"/>
-      <c r="M96" s="7"/>
-    </row>
-    <row r="97" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B97" s="7"/>
-      <c r="H97" s="7"/>
-      <c r="M97" s="7"/>
-    </row>
-    <row r="98" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B98" s="7"/>
-      <c r="H98" s="7"/>
-      <c r="M98" s="7"/>
-    </row>
-    <row r="99" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B99" s="7"/>
-      <c r="H99" s="7"/>
-      <c r="M99" s="7"/>
-    </row>
-    <row r="100" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B100" s="7"/>
-      <c r="H100" s="7"/>
-      <c r="M100" s="7"/>
-    </row>
-    <row r="101" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B101" s="7"/>
-      <c r="H101" s="7"/>
-      <c r="M101" s="7"/>
-    </row>
-    <row r="102" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B102" s="7"/>
-      <c r="H102" s="7"/>
-      <c r="M102" s="7"/>
-    </row>
-    <row r="103" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B103" s="7"/>
-      <c r="H103" s="7"/>
-      <c r="M103" s="7"/>
-    </row>
-    <row r="104" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B104" s="7"/>
-      <c r="H104" s="7"/>
-      <c r="M104" s="7"/>
-    </row>
-    <row r="105" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B105" s="7"/>
-      <c r="H105" s="7"/>
-      <c r="M105" s="7"/>
-    </row>
-    <row r="106" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B106" s="7"/>
-      <c r="H106" s="7"/>
-      <c r="M106" s="7"/>
-    </row>
-    <row r="107" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B107" s="7"/>
-      <c r="H107" s="7"/>
-      <c r="M107" s="7"/>
-    </row>
-    <row r="108" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B108" s="7"/>
-      <c r="H108" s="7"/>
-      <c r="M108" s="7"/>
-    </row>
-    <row r="109" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B109" s="7"/>
-      <c r="H109" s="7"/>
-      <c r="M109" s="7"/>
-    </row>
-    <row r="110" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B110" s="7"/>
-      <c r="H110" s="7"/>
-      <c r="M110" s="7"/>
-    </row>
-    <row r="111" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B111" s="7"/>
-      <c r="H111" s="7"/>
-      <c r="M111" s="7"/>
-    </row>
-    <row r="112" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B112" s="7"/>
-      <c r="H112" s="7"/>
-      <c r="M112" s="7"/>
-    </row>
-    <row r="113" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B113" s="7"/>
-      <c r="H113" s="7"/>
-      <c r="M113" s="7"/>
-    </row>
-    <row r="114" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B114" s="7"/>
-      <c r="H114" s="7"/>
-      <c r="M114" s="7"/>
-    </row>
-    <row r="115" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B115" s="7"/>
-      <c r="H115" s="7"/>
-      <c r="M115" s="7"/>
-    </row>
-    <row r="116" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B116" s="7"/>
-      <c r="H116" s="7"/>
-      <c r="M116" s="7"/>
-    </row>
-    <row r="117" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B117" s="7"/>
-      <c r="H117" s="7"/>
-      <c r="M117" s="7"/>
-    </row>
-    <row r="118" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B118" s="7"/>
-      <c r="H118" s="7"/>
-      <c r="M118" s="7"/>
-    </row>
-    <row r="119" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B119" s="7"/>
-      <c r="H119" s="7"/>
-      <c r="M119" s="7"/>
-    </row>
-    <row r="120" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B120" s="7"/>
-      <c r="H120" s="7"/>
-      <c r="M120" s="7"/>
-    </row>
-    <row r="121" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B121" s="7"/>
-      <c r="H121" s="7"/>
-      <c r="M121" s="7"/>
-    </row>
-    <row r="122" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B122" s="7"/>
-      <c r="H122" s="7"/>
-      <c r="M122" s="7"/>
-    </row>
-    <row r="123" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B123" s="7"/>
-      <c r="H123" s="7"/>
-      <c r="M123" s="7"/>
-    </row>
-    <row r="124" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B124" s="7"/>
-      <c r="H124" s="7"/>
-      <c r="M124" s="7"/>
-    </row>
-    <row r="125" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B125" s="7"/>
-      <c r="H125" s="7"/>
-      <c r="M125" s="7"/>
-    </row>
-    <row r="126" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B126" s="7"/>
-      <c r="H126" s="7"/>
-      <c r="M126" s="7"/>
-    </row>
-    <row r="127" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B127" s="7"/>
-      <c r="H127" s="7"/>
-      <c r="M127" s="7"/>
-    </row>
-    <row r="128" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B128" s="7"/>
-      <c r="H128" s="7"/>
-      <c r="M128" s="7"/>
-    </row>
-    <row r="129" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B129" s="7"/>
-      <c r="H129" s="7"/>
-      <c r="M129" s="7"/>
-    </row>
-    <row r="130" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B130" s="7"/>
-      <c r="H130" s="7"/>
-      <c r="M130" s="7"/>
-    </row>
-    <row r="131" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B131" s="7"/>
-      <c r="H131" s="7"/>
-      <c r="M131" s="7"/>
-    </row>
-    <row r="132" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B132" s="7"/>
-      <c r="H132" s="7"/>
-      <c r="M132" s="7"/>
-    </row>
-    <row r="133" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B133" s="7"/>
-      <c r="H133" s="7"/>
-      <c r="M133" s="7"/>
-    </row>
-    <row r="134" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B134" s="7"/>
-      <c r="H134" s="7"/>
-      <c r="M134" s="7"/>
-    </row>
-    <row r="135" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B135" s="7"/>
-      <c r="H135" s="7"/>
-      <c r="M135" s="7"/>
-    </row>
-    <row r="136" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B136" s="7"/>
-      <c r="H136" s="7"/>
-      <c r="M136" s="7"/>
-    </row>
-    <row r="137" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B137" s="7"/>
-      <c r="H137" s="7"/>
-      <c r="M137" s="7"/>
-    </row>
-    <row r="138" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B138" s="7"/>
-      <c r="H138" s="7"/>
-      <c r="M138" s="7"/>
-    </row>
-    <row r="139" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B139" s="7"/>
-      <c r="H139" s="7"/>
-      <c r="M139" s="7"/>
-    </row>
+    <row r="75" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="81" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="82" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="83" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="84" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="85" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="86" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="87" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="88" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="89" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="90" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="91" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="92" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="93" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="94" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="95" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="96" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="97" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="98" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="99" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="100" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="101" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="102" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="103" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="104" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="105" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="106" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="107" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="108" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="109" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="110" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="111" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="112" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="113" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="114" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="115" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="116" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="117" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="118" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="119" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="120" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="121" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="122" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="123" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="124" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="125" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="126" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="127" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="128" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="129" spans="2:13" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="130" spans="2:13" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="131" spans="2:13" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="132" spans="2:13" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="133" spans="2:13" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="134" spans="2:13" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="135" spans="2:13" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="136" spans="2:13" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="137" spans="2:13" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="138" spans="2:13" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="139" spans="2:13" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="140" spans="2:13" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B140" s="7"/>
       <c r="H140" s="7"/>
@@ -44560,19 +44201,19 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]Report!#REF!</xm:f>
+            <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>M51:M74</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]Report!#REF!</xm:f>
+            <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E51:E74</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[TestCaseData.xlsx]Report!#REF!</xm:f>
+            <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G51:G74</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
update to test class + set all values in annotation to FALSE in Views sheet
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -15420,8 +15420,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD40"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16999,7 +16999,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="19" t="b">
         <v>0</v>
@@ -17014,7 +17014,7 @@
         <v>1</v>
       </c>
       <c r="L36" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="19" t="s">
         <v>83</v>
@@ -17087,7 +17087,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="19" t="b">
         <v>0</v>
@@ -17102,7 +17102,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38" s="19" t="s">
         <v>83</v>
@@ -17974,13 +17974,13 @@
           <x14:formula1>
             <xm:f>General!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:L35 C41:L1048576</xm:sqref>
+          <xm:sqref>C2:L35 C41:L1048576 L36:L40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>General!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C36:L40</xm:sqref>
+          <xm:sqref>C36:K40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -18528,7 +18528,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30756,8 +30756,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated locator for in progress Copy and Cancel
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -1746,9 +1746,6 @@
     <t>TC13</t>
   </si>
   <si>
-    <t>11,38,39</t>
-  </si>
-  <si>
     <t>Annotations, Isotopic, Assets, Boundaries = TRUE, (BaseMap=Map)</t>
   </si>
   <si>
@@ -1758,13 +1755,16 @@
     <t>LISAs, Indications, Field Notes, Gaps = TRUE, (BaseMap=Satellite)</t>
   </si>
   <si>
-    <t>FOV, Isotopic Analysis, Assets, Boundaries = TRUE, (BaseMap=Map)</t>
-  </si>
-  <si>
     <t>stnd-pic</t>
   </si>
   <si>
     <t>iso-cap</t>
+  </si>
+  <si>
+    <t>FOV, Indication, Isotopic Analysis, Assets, Boundaries = TRUE, (BaseMap=Map)</t>
+  </si>
+  <si>
+    <t>18,38,39</t>
   </si>
 </sst>
 </file>
@@ -1982,7 +1982,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2022,6 +2022,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1 2" xfId="7"/>
@@ -3052,7 +3053,7 @@
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
       <c r="D27" s="19" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
@@ -3075,7 +3076,7 @@
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
@@ -15391,8 +15392,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD40"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15429,7 +15430,7 @@
       <c r="F1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="21" t="s">
         <v>77</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -16970,7 +16971,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="19" t="b">
         <v>0</v>
@@ -16985,13 +16986,13 @@
         <v>1</v>
       </c>
       <c r="L36" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="19" t="s">
         <v>83</v>
       </c>
       <c r="N36" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17058,7 +17059,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="19" t="b">
         <v>0</v>
@@ -17073,13 +17074,13 @@
         <v>0</v>
       </c>
       <c r="L38" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38" s="19" t="s">
         <v>83</v>
       </c>
       <c r="N38" s="19" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17123,7 +17124,7 @@
         <v>84</v>
       </c>
       <c r="N39" s="19" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17167,7 +17168,7 @@
         <v>83</v>
       </c>
       <c r="N40" s="19" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -17932,6 +17933,7 @@
     <row r="800" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
@@ -17945,13 +17947,13 @@
           <x14:formula1>
             <xm:f>General!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:L35 C41:L1048576</xm:sqref>
+          <xm:sqref>C2:L35 C41:L1048576 G36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>General!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C36:L40</xm:sqref>
+          <xm:sqref>C36:F40 G37 H36:L40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -18100,10 +18102,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18487,6 +18489,11 @@
       </c>
       <c r="E22" s="12" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="19">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -30727,8 +30734,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51:C74"/>
+    <sheetView topLeftCell="P70" workbookViewId="0">
+      <selection activeCell="S74" sqref="S74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34793,10 +34800,10 @@
         <v>18</v>
       </c>
       <c r="T73" s="20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U73" s="20">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="V73" s="19">
         <v>27</v>
@@ -34851,13 +34858,13 @@
         <v>20</v>
       </c>
       <c r="S74" s="20" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="T74" s="20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U74" s="20">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="V74" s="19">
         <v>27</v>

</xml_diff>

<commit_message>
add ability to trigger survey upload from CI
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="15" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -144,6 +144,233 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Shirish Pulikkal</author>
+  </authors>
+  <commentList>
+    <comment ref="B43" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Test data survey. Used when uploading survey data to different environments. It is recommended to NOT use this tag for creation of survey in driver view for other purposes as it might create duplicate surveys with the same tag in the environment.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Test data survey. Used when uploading survey data to different environments. It is recommended to NOT use this tag for creation of survey in driver view for other purposes as it might create duplicate surveys with the same tag in the environment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B45" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Test data survey. Used when uploading survey data to different environments. It is recommended to NOT use this tag for creation of survey in driver view for other purposes as it might create duplicate surveys with the same tag in the environment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B46" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Test data survey. Used when uploading survey data to different environments. It is recommended to NOT use this tag for creation of survey in driver view for other purposes as it might create duplicate surveys with the same tag in the environment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B47" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Test data survey. Used when uploading survey data to different environments. It is recommended to NOT use this tag for creation of survey in driver view for other purposes as it might create duplicate surveys with the same tag in the environment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B48" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Test data survey. Used when uploading survey data to different environments. It is recommended to NOT use this tag for creation of survey in driver view for other purposes as it might create duplicate surveys with the same tag in the environment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B49" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Test data survey. Used when uploading survey data to different environments. It is recommended to NOT use this tag for creation of survey in driver view for other purposes as it might create duplicate surveys with the same tag in the environment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B50" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Test data survey. Used when uploading survey data to different environments. It is recommended to NOT use this tag for creation of survey in driver view for other purposes as it might create duplicate surveys with the same tag in the environment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B51" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Shirish Pulikkal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Test data survey. Used when uploading survey data to different environments. It is recommended to NOT use this tag for creation of survey in driver view for other purposes as it might create duplicate surveys with the same tag in the environment.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Shirish Pulikkal</author>
@@ -314,7 +541,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Shirish Pulikkal</author>
@@ -1752,7 +1979,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1855,6 +2082,19 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2378,7 +2618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1138"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -19686,7 +19926,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -28812,12 +29052,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H1073"/>
   <sheetViews>
-    <sheetView topLeftCell="D16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35068,6 +35308,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">

</xml_diff>

<commit_message>
additional comprpt page actions + some fixes
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="433">
   <si>
     <t>Enabled</t>
   </si>
@@ -1653,9 +1653,6 @@
     <t>Over700</t>
   </si>
   <si>
-    <t>TC1091 Report558596</t>
-  </si>
-  <si>
     <t>TC1319</t>
   </si>
   <si>
@@ -1795,6 +1792,9 @@
   </si>
   <si>
     <t>iso-cap</t>
+  </si>
+  <si>
+    <t>TC824 Report992104</t>
   </si>
 </sst>
 </file>
@@ -3081,7 +3081,7 @@
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
       <c r="D27" s="19" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
@@ -3104,7 +3104,7 @@
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
@@ -15420,8 +15420,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17020,7 +17020,7 @@
         <v>83</v>
       </c>
       <c r="N36" s="19" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17108,7 +17108,7 @@
         <v>83</v>
       </c>
       <c r="N38" s="19" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17152,7 +17152,7 @@
         <v>84</v>
       </c>
       <c r="N39" s="19" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17196,7 +17196,7 @@
         <v>83</v>
       </c>
       <c r="N40" s="19" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -20802,7 +20802,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30756,8 +30756,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33437,10 +33437,10 @@
         <v>340</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>385</v>
+        <v>432</v>
       </c>
       <c r="D50" s="7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>162</v>
@@ -33494,10 +33494,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="19" t="s">
+        <v>385</v>
+      </c>
+      <c r="C51" s="19" t="s">
         <v>386</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>387</v>
       </c>
       <c r="D51" s="19">
         <v>1</v>
@@ -33515,7 +33515,7 @@
         <v>236</v>
       </c>
       <c r="N51" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O51" s="19">
         <v>0.5</v>
@@ -33539,7 +33539,7 @@
         <v>1</v>
       </c>
       <c r="V51" s="19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="52" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33547,10 +33547,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D52" s="19">
         <v>1</v>
@@ -33568,7 +33568,7 @@
         <v>236</v>
       </c>
       <c r="N52" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O52" s="19">
         <v>0.5</v>
@@ -33592,7 +33592,7 @@
         <v>1</v>
       </c>
       <c r="V52" s="19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="53" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33600,10 +33600,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D53" s="19">
         <v>1</v>
@@ -33621,7 +33621,7 @@
         <v>236</v>
       </c>
       <c r="N53" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O53" s="19">
         <v>0.5</v>
@@ -33645,7 +33645,7 @@
         <v>1</v>
       </c>
       <c r="V53" s="19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="54" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33653,10 +33653,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D54" s="19">
         <v>1</v>
@@ -33674,7 +33674,7 @@
         <v>236</v>
       </c>
       <c r="N54" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O54" s="19">
         <v>0.5</v>
@@ -33698,7 +33698,7 @@
         <v>1</v>
       </c>
       <c r="V54" s="19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="55" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33706,10 +33706,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D55" s="19">
         <v>1</v>
@@ -33727,7 +33727,7 @@
         <v>236</v>
       </c>
       <c r="N55" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O55" s="19">
         <v>0.5</v>
@@ -33751,7 +33751,7 @@
         <v>1</v>
       </c>
       <c r="V55" s="19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="56" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33759,10 +33759,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D56" s="19">
         <v>1</v>
@@ -33780,7 +33780,7 @@
         <v>236</v>
       </c>
       <c r="N56" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O56" s="19">
         <v>0.5</v>
@@ -33804,7 +33804,7 @@
         <v>1</v>
       </c>
       <c r="V56" s="19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="57" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33812,10 +33812,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D57" s="19">
         <v>1</v>
@@ -33833,7 +33833,7 @@
         <v>236</v>
       </c>
       <c r="N57" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O57" s="19">
         <v>0.5</v>
@@ -33857,7 +33857,7 @@
         <v>1</v>
       </c>
       <c r="V57" s="19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="58" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33865,10 +33865,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D58" s="19">
         <v>1</v>
@@ -33886,7 +33886,7 @@
         <v>236</v>
       </c>
       <c r="N58" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O58" s="19">
         <v>0.5</v>
@@ -33910,7 +33910,7 @@
         <v>1</v>
       </c>
       <c r="V58" s="19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="59" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33918,10 +33918,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="C59" s="19" t="s">
         <v>397</v>
-      </c>
-      <c r="C59" s="19" t="s">
-        <v>398</v>
       </c>
       <c r="D59" s="19">
         <v>1</v>
@@ -33939,7 +33939,7 @@
         <v>236</v>
       </c>
       <c r="N59" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O59" s="19">
         <v>0.5</v>
@@ -33971,10 +33971,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="C60" s="19" t="s">
         <v>399</v>
-      </c>
-      <c r="C60" s="19" t="s">
-        <v>400</v>
       </c>
       <c r="D60" s="19">
         <v>1</v>
@@ -33992,7 +33992,7 @@
         <v>236</v>
       </c>
       <c r="N60" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O60" s="19">
         <v>0.5</v>
@@ -34016,7 +34016,7 @@
         <v>1</v>
       </c>
       <c r="V60" s="19" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="61" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -34024,10 +34024,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D61" s="19">
         <v>1</v>
@@ -34045,7 +34045,7 @@
         <v>236</v>
       </c>
       <c r="N61" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O61" s="19">
         <v>0.5</v>
@@ -34069,7 +34069,7 @@
         <v>1</v>
       </c>
       <c r="V61" s="19" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="62" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -34077,10 +34077,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="C62" s="19" t="s">
         <v>403</v>
-      </c>
-      <c r="C62" s="19" t="s">
-        <v>404</v>
       </c>
       <c r="D62" s="19">
         <v>1</v>
@@ -34098,7 +34098,7 @@
         <v>236</v>
       </c>
       <c r="N62" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O62" s="19">
         <v>0.5</v>
@@ -34130,10 +34130,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="19" t="s">
+        <v>404</v>
+      </c>
+      <c r="C63" s="19" t="s">
         <v>405</v>
-      </c>
-      <c r="C63" s="19" t="s">
-        <v>406</v>
       </c>
       <c r="D63" s="19">
         <v>1</v>
@@ -34151,7 +34151,7 @@
         <v>236</v>
       </c>
       <c r="N63" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O63" s="19">
         <v>0.5</v>
@@ -34175,7 +34175,7 @@
         <v>1</v>
       </c>
       <c r="V63" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="64" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -34183,10 +34183,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="C64" s="19" t="s">
         <v>408</v>
-      </c>
-      <c r="C64" s="19" t="s">
-        <v>409</v>
       </c>
       <c r="D64" s="19">
         <v>1</v>
@@ -34204,7 +34204,7 @@
         <v>236</v>
       </c>
       <c r="N64" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O64" s="19">
         <v>0.5</v>
@@ -34228,7 +34228,7 @@
         <v>1</v>
       </c>
       <c r="V64" s="19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="65" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -34236,10 +34236,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D65" s="19">
         <v>1</v>
@@ -34257,7 +34257,7 @@
         <v>236</v>
       </c>
       <c r="N65" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O65" s="19">
         <v>0.5</v>
@@ -34281,7 +34281,7 @@
         <v>1</v>
       </c>
       <c r="V65" s="19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="66" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -34289,10 +34289,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="C66" s="19" t="s">
         <v>412</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>413</v>
       </c>
       <c r="D66" s="19">
         <v>1</v>
@@ -34310,7 +34310,7 @@
         <v>236</v>
       </c>
       <c r="N66" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O66" s="19">
         <v>0.5</v>
@@ -34334,7 +34334,7 @@
         <v>1</v>
       </c>
       <c r="V66" s="19" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="67" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -34342,10 +34342,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="19" t="s">
+        <v>414</v>
+      </c>
+      <c r="C67" s="19" t="s">
         <v>415</v>
-      </c>
-      <c r="C67" s="19" t="s">
-        <v>416</v>
       </c>
       <c r="D67" s="19">
         <v>1</v>
@@ -34401,10 +34401,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D68" s="19">
         <v>1</v>
@@ -34460,10 +34460,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D69" s="19">
         <v>1</v>
@@ -34519,10 +34519,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="C70" s="19" t="s">
         <v>419</v>
-      </c>
-      <c r="C70" s="19" t="s">
-        <v>420</v>
       </c>
       <c r="D70" s="19">
         <v>1</v>
@@ -34540,7 +34540,7 @@
         <v>236</v>
       </c>
       <c r="N70" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O70" s="19">
         <v>0.5</v>
@@ -34572,10 +34572,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="19" t="s">
+        <v>420</v>
+      </c>
+      <c r="C71" s="19" t="s">
         <v>421</v>
-      </c>
-      <c r="C71" s="19" t="s">
-        <v>422</v>
       </c>
       <c r="D71" s="19">
         <v>1</v>
@@ -34614,7 +34614,7 @@
         <v>11</v>
       </c>
       <c r="S71" s="19" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="T71" s="19">
         <v>1</v>
@@ -34631,10 +34631,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D72" s="19">
         <v>1</v>
@@ -34652,7 +34652,7 @@
         <v>236</v>
       </c>
       <c r="N72" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O72" s="19">
         <v>0.5</v>
@@ -34681,10 +34681,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D73" s="19">
         <v>1</v>
@@ -34740,10 +34740,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C74" s="19" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D74" s="19">
         <v>1</v>
@@ -34782,7 +34782,7 @@
         <v>20</v>
       </c>
       <c r="S74" s="19" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="T74" s="19">
         <v>1</v>
@@ -34794,7 +34794,57 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A75" s="19">
+        <v>74</v>
+      </c>
+      <c r="B75" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="C75" s="18"/>
+      <c r="D75" s="19">
+        <v>1</v>
+      </c>
+      <c r="E75" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="F75" s="19">
+        <v>0</v>
+      </c>
+      <c r="G75" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I75" s="19">
+        <v>37.4102286146667</v>
+      </c>
+      <c r="J75" s="19">
+        <v>-121.98135786749999</v>
+      </c>
+      <c r="K75" s="19">
+        <v>37.410229614666697</v>
+      </c>
+      <c r="L75" s="19">
+        <v>-121.984789916667</v>
+      </c>
+      <c r="Q75" s="19">
+        <v>8.5</v>
+      </c>
+      <c r="R75" s="19">
+        <v>11</v>
+      </c>
+      <c r="S75" s="19">
+        <v>23</v>
+      </c>
+      <c r="T75" s="19">
+        <v>1</v>
+      </c>
+      <c r="U75" s="19">
+        <v>11</v>
+      </c>
+      <c r="V75" s="19">
+        <v>4</v>
+      </c>
+    </row>
     <row r="76" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="77" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="78" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Actions required for comp reports page tests 7,8,9
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -1788,13 +1788,13 @@
     <t>iso-cap</t>
   </si>
   <si>
-    <t>TC824 Report992104</t>
-  </si>
-  <si>
     <t>ONLY Assets and Gaps TRUE</t>
   </si>
   <si>
     <t>FOV and Breadcrumb</t>
+  </si>
+  <si>
+    <t>6636dcfa8b4f416d828b</t>
   </si>
 </sst>
 </file>
@@ -15420,7 +15420,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+    <sheetView topLeftCell="D7" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -16668,7 +16668,7 @@
         <v>83</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="29" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16712,7 +16712,7 @@
         <v>83</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20470,7 +20470,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30756,8 +30756,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33437,10 +33437,10 @@
         <v>338</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D50" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>162</v>

</xml_diff>

<commit_message>
Enabled 17 tests in setIII
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="430">
   <si>
     <t>Enabled</t>
   </si>
@@ -1704,9 +1704,6 @@
     <t>TC1352</t>
   </si>
   <si>
-    <t>31,26,27,30</t>
-  </si>
-  <si>
     <t>TC1370</t>
   </si>
   <si>
@@ -1737,9 +1734,6 @@
     <t>TC149</t>
   </si>
   <si>
-    <t>35,36,37</t>
-  </si>
-  <si>
     <t>TC12</t>
   </si>
   <si>
@@ -1765,6 +1759,33 @@
   </si>
   <si>
     <t>18,38,39</t>
+  </si>
+  <si>
+    <t>30,26</t>
+  </si>
+  <si>
+    <t>All FALSE, Base Map=Map</t>
+  </si>
+  <si>
+    <t>TestView1</t>
+  </si>
+  <si>
+    <t>TestView2</t>
+  </si>
+  <si>
+    <t>TestView3</t>
+  </si>
+  <si>
+    <t>LISA, FOV, Breadcrumbs TRUE, (BaseMap=Satellite)</t>
+  </si>
+  <si>
+    <t>35,41,37</t>
+  </si>
+  <si>
+    <t>std test</t>
+  </si>
+  <si>
+    <t>32,26,27,30</t>
   </si>
 </sst>
 </file>
@@ -1982,7 +2003,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2023,6 +2044,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1 2" xfId="7"/>
@@ -2396,10 +2419,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1138"/>
+  <dimension ref="A1:K1137"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3053,7 +3076,7 @@
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
       <c r="D27" s="19" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
@@ -3076,7 +3099,7 @@
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
@@ -3162,7 +3185,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="19">
+      <c r="A32" s="22">
         <v>31</v>
       </c>
       <c r="B32" s="19"/>
@@ -3184,29 +3207,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="22">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19">
+        <v>1</v>
+      </c>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="22">
+        <v>33</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19">
+        <v>1</v>
+      </c>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -3217,7 +3260,7 @@
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -3228,7 +3271,7 @@
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -3239,7 +3282,7 @@
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -3250,7 +3293,7 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -3261,7 +3304,7 @@
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -3272,7 +3315,7 @@
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -3283,7 +3326,7 @@
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -3294,7 +3337,7 @@
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
@@ -3305,7 +3348,7 @@
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -3316,7 +3359,7 @@
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
@@ -3327,7 +3370,7 @@
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -3338,7 +3381,7 @@
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -3349,7 +3392,7 @@
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -10368,15 +10411,15 @@
       <c r="J685" s="7"/>
     </row>
     <row r="686" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B686" s="7"/>
-      <c r="C686" s="7"/>
-      <c r="D686" s="7"/>
-      <c r="E686" s="7"/>
-      <c r="F686" s="7"/>
-      <c r="G686" s="7"/>
-      <c r="H686" s="7"/>
-      <c r="I686" s="7"/>
-      <c r="J686" s="7"/>
+      <c r="B686" s="5"/>
+      <c r="C686" s="5"/>
+      <c r="D686" s="5"/>
+      <c r="E686" s="5"/>
+      <c r="F686" s="5"/>
+      <c r="G686" s="5"/>
+      <c r="H686" s="5"/>
+      <c r="I686" s="5"/>
+      <c r="J686" s="5"/>
     </row>
     <row r="687" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B687" s="5"/>
@@ -15338,17 +15381,6 @@
       <c r="H1137" s="5"/>
       <c r="I1137" s="5"/>
       <c r="J1137" s="5"/>
-    </row>
-    <row r="1138" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B1138" s="5"/>
-      <c r="C1138" s="5"/>
-      <c r="D1138" s="5"/>
-      <c r="E1138" s="5"/>
-      <c r="F1138" s="5"/>
-      <c r="G1138" s="5"/>
-      <c r="H1138" s="5"/>
-      <c r="I1138" s="5"/>
-      <c r="J1138" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15361,25 +15393,25 @@
           <x14:formula1>
             <xm:f>General!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J33:J1048576 J2:J26 H1:H26 H33:H1048576</xm:sqref>
+          <xm:sqref>J2:J26 H1:H26 J35:J1048576 J33 H33 H35:H1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Report!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G26 G33:G1048576</xm:sqref>
+          <xm:sqref>G1:G26 G33 G35:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>G27:G32</xm:sqref>
+          <xm:sqref>G27:G32 G34</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>General!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>J27:J32 H27:H32</xm:sqref>
+          <xm:sqref>J27:J32 H27:H32 J34 H34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -15392,8 +15424,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16956,7 +16988,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>99</v>
+        <v>423</v>
       </c>
       <c r="C36" s="19" t="b">
         <v>0</v>
@@ -16992,7 +17024,7 @@
         <v>83</v>
       </c>
       <c r="N36" s="19" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17000,7 +17032,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>99</v>
+        <v>424</v>
       </c>
       <c r="C37" s="19" t="b">
         <v>1</v>
@@ -17036,7 +17068,7 @@
         <v>84</v>
       </c>
       <c r="N37" s="19" t="s">
-        <v>299</v>
+        <v>426</v>
       </c>
     </row>
     <row r="38" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17044,7 +17076,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>99</v>
+        <v>425</v>
       </c>
       <c r="C38" s="19" t="b">
         <v>0</v>
@@ -17080,7 +17112,7 @@
         <v>83</v>
       </c>
       <c r="N38" s="19" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17124,7 +17156,7 @@
         <v>84</v>
       </c>
       <c r="N39" s="19" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17168,11 +17200,97 @@
         <v>83</v>
       </c>
       <c r="N40" s="19" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A41" s="19">
+        <v>40</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="M41" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="N41" s="19" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A42" s="19">
+        <v>41</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>424</v>
+      </c>
+      <c r="C42" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L42" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="M42" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="N42" s="19" t="s">
+        <v>299</v>
+      </c>
+    </row>
     <row r="43" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="45" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -17941,25 +18059,25 @@
           <x14:formula1>
             <xm:f>Report!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>M1:M35 M41:M1048576</xm:sqref>
+          <xm:sqref>M1:M35 M43:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>General!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:L35 C41:L1048576 G36</xm:sqref>
+          <xm:sqref>C2:L35 G36 C43:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>General!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C36:F40 G37 H36:L40</xm:sqref>
+          <xm:sqref>F36:F40 G37 C36:C42 D36:D40 E36:E42 H36:H42 L36:L42 I36:K40 F42:G42 D42 I42:K42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>M36:M40</xm:sqref>
+          <xm:sqref>M36:M41</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -17972,7 +18090,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18104,8 +18222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18632,7 +18750,7 @@
   <dimension ref="A1:H578"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28774,7 +28892,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H1072"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -30734,8 +30852,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView topLeftCell="P70" workbookViewId="0">
-      <selection activeCell="S74" sqref="S74"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53:C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33648,7 +33766,7 @@
       <c r="B54" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D54" s="20">
@@ -33706,7 +33824,7 @@
       <c r="B55" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C55" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D55" s="20">
@@ -33764,7 +33882,7 @@
       <c r="B56" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C56" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D56" s="20">
@@ -33822,7 +33940,7 @@
       <c r="B57" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="C57" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D57" s="20">
@@ -33880,7 +33998,7 @@
       <c r="B58" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="C58" s="19" t="s">
+      <c r="C58" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D58" s="20">
@@ -33938,7 +34056,7 @@
       <c r="B59" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="C59" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D59" s="20">
@@ -33996,7 +34114,7 @@
       <c r="B60" s="19" t="s">
         <v>397</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="C60" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D60" s="20">
@@ -34054,7 +34172,7 @@
       <c r="B61" s="19" t="s">
         <v>399</v>
       </c>
-      <c r="C61" s="19" t="s">
+      <c r="C61" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D61" s="20">
@@ -34112,7 +34230,7 @@
       <c r="B62" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D62" s="20">
@@ -34170,7 +34288,7 @@
       <c r="B63" s="19" t="s">
         <v>401</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="C63" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D63" s="20">
@@ -34218,7 +34336,7 @@
         <v>1</v>
       </c>
       <c r="V63" s="20" t="s">
-        <v>402</v>
+        <v>429</v>
       </c>
     </row>
     <row r="64" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -34226,9 +34344,9 @@
         <v>63</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>403</v>
-      </c>
-      <c r="C64" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="C64" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D64" s="20">
@@ -34276,7 +34394,7 @@
         <v>1</v>
       </c>
       <c r="V64" s="20" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="65" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -34284,9 +34402,9 @@
         <v>64</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>405</v>
-      </c>
-      <c r="C65" s="19" t="s">
+        <v>404</v>
+      </c>
+      <c r="C65" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D65" s="20">
@@ -34325,7 +34443,7 @@
         <v>11</v>
       </c>
       <c r="S65" s="20">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="T65" s="20">
         <v>1</v>
@@ -34334,7 +34452,7 @@
         <v>1</v>
       </c>
       <c r="V65" s="20" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="66" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -34342,9 +34460,9 @@
         <v>65</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>406</v>
-      </c>
-      <c r="C66" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="C66" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D66" s="20">
@@ -34383,7 +34501,7 @@
         <v>11</v>
       </c>
       <c r="S66" s="20">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="T66" s="20">
         <v>1</v>
@@ -34392,7 +34510,7 @@
         <v>1</v>
       </c>
       <c r="V66" s="20" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="67" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -34400,9 +34518,9 @@
         <v>66</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>408</v>
-      </c>
-      <c r="C67" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="C67" s="22" t="s">
         <v>177</v>
       </c>
       <c r="D67" s="20">
@@ -34444,16 +34562,16 @@
         <v>11</v>
       </c>
       <c r="S67" s="20">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="T67" s="20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="U67" s="20">
         <v>7</v>
       </c>
-      <c r="V67" s="20">
-        <v>30</v>
+      <c r="V67" s="23" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="68" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
@@ -34461,7 +34579,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C68" s="19" t="s">
         <v>177</v>
@@ -34522,7 +34640,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C69" s="19" t="s">
         <v>177</v>
@@ -34583,7 +34701,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C70" s="19" t="s">
         <v>177</v>
@@ -34637,7 +34755,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C71" s="19" t="s">
         <v>177</v>
@@ -34681,7 +34799,7 @@
         <v>11</v>
       </c>
       <c r="S71" s="20" t="s">
-        <v>413</v>
+        <v>427</v>
       </c>
       <c r="T71" s="20">
         <v>1</v>
@@ -34690,14 +34808,14 @@
         <v>7</v>
       </c>
       <c r="V71" s="20">
-        <v>1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="72" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="19">
         <v>71</v>
       </c>
-      <c r="B72" s="19" t="s">
+      <c r="B72" s="5" t="s">
         <v>400</v>
       </c>
       <c r="C72" s="19" t="s">
@@ -34747,13 +34865,16 @@
       <c r="U72" s="20">
         <v>1</v>
       </c>
+      <c r="V72" s="20" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="73" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="19">
         <v>72</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C73" s="19" t="s">
         <v>177</v>
@@ -34814,7 +34935,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C74" s="19" t="s">
         <v>177</v>
@@ -34858,37 +34979,249 @@
         <v>20</v>
       </c>
       <c r="S74" s="20" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="T74" s="20">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="U74" s="20">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="V74" s="19">
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B75" s="7"/>
-      <c r="H75" s="7"/>
-      <c r="M75" s="7"/>
-    </row>
-    <row r="76" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B76" s="7"/>
-      <c r="H76" s="7"/>
-      <c r="M76" s="7"/>
-    </row>
-    <row r="77" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B77" s="7"/>
-      <c r="H77" s="7"/>
-      <c r="M77" s="7"/>
-    </row>
-    <row r="78" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="B78" s="7"/>
-      <c r="H78" s="7"/>
-      <c r="M78" s="7"/>
+    <row r="75" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="19">
+        <v>74</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D75" s="20">
+        <v>1</v>
+      </c>
+      <c r="E75" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="F75" s="20">
+        <v>0</v>
+      </c>
+      <c r="G75" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H75" s="20"/>
+      <c r="I75" s="20"/>
+      <c r="J75" s="20"/>
+      <c r="K75" s="20"/>
+      <c r="L75" s="20"/>
+      <c r="M75" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="N75" t="s">
+        <v>387</v>
+      </c>
+      <c r="O75" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="P75" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="Q75" s="20">
+        <v>8.5</v>
+      </c>
+      <c r="R75" s="20">
+        <v>11</v>
+      </c>
+      <c r="S75" s="20">
+        <v>11</v>
+      </c>
+      <c r="T75" s="20">
+        <v>1</v>
+      </c>
+      <c r="U75" s="20">
+        <v>1</v>
+      </c>
+      <c r="V75" s="20" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="19">
+        <v>75</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D76" s="20">
+        <v>1</v>
+      </c>
+      <c r="E76" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="F76" s="20">
+        <v>0</v>
+      </c>
+      <c r="G76" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H76" s="20"/>
+      <c r="I76" s="20"/>
+      <c r="J76" s="20"/>
+      <c r="K76" s="20"/>
+      <c r="L76" s="20"/>
+      <c r="M76" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="N76" t="s">
+        <v>387</v>
+      </c>
+      <c r="O76" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="P76" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="Q76" s="20">
+        <v>8.5</v>
+      </c>
+      <c r="R76" s="20">
+        <v>11</v>
+      </c>
+      <c r="S76" s="20">
+        <v>11</v>
+      </c>
+      <c r="T76" s="20">
+        <v>1</v>
+      </c>
+      <c r="U76" s="20">
+        <v>1</v>
+      </c>
+      <c r="V76" s="20">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="19">
+        <v>76</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D77" s="20">
+        <v>1</v>
+      </c>
+      <c r="E77" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="F77" s="20">
+        <v>0</v>
+      </c>
+      <c r="G77" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H77" s="20"/>
+      <c r="I77" s="20"/>
+      <c r="J77" s="20"/>
+      <c r="K77" s="20"/>
+      <c r="L77" s="20"/>
+      <c r="M77" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="N77" t="s">
+        <v>387</v>
+      </c>
+      <c r="O77" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="P77" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="Q77" s="20">
+        <v>8.5</v>
+      </c>
+      <c r="R77" s="20">
+        <v>11</v>
+      </c>
+      <c r="S77" s="20">
+        <v>40</v>
+      </c>
+      <c r="T77" s="20">
+        <v>4</v>
+      </c>
+      <c r="U77" s="20">
+        <v>6</v>
+      </c>
+      <c r="V77" s="20">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="19">
+        <v>77</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D78" s="20">
+        <v>1</v>
+      </c>
+      <c r="E78" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="F78" s="20">
+        <v>0</v>
+      </c>
+      <c r="G78" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H78" s="20"/>
+      <c r="I78" s="20"/>
+      <c r="J78" s="20"/>
+      <c r="K78" s="20"/>
+      <c r="L78" s="20"/>
+      <c r="M78" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="N78" t="s">
+        <v>387</v>
+      </c>
+      <c r="O78" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="P78" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="Q78" s="20">
+        <v>8.5</v>
+      </c>
+      <c r="R78" s="20">
+        <v>11</v>
+      </c>
+      <c r="S78" s="20">
+        <v>40</v>
+      </c>
+      <c r="T78" s="20">
+        <v>4</v>
+      </c>
+      <c r="U78" s="20">
+        <v>6</v>
+      </c>
+      <c r="V78" s="20" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="79" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="B79" s="7"/>
@@ -44515,7 +44848,7 @@
           <x14:formula1>
             <xm:f>Report!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H2828:H1048576 G1:G50 G75:G1048576</xm:sqref>
+          <xm:sqref>H2828:H1048576 G1:G50 G79:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -44527,31 +44860,31 @@
           <x14:formula1>
             <xm:f>Report!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E50 E75:E1048576</xm:sqref>
+          <xm:sqref>E1:E50 E79:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Report!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M50 M75:M2824</xm:sqref>
+          <xm:sqref>M2:M50 M79:M2824</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>M51:M74</xm:sqref>
+          <xm:sqref>M51:M78</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>E51:E74</xm:sqref>
+          <xm:sqref>E51:E78</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Report!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>G51:G74</xm:sqref>
+          <xm:sqref>G51:G78</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
bug fixes pageTest6 + some other fixes
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="434">
   <si>
     <t>Enabled</t>
   </si>
@@ -1794,7 +1794,10 @@
     <t>FOV and Breadcrumb</t>
   </si>
   <si>
-    <t>6636dcfa8b4f416d828b</t>
+    <t>ONLY Gaps TRUE</t>
+  </si>
+  <si>
+    <t>68494f345cb849a1ac85</t>
   </si>
 </sst>
 </file>
@@ -15420,8 +15423,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17199,7 +17202,50 @@
         <v>427</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A41" s="19">
+        <v>40</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L41" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="M41" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
     <row r="42" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -17974,7 +18020,7 @@
           <x14:formula1>
             <xm:f>General!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>L36:L40 C41:L1048576 C2:L35</xm:sqref>
+          <xm:sqref>L36:L40 C2:L35 C41:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -18654,7 +18700,7 @@
   <dimension ref="A1:H578"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30756,8 +30802,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32993,7 +33039,7 @@
         <v>11</v>
       </c>
       <c r="S41" s="7">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="T41" s="7">
         <v>4</v>
@@ -33158,7 +33204,7 @@
         <v>4</v>
       </c>
       <c r="U44" s="7">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="V44" s="7">
         <v>4</v>
@@ -33429,63 +33475,56 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:22" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
+    <row r="50" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A50" s="19">
         <v>49</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>338</v>
+      <c r="B50" s="19" t="s">
+        <v>296</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>432</v>
-      </c>
-      <c r="D50" s="7">
-        <v>2</v>
-      </c>
-      <c r="E50" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="D50" s="19">
+        <v>1</v>
+      </c>
+      <c r="E50" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F50" s="7">
+      <c r="F50" s="19">
         <v>0</v>
       </c>
-      <c r="G50" s="7" t="s">
+      <c r="G50" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7">
+      <c r="I50" s="19">
         <v>37.4206</v>
       </c>
-      <c r="J50" s="7">
+      <c r="J50" s="19">
         <v>-121.9725</v>
       </c>
-      <c r="K50" s="7">
+      <c r="K50" s="19">
         <v>37.415700000000001</v>
       </c>
-      <c r="L50" s="7">
+      <c r="L50" s="19">
         <v>-121.98390000000001</v>
       </c>
-      <c r="M50" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="N50" s="7"/>
-      <c r="O50" s="7"/>
-      <c r="P50" s="7"/>
-      <c r="Q50" s="7">
+      <c r="Q50" s="19">
         <v>8.5</v>
       </c>
-      <c r="R50" s="7">
+      <c r="R50" s="19">
         <v>11</v>
       </c>
-      <c r="S50" s="7">
-        <v>23</v>
-      </c>
-      <c r="T50" s="7">
-        <v>1</v>
-      </c>
-      <c r="U50" s="7">
-        <v>11</v>
-      </c>
-      <c r="V50" s="7">
+      <c r="S50" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="T50" s="19">
+        <v>8</v>
+      </c>
+      <c r="U50" s="19">
+        <v>9</v>
+      </c>
+      <c r="V50" s="19">
         <v>4</v>
       </c>
     </row>
@@ -44229,7 +44268,7 @@
           <x14:formula1>
             <xm:f>Report!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H2828:H1048576 G1:G50 G75:G1048576</xm:sqref>
+          <xm:sqref>H2828:H1048576 G75:G1048576 G1:G50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -44241,13 +44280,13 @@
           <x14:formula1>
             <xm:f>Report!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E50 E75:E1048576</xm:sqref>
+          <xm:sqref>E75:E1048576 E1:E50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Report!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M50 M75:M2824</xm:sqref>
+          <xm:sqref>M75:M2824 M2:M50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
fixes for shape file baselines + some fixes in page test 6
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="459">
   <si>
     <t>Enabled</t>
   </si>
@@ -1798,6 +1798,81 @@
   </si>
   <si>
     <t>68494f345cb849a1ac85</t>
+  </si>
+  <si>
+    <t>View002</t>
+  </si>
+  <si>
+    <t>View009</t>
+  </si>
+  <si>
+    <t>View011</t>
+  </si>
+  <si>
+    <t>View012</t>
+  </si>
+  <si>
+    <t>View015</t>
+  </si>
+  <si>
+    <t>View016</t>
+  </si>
+  <si>
+    <t>View017</t>
+  </si>
+  <si>
+    <t>View018</t>
+  </si>
+  <si>
+    <t>View019</t>
+  </si>
+  <si>
+    <t>View020</t>
+  </si>
+  <si>
+    <t>View021</t>
+  </si>
+  <si>
+    <t>View022</t>
+  </si>
+  <si>
+    <t>View023</t>
+  </si>
+  <si>
+    <t>View024</t>
+  </si>
+  <si>
+    <t>View025</t>
+  </si>
+  <si>
+    <t>View026</t>
+  </si>
+  <si>
+    <t>View027</t>
+  </si>
+  <si>
+    <t>View028</t>
+  </si>
+  <si>
+    <t>View029</t>
+  </si>
+  <si>
+    <t>View030</t>
+  </si>
+  <si>
+    <t>View031</t>
+  </si>
+  <si>
+    <t>View032</t>
+  </si>
+  <si>
+    <t>View033</t>
+  </si>
+  <si>
+    <t>View034</t>
+  </si>
+  <si>
+    <t>View040</t>
   </si>
 </sst>
 </file>
@@ -15423,8 +15498,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15535,7 +15610,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>434</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -15843,7 +15918,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>99</v>
+        <v>435</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>
@@ -15931,7 +16006,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>99</v>
+        <v>436</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>1</v>
@@ -15975,7 +16050,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>99</v>
+        <v>437</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>1</v>
@@ -16107,7 +16182,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>99</v>
+        <v>438</v>
       </c>
       <c r="C16" s="7" t="b">
         <v>1</v>
@@ -16151,7 +16226,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>99</v>
+        <v>439</v>
       </c>
       <c r="C17" s="7" t="b">
         <v>1</v>
@@ -16195,7 +16270,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>99</v>
+        <v>440</v>
       </c>
       <c r="C18" s="7" t="b">
         <v>1</v>
@@ -16239,7 +16314,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>99</v>
+        <v>441</v>
       </c>
       <c r="C19" s="7" t="b">
         <v>1</v>
@@ -16283,7 +16358,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>99</v>
+        <v>442</v>
       </c>
       <c r="C20" s="7" t="b">
         <v>1</v>
@@ -16327,7 +16402,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>99</v>
+        <v>443</v>
       </c>
       <c r="C21" s="7" t="b">
         <v>1</v>
@@ -16371,7 +16446,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>99</v>
+        <v>444</v>
       </c>
       <c r="C22" s="7" t="b">
         <v>0</v>
@@ -16415,7 +16490,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>99</v>
+        <v>445</v>
       </c>
       <c r="C23" s="7" t="b">
         <v>0</v>
@@ -16459,7 +16534,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>99</v>
+        <v>446</v>
       </c>
       <c r="C24" s="7" t="b">
         <v>0</v>
@@ -16503,7 +16578,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>99</v>
+        <v>447</v>
       </c>
       <c r="C25" s="2" t="b">
         <v>1</v>
@@ -16546,8 +16621,8 @@
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>99</v>
+      <c r="B26" s="19" t="s">
+        <v>448</v>
       </c>
       <c r="C26" s="7" t="b">
         <v>0</v>
@@ -16590,8 +16665,8 @@
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>99</v>
+      <c r="B27" s="19" t="s">
+        <v>449</v>
       </c>
       <c r="C27" s="7" t="b">
         <v>0</v>
@@ -16634,8 +16709,8 @@
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>99</v>
+      <c r="B28" s="19" t="s">
+        <v>450</v>
       </c>
       <c r="C28" s="7" t="b">
         <v>0</v>
@@ -16678,8 +16753,8 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>99</v>
+      <c r="B29" s="19" t="s">
+        <v>451</v>
       </c>
       <c r="C29" s="7" t="b">
         <v>0</v>
@@ -16722,8 +16797,8 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>99</v>
+      <c r="B30" s="19" t="s">
+        <v>452</v>
       </c>
       <c r="C30" s="7" t="b">
         <v>1</v>
@@ -16767,7 +16842,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>99</v>
+        <v>453</v>
       </c>
       <c r="C31" s="7" t="b">
         <v>1</v>
@@ -16811,7 +16886,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>99</v>
+        <v>454</v>
       </c>
       <c r="C32" s="7" t="b">
         <v>1</v>
@@ -16855,7 +16930,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>99</v>
+        <v>455</v>
       </c>
       <c r="C33" s="7" t="b">
         <v>1</v>
@@ -16899,7 +16974,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>99</v>
+        <v>456</v>
       </c>
       <c r="C34" s="7" t="b">
         <v>1</v>
@@ -16943,7 +17018,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>99</v>
+        <v>457</v>
       </c>
       <c r="C35" s="7" t="b">
         <v>0</v>
@@ -17207,7 +17282,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>99</v>
+        <v>458</v>
       </c>
       <c r="C41" s="19" t="b">
         <v>0</v>
@@ -30802,8 +30877,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32336,7 +32411,7 @@
         <v>27</v>
       </c>
       <c r="T28" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U28" s="7">
         <v>2</v>

</xml_diff>

<commit_message>
fixes in page actions and page test6 tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="461">
   <si>
     <t>Enabled</t>
   </si>
@@ -1362,9 +1362,6 @@
     <t>TC237</t>
   </si>
   <si>
-    <t>Level 2-AB</t>
-  </si>
-  <si>
     <t>Level 2-A</t>
   </si>
   <si>
@@ -1872,7 +1869,16 @@
     <t>z`z`</t>
   </si>
   <si>
-    <t>93a1271f53414db5bd8e</t>
+    <t>TestPlat-Auto-1.5km</t>
+  </si>
+  <si>
+    <t>View014</t>
+  </si>
+  <si>
+    <t>View013</t>
+  </si>
+  <si>
+    <t>187fe14bab984102947a</t>
   </si>
 </sst>
 </file>
@@ -2439,19 +2445,19 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2459,10 +2465,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D2" s="9">
         <v>1</v>
@@ -2471,7 +2477,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2479,10 +2485,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>351</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>352</v>
       </c>
       <c r="D3" s="7">
         <v>2</v>
@@ -2491,7 +2497,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -2554,7 +2560,7 @@
         <v>279</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -3134,7 +3140,7 @@
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
       <c r="D26" s="19" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
@@ -3159,7 +3165,7 @@
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
       <c r="D27" s="19" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
@@ -3182,7 +3188,7 @@
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
@@ -15498,8 +15504,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N800"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15610,7 +15616,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -15778,7 +15784,7 @@
         <v>83</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15822,7 +15828,7 @@
         <v>84</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15866,7 +15872,7 @@
         <v>83</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15910,7 +15916,7 @@
         <v>84</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -15918,7 +15924,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>
@@ -16006,7 +16012,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>1</v>
@@ -16050,7 +16056,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>1</v>
@@ -16086,7 +16092,7 @@
         <v>83</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16094,7 +16100,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>99</v>
+        <v>459</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>1</v>
@@ -16138,7 +16144,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>99</v>
+        <v>458</v>
       </c>
       <c r="C15" s="7" t="b">
         <v>0</v>
@@ -16182,7 +16188,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C16" s="7" t="b">
         <v>1</v>
@@ -16226,7 +16232,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C17" s="7" t="b">
         <v>1</v>
@@ -16262,7 +16268,7 @@
         <v>84</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16270,7 +16276,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C18" s="7" t="b">
         <v>1</v>
@@ -16306,7 +16312,7 @@
         <v>85</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16314,7 +16320,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C19" s="7" t="b">
         <v>1</v>
@@ -16350,7 +16356,7 @@
         <v>83</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16358,7 +16364,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C20" s="7" t="b">
         <v>1</v>
@@ -16394,7 +16400,7 @@
         <v>84</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16402,7 +16408,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C21" s="7" t="b">
         <v>1</v>
@@ -16438,7 +16444,7 @@
         <v>83</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16446,7 +16452,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C22" s="7" t="b">
         <v>0</v>
@@ -16482,7 +16488,7 @@
         <v>83</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16490,7 +16496,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C23" s="7" t="b">
         <v>0</v>
@@ -16526,7 +16532,7 @@
         <v>83</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16534,7 +16540,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C24" s="7" t="b">
         <v>0</v>
@@ -16570,7 +16576,7 @@
         <v>83</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16578,7 +16584,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C25" s="2" t="b">
         <v>1</v>
@@ -16614,7 +16620,7 @@
         <v>83</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16622,7 +16628,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C26" s="7" t="b">
         <v>0</v>
@@ -16658,7 +16664,7 @@
         <v>83</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16666,7 +16672,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C27" s="7" t="b">
         <v>0</v>
@@ -16702,7 +16708,7 @@
         <v>83</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16710,7 +16716,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C28" s="7" t="b">
         <v>0</v>
@@ -16746,7 +16752,7 @@
         <v>83</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="29" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16754,7 +16760,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C29" s="7" t="b">
         <v>0</v>
@@ -16790,7 +16796,7 @@
         <v>83</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16798,7 +16804,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C30" s="7" t="b">
         <v>1</v>
@@ -16834,7 +16840,7 @@
         <v>83</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="31" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16842,7 +16848,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C31" s="7" t="b">
         <v>1</v>
@@ -16878,7 +16884,7 @@
         <v>84</v>
       </c>
       <c r="N31" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16886,7 +16892,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C32" s="7" t="b">
         <v>1</v>
@@ -16922,7 +16928,7 @@
         <v>84</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16930,7 +16936,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C33" s="7" t="b">
         <v>1</v>
@@ -16966,7 +16972,7 @@
         <v>83</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="34" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -16974,7 +16980,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C34" s="7" t="b">
         <v>1</v>
@@ -17010,7 +17016,7 @@
         <v>83</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17018,7 +17024,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C35" s="7" t="b">
         <v>0</v>
@@ -17054,7 +17060,7 @@
         <v>83</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="36" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17098,7 +17104,7 @@
         <v>83</v>
       </c>
       <c r="N36" s="19" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17142,7 +17148,7 @@
         <v>84</v>
       </c>
       <c r="N37" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="38" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17186,7 +17192,7 @@
         <v>83</v>
       </c>
       <c r="N38" s="19" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17230,7 +17236,7 @@
         <v>84</v>
       </c>
       <c r="N39" s="19" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17274,7 +17280,7 @@
         <v>83</v>
       </c>
       <c r="N40" s="19" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17282,7 +17288,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C41" s="19" t="b">
         <v>0</v>
@@ -17318,7 +17324,7 @@
         <v>83</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -19047,7 +19053,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -19073,7 +19079,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -19099,7 +19105,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -19703,22 +19709,22 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -19928,7 +19934,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B3" t="s">
         <v>48</v>
@@ -19945,7 +19951,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -19962,7 +19968,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C5" t="s">
         <v>236</v>
@@ -19973,7 +19979,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C6" t="s">
         <v>237</v>
@@ -20012,13 +20018,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -20026,7 +20032,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
@@ -20040,7 +20046,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
@@ -20131,7 +20137,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>160</v>
@@ -20166,7 +20172,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>164</v>
@@ -20202,7 +20208,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>165</v>
@@ -20238,7 +20244,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>166</v>
@@ -20306,7 +20312,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>167</v>
@@ -20342,7 +20348,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -20374,7 +20380,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -20406,7 +20412,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -20438,7 +20444,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>167</v>
@@ -20465,7 +20471,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>196</v>
@@ -20494,7 +20500,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>196</v>
@@ -20503,7 +20509,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -20526,7 +20532,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>196</v>
@@ -20535,7 +20541,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>162</v>
@@ -20626,40 +20632,40 @@
         <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>364</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -21036,7 +21042,7 @@
         <v>145</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -21053,7 +21059,7 @@
         <v>145</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -21070,7 +21076,7 @@
         <v>145</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -30877,8 +30883,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31042,7 +31049,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -31085,7 +31092,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="2">
@@ -31140,7 +31147,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
@@ -31197,7 +31204,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F6" s="7">
         <v>0</v>
@@ -31253,7 +31260,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F7" s="7">
         <v>0</v>
@@ -31309,7 +31316,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F8" s="7">
         <v>0</v>
@@ -31368,7 +31375,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F9" s="7">
         <v>0</v>
@@ -31424,7 +31431,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F10" s="7">
         <v>0</v>
@@ -31704,7 +31711,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F15" s="7">
         <v>0</v>
@@ -31760,7 +31767,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F16" s="7">
         <v>0</v>
@@ -31816,7 +31823,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F17" s="7">
         <v>0</v>
@@ -31828,7 +31835,7 @@
         <v>236</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Q17" s="7">
         <v>8.5</v>
@@ -31854,7 +31861,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>177</v>
@@ -31890,7 +31897,7 @@
         <v>11</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="T18" s="7">
         <v>1</v>
@@ -31907,7 +31914,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>177</v>
@@ -31916,7 +31923,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F19" s="7">
         <v>0</v>
@@ -31960,7 +31967,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>177</v>
@@ -31969,7 +31976,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F20" s="7">
         <v>0</v>
@@ -32013,7 +32020,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>177</v>
@@ -32022,7 +32029,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F21" s="7">
         <v>0</v>
@@ -32071,7 +32078,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>177</v>
@@ -32080,7 +32087,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F22" s="7">
         <v>0</v>
@@ -32097,7 +32104,7 @@
         <v>236</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>288</v>
+        <v>457</v>
       </c>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
@@ -32108,10 +32115,10 @@
         <v>11</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="T22" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="U22" s="7">
         <v>2</v>
@@ -32125,7 +32132,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>177</v>
@@ -32166,7 +32173,7 @@
         <v>11</v>
       </c>
       <c r="S23" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="T23" s="7">
         <v>8</v>
@@ -32183,7 +32190,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H24" s="7"/>
       <c r="M24" s="7"/>
@@ -32193,7 +32200,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>177</v>
@@ -32251,7 +32258,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>177</v>
@@ -32309,7 +32316,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>177</v>
@@ -32367,7 +32374,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>177</v>
@@ -32425,7 +32432,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>177</v>
@@ -32483,7 +32490,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>177</v>
@@ -32541,7 +32548,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>177</v>
@@ -32594,7 +32601,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>177</v>
@@ -32647,7 +32654,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>177</v>
@@ -32700,7 +32707,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>177</v>
@@ -32753,7 +32760,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>177</v>
@@ -32806,7 +32813,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>177</v>
@@ -32842,7 +32849,7 @@
         <v>11</v>
       </c>
       <c r="S36" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="T36" s="7">
         <v>4</v>
@@ -32859,7 +32866,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>177</v>
@@ -32917,7 +32924,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>177</v>
@@ -32972,7 +32979,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>177</v>
@@ -33025,7 +33032,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>177</v>
@@ -33034,7 +33041,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F40" s="7">
         <v>0</v>
@@ -33078,7 +33085,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>177</v>
@@ -33087,7 +33094,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F41" s="7">
         <v>0</v>
@@ -33131,7 +33138,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>177</v>
@@ -33140,7 +33147,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F42" s="7">
         <v>0</v>
@@ -33184,7 +33191,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>177</v>
@@ -33193,7 +33200,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F43" s="7">
         <v>0</v>
@@ -33237,7 +33244,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>177</v>
@@ -33246,7 +33253,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F44" s="7">
         <v>0</v>
@@ -33290,7 +33297,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>177</v>
@@ -33299,7 +33306,7 @@
         <v>8</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F45" s="7">
         <v>0</v>
@@ -33343,7 +33350,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>177</v>
@@ -33352,7 +33359,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F46" s="7">
         <v>0</v>
@@ -33396,7 +33403,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>177</v>
@@ -33405,7 +33412,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F47" s="7">
         <v>0</v>
@@ -33449,7 +33456,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>177</v>
@@ -33458,7 +33465,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F48" s="7">
         <v>0</v>
@@ -33502,7 +33509,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>177</v>
@@ -33511,7 +33518,7 @@
         <v>6</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F49" s="7">
         <v>0</v>
@@ -33555,19 +33562,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>338</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>458</v>
+        <v>337</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>460</v>
       </c>
       <c r="D50" s="19">
         <v>1</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>162</v>
+        <v>366</v>
       </c>
       <c r="F50" s="19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G50" s="19" t="s">
         <v>22</v>
@@ -33590,17 +33597,17 @@
       <c r="R50" s="19">
         <v>11</v>
       </c>
-      <c r="S50" s="19" t="s">
-        <v>380</v>
+      <c r="S50" s="19">
+        <v>24</v>
       </c>
       <c r="T50" s="19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U50" s="19">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="V50" s="19">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33608,16 +33615,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="C51" s="19" t="s">
         <v>383</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>384</v>
       </c>
       <c r="D51" s="19">
         <v>1</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F51" s="19">
         <v>0</v>
@@ -33629,7 +33636,7 @@
         <v>236</v>
       </c>
       <c r="N51" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O51" s="19">
         <v>0.5</v>
@@ -33653,7 +33660,7 @@
         <v>1</v>
       </c>
       <c r="V51" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="52" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33661,16 +33668,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D52" s="19">
         <v>1</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F52" s="19">
         <v>0</v>
@@ -33682,7 +33689,7 @@
         <v>236</v>
       </c>
       <c r="N52" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O52" s="19">
         <v>0.5</v>
@@ -33706,7 +33713,7 @@
         <v>1</v>
       </c>
       <c r="V52" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="53" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33714,16 +33721,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D53" s="19">
         <v>1</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F53" s="19">
         <v>0</v>
@@ -33735,7 +33742,7 @@
         <v>236</v>
       </c>
       <c r="N53" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O53" s="19">
         <v>0.5</v>
@@ -33759,7 +33766,7 @@
         <v>1</v>
       </c>
       <c r="V53" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="54" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33767,16 +33774,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D54" s="19">
         <v>1</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F54" s="19">
         <v>0</v>
@@ -33788,7 +33795,7 @@
         <v>236</v>
       </c>
       <c r="N54" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O54" s="19">
         <v>0.5</v>
@@ -33812,7 +33819,7 @@
         <v>1</v>
       </c>
       <c r="V54" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="55" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33820,16 +33827,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D55" s="19">
         <v>1</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F55" s="19">
         <v>0</v>
@@ -33841,7 +33848,7 @@
         <v>236</v>
       </c>
       <c r="N55" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O55" s="19">
         <v>0.5</v>
@@ -33865,7 +33872,7 @@
         <v>1</v>
       </c>
       <c r="V55" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="56" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33873,16 +33880,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D56" s="19">
         <v>1</v>
       </c>
       <c r="E56" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F56" s="19">
         <v>0</v>
@@ -33894,7 +33901,7 @@
         <v>236</v>
       </c>
       <c r="N56" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O56" s="19">
         <v>0.5</v>
@@ -33918,7 +33925,7 @@
         <v>1</v>
       </c>
       <c r="V56" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="57" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33926,16 +33933,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D57" s="19">
         <v>1</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F57" s="19">
         <v>0</v>
@@ -33947,7 +33954,7 @@
         <v>236</v>
       </c>
       <c r="N57" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O57" s="19">
         <v>0.5</v>
@@ -33971,7 +33978,7 @@
         <v>1</v>
       </c>
       <c r="V57" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="58" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -33979,16 +33986,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D58" s="19">
         <v>1</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F58" s="19">
         <v>0</v>
@@ -34000,7 +34007,7 @@
         <v>236</v>
       </c>
       <c r="N58" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O58" s="19">
         <v>0.5</v>
@@ -34024,7 +34031,7 @@
         <v>1</v>
       </c>
       <c r="V58" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="59" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -34032,16 +34039,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="C59" s="19" t="s">
         <v>394</v>
-      </c>
-      <c r="C59" s="19" t="s">
-        <v>395</v>
       </c>
       <c r="D59" s="19">
         <v>1</v>
       </c>
       <c r="E59" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F59" s="19">
         <v>0</v>
@@ -34053,7 +34060,7 @@
         <v>236</v>
       </c>
       <c r="N59" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O59" s="19">
         <v>0.5</v>
@@ -34085,16 +34092,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D60" s="19">
         <v>1</v>
       </c>
       <c r="E60" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F60" s="19">
         <v>0</v>
@@ -34106,7 +34113,7 @@
         <v>236</v>
       </c>
       <c r="N60" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O60" s="19">
         <v>0.5</v>
@@ -34130,7 +34137,7 @@
         <v>1</v>
       </c>
       <c r="V60" s="19" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="61" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -34138,16 +34145,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D61" s="19">
         <v>1</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F61" s="19">
         <v>0</v>
@@ -34159,7 +34166,7 @@
         <v>236</v>
       </c>
       <c r="N61" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O61" s="19">
         <v>0.5</v>
@@ -34183,7 +34190,7 @@
         <v>1</v>
       </c>
       <c r="V61" s="19" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="62" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -34191,16 +34198,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="C62" s="19" t="s">
         <v>399</v>
-      </c>
-      <c r="C62" s="19" t="s">
-        <v>400</v>
       </c>
       <c r="D62" s="19">
         <v>1</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F62" s="19">
         <v>0</v>
@@ -34212,7 +34219,7 @@
         <v>236</v>
       </c>
       <c r="N62" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O62" s="19">
         <v>0.5</v>
@@ -34244,16 +34251,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="C63" s="19" t="s">
         <v>401</v>
-      </c>
-      <c r="C63" s="19" t="s">
-        <v>402</v>
       </c>
       <c r="D63" s="19">
         <v>1</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F63" s="19">
         <v>0</v>
@@ -34265,7 +34272,7 @@
         <v>236</v>
       </c>
       <c r="N63" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O63" s="19">
         <v>0.5</v>
@@ -34289,7 +34296,7 @@
         <v>1</v>
       </c>
       <c r="V63" s="19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="64" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -34297,10 +34304,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="C64" s="19" t="s">
         <v>404</v>
-      </c>
-      <c r="C64" s="19" t="s">
-        <v>405</v>
       </c>
       <c r="D64" s="19">
         <v>1</v>
@@ -34318,7 +34325,7 @@
         <v>236</v>
       </c>
       <c r="N64" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O64" s="19">
         <v>0.5</v>
@@ -34342,7 +34349,7 @@
         <v>1</v>
       </c>
       <c r="V64" s="19" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="65" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -34350,10 +34357,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D65" s="19">
         <v>1</v>
@@ -34371,7 +34378,7 @@
         <v>236</v>
       </c>
       <c r="N65" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O65" s="19">
         <v>0.5</v>
@@ -34395,7 +34402,7 @@
         <v>1</v>
       </c>
       <c r="V65" s="19" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="66" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -34403,10 +34410,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="C66" s="19" t="s">
         <v>408</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>409</v>
       </c>
       <c r="D66" s="19">
         <v>1</v>
@@ -34424,7 +34431,7 @@
         <v>236</v>
       </c>
       <c r="N66" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O66" s="19">
         <v>0.5</v>
@@ -34448,7 +34455,7 @@
         <v>1</v>
       </c>
       <c r="V66" s="19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="67" spans="1:22" s="19" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -34456,10 +34463,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="19" t="s">
+        <v>410</v>
+      </c>
+      <c r="C67" s="19" t="s">
         <v>411</v>
-      </c>
-      <c r="C67" s="19" t="s">
-        <v>412</v>
       </c>
       <c r="D67" s="19">
         <v>1</v>
@@ -34515,10 +34522,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D68" s="19">
         <v>1</v>
@@ -34574,10 +34581,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D69" s="19">
         <v>1</v>
@@ -34633,10 +34640,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="19" t="s">
+        <v>414</v>
+      </c>
+      <c r="C70" s="19" t="s">
         <v>415</v>
-      </c>
-      <c r="C70" s="19" t="s">
-        <v>416</v>
       </c>
       <c r="D70" s="19">
         <v>1</v>
@@ -34654,7 +34661,7 @@
         <v>236</v>
       </c>
       <c r="N70" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O70" s="19">
         <v>0.5</v>
@@ -34686,10 +34693,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="19" t="s">
+        <v>416</v>
+      </c>
+      <c r="C71" s="19" t="s">
         <v>417</v>
-      </c>
-      <c r="C71" s="19" t="s">
-        <v>418</v>
       </c>
       <c r="D71" s="19">
         <v>1</v>
@@ -34728,7 +34735,7 @@
         <v>11</v>
       </c>
       <c r="S71" s="19" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="T71" s="19">
         <v>1</v>
@@ -34745,16 +34752,16 @@
         <v>71</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D72" s="19">
         <v>1</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F72" s="19">
         <v>0</v>
@@ -34766,7 +34773,7 @@
         <v>236</v>
       </c>
       <c r="N72" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O72" s="19">
         <v>0.5</v>
@@ -34795,16 +34802,16 @@
         <v>72</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D73" s="19">
         <v>1</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F73" s="19">
         <v>0</v>
@@ -34854,16 +34861,16 @@
         <v>73</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C74" s="19" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D74" s="19">
         <v>1</v>
       </c>
       <c r="E74" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F74" s="19">
         <v>0</v>
@@ -34896,7 +34903,7 @@
         <v>20</v>
       </c>
       <c r="S74" s="19" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="T74" s="19">
         <v>1</v>
@@ -34913,7 +34920,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C75" s="18"/>
       <c r="D75" s="19">

</xml_diff>

<commit_message>
Refined test code for compliance reports SetII and SetIII
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxiang\dev\surveyor-qa\selenium-wd\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="11" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -650,7 +650,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="465">
   <si>
     <t>Enabled</t>
   </si>
@@ -2043,11 +2043,14 @@
   <si>
     <t>32,26,27,30</t>
   </si>
+  <si>
+    <t>Keep this empty line for some tests</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -2661,7 +2664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -2744,7 +2747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
@@ -15746,7 +15749,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AA800"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -19178,7 +19181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -19309,10 +19312,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19322,6 +19325,7 @@
     <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -19596,7 +19600,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -19613,7 +19617,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -19630,7 +19634,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -19647,7 +19651,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -19664,7 +19668,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -19681,7 +19685,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -19696,6 +19700,14 @@
       </c>
       <c r="E22" s="12" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="22">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s">
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -36860,7 +36872,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changed test cases according to review comments
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -625,7 +625,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="477">
   <si>
     <t>Enabled</t>
   </si>
@@ -2054,6 +2054,9 @@
   <si>
     <t>TC1532</t>
   </si>
+  <si>
+    <t>All Except LISA and GAP</t>
+  </si>
 </sst>
 </file>
 
@@ -15682,8 +15685,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AA800"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17966,20 +17969,48 @@
       </c>
     </row>
     <row r="43" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
+      <c r="A43" s="22">
+        <v>42</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D43" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E43" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J43" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K43" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="L43" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M43" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="N43" s="22" t="s">
+        <v>476</v>
+      </c>
       <c r="O43" s="22"/>
       <c r="P43" s="22"/>
       <c r="Q43" s="22"/>
@@ -36805,8 +36836,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView tabSelected="1" topLeftCell="L62" workbookViewId="0">
+      <selection activeCell="S85" sqref="S85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41843,13 +41874,13 @@
         <v>11</v>
       </c>
       <c r="S85" s="22">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="T85" s="22">
         <v>1</v>
       </c>
       <c r="U85" s="22">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="V85" s="22" t="s">
         <v>474</v>
@@ -41914,7 +41945,7 @@
         <v>4</v>
       </c>
       <c r="U86" s="19">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="V86" s="19">
         <v>4</v>

</xml_diff>

<commit_message>
fixes for pagetest6 + new baseline shape files for data provider page action tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" tabRatio="799" firstSheet="10" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" tabRatio="799" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -625,7 +625,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="475">
   <si>
     <t>Enabled</t>
   </si>
@@ -1521,15 +1521,6 @@
     <t>TC526</t>
   </si>
   <si>
-    <t>TC678</t>
-  </si>
-  <si>
-    <t>TC680</t>
-  </si>
-  <si>
-    <t>TC681</t>
-  </si>
-  <si>
     <t>ONLY LISA TRUE</t>
   </si>
   <si>
@@ -2020,6 +2011,45 @@
   </si>
   <si>
     <t>Keep this empty line for test cases</t>
+  </si>
+  <si>
+    <t>TC678-0</t>
+  </si>
+  <si>
+    <t>TC678-1</t>
+  </si>
+  <si>
+    <t>TC678-2</t>
+  </si>
+  <si>
+    <t>TC678-3</t>
+  </si>
+  <si>
+    <t>TC678-4</t>
+  </si>
+  <si>
+    <t>TC678-5</t>
+  </si>
+  <si>
+    <t>TC680-0</t>
+  </si>
+  <si>
+    <t>TC680-1</t>
+  </si>
+  <si>
+    <t>TC680-2</t>
+  </si>
+  <si>
+    <t>TC680-3</t>
+  </si>
+  <si>
+    <t>TC680-4</t>
+  </si>
+  <si>
+    <t>TC681-0</t>
+  </si>
+  <si>
+    <t>TC681-1</t>
   </si>
 </sst>
 </file>
@@ -2642,19 +2672,19 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2662,10 +2692,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D2" s="9">
         <v>1</v>
@@ -2674,7 +2704,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2682,10 +2712,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D3" s="7">
         <v>2</v>
@@ -2694,7 +2724,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -2757,7 +2787,7 @@
         <v>269</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -2873,7 +2903,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="H6" s="22" t="b">
         <v>0</v>
@@ -2893,7 +2923,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="H7" s="22" t="b">
         <v>0</v>
@@ -2913,7 +2943,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="H8" s="22" t="b">
         <v>0</v>
@@ -2933,7 +2963,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="H9" s="22" t="b">
         <v>0</v>
@@ -2953,7 +2983,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="H10" s="22" t="b">
         <v>0</v>
@@ -2973,7 +3003,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="H11" s="22" t="b">
         <v>0</v>
@@ -2993,7 +3023,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="H12" s="22" t="b">
         <v>0</v>
@@ -3013,7 +3043,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="H13" s="22" t="b">
         <v>0</v>
@@ -3033,7 +3063,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="H14" s="22" t="b">
         <v>0</v>
@@ -3283,7 +3313,7 @@
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
@@ -3308,7 +3338,7 @@
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
@@ -3331,7 +3361,7 @@
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
@@ -3458,7 +3488,7 @@
         <v>33</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="I34" s="22">
         <v>1</v>
@@ -15635,8 +15665,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AA800"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15747,7 +15777,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C3" s="29" t="b">
         <v>1</v>
@@ -16133,7 +16163,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C10" s="22" t="b">
         <v>0</v>
@@ -16247,7 +16277,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C12" s="22" t="b">
         <v>1</v>
@@ -16304,7 +16334,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C13" s="22" t="b">
         <v>1</v>
@@ -16340,7 +16370,7 @@
         <v>83</v>
       </c>
       <c r="N13" s="22" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="O13" s="22"/>
       <c r="P13" s="22"/>
@@ -16361,7 +16391,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C14" s="22" t="b">
         <v>1</v>
@@ -16418,7 +16448,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C15" s="22" t="b">
         <v>0</v>
@@ -16475,7 +16505,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C16" s="22" t="b">
         <v>1</v>
@@ -16532,7 +16562,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C17" s="22" t="b">
         <v>1</v>
@@ -16568,7 +16598,7 @@
         <v>84</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="O17" s="22"/>
       <c r="P17" s="22"/>
@@ -16589,7 +16619,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C18" s="22" t="b">
         <v>1</v>
@@ -16625,7 +16655,7 @@
         <v>85</v>
       </c>
       <c r="N18" s="22" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="O18" s="22"/>
       <c r="P18" s="22"/>
@@ -16646,7 +16676,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C19" s="22" t="b">
         <v>1</v>
@@ -16703,7 +16733,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C20" s="22" t="b">
         <v>1</v>
@@ -16760,7 +16790,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C21" s="22" t="b">
         <v>1</v>
@@ -16817,7 +16847,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C22" s="22" t="b">
         <v>0</v>
@@ -16874,7 +16904,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C23" s="22" t="b">
         <v>0</v>
@@ -16931,7 +16961,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C24" s="22" t="b">
         <v>0</v>
@@ -16988,7 +17018,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C25" s="22" t="b">
         <v>1</v>
@@ -17024,7 +17054,7 @@
         <v>83</v>
       </c>
       <c r="N25" s="22" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="O25" s="22"/>
       <c r="P25" s="22"/>
@@ -17045,7 +17075,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C26" s="22" t="b">
         <v>0</v>
@@ -17081,7 +17111,7 @@
         <v>83</v>
       </c>
       <c r="N26" s="22" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="O26" s="22"/>
       <c r="P26" s="22"/>
@@ -17102,7 +17132,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C27" s="22" t="b">
         <v>0</v>
@@ -17138,7 +17168,7 @@
         <v>83</v>
       </c>
       <c r="N27" s="22" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="O27" s="22"/>
       <c r="P27" s="22"/>
@@ -17159,7 +17189,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C28" s="22" t="b">
         <v>0</v>
@@ -17195,7 +17225,7 @@
         <v>83</v>
       </c>
       <c r="N28" s="22" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="O28" s="22"/>
       <c r="P28" s="22"/>
@@ -17216,7 +17246,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C29" s="22" t="b">
         <v>0</v>
@@ -17252,7 +17282,7 @@
         <v>83</v>
       </c>
       <c r="N29" s="22" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="O29" s="22"/>
       <c r="P29" s="22"/>
@@ -17273,7 +17303,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C30" s="22" t="b">
         <v>1</v>
@@ -17309,7 +17339,7 @@
         <v>83</v>
       </c>
       <c r="N30" s="22" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="O30" s="22"/>
       <c r="P30" s="22"/>
@@ -17330,7 +17360,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C31" s="22" t="b">
         <v>1</v>
@@ -17366,7 +17396,7 @@
         <v>84</v>
       </c>
       <c r="N31" s="22" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="O31" s="22"/>
       <c r="P31" s="22"/>
@@ -17387,7 +17417,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C32" s="22" t="b">
         <v>1</v>
@@ -17423,7 +17453,7 @@
         <v>84</v>
       </c>
       <c r="N32" s="22" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="O32" s="22"/>
       <c r="P32" s="22"/>
@@ -17444,7 +17474,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C33" s="22" t="b">
         <v>1</v>
@@ -17480,7 +17510,7 @@
         <v>83</v>
       </c>
       <c r="N33" s="22" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="O33" s="22"/>
       <c r="P33" s="22"/>
@@ -17501,7 +17531,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C34" s="22" t="b">
         <v>1</v>
@@ -17537,7 +17567,7 @@
         <v>83</v>
       </c>
       <c r="N34" s="22" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="O34" s="22"/>
       <c r="P34" s="22"/>
@@ -17558,7 +17588,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C35" s="22" t="b">
         <v>0</v>
@@ -17594,7 +17624,7 @@
         <v>83</v>
       </c>
       <c r="N35" s="22" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="O35" s="22"/>
       <c r="P35" s="22"/>
@@ -17615,7 +17645,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C36" s="22" t="b">
         <v>0</v>
@@ -17651,7 +17681,7 @@
         <v>83</v>
       </c>
       <c r="N36" s="22" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="37" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17659,7 +17689,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C37" s="22" t="b">
         <v>1</v>
@@ -17695,7 +17725,7 @@
         <v>84</v>
       </c>
       <c r="N37" s="22" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="38" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17703,7 +17733,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C38" s="22" t="b">
         <v>0</v>
@@ -17739,7 +17769,7 @@
         <v>83</v>
       </c>
       <c r="N38" s="22" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="39" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17783,7 +17813,7 @@
         <v>84</v>
       </c>
       <c r="N39" s="22" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="40" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17827,7 +17857,7 @@
         <v>83</v>
       </c>
       <c r="N40" s="22" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="41" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17835,7 +17865,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C41" s="22" t="b">
         <v>0</v>
@@ -17871,7 +17901,7 @@
         <v>83</v>
       </c>
       <c r="N41" s="22" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="42" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -17879,7 +17909,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C42" s="22" t="b">
         <v>1</v>
@@ -19068,7 +19098,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19592,7 +19622,7 @@
         <v>22</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -20029,7 +20059,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:28" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -20055,7 +20085,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
@@ -20666,7 +20696,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -20679,22 +20709,22 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -20904,7 +20934,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B3" t="s">
         <v>48</v>
@@ -20921,7 +20951,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -20938,7 +20968,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C5" t="s">
         <v>226</v>
@@ -20949,7 +20979,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C6" t="s">
         <v>227</v>
@@ -20988,13 +21018,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -21002,7 +21032,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
@@ -21016,7 +21046,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C3" s="7">
         <v>1</v>
@@ -21107,7 +21137,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>160</v>
@@ -21142,7 +21172,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>164</v>
@@ -21178,7 +21208,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>165</v>
@@ -21214,7 +21244,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>166</v>
@@ -21282,7 +21312,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>167</v>
@@ -21318,7 +21348,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -21350,7 +21380,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -21382,7 +21412,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -21414,7 +21444,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>167</v>
@@ -21441,7 +21471,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>195</v>
@@ -21470,7 +21500,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>195</v>
@@ -21479,7 +21509,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -21502,7 +21532,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>195</v>
@@ -21511,7 +21541,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>162</v>
@@ -21602,40 +21632,40 @@
         <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>354</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -22012,7 +22042,7 @@
         <v>145</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -22029,7 +22059,7 @@
         <v>145</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -22046,7 +22076,7 @@
         <v>145</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -22558,13 +22588,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E23" s="29" t="s">
         <v>26</v>
@@ -22598,10 +22628,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D24" s="29" t="s">
         <v>132</v>
@@ -22638,10 +22668,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D25" s="29" t="s">
         <v>27</v>
@@ -22678,10 +22708,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D26" s="29" t="s">
         <v>268</v>
@@ -22718,10 +22748,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>268</v>
@@ -22758,13 +22788,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>26</v>
@@ -22798,10 +22828,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D29" s="29" t="s">
         <v>132</v>
@@ -22838,13 +22868,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="E30" s="29" t="s">
         <v>26</v>
@@ -22878,10 +22908,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D31" s="29" t="s">
         <v>27</v>
@@ -31214,7 +31244,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C43" s="22" t="s">
         <v>19</v>
@@ -31234,7 +31264,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C44" s="22" t="s">
         <v>19</v>
@@ -31254,7 +31284,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C45" s="22" t="s">
         <v>19</v>
@@ -31274,7 +31304,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>19</v>
@@ -31297,7 +31327,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>19</v>
@@ -31340,7 +31370,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>19</v>
@@ -31360,7 +31390,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C50" s="22" t="s">
         <v>19</v>
@@ -31380,7 +31410,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C51" s="22" t="s">
         <v>19</v>
@@ -36758,8 +36788,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36923,7 +36953,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F3" s="22">
         <v>0</v>
@@ -36978,7 +37008,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
@@ -37041,7 +37071,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F5" s="22">
         <v>0</v>
@@ -37106,7 +37136,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F6" s="22">
         <v>0</v>
@@ -37171,7 +37201,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F7" s="22">
         <v>0</v>
@@ -37236,7 +37266,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F8" s="22">
         <v>0</v>
@@ -37303,7 +37333,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F9" s="22">
         <v>0</v>
@@ -37368,7 +37398,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F10" s="22">
         <v>0</v>
@@ -37570,7 +37600,7 @@
         <v>11</v>
       </c>
       <c r="S13" s="22" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="T13" s="22">
         <v>7</v>
@@ -37649,7 +37679,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F15" s="22">
         <v>0</v>
@@ -37714,7 +37744,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F16" s="22">
         <v>0</v>
@@ -37779,7 +37809,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F17" s="22">
         <v>0</v>
@@ -37870,7 +37900,7 @@
         <v>11</v>
       </c>
       <c r="S18" s="22" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="T18" s="22">
         <v>1</v>
@@ -37901,7 +37931,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F19" s="22">
         <v>0</v>
@@ -37964,7 +37994,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F20" s="22">
         <v>0</v>
@@ -38027,7 +38057,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F21" s="22">
         <v>0</v>
@@ -38090,7 +38120,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F22" s="22">
         <v>0</v>
@@ -38107,7 +38137,7 @@
         <v>226</v>
       </c>
       <c r="N22" s="22" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="O22" s="22"/>
       <c r="P22" s="22"/>
@@ -38236,7 +38266,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>298</v>
+        <v>462</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>177</v>
@@ -38299,7 +38329,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>298</v>
+        <v>463</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>177</v>
@@ -38362,7 +38392,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>298</v>
+        <v>464</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>177</v>
@@ -38425,7 +38455,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>298</v>
+        <v>465</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>177</v>
@@ -38488,7 +38518,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>298</v>
+        <v>466</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>177</v>
@@ -38551,7 +38581,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>298</v>
+        <v>467</v>
       </c>
       <c r="C30" s="22" t="s">
         <v>177</v>
@@ -38614,7 +38644,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>299</v>
+        <v>468</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>177</v>
@@ -38677,7 +38707,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>299</v>
+        <v>469</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>177</v>
@@ -38740,7 +38770,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>299</v>
+        <v>470</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>177</v>
@@ -38803,7 +38833,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>299</v>
+        <v>471</v>
       </c>
       <c r="C34" s="22" t="s">
         <v>177</v>
@@ -38847,7 +38877,7 @@
         <v>27</v>
       </c>
       <c r="T34" s="22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U34" s="22">
         <v>2</v>
@@ -38866,7 +38896,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>299</v>
+        <v>472</v>
       </c>
       <c r="C35" s="22" t="s">
         <v>177</v>
@@ -38929,7 +38959,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>300</v>
+        <v>473</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>177</v>
@@ -38970,7 +39000,7 @@
         <v>11</v>
       </c>
       <c r="S36" s="22" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="T36" s="22">
         <v>4</v>
@@ -38992,7 +39022,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>300</v>
+        <v>474</v>
       </c>
       <c r="C37" s="22" t="s">
         <v>177</v>
@@ -39055,7 +39085,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C38" s="22" t="s">
         <v>177</v>
@@ -39118,7 +39148,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C39" s="22" t="s">
         <v>177</v>
@@ -39181,7 +39211,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C40" s="22" t="s">
         <v>177</v>
@@ -39190,7 +39220,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F40" s="22">
         <v>0</v>
@@ -39244,7 +39274,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C41" s="22" t="s">
         <v>177</v>
@@ -39253,7 +39283,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F41" s="22">
         <v>0</v>
@@ -39307,7 +39337,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C42" s="22" t="s">
         <v>177</v>
@@ -39316,7 +39346,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F42" s="22">
         <v>0</v>
@@ -39370,7 +39400,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C43" s="22" t="s">
         <v>177</v>
@@ -39379,7 +39409,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F43" s="22">
         <v>0</v>
@@ -39433,7 +39463,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C44" s="22" t="s">
         <v>177</v>
@@ -39442,7 +39472,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F44" s="22">
         <v>0</v>
@@ -39496,7 +39526,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C45" s="22" t="s">
         <v>177</v>
@@ -39505,7 +39535,7 @@
         <v>8</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F45" s="22">
         <v>0</v>
@@ -39559,7 +39589,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C46" s="22" t="s">
         <v>177</v>
@@ -39568,7 +39598,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F46" s="22">
         <v>0</v>
@@ -39622,7 +39652,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C47" s="22" t="s">
         <v>177</v>
@@ -39631,7 +39661,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F47" s="22">
         <v>0</v>
@@ -39685,7 +39715,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>177</v>
@@ -39694,7 +39724,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F48" s="22">
         <v>0</v>
@@ -39748,7 +39778,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>177</v>
@@ -39757,7 +39787,7 @@
         <v>6</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F49" s="22">
         <v>0</v>
@@ -39811,16 +39841,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D50" s="22">
         <v>1</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F50" s="22">
         <v>0</v>
@@ -39867,7 +39897,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C51" s="22" t="s">
         <v>177</v>
@@ -39876,7 +39906,7 @@
         <v>1</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F51" s="22">
         <v>0</v>
@@ -39888,7 +39918,7 @@
         <v>226</v>
       </c>
       <c r="N51" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O51" s="22">
         <v>0.5</v>
@@ -39912,7 +39942,7 @@
         <v>1</v>
       </c>
       <c r="V51" s="22" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="52" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -39920,7 +39950,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C52" s="22" t="s">
         <v>177</v>
@@ -39929,7 +39959,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F52" s="22">
         <v>0</v>
@@ -39941,7 +39971,7 @@
         <v>226</v>
       </c>
       <c r="N52" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O52" s="22">
         <v>0.5</v>
@@ -39965,7 +39995,7 @@
         <v>1</v>
       </c>
       <c r="V52" s="22" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="53" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -39973,7 +40003,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C53" s="22" t="s">
         <v>177</v>
@@ -39982,7 +40012,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F53" s="22">
         <v>0</v>
@@ -39994,7 +40024,7 @@
         <v>226</v>
       </c>
       <c r="N53" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O53" s="22">
         <v>0.5</v>
@@ -40018,7 +40048,7 @@
         <v>1</v>
       </c>
       <c r="V53" s="22" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="54" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40026,7 +40056,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C54" s="22" t="s">
         <v>177</v>
@@ -40035,7 +40065,7 @@
         <v>1</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F54" s="22">
         <v>0</v>
@@ -40047,7 +40077,7 @@
         <v>226</v>
       </c>
       <c r="N54" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O54" s="22">
         <v>0.5</v>
@@ -40071,7 +40101,7 @@
         <v>1</v>
       </c>
       <c r="V54" s="22" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="55" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40079,7 +40109,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C55" s="22" t="s">
         <v>177</v>
@@ -40088,7 +40118,7 @@
         <v>1</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F55" s="22">
         <v>0</v>
@@ -40100,7 +40130,7 @@
         <v>226</v>
       </c>
       <c r="N55" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O55" s="22">
         <v>0.5</v>
@@ -40124,7 +40154,7 @@
         <v>1</v>
       </c>
       <c r="V55" s="22" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="56" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40132,7 +40162,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C56" s="22" t="s">
         <v>177</v>
@@ -40141,7 +40171,7 @@
         <v>1</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F56" s="22">
         <v>0</v>
@@ -40153,7 +40183,7 @@
         <v>226</v>
       </c>
       <c r="N56" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O56" s="22">
         <v>0.5</v>
@@ -40177,7 +40207,7 @@
         <v>1</v>
       </c>
       <c r="V56" s="22" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="57" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40185,7 +40215,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C57" s="22" t="s">
         <v>177</v>
@@ -40194,7 +40224,7 @@
         <v>1</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F57" s="22">
         <v>0</v>
@@ -40206,7 +40236,7 @@
         <v>226</v>
       </c>
       <c r="N57" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O57" s="22">
         <v>0.5</v>
@@ -40230,7 +40260,7 @@
         <v>1</v>
       </c>
       <c r="V57" s="22" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="58" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40238,7 +40268,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C58" s="22" t="s">
         <v>177</v>
@@ -40247,7 +40277,7 @@
         <v>1</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F58" s="22">
         <v>0</v>
@@ -40259,7 +40289,7 @@
         <v>226</v>
       </c>
       <c r="N58" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O58" s="22">
         <v>0.5</v>
@@ -40283,7 +40313,7 @@
         <v>1</v>
       </c>
       <c r="V58" s="22" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="59" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40291,7 +40321,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C59" s="22" t="s">
         <v>177</v>
@@ -40300,7 +40330,7 @@
         <v>1</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F59" s="22">
         <v>0</v>
@@ -40312,7 +40342,7 @@
         <v>226</v>
       </c>
       <c r="N59" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O59" s="22">
         <v>0.5</v>
@@ -40344,7 +40374,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C60" s="22" t="s">
         <v>177</v>
@@ -40353,7 +40383,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F60" s="22">
         <v>0</v>
@@ -40365,7 +40395,7 @@
         <v>226</v>
       </c>
       <c r="N60" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O60" s="22">
         <v>0.5</v>
@@ -40389,7 +40419,7 @@
         <v>1</v>
       </c>
       <c r="V60" s="22" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="61" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40397,7 +40427,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C61" s="22" t="s">
         <v>177</v>
@@ -40406,7 +40436,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F61" s="22">
         <v>0</v>
@@ -40418,7 +40448,7 @@
         <v>226</v>
       </c>
       <c r="N61" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O61" s="22">
         <v>0.5</v>
@@ -40442,7 +40472,7 @@
         <v>1</v>
       </c>
       <c r="V61" s="22" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="62" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40450,7 +40480,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C62" s="22" t="s">
         <v>177</v>
@@ -40459,7 +40489,7 @@
         <v>1</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F62" s="22">
         <v>0</v>
@@ -40471,7 +40501,7 @@
         <v>226</v>
       </c>
       <c r="N62" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O62" s="22">
         <v>0.5</v>
@@ -40503,7 +40533,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C63" s="22" t="s">
         <v>177</v>
@@ -40512,7 +40542,7 @@
         <v>1</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F63" s="22">
         <v>0</v>
@@ -40524,7 +40554,7 @@
         <v>226</v>
       </c>
       <c r="N63" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O63" s="22">
         <v>0.5</v>
@@ -40548,7 +40578,7 @@
         <v>1</v>
       </c>
       <c r="V63" s="22" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="64" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40556,7 +40586,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C64" s="22" t="s">
         <v>177</v>
@@ -40577,7 +40607,7 @@
         <v>226</v>
       </c>
       <c r="N64" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O64" s="22">
         <v>0.5</v>
@@ -40601,7 +40631,7 @@
         <v>1</v>
       </c>
       <c r="V64" s="22" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="65" spans="1:22" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40609,7 +40639,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C65" s="22" t="s">
         <v>177</v>
@@ -40630,7 +40660,7 @@
         <v>226</v>
       </c>
       <c r="N65" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O65" s="22">
         <v>0.5</v>
@@ -40654,7 +40684,7 @@
         <v>1</v>
       </c>
       <c r="V65" s="22" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="66" spans="1:22" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40662,7 +40692,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C66" s="22" t="s">
         <v>177</v>
@@ -40683,7 +40713,7 @@
         <v>226</v>
       </c>
       <c r="N66" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O66" s="22">
         <v>0.5</v>
@@ -40707,7 +40737,7 @@
         <v>1</v>
       </c>
       <c r="V66" s="22" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="67" spans="1:22" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40715,7 +40745,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C67" s="22" t="s">
         <v>177</v>
@@ -40766,7 +40796,7 @@
         <v>7</v>
       </c>
       <c r="V67" s="22" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="68" spans="1:22" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40774,7 +40804,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C68" s="22" t="s">
         <v>177</v>
@@ -40833,7 +40863,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C69" s="22" t="s">
         <v>177</v>
@@ -40892,7 +40922,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C70" s="22" t="s">
         <v>177</v>
@@ -40913,7 +40943,7 @@
         <v>226</v>
       </c>
       <c r="N70" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O70" s="22">
         <v>0.5</v>
@@ -40945,7 +40975,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C71" s="22" t="s">
         <v>177</v>
@@ -40987,7 +41017,7 @@
         <v>11</v>
       </c>
       <c r="S71" s="22" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="T71" s="22">
         <v>1</v>
@@ -41004,7 +41034,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C72" s="22" t="s">
         <v>177</v>
@@ -41013,7 +41043,7 @@
         <v>1</v>
       </c>
       <c r="E72" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F72" s="22">
         <v>0</v>
@@ -41025,7 +41055,7 @@
         <v>226</v>
       </c>
       <c r="N72" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O72" s="22">
         <v>0.5</v>
@@ -41049,7 +41079,7 @@
         <v>1</v>
       </c>
       <c r="V72" s="22" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="73" spans="1:22" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -41057,7 +41087,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C73" s="22" t="s">
         <v>177</v>
@@ -41066,7 +41096,7 @@
         <v>1</v>
       </c>
       <c r="E73" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F73" s="22">
         <v>0</v>
@@ -41116,7 +41146,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C74" s="22" t="s">
         <v>177</v>
@@ -41125,7 +41155,7 @@
         <v>1</v>
       </c>
       <c r="E74" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F74" s="22">
         <v>0</v>
@@ -41158,7 +41188,7 @@
         <v>20</v>
       </c>
       <c r="S74" s="22" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="T74" s="22">
         <v>8</v>
@@ -41175,7 +41205,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="22" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D75" s="22">
         <v>1</v>
@@ -41225,7 +41255,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C76" s="22" t="s">
         <v>177</v>
@@ -41234,7 +41264,7 @@
         <v>1</v>
       </c>
       <c r="E76" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F76" s="22">
         <v>0</v>
@@ -41246,7 +41276,7 @@
         <v>226</v>
       </c>
       <c r="N76" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O76" s="22">
         <v>0.5</v>
@@ -41270,7 +41300,7 @@
         <v>1</v>
       </c>
       <c r="V76" s="22" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="77" spans="1:22" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -41278,7 +41308,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="22" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C77" s="22" t="s">
         <v>177</v>
@@ -41287,7 +41317,7 @@
         <v>1</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F77" s="22">
         <v>0</v>
@@ -41299,7 +41329,7 @@
         <v>226</v>
       </c>
       <c r="N77" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O77" s="22">
         <v>0.5</v>
@@ -41331,7 +41361,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="22" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C78" s="22" t="s">
         <v>177</v>
@@ -41340,7 +41370,7 @@
         <v>1</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F78" s="22">
         <v>0</v>
@@ -41352,7 +41382,7 @@
         <v>226</v>
       </c>
       <c r="N78" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O78" s="22">
         <v>0.5</v>
@@ -41384,7 +41414,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="22" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C79" s="22" t="s">
         <v>177</v>
@@ -41393,7 +41423,7 @@
         <v>1</v>
       </c>
       <c r="E79" s="22" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F79" s="22">
         <v>0</v>
@@ -41405,7 +41435,7 @@
         <v>226</v>
       </c>
       <c r="N79" s="22" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="O79" s="22">
         <v>0.5</v>
@@ -41429,7 +41459,7 @@
         <v>6</v>
       </c>
       <c r="V79" s="22" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="80" spans="1:22" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed bugs in compliance report tests - Set VIII
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12264" windowHeight="4116" tabRatio="799" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -37042,8 +37042,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q94" workbookViewId="0">
-      <selection activeCell="S118" sqref="S118"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43289,7 +43289,7 @@
     </row>
     <row r="117" spans="1:24" s="29" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A117" s="29">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B117" s="33" t="s">
         <v>499</v>
@@ -43336,7 +43336,7 @@
         <v>11</v>
       </c>
       <c r="S117" s="33">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="T117" s="33">
         <v>4</v>

</xml_diff>

<commit_message>
Added isManualSurveyModeSelected to reportsBasePage
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -625,7 +625,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="508">
   <si>
     <t>Enabled</t>
   </si>
@@ -2144,6 +2144,12 @@
   <si>
     <t>TC705</t>
   </si>
+  <si>
+    <t>View042</t>
+  </si>
+  <si>
+    <t>ONLY Field Notes TRUE</t>
+  </si>
 </sst>
 </file>
 
@@ -2403,7 +2409,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2458,6 +2464,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1 2" xfId="7"/>
@@ -15780,8 +15787,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AA800"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:N43"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18120,34 +18127,62 @@
       <c r="Z43" s="22"/>
       <c r="AA43" s="22"/>
     </row>
-    <row r="44" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="22"/>
-      <c r="S44" s="22"/>
-      <c r="T44" s="22"/>
-      <c r="U44" s="22"/>
-      <c r="V44" s="22"/>
-      <c r="W44" s="22"/>
-      <c r="X44" s="22"/>
-      <c r="Y44" s="22"/>
-      <c r="Z44" s="22"/>
-      <c r="AA44" s="22"/>
+    <row r="44" spans="1:27" s="33" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A44" s="36">
+        <v>43</v>
+      </c>
+      <c r="B44" s="36" t="s">
+        <v>506</v>
+      </c>
+      <c r="C44" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="D44" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J44" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K44" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="L44" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="M44" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="N44" s="36" t="s">
+        <v>507</v>
+      </c>
+      <c r="O44" s="36"/>
+      <c r="P44" s="36"/>
+      <c r="Q44" s="36"/>
+      <c r="R44" s="36"/>
+      <c r="S44" s="36"/>
+      <c r="T44" s="36"/>
+      <c r="U44" s="36"/>
+      <c r="V44" s="36"/>
+      <c r="W44" s="36"/>
+      <c r="X44" s="36"/>
+      <c r="Y44" s="36"/>
+      <c r="Z44" s="36"/>
+      <c r="AA44" s="36"/>
     </row>
     <row r="45" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A45" s="22"/>
@@ -36931,8 +36966,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86:A106"/>
+    <sheetView tabSelected="1" topLeftCell="N70" workbookViewId="0">
+      <selection activeCell="Q85" sqref="A85:XFD85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43106,10 +43141,10 @@
         <v>11</v>
       </c>
       <c r="S103" s="35">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T103" s="35">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="U103" s="35">
         <v>6</v>
@@ -43170,10 +43205,10 @@
         <v>11</v>
       </c>
       <c r="S104" s="35">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T104" s="35">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="U104" s="35">
         <v>6</v>

</xml_diff>

<commit_message>
Updated test data for test 8
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -625,7 +625,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="507">
   <si>
     <t>Enabled</t>
   </si>
@@ -2082,9 +2082,6 @@
     <t>TC1532</t>
   </si>
   <si>
-    <t>ethane</t>
-  </si>
-  <si>
     <t>All Except LISA and GAP</t>
   </si>
   <si>
@@ -2145,10 +2142,10 @@
     <t>TC705</t>
   </si>
   <si>
-    <t>View042</t>
+    <t>ONLY Field Notes TRUE</t>
   </si>
   <si>
-    <t>ONLY Field Notes TRUE</t>
+    <t>Ethane1MinSurvey</t>
   </si>
 </sst>
 </file>
@@ -2840,15 +2837,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1138"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:P35"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.21875" customWidth="1"/>
     <col min="5" max="5" width="27.5546875" customWidth="1"/>
     <col min="6" max="6" width="23.88671875" customWidth="1"/>
     <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
@@ -3607,7 +3604,7 @@
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22" t="s">
-        <v>485</v>
+        <v>506</v>
       </c>
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
@@ -15787,8 +15784,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AA800"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18111,7 +18108,7 @@
         <v>83</v>
       </c>
       <c r="N43" s="22" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="O43" s="22"/>
       <c r="P43" s="22"/>
@@ -18132,7 +18129,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>506</v>
+        <v>441</v>
       </c>
       <c r="C44" s="36" t="b">
         <v>0</v>
@@ -18168,7 +18165,7 @@
         <v>83</v>
       </c>
       <c r="N44" s="36" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="O44" s="36"/>
       <c r="P44" s="36"/>
@@ -19408,7 +19405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -36966,8 +36963,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N70" workbookViewId="0">
-      <selection activeCell="Q85" sqref="A85:XFD85"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42088,7 +42085,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="35" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C87" s="33" t="s">
         <v>177</v>
@@ -42152,7 +42149,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="35" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C88" s="33" t="s">
         <v>177</v>
@@ -42216,7 +42213,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="35" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C89" s="33" t="s">
         <v>177</v>
@@ -42280,7 +42277,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="33" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C90" s="33" t="s">
         <v>177</v>
@@ -42317,7 +42314,7 @@
         <v>11</v>
       </c>
       <c r="S90" s="33" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="T90" s="33">
         <v>1</v>
@@ -42336,7 +42333,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="35" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C91" s="33" t="s">
         <v>177</v>
@@ -42400,7 +42397,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="33" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C92" s="33" t="s">
         <v>177</v>
@@ -42437,7 +42434,7 @@
         <v>11</v>
       </c>
       <c r="S92" s="33" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="T92" s="33">
         <v>1</v>
@@ -42456,7 +42453,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="35" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C93" s="33" t="s">
         <v>177</v>
@@ -42520,7 +42517,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="35" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C94" s="33" t="s">
         <v>177</v>
@@ -42584,7 +42581,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="35" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C95" s="33" t="s">
         <v>177</v>
@@ -42648,7 +42645,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="35" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C96" s="33" t="s">
         <v>177</v>
@@ -42712,7 +42709,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="35" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C97" s="33" t="s">
         <v>177</v>
@@ -42776,13 +42773,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="35" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C98" s="33" t="s">
         <v>177</v>
       </c>
       <c r="D98" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E98" s="35" t="s">
         <v>356</v>
@@ -42840,7 +42837,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="35" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C99" s="33" t="s">
         <v>177</v>
@@ -42904,7 +42901,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="35" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C100" s="33" t="s">
         <v>177</v>
@@ -42968,7 +42965,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="35" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C101" s="33" t="s">
         <v>177</v>
@@ -43032,7 +43029,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C102" s="33" t="s">
         <v>177</v>
@@ -43096,7 +43093,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="35" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C103" s="33" t="s">
         <v>177</v>
@@ -43144,7 +43141,7 @@
         <v>43</v>
       </c>
       <c r="T103" s="35">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="U103" s="35">
         <v>6</v>
@@ -43160,7 +43157,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="35" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C104" s="33" t="s">
         <v>177</v>
@@ -43208,7 +43205,7 @@
         <v>43</v>
       </c>
       <c r="T104" s="35">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="U104" s="35">
         <v>6</v>
@@ -43224,7 +43221,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="35" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C105" s="33" t="s">
         <v>177</v>
@@ -43288,7 +43285,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="35" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C106" s="33" t="s">
         <v>177</v>

</xml_diff>

<commit_message>
report job perf tests with multiple views and large PDF size
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -625,7 +625,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="494">
   <si>
     <t>Enabled</t>
   </si>
@@ -2087,6 +2087,27 @@
   <si>
     <t>All Except LISA and GAP</t>
   </si>
+  <si>
+    <t>TC1844-1</t>
+  </si>
+  <si>
+    <t>TC1844-2</t>
+  </si>
+  <si>
+    <t>TC1843-1</t>
+  </si>
+  <si>
+    <t>TC1843-2</t>
+  </si>
+  <si>
+    <t>10,11,12,13,14,15,24</t>
+  </si>
+  <si>
+    <t>10,11,12,13,14,15,25</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,8</t>
+  </si>
 </sst>
 </file>
 
@@ -15720,8 +15741,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AA800"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:N43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36871,8 +36892,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80:V86"/>
+    <sheetView tabSelected="1" topLeftCell="L65" workbookViewId="0">
+      <selection activeCell="S91" sqref="S91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41988,109 +42009,205 @@
       <c r="W86" s="19"/>
       <c r="X86" s="19"/>
     </row>
-    <row r="87" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A87" s="19"/>
-      <c r="B87" s="19"/>
-      <c r="C87" s="19"/>
-      <c r="D87" s="19"/>
-      <c r="E87" s="19"/>
-      <c r="F87" s="19"/>
-      <c r="G87" s="19"/>
-      <c r="H87" s="19"/>
-      <c r="I87" s="19"/>
-      <c r="J87" s="19"/>
-      <c r="K87" s="19"/>
-      <c r="L87" s="19"/>
-      <c r="M87" s="19"/>
-      <c r="N87" s="19"/>
-      <c r="O87" s="19"/>
-      <c r="P87" s="19"/>
-      <c r="Q87" s="19"/>
-      <c r="R87" s="19"/>
-      <c r="S87" s="19"/>
-      <c r="T87" s="19"/>
-      <c r="U87" s="19"/>
-      <c r="V87" s="19"/>
-      <c r="W87" s="19"/>
-      <c r="X87" s="19"/>
-    </row>
-    <row r="88" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A88" s="19"/>
-      <c r="B88" s="19"/>
-      <c r="C88" s="19"/>
-      <c r="D88" s="19"/>
-      <c r="E88" s="19"/>
-      <c r="F88" s="19"/>
-      <c r="G88" s="19"/>
-      <c r="H88" s="19"/>
-      <c r="I88" s="19"/>
-      <c r="J88" s="19"/>
-      <c r="K88" s="19"/>
-      <c r="L88" s="19"/>
-      <c r="M88" s="19"/>
-      <c r="N88" s="19"/>
-      <c r="O88" s="19"/>
-      <c r="P88" s="19"/>
-      <c r="Q88" s="19"/>
-      <c r="R88" s="19"/>
-      <c r="S88" s="19"/>
-      <c r="T88" s="19"/>
-      <c r="U88" s="19"/>
-      <c r="V88" s="19"/>
-      <c r="W88" s="19"/>
-      <c r="X88" s="19"/>
-    </row>
-    <row r="89" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A89" s="19"/>
-      <c r="B89" s="19"/>
-      <c r="C89" s="19"/>
-      <c r="D89" s="19"/>
-      <c r="E89" s="19"/>
-      <c r="F89" s="19"/>
-      <c r="G89" s="19"/>
-      <c r="H89" s="19"/>
-      <c r="I89" s="19"/>
-      <c r="J89" s="19"/>
-      <c r="K89" s="19"/>
-      <c r="L89" s="19"/>
-      <c r="M89" s="19"/>
-      <c r="N89" s="19"/>
-      <c r="O89" s="19"/>
-      <c r="P89" s="19"/>
-      <c r="Q89" s="19"/>
-      <c r="R89" s="19"/>
-      <c r="S89" s="19"/>
-      <c r="T89" s="19"/>
-      <c r="U89" s="19"/>
-      <c r="V89" s="19"/>
-      <c r="W89" s="19"/>
-      <c r="X89" s="19"/>
-    </row>
-    <row r="90" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A90" s="19"/>
-      <c r="B90" s="19"/>
-      <c r="C90" s="19"/>
-      <c r="D90" s="19"/>
-      <c r="E90" s="19"/>
-      <c r="F90" s="19"/>
-      <c r="G90" s="19"/>
-      <c r="H90" s="19"/>
-      <c r="I90" s="19"/>
-      <c r="J90" s="19"/>
-      <c r="K90" s="19"/>
-      <c r="L90" s="19"/>
-      <c r="M90" s="19"/>
-      <c r="N90" s="19"/>
-      <c r="O90" s="19"/>
-      <c r="P90" s="19"/>
-      <c r="Q90" s="19"/>
-      <c r="R90" s="19"/>
-      <c r="S90" s="19"/>
-      <c r="T90" s="19"/>
-      <c r="U90" s="19"/>
-      <c r="V90" s="19"/>
-      <c r="W90" s="19"/>
-      <c r="X90" s="19"/>
+    <row r="87" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A87" s="22">
+        <v>86</v>
+      </c>
+      <c r="B87" s="22" t="s">
+        <v>489</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D87" s="22">
+        <v>5</v>
+      </c>
+      <c r="E87" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="F87" s="22">
+        <v>0</v>
+      </c>
+      <c r="G87" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M87" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="N87" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q87" s="22">
+        <v>40</v>
+      </c>
+      <c r="R87" s="22">
+        <v>40</v>
+      </c>
+      <c r="S87" s="22" t="s">
+        <v>491</v>
+      </c>
+      <c r="T87" s="22">
+        <v>7</v>
+      </c>
+      <c r="U87" s="22">
+        <v>10</v>
+      </c>
+      <c r="V87" s="22" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="88" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A88" s="22">
+        <v>87</v>
+      </c>
+      <c r="B88" s="22" t="s">
+        <v>487</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D88" s="22">
+        <v>5</v>
+      </c>
+      <c r="E88" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="F88" s="22">
+        <v>0</v>
+      </c>
+      <c r="G88" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="I88" s="22">
+        <v>29.757819448754098</v>
+      </c>
+      <c r="J88" s="22">
+        <v>-95.353906211853001</v>
+      </c>
+      <c r="K88" s="22">
+        <v>29.7362085557276</v>
+      </c>
+      <c r="L88" s="22">
+        <v>-95.381543693542397</v>
+      </c>
+      <c r="Q88" s="22">
+        <v>40</v>
+      </c>
+      <c r="R88" s="22">
+        <v>40</v>
+      </c>
+      <c r="S88" s="22" t="s">
+        <v>492</v>
+      </c>
+      <c r="T88" s="22">
+        <v>7</v>
+      </c>
+      <c r="U88" s="22">
+        <v>8</v>
+      </c>
+      <c r="V88" s="22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A89" s="22">
+        <v>88</v>
+      </c>
+      <c r="B89" s="22" t="s">
+        <v>490</v>
+      </c>
+      <c r="C89" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D89" s="22">
+        <v>5</v>
+      </c>
+      <c r="E89" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="F89" s="22">
+        <v>0</v>
+      </c>
+      <c r="G89" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M89" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="N89" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q89" s="22">
+        <v>48</v>
+      </c>
+      <c r="R89" s="22">
+        <v>45</v>
+      </c>
+      <c r="S89" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="T89" s="22">
+        <v>7</v>
+      </c>
+      <c r="U89" s="22">
+        <v>10</v>
+      </c>
+      <c r="V89" s="22" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A90" s="22">
+        <v>89</v>
+      </c>
+      <c r="B90" s="22" t="s">
+        <v>488</v>
+      </c>
+      <c r="C90" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D90" s="22">
+        <v>5</v>
+      </c>
+      <c r="E90" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="F90" s="22">
+        <v>0</v>
+      </c>
+      <c r="G90" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="I90" s="22">
+        <v>29.757819448754098</v>
+      </c>
+      <c r="J90" s="22">
+        <v>-95.353906211853001</v>
+      </c>
+      <c r="K90" s="22">
+        <v>29.7362085557276</v>
+      </c>
+      <c r="L90" s="22">
+        <v>-95.381543693542397</v>
+      </c>
+      <c r="Q90" s="22">
+        <v>48</v>
+      </c>
+      <c r="R90" s="22">
+        <v>45</v>
+      </c>
+      <c r="S90" s="22" t="s">
+        <v>493</v>
+      </c>
+      <c r="T90" s="22">
+        <v>7</v>
+      </c>
+      <c r="U90" s="22">
+        <v>8</v>
+      </c>
+      <c r="V90" s="22">
+        <v>25</v>
+      </c>
     </row>
     <row r="91" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A91" s="19"/>

</xml_diff>

<commit_message>
additional test cases for max pdf size
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -625,7 +625,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="497">
   <si>
     <t>Enabled</t>
   </si>
@@ -2108,6 +2108,15 @@
   <si>
     <t>1,2,3,4,5,6,8</t>
   </si>
+  <si>
+    <t>TC1844-3</t>
+  </si>
+  <si>
+    <t>TC1843-3</t>
+  </si>
+  <si>
+    <t>43,43,43,43,43,43,43</t>
+  </si>
 </sst>
 </file>
 
@@ -15741,8 +15750,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AA800"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18081,34 +18090,49 @@
       <c r="Z43" s="22"/>
       <c r="AA43" s="22"/>
     </row>
-    <row r="44" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="22"/>
-      <c r="S44" s="22"/>
-      <c r="T44" s="22"/>
-      <c r="U44" s="22"/>
-      <c r="V44" s="22"/>
-      <c r="W44" s="22"/>
-      <c r="X44" s="22"/>
-      <c r="Y44" s="22"/>
-      <c r="Z44" s="22"/>
-      <c r="AA44" s="22"/>
+    <row r="44" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A44" s="22">
+        <v>43</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K44" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="L44" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="M44" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="N44" s="22" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="45" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A45" s="22"/>
@@ -36892,8 +36916,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L65" workbookViewId="0">
-      <selection activeCell="S91" sqref="S91"/>
+    <sheetView tabSelected="1" topLeftCell="N61" workbookViewId="0">
+      <selection activeCell="S92" sqref="S92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42138,10 +42162,10 @@
         <v>186</v>
       </c>
       <c r="Q89" s="22">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="R89" s="22">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="S89" s="22" t="s">
         <v>305</v>
@@ -42191,10 +42215,10 @@
         <v>-95.381543693542397</v>
       </c>
       <c r="Q90" s="22">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="R90" s="22">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="S90" s="22" t="s">
         <v>493</v>
@@ -42209,57 +42233,105 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A91" s="19"/>
-      <c r="B91" s="19"/>
-      <c r="C91" s="19"/>
-      <c r="D91" s="19"/>
-      <c r="E91" s="19"/>
-      <c r="F91" s="19"/>
-      <c r="G91" s="19"/>
-      <c r="H91" s="19"/>
-      <c r="I91" s="19"/>
-      <c r="J91" s="19"/>
-      <c r="K91" s="19"/>
-      <c r="L91" s="19"/>
-      <c r="M91" s="19"/>
-      <c r="N91" s="19"/>
-      <c r="O91" s="19"/>
-      <c r="P91" s="19"/>
-      <c r="Q91" s="19"/>
-      <c r="R91" s="19"/>
-      <c r="S91" s="19"/>
-      <c r="T91" s="19"/>
-      <c r="U91" s="19"/>
-      <c r="V91" s="19"/>
-      <c r="W91" s="19"/>
-      <c r="X91" s="19"/>
-    </row>
-    <row r="92" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A92" s="19"/>
-      <c r="B92" s="19"/>
-      <c r="C92" s="19"/>
-      <c r="D92" s="19"/>
-      <c r="E92" s="19"/>
-      <c r="F92" s="19"/>
-      <c r="G92" s="19"/>
-      <c r="H92" s="19"/>
-      <c r="I92" s="19"/>
-      <c r="J92" s="19"/>
-      <c r="K92" s="19"/>
-      <c r="L92" s="19"/>
-      <c r="M92" s="19"/>
-      <c r="N92" s="19"/>
-      <c r="O92" s="19"/>
-      <c r="P92" s="19"/>
-      <c r="Q92" s="19"/>
-      <c r="R92" s="19"/>
-      <c r="S92" s="19"/>
-      <c r="T92" s="19"/>
-      <c r="U92" s="19"/>
-      <c r="V92" s="19"/>
-      <c r="W92" s="19"/>
-      <c r="X92" s="19"/>
+    <row r="91" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A91" s="22">
+        <v>90</v>
+      </c>
+      <c r="B91" s="22" t="s">
+        <v>495</v>
+      </c>
+      <c r="C91" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D91" s="22">
+        <v>5</v>
+      </c>
+      <c r="E91" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="F91" s="22">
+        <v>0</v>
+      </c>
+      <c r="G91" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M91" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="N91" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q91" s="22">
+        <v>40</v>
+      </c>
+      <c r="R91" s="22">
+        <v>40</v>
+      </c>
+      <c r="S91" s="22" t="s">
+        <v>496</v>
+      </c>
+      <c r="T91" s="22">
+        <v>7</v>
+      </c>
+      <c r="U91" s="22">
+        <v>10</v>
+      </c>
+      <c r="V91" s="22" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A92" s="22">
+        <v>91</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>494</v>
+      </c>
+      <c r="C92" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D92" s="22">
+        <v>5</v>
+      </c>
+      <c r="E92" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="F92" s="22">
+        <v>0</v>
+      </c>
+      <c r="G92" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="I92" s="22">
+        <v>29.757819448754098</v>
+      </c>
+      <c r="J92" s="22">
+        <v>-95.353906211853001</v>
+      </c>
+      <c r="K92" s="22">
+        <v>29.7362085557276</v>
+      </c>
+      <c r="L92" s="22">
+        <v>-95.381543693542397</v>
+      </c>
+      <c r="Q92" s="22">
+        <v>40</v>
+      </c>
+      <c r="R92" s="22">
+        <v>40</v>
+      </c>
+      <c r="S92" s="22" t="s">
+        <v>496</v>
+      </c>
+      <c r="T92" s="22">
+        <v>7</v>
+      </c>
+      <c r="U92" s="22">
+        <v>8</v>
+      </c>
+      <c r="V92" s="22">
+        <v>25</v>
+      </c>
     </row>
     <row r="93" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A93" s="19"/>

</xml_diff>

<commit_message>
changes in page objects and actions for driver view page as per product changes
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -15720,7 +15720,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AA800"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A43" sqref="A43:N43"/>
     </sheetView>
   </sheetViews>
@@ -21148,8 +21148,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22280,8 +22280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1069"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22353,7 +22353,7 @@
       <c r="C4" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="22" t="s">
         <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -30417,8 +30417,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AB1073"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added support for 2 highlight checkboxes in compliance report
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -625,7 +625,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="512">
   <si>
     <t>Enabled</t>
   </si>
@@ -2156,6 +2156,12 @@
   <si>
     <t>View042</t>
   </si>
+  <si>
+    <t>Highlight LISA Assets</t>
+  </si>
+  <si>
+    <t>Highlight GAP Assets</t>
+  </si>
 </sst>
 </file>
 
@@ -2415,7 +2421,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2472,6 +2478,7 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1 2" xfId="7"/>
@@ -15792,10 +15799,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:AA800"/>
+  <dimension ref="A1:AC800"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15810,10 +15817,12 @@
     <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="10.44140625" customWidth="1"/>
     <col min="13" max="13" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.88671875" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" customWidth="1"/>
+    <col min="16" max="16" width="35.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -15854,10 +15863,16 @@
         <v>81</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -15897,11 +15912,13 @@
       <c r="M2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="29" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" s="29" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A3" s="29">
         <v>2</v>
       </c>
@@ -15941,11 +15958,13 @@
       <c r="M3" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="N3" s="29" t="s">
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="29" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -15985,11 +16004,11 @@
       <c r="M4" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="22"/>
@@ -16001,8 +16020,10 @@
       <c r="Y4" s="22"/>
       <c r="Z4" s="22"/>
       <c r="AA4" s="22"/>
-    </row>
-    <row r="5" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+    </row>
+    <row r="5" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -16042,11 +16063,11 @@
       <c r="M5" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N5" s="22" t="s">
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="22"/>
@@ -16058,8 +16079,10 @@
       <c r="Y5" s="22"/>
       <c r="Z5" s="22"/>
       <c r="AA5" s="22"/>
-    </row>
-    <row r="6" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22"/>
+    </row>
+    <row r="6" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -16099,11 +16122,11 @@
       <c r="M6" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N6" s="22" t="s">
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22" t="s">
         <v>290</v>
       </c>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
@@ -16115,8 +16138,10 @@
       <c r="Y6" s="22"/>
       <c r="Z6" s="22"/>
       <c r="AA6" s="22"/>
-    </row>
-    <row r="7" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+    </row>
+    <row r="7" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -16156,11 +16181,11 @@
       <c r="M7" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N7" s="22" t="s">
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22" t="s">
         <v>293</v>
       </c>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
@@ -16172,8 +16197,10 @@
       <c r="Y7" s="22"/>
       <c r="Z7" s="22"/>
       <c r="AA7" s="22"/>
-    </row>
-    <row r="8" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22"/>
+    </row>
+    <row r="8" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -16213,11 +16240,11 @@
       <c r="M8" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N8" s="22" t="s">
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22" t="s">
         <v>292</v>
       </c>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
@@ -16229,8 +16256,10 @@
       <c r="Y8" s="22"/>
       <c r="Z8" s="22"/>
       <c r="AA8" s="22"/>
-    </row>
-    <row r="9" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+    </row>
+    <row r="9" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A9" s="22">
         <v>8</v>
       </c>
@@ -16270,11 +16299,11 @@
       <c r="M9" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N9" s="22" t="s">
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
@@ -16286,8 +16315,10 @@
       <c r="Y9" s="22"/>
       <c r="Z9" s="22"/>
       <c r="AA9" s="22"/>
-    </row>
-    <row r="10" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+    </row>
+    <row r="10" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A10" s="22">
         <v>9</v>
       </c>
@@ -16327,11 +16358,11 @@
       <c r="M10" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N10" s="22" t="s">
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
       <c r="Q10" s="22"/>
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
@@ -16343,8 +16374,10 @@
       <c r="Y10" s="22"/>
       <c r="Z10" s="22"/>
       <c r="AA10" s="22"/>
-    </row>
-    <row r="11" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+    </row>
+    <row r="11" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A11" s="22">
         <v>10</v>
       </c>
@@ -16384,11 +16417,11 @@
       <c r="M11" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N11" s="22" t="s">
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
       <c r="Q11" s="22"/>
       <c r="R11" s="22"/>
       <c r="S11" s="22"/>
@@ -16400,8 +16433,10 @@
       <c r="Y11" s="22"/>
       <c r="Z11" s="22"/>
       <c r="AA11" s="22"/>
-    </row>
-    <row r="12" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB11" s="22"/>
+      <c r="AC11" s="22"/>
+    </row>
+    <row r="12" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A12" s="22">
         <v>11</v>
       </c>
@@ -16441,11 +16476,11 @@
       <c r="M12" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N12" s="22" t="s">
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
       <c r="Q12" s="22"/>
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
@@ -16457,8 +16492,10 @@
       <c r="Y12" s="22"/>
       <c r="Z12" s="22"/>
       <c r="AA12" s="22"/>
-    </row>
-    <row r="13" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB12" s="22"/>
+      <c r="AC12" s="22"/>
+    </row>
+    <row r="13" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A13" s="22">
         <v>12</v>
       </c>
@@ -16498,11 +16535,11 @@
       <c r="M13" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N13" s="22" t="s">
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="22" t="s">
         <v>366</v>
       </c>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
       <c r="Q13" s="22"/>
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
@@ -16514,8 +16551,10 @@
       <c r="Y13" s="22"/>
       <c r="Z13" s="22"/>
       <c r="AA13" s="22"/>
-    </row>
-    <row r="14" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB13" s="22"/>
+      <c r="AC13" s="22"/>
+    </row>
+    <row r="14" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A14" s="22">
         <v>13</v>
       </c>
@@ -16555,11 +16594,11 @@
       <c r="M14" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N14" s="22" t="s">
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
       <c r="Q14" s="22"/>
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
@@ -16571,8 +16610,10 @@
       <c r="Y14" s="22"/>
       <c r="Z14" s="22"/>
       <c r="AA14" s="22"/>
-    </row>
-    <row r="15" spans="1:27" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB14" s="22"/>
+      <c r="AC14" s="22"/>
+    </row>
+    <row r="15" spans="1:29" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A15" s="22">
         <v>14</v>
       </c>
@@ -16612,11 +16653,11 @@
       <c r="M15" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N15" s="22" t="s">
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22" t="s">
         <v>272</v>
       </c>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="22"/>
@@ -16628,8 +16669,10 @@
       <c r="Y15" s="22"/>
       <c r="Z15" s="22"/>
       <c r="AA15" s="22"/>
-    </row>
-    <row r="16" spans="1:27" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB15" s="22"/>
+      <c r="AC15" s="22"/>
+    </row>
+    <row r="16" spans="1:29" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A16" s="22">
         <v>15</v>
       </c>
@@ -16669,11 +16712,11 @@
       <c r="M16" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N16" s="22" t="s">
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22" t="s">
         <v>276</v>
       </c>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
@@ -16685,8 +16728,10 @@
       <c r="Y16" s="22"/>
       <c r="Z16" s="22"/>
       <c r="AA16" s="22"/>
-    </row>
-    <row r="17" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB16" s="22"/>
+      <c r="AC16" s="22"/>
+    </row>
+    <row r="17" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A17" s="22">
         <v>16</v>
       </c>
@@ -16726,11 +16771,11 @@
       <c r="M17" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N17" s="22" t="s">
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22" t="s">
         <v>364</v>
       </c>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
       <c r="Q17" s="22"/>
       <c r="R17" s="22"/>
       <c r="S17" s="22"/>
@@ -16742,8 +16787,10 @@
       <c r="Y17" s="22"/>
       <c r="Z17" s="22"/>
       <c r="AA17" s="22"/>
-    </row>
-    <row r="18" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+    </row>
+    <row r="18" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A18" s="22">
         <v>17</v>
       </c>
@@ -16783,11 +16830,11 @@
       <c r="M18" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="N18" s="22" t="s">
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22" t="s">
         <v>365</v>
       </c>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
       <c r="Q18" s="22"/>
       <c r="R18" s="22"/>
       <c r="S18" s="22"/>
@@ -16799,8 +16846,10 @@
       <c r="Y18" s="22"/>
       <c r="Z18" s="22"/>
       <c r="AA18" s="22"/>
-    </row>
-    <row r="19" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="22"/>
+    </row>
+    <row r="19" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A19" s="22">
         <v>18</v>
       </c>
@@ -16840,11 +16889,11 @@
       <c r="M19" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N19" s="22" t="s">
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
       <c r="Q19" s="22"/>
       <c r="R19" s="22"/>
       <c r="S19" s="22"/>
@@ -16856,8 +16905,10 @@
       <c r="Y19" s="22"/>
       <c r="Z19" s="22"/>
       <c r="AA19" s="22"/>
-    </row>
-    <row r="20" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB19" s="22"/>
+      <c r="AC19" s="22"/>
+    </row>
+    <row r="20" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A20" s="22">
         <v>19</v>
       </c>
@@ -16897,11 +16948,11 @@
       <c r="M20" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N20" s="22" t="s">
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
       <c r="Q20" s="22"/>
       <c r="R20" s="22"/>
       <c r="S20" s="22"/>
@@ -16913,8 +16964,10 @@
       <c r="Y20" s="22"/>
       <c r="Z20" s="22"/>
       <c r="AA20" s="22"/>
-    </row>
-    <row r="21" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB20" s="22"/>
+      <c r="AC20" s="22"/>
+    </row>
+    <row r="21" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A21" s="22">
         <v>20</v>
       </c>
@@ -16954,11 +17007,11 @@
       <c r="M21" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N21" s="22" t="s">
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="O21" s="22"/>
-      <c r="P21" s="22"/>
       <c r="Q21" s="22"/>
       <c r="R21" s="22"/>
       <c r="S21" s="22"/>
@@ -16970,8 +17023,10 @@
       <c r="Y21" s="22"/>
       <c r="Z21" s="22"/>
       <c r="AA21" s="22"/>
-    </row>
-    <row r="22" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB21" s="22"/>
+      <c r="AC21" s="22"/>
+    </row>
+    <row r="22" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A22" s="22">
         <v>21</v>
       </c>
@@ -17011,11 +17066,11 @@
       <c r="M22" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N22" s="22" t="s">
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
       <c r="Q22" s="22"/>
       <c r="R22" s="22"/>
       <c r="S22" s="22"/>
@@ -17027,8 +17082,10 @@
       <c r="Y22" s="22"/>
       <c r="Z22" s="22"/>
       <c r="AA22" s="22"/>
-    </row>
-    <row r="23" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB22" s="22"/>
+      <c r="AC22" s="22"/>
+    </row>
+    <row r="23" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A23" s="22">
         <v>22</v>
       </c>
@@ -17068,11 +17125,11 @@
       <c r="M23" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N23" s="22" t="s">
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22" t="s">
         <v>294</v>
       </c>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
       <c r="Q23" s="22"/>
       <c r="R23" s="22"/>
       <c r="S23" s="22"/>
@@ -17084,8 +17141,10 @@
       <c r="Y23" s="22"/>
       <c r="Z23" s="22"/>
       <c r="AA23" s="22"/>
-    </row>
-    <row r="24" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB23" s="22"/>
+      <c r="AC23" s="22"/>
+    </row>
+    <row r="24" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A24" s="22">
         <v>23</v>
       </c>
@@ -17125,11 +17184,11 @@
       <c r="M24" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N24" s="22" t="s">
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
       <c r="Q24" s="22"/>
       <c r="R24" s="22"/>
       <c r="S24" s="22"/>
@@ -17141,8 +17200,10 @@
       <c r="Y24" s="22"/>
       <c r="Z24" s="22"/>
       <c r="AA24" s="22"/>
-    </row>
-    <row r="25" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB24" s="22"/>
+      <c r="AC24" s="22"/>
+    </row>
+    <row r="25" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A25" s="22">
         <v>24</v>
       </c>
@@ -17182,11 +17243,11 @@
       <c r="M25" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N25" s="22" t="s">
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22" t="s">
         <v>298</v>
       </c>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
       <c r="Q25" s="22"/>
       <c r="R25" s="22"/>
       <c r="S25" s="22"/>
@@ -17198,8 +17259,10 @@
       <c r="Y25" s="22"/>
       <c r="Z25" s="22"/>
       <c r="AA25" s="22"/>
-    </row>
-    <row r="26" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB25" s="22"/>
+      <c r="AC25" s="22"/>
+    </row>
+    <row r="26" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A26" s="22">
         <v>25</v>
       </c>
@@ -17239,11 +17302,11 @@
       <c r="M26" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N26" s="22" t="s">
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22" t="s">
         <v>299</v>
       </c>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
       <c r="Q26" s="22"/>
       <c r="R26" s="22"/>
       <c r="S26" s="22"/>
@@ -17255,8 +17318,10 @@
       <c r="Y26" s="22"/>
       <c r="Z26" s="22"/>
       <c r="AA26" s="22"/>
-    </row>
-    <row r="27" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB26" s="22"/>
+      <c r="AC26" s="22"/>
+    </row>
+    <row r="27" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A27" s="22">
         <v>26</v>
       </c>
@@ -17296,11 +17361,11 @@
       <c r="M27" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N27" s="22" t="s">
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="22"/>
@@ -17312,8 +17377,10 @@
       <c r="Y27" s="22"/>
       <c r="Z27" s="22"/>
       <c r="AA27" s="22"/>
-    </row>
-    <row r="28" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB27" s="22"/>
+      <c r="AC27" s="22"/>
+    </row>
+    <row r="28" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A28" s="22">
         <v>27</v>
       </c>
@@ -17353,11 +17420,11 @@
       <c r="M28" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N28" s="22" t="s">
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22" t="s">
         <v>437</v>
       </c>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
       <c r="Q28" s="22"/>
       <c r="R28" s="22"/>
       <c r="S28" s="22"/>
@@ -17369,8 +17436,10 @@
       <c r="Y28" s="22"/>
       <c r="Z28" s="22"/>
       <c r="AA28" s="22"/>
-    </row>
-    <row r="29" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB28" s="22"/>
+      <c r="AC28" s="22"/>
+    </row>
+    <row r="29" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A29" s="22">
         <v>28</v>
       </c>
@@ -17410,11 +17479,11 @@
       <c r="M29" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N29" s="22" t="s">
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22" t="s">
         <v>438</v>
       </c>
-      <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
       <c r="Q29" s="22"/>
       <c r="R29" s="22"/>
       <c r="S29" s="22"/>
@@ -17426,8 +17495,10 @@
       <c r="Y29" s="22"/>
       <c r="Z29" s="22"/>
       <c r="AA29" s="22"/>
-    </row>
-    <row r="30" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB29" s="22"/>
+      <c r="AC29" s="22"/>
+    </row>
+    <row r="30" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A30" s="22">
         <v>29</v>
       </c>
@@ -17467,11 +17538,11 @@
       <c r="M30" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N30" s="22" t="s">
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22" t="s">
         <v>302</v>
       </c>
-      <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
       <c r="Q30" s="22"/>
       <c r="R30" s="22"/>
       <c r="S30" s="22"/>
@@ -17483,8 +17554,10 @@
       <c r="Y30" s="22"/>
       <c r="Z30" s="22"/>
       <c r="AA30" s="22"/>
-    </row>
-    <row r="31" spans="1:27" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB30" s="22"/>
+      <c r="AC30" s="22"/>
+    </row>
+    <row r="31" spans="1:29" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A31" s="22">
         <v>30</v>
       </c>
@@ -17524,11 +17597,11 @@
       <c r="M31" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N31" s="22" t="s">
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="O31" s="22"/>
-      <c r="P31" s="22"/>
       <c r="Q31" s="22"/>
       <c r="R31" s="22"/>
       <c r="S31" s="22"/>
@@ -17540,8 +17613,10 @@
       <c r="Y31" s="22"/>
       <c r="Z31" s="22"/>
       <c r="AA31" s="22"/>
-    </row>
-    <row r="32" spans="1:27" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB31" s="22"/>
+      <c r="AC31" s="22"/>
+    </row>
+    <row r="32" spans="1:29" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A32" s="22">
         <v>31</v>
       </c>
@@ -17581,11 +17656,11 @@
       <c r="M32" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N32" s="22" t="s">
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22" t="s">
         <v>314</v>
       </c>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
       <c r="Q32" s="22"/>
       <c r="R32" s="22"/>
       <c r="S32" s="22"/>
@@ -17597,8 +17672,10 @@
       <c r="Y32" s="22"/>
       <c r="Z32" s="22"/>
       <c r="AA32" s="22"/>
-    </row>
-    <row r="33" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB32" s="22"/>
+      <c r="AC32" s="22"/>
+    </row>
+    <row r="33" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A33" s="22">
         <v>32</v>
       </c>
@@ -17638,11 +17715,11 @@
       <c r="M33" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N33" s="22" t="s">
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
       <c r="Q33" s="22"/>
       <c r="R33" s="22"/>
       <c r="S33" s="22"/>
@@ -17654,8 +17731,10 @@
       <c r="Y33" s="22"/>
       <c r="Z33" s="22"/>
       <c r="AA33" s="22"/>
-    </row>
-    <row r="34" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB33" s="22"/>
+      <c r="AC33" s="22"/>
+    </row>
+    <row r="34" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A34" s="22">
         <v>33</v>
       </c>
@@ -17695,11 +17774,15 @@
       <c r="M34" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N34" s="22" t="s">
+      <c r="N34" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="O34" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="P34" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
       <c r="Q34" s="22"/>
       <c r="R34" s="22"/>
       <c r="S34" s="22"/>
@@ -17711,8 +17794,10 @@
       <c r="Y34" s="22"/>
       <c r="Z34" s="22"/>
       <c r="AA34" s="22"/>
-    </row>
-    <row r="35" spans="1:27" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB34" s="22"/>
+      <c r="AC34" s="22"/>
+    </row>
+    <row r="35" spans="1:29" s="7" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A35" s="22">
         <v>34</v>
       </c>
@@ -17752,11 +17837,11 @@
       <c r="M35" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N35" s="22" t="s">
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
       <c r="Q35" s="22"/>
       <c r="R35" s="22"/>
       <c r="S35" s="22"/>
@@ -17768,8 +17853,10 @@
       <c r="Y35" s="22"/>
       <c r="Z35" s="22"/>
       <c r="AA35" s="22"/>
-    </row>
-    <row r="36" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB35" s="22"/>
+      <c r="AC35" s="22"/>
+    </row>
+    <row r="36" spans="1:29" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A36" s="22">
         <v>35</v>
       </c>
@@ -17809,11 +17896,11 @@
       <c r="M36" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N36" s="22" t="s">
+      <c r="P36" s="22" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="37" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A37" s="22">
         <v>36</v>
       </c>
@@ -17853,11 +17940,11 @@
       <c r="M37" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N37" s="22" t="s">
+      <c r="P37" s="22" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="38" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A38" s="22">
         <v>37</v>
       </c>
@@ -17897,11 +17984,11 @@
       <c r="M38" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N38" s="22" t="s">
+      <c r="P38" s="22" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="39" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A39" s="22">
         <v>38</v>
       </c>
@@ -17941,11 +18028,11 @@
       <c r="M39" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N39" s="22" t="s">
+      <c r="P39" s="22" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="40" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A40" s="22">
         <v>39</v>
       </c>
@@ -17985,11 +18072,11 @@
       <c r="M40" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N40" s="22" t="s">
+      <c r="P40" s="22" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="41" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A41" s="22">
         <v>40</v>
       </c>
@@ -18029,11 +18116,11 @@
       <c r="M41" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N41" s="22" t="s">
+      <c r="P41" s="22" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="42" spans="1:27" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A42" s="22">
         <v>41</v>
       </c>
@@ -18073,11 +18160,11 @@
       <c r="M42" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N42" s="22" t="s">
+      <c r="P42" s="22" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="43" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A43" s="22">
         <v>42</v>
       </c>
@@ -18117,11 +18204,11 @@
       <c r="M43" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N43" s="22" t="s">
+      <c r="N43" s="22"/>
+      <c r="O43" s="22"/>
+      <c r="P43" s="22" t="s">
         <v>485</v>
       </c>
-      <c r="O43" s="22"/>
-      <c r="P43" s="22"/>
       <c r="Q43" s="22"/>
       <c r="R43" s="22"/>
       <c r="S43" s="22"/>
@@ -18133,8 +18220,10 @@
       <c r="Y43" s="22"/>
       <c r="Z43" s="22"/>
       <c r="AA43" s="22"/>
-    </row>
-    <row r="44" spans="1:27" s="33" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB43" s="22"/>
+      <c r="AC43" s="22"/>
+    </row>
+    <row r="44" spans="1:29" s="33" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A44" s="35">
         <v>43</v>
       </c>
@@ -18174,11 +18263,11 @@
       <c r="M44" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="N44" s="35" t="s">
+      <c r="N44" s="37"/>
+      <c r="O44" s="37"/>
+      <c r="P44" s="35" t="s">
         <v>486</v>
       </c>
-      <c r="O44" s="35"/>
-      <c r="P44" s="35"/>
       <c r="Q44" s="35"/>
       <c r="R44" s="35"/>
       <c r="S44" s="35"/>
@@ -18190,8 +18279,10 @@
       <c r="Y44" s="35"/>
       <c r="Z44" s="35"/>
       <c r="AA44" s="35"/>
-    </row>
-    <row r="45" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB44" s="35"/>
+      <c r="AC44" s="35"/>
+    </row>
+    <row r="45" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A45" s="22"/>
       <c r="B45" s="22"/>
       <c r="C45" s="22"/>
@@ -18219,8 +18310,10 @@
       <c r="Y45" s="22"/>
       <c r="Z45" s="22"/>
       <c r="AA45" s="22"/>
-    </row>
-    <row r="46" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB45" s="22"/>
+      <c r="AC45" s="22"/>
+    </row>
+    <row r="46" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A46" s="22"/>
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
@@ -18248,8 +18341,10 @@
       <c r="Y46" s="22"/>
       <c r="Z46" s="22"/>
       <c r="AA46" s="22"/>
-    </row>
-    <row r="47" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB46" s="22"/>
+      <c r="AC46" s="22"/>
+    </row>
+    <row r="47" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A47" s="22"/>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
@@ -18277,8 +18372,10 @@
       <c r="Y47" s="22"/>
       <c r="Z47" s="22"/>
       <c r="AA47" s="22"/>
-    </row>
-    <row r="48" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB47" s="22"/>
+      <c r="AC47" s="22"/>
+    </row>
+    <row r="48" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A48" s="22"/>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
@@ -18306,8 +18403,10 @@
       <c r="Y48" s="22"/>
       <c r="Z48" s="22"/>
       <c r="AA48" s="22"/>
-    </row>
-    <row r="49" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB48" s="22"/>
+      <c r="AC48" s="22"/>
+    </row>
+    <row r="49" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A49" s="22"/>
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
@@ -18335,8 +18434,10 @@
       <c r="Y49" s="22"/>
       <c r="Z49" s="22"/>
       <c r="AA49" s="22"/>
-    </row>
-    <row r="50" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB49" s="22"/>
+      <c r="AC49" s="22"/>
+    </row>
+    <row r="50" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A50" s="22"/>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
@@ -18364,8 +18465,10 @@
       <c r="Y50" s="22"/>
       <c r="Z50" s="22"/>
       <c r="AA50" s="22"/>
-    </row>
-    <row r="51" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB50" s="22"/>
+      <c r="AC50" s="22"/>
+    </row>
+    <row r="51" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A51" s="22"/>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
@@ -18393,8 +18496,10 @@
       <c r="Y51" s="22"/>
       <c r="Z51" s="22"/>
       <c r="AA51" s="22"/>
-    </row>
-    <row r="52" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB51" s="22"/>
+      <c r="AC51" s="22"/>
+    </row>
+    <row r="52" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A52" s="22"/>
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
@@ -18422,8 +18527,10 @@
       <c r="Y52" s="22"/>
       <c r="Z52" s="22"/>
       <c r="AA52" s="22"/>
-    </row>
-    <row r="53" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB52" s="22"/>
+      <c r="AC52" s="22"/>
+    </row>
+    <row r="53" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A53" s="22"/>
       <c r="B53" s="22"/>
       <c r="C53" s="22"/>
@@ -18451,8 +18558,10 @@
       <c r="Y53" s="22"/>
       <c r="Z53" s="22"/>
       <c r="AA53" s="22"/>
-    </row>
-    <row r="54" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB53" s="22"/>
+      <c r="AC53" s="22"/>
+    </row>
+    <row r="54" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A54" s="22"/>
       <c r="B54" s="22"/>
       <c r="C54" s="22"/>
@@ -18480,8 +18589,10 @@
       <c r="Y54" s="22"/>
       <c r="Z54" s="22"/>
       <c r="AA54" s="22"/>
-    </row>
-    <row r="55" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="AB54" s="22"/>
+      <c r="AC54" s="22"/>
+    </row>
+    <row r="55" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A55" s="22"/>
       <c r="B55" s="22"/>
       <c r="C55" s="22"/>
@@ -18509,416 +18620,1609 @@
       <c r="Y55" s="22"/>
       <c r="Z55" s="22"/>
       <c r="AA55" s="22"/>
-    </row>
-    <row r="56" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="65" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="66" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="67" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="68" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="69" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="70" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="71" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="72" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="73" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="74" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="75" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="76" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="77" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="78" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="79" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="80" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="81" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="82" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="83" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="84" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="85" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="86" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="87" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="88" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="89" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="90" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="91" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="92" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="93" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="94" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="95" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="96" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="97" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="98" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="99" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="100" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="101" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="102" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="103" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="104" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="105" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="106" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="107" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="108" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="109" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="110" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="111" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="112" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="113" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="114" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="115" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="116" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="117" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="118" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="119" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="120" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="121" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="122" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="123" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="124" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="125" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="126" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="127" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="128" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="129" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="130" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="131" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="132" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="133" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="134" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="135" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="136" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="137" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="138" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="139" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="140" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="141" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="142" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="143" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="144" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="145" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="146" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="147" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="148" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="149" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="150" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="151" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="152" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="153" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="154" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="155" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="156" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="157" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="158" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="159" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="160" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="161" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="162" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="163" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="164" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="165" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="166" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="167" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="168" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="169" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="170" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="171" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="172" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="173" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="174" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="175" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="176" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="177" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="178" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="179" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="180" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="181" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="182" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="183" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="184" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="185" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="186" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="187" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="188" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="189" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="190" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="191" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="192" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="193" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="194" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="195" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="196" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="197" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="198" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="199" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="200" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="201" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="202" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="203" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="204" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="205" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="206" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="207" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="208" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="209" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="210" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="211" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="212" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="213" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="214" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="215" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="216" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="217" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="218" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="219" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="220" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="221" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="222" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="223" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="224" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="225" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="226" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="227" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="228" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="229" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="230" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="231" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="232" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="233" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="234" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="235" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="236" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="237" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="238" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="239" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="240" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="241" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="242" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="243" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="244" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="245" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="246" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="247" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="248" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="249" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="250" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="251" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="252" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="253" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="254" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="255" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="256" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="257" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="258" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="259" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="260" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="261" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="262" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="263" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="264" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="265" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="266" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="267" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="268" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="269" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="270" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="271" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="272" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="273" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="274" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="275" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="276" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="277" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="278" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="279" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="280" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="281" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="282" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="283" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="284" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="285" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="286" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="287" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="288" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="289" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="290" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="291" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="292" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="293" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="294" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="295" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="296" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="297" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="298" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="299" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="300" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="301" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="302" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="303" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="304" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="305" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="306" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="307" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="308" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="309" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="310" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="311" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="312" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="313" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="314" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="315" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="316" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="317" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="318" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="319" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="320" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="321" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="322" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="323" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="324" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="325" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="326" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="327" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="328" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="329" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="330" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="331" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="332" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="333" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="334" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="335" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="336" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="337" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="338" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="339" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="340" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="341" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="342" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="343" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="344" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="345" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="346" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="347" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="348" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="349" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="350" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="351" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="352" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="353" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="354" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="355" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="356" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="357" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="358" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="359" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="360" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="361" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="362" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="363" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="364" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="365" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="366" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="367" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="368" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="369" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="370" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="371" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="372" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="373" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="374" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="375" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="376" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="377" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="378" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="379" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="380" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="381" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="382" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="383" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="384" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="385" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="386" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="387" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="388" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="389" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="390" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="391" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="392" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="393" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="394" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="395" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="396" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="397" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="398" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="399" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="400" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="401" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="402" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="403" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="404" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="405" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="406" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="407" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="408" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="409" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="410" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="411" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="412" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="413" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="414" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="415" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="416" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="417" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="418" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="419" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="420" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="421" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="422" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="423" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="424" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="425" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="426" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="427" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="428" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="429" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="430" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="431" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="432" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="433" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="434" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="435" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="436" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="437" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="438" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="439" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="440" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="441" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="442" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="443" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="444" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="445" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="446" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="447" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="448" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="449" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="450" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="451" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="452" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="453" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="454" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="455" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="456" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="457" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="458" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="459" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="460" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="461" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="462" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="463" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
-    <row r="464" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+      <c r="AB55" s="22"/>
+      <c r="AC55" s="22"/>
+    </row>
+    <row r="56" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N56" s="22"/>
+      <c r="O56" s="22"/>
+    </row>
+    <row r="57" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N57" s="22"/>
+      <c r="O57" s="22"/>
+    </row>
+    <row r="58" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N58" s="22"/>
+      <c r="O58" s="22"/>
+    </row>
+    <row r="59" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N59" s="22"/>
+      <c r="O59" s="22"/>
+    </row>
+    <row r="60" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N60" s="22"/>
+      <c r="O60" s="22"/>
+    </row>
+    <row r="61" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N61" s="22"/>
+      <c r="O61" s="22"/>
+    </row>
+    <row r="62" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N62" s="22"/>
+      <c r="O62" s="22"/>
+    </row>
+    <row r="63" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N63" s="22"/>
+      <c r="O63" s="22"/>
+    </row>
+    <row r="64" spans="1:29" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N64" s="22"/>
+      <c r="O64" s="22"/>
+    </row>
+    <row r="65" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N65" s="22"/>
+      <c r="O65" s="22"/>
+    </row>
+    <row r="66" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N66" s="22"/>
+      <c r="O66" s="22"/>
+    </row>
+    <row r="67" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N67" s="22"/>
+      <c r="O67" s="22"/>
+    </row>
+    <row r="68" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N68" s="22"/>
+      <c r="O68" s="22"/>
+    </row>
+    <row r="69" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N69" s="22"/>
+      <c r="O69" s="22"/>
+    </row>
+    <row r="70" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N70" s="22"/>
+      <c r="O70" s="22"/>
+    </row>
+    <row r="71" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N71" s="22"/>
+      <c r="O71" s="22"/>
+    </row>
+    <row r="72" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N72" s="22"/>
+      <c r="O72" s="22"/>
+    </row>
+    <row r="73" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N73" s="22"/>
+      <c r="O73" s="22"/>
+    </row>
+    <row r="74" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N74" s="22"/>
+      <c r="O74" s="22"/>
+    </row>
+    <row r="75" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N75" s="22"/>
+      <c r="O75" s="22"/>
+    </row>
+    <row r="76" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N76" s="22"/>
+      <c r="O76" s="22"/>
+    </row>
+    <row r="77" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N77" s="22"/>
+      <c r="O77" s="22"/>
+    </row>
+    <row r="78" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N78" s="22"/>
+      <c r="O78" s="22"/>
+    </row>
+    <row r="79" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N79" s="22"/>
+      <c r="O79" s="22"/>
+    </row>
+    <row r="80" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N80" s="22"/>
+      <c r="O80" s="22"/>
+    </row>
+    <row r="81" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N81" s="22"/>
+      <c r="O81" s="22"/>
+    </row>
+    <row r="82" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N82" s="22"/>
+      <c r="O82" s="22"/>
+    </row>
+    <row r="83" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N83" s="22"/>
+      <c r="O83" s="22"/>
+    </row>
+    <row r="84" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N84" s="22"/>
+      <c r="O84" s="22"/>
+    </row>
+    <row r="85" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N85" s="22"/>
+      <c r="O85" s="22"/>
+    </row>
+    <row r="86" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N86" s="22"/>
+      <c r="O86" s="22"/>
+    </row>
+    <row r="87" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N87" s="22"/>
+      <c r="O87" s="22"/>
+    </row>
+    <row r="88" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N88" s="22"/>
+      <c r="O88" s="22"/>
+    </row>
+    <row r="89" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N89" s="22"/>
+      <c r="O89" s="22"/>
+    </row>
+    <row r="90" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N90" s="22"/>
+      <c r="O90" s="22"/>
+    </row>
+    <row r="91" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N91" s="22"/>
+      <c r="O91" s="22"/>
+    </row>
+    <row r="92" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N92" s="22"/>
+      <c r="O92" s="22"/>
+    </row>
+    <row r="93" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N93" s="22"/>
+      <c r="O93" s="22"/>
+    </row>
+    <row r="94" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N94" s="22"/>
+      <c r="O94" s="22"/>
+    </row>
+    <row r="95" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N95" s="22"/>
+      <c r="O95" s="22"/>
+    </row>
+    <row r="96" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N96" s="22"/>
+      <c r="O96" s="22"/>
+    </row>
+    <row r="97" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N97" s="22"/>
+      <c r="O97" s="22"/>
+    </row>
+    <row r="98" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N98" s="22"/>
+      <c r="O98" s="22"/>
+    </row>
+    <row r="99" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N99" s="22"/>
+      <c r="O99" s="22"/>
+    </row>
+    <row r="100" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N100" s="22"/>
+      <c r="O100" s="22"/>
+    </row>
+    <row r="101" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N101" s="22"/>
+      <c r="O101" s="22"/>
+    </row>
+    <row r="102" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N102" s="22"/>
+      <c r="O102" s="22"/>
+    </row>
+    <row r="103" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N103" s="22"/>
+      <c r="O103" s="22"/>
+    </row>
+    <row r="104" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N104" s="22"/>
+      <c r="O104" s="22"/>
+    </row>
+    <row r="105" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N105" s="22"/>
+      <c r="O105" s="22"/>
+    </row>
+    <row r="106" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N106" s="22"/>
+      <c r="O106" s="22"/>
+    </row>
+    <row r="107" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N107" s="22"/>
+      <c r="O107" s="22"/>
+    </row>
+    <row r="108" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N108" s="22"/>
+      <c r="O108" s="22"/>
+    </row>
+    <row r="109" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N109" s="22"/>
+      <c r="O109" s="22"/>
+    </row>
+    <row r="110" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N110" s="22"/>
+      <c r="O110" s="22"/>
+    </row>
+    <row r="111" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N111" s="22"/>
+      <c r="O111" s="22"/>
+    </row>
+    <row r="112" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N112" s="22"/>
+      <c r="O112" s="22"/>
+    </row>
+    <row r="113" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N113" s="22"/>
+      <c r="O113" s="22"/>
+    </row>
+    <row r="114" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N114" s="22"/>
+      <c r="O114" s="22"/>
+    </row>
+    <row r="115" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N115" s="22"/>
+      <c r="O115" s="22"/>
+    </row>
+    <row r="116" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N116" s="22"/>
+      <c r="O116" s="22"/>
+    </row>
+    <row r="117" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N117" s="22"/>
+      <c r="O117" s="22"/>
+    </row>
+    <row r="118" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N118" s="22"/>
+      <c r="O118" s="22"/>
+    </row>
+    <row r="119" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N119" s="22"/>
+      <c r="O119" s="22"/>
+    </row>
+    <row r="120" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N120" s="22"/>
+      <c r="O120" s="22"/>
+    </row>
+    <row r="121" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N121" s="22"/>
+      <c r="O121" s="22"/>
+    </row>
+    <row r="122" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N122" s="22"/>
+      <c r="O122" s="22"/>
+    </row>
+    <row r="123" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N123" s="22"/>
+      <c r="O123" s="22"/>
+    </row>
+    <row r="124" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N124" s="22"/>
+      <c r="O124" s="22"/>
+    </row>
+    <row r="125" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N125" s="22"/>
+      <c r="O125" s="22"/>
+    </row>
+    <row r="126" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N126" s="22"/>
+      <c r="O126" s="22"/>
+    </row>
+    <row r="127" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N127" s="22"/>
+      <c r="O127" s="22"/>
+    </row>
+    <row r="128" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N128" s="22"/>
+      <c r="O128" s="22"/>
+    </row>
+    <row r="129" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N129" s="22"/>
+      <c r="O129" s="22"/>
+    </row>
+    <row r="130" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N130" s="22"/>
+      <c r="O130" s="22"/>
+    </row>
+    <row r="131" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N131" s="22"/>
+      <c r="O131" s="22"/>
+    </row>
+    <row r="132" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N132" s="22"/>
+      <c r="O132" s="22"/>
+    </row>
+    <row r="133" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N133" s="22"/>
+      <c r="O133" s="22"/>
+    </row>
+    <row r="134" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N134" s="22"/>
+      <c r="O134" s="22"/>
+    </row>
+    <row r="135" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N135" s="22"/>
+      <c r="O135" s="22"/>
+    </row>
+    <row r="136" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N136" s="22"/>
+      <c r="O136" s="22"/>
+    </row>
+    <row r="137" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N137" s="22"/>
+      <c r="O137" s="22"/>
+    </row>
+    <row r="138" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N138" s="22"/>
+      <c r="O138" s="22"/>
+    </row>
+    <row r="139" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N139" s="22"/>
+      <c r="O139" s="22"/>
+    </row>
+    <row r="140" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N140" s="22"/>
+      <c r="O140" s="22"/>
+    </row>
+    <row r="141" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N141" s="22"/>
+      <c r="O141" s="22"/>
+    </row>
+    <row r="142" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N142" s="22"/>
+      <c r="O142" s="22"/>
+    </row>
+    <row r="143" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N143" s="22"/>
+      <c r="O143" s="22"/>
+    </row>
+    <row r="144" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N144" s="22"/>
+      <c r="O144" s="22"/>
+    </row>
+    <row r="145" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N145" s="22"/>
+      <c r="O145" s="22"/>
+    </row>
+    <row r="146" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N146" s="22"/>
+      <c r="O146" s="22"/>
+    </row>
+    <row r="147" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N147" s="22"/>
+      <c r="O147" s="22"/>
+    </row>
+    <row r="148" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N148" s="22"/>
+      <c r="O148" s="22"/>
+    </row>
+    <row r="149" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N149" s="22"/>
+      <c r="O149" s="22"/>
+    </row>
+    <row r="150" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N150" s="22"/>
+      <c r="O150" s="22"/>
+    </row>
+    <row r="151" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N151" s="22"/>
+      <c r="O151" s="22"/>
+    </row>
+    <row r="152" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N152" s="22"/>
+      <c r="O152" s="22"/>
+    </row>
+    <row r="153" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N153" s="22"/>
+      <c r="O153" s="22"/>
+    </row>
+    <row r="154" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N154" s="22"/>
+      <c r="O154" s="22"/>
+    </row>
+    <row r="155" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N155" s="22"/>
+      <c r="O155" s="22"/>
+    </row>
+    <row r="156" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N156" s="22"/>
+      <c r="O156" s="22"/>
+    </row>
+    <row r="157" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N157" s="22"/>
+      <c r="O157" s="22"/>
+    </row>
+    <row r="158" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N158" s="22"/>
+      <c r="O158" s="22"/>
+    </row>
+    <row r="159" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N159" s="22"/>
+      <c r="O159" s="22"/>
+    </row>
+    <row r="160" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N160" s="22"/>
+      <c r="O160" s="22"/>
+    </row>
+    <row r="161" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N161" s="22"/>
+      <c r="O161" s="22"/>
+    </row>
+    <row r="162" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N162" s="22"/>
+      <c r="O162" s="22"/>
+    </row>
+    <row r="163" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N163" s="22"/>
+      <c r="O163" s="22"/>
+    </row>
+    <row r="164" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N164" s="22"/>
+      <c r="O164" s="22"/>
+    </row>
+    <row r="165" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N165" s="22"/>
+      <c r="O165" s="22"/>
+    </row>
+    <row r="166" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N166" s="22"/>
+      <c r="O166" s="22"/>
+    </row>
+    <row r="167" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N167" s="22"/>
+      <c r="O167" s="22"/>
+    </row>
+    <row r="168" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N168" s="22"/>
+      <c r="O168" s="22"/>
+    </row>
+    <row r="169" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N169" s="22"/>
+      <c r="O169" s="22"/>
+    </row>
+    <row r="170" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N170" s="22"/>
+      <c r="O170" s="22"/>
+    </row>
+    <row r="171" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N171" s="22"/>
+      <c r="O171" s="22"/>
+    </row>
+    <row r="172" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N172" s="22"/>
+      <c r="O172" s="22"/>
+    </row>
+    <row r="173" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N173" s="22"/>
+      <c r="O173" s="22"/>
+    </row>
+    <row r="174" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N174" s="22"/>
+      <c r="O174" s="22"/>
+    </row>
+    <row r="175" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N175" s="22"/>
+      <c r="O175" s="22"/>
+    </row>
+    <row r="176" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N176" s="22"/>
+      <c r="O176" s="22"/>
+    </row>
+    <row r="177" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N177" s="22"/>
+      <c r="O177" s="22"/>
+    </row>
+    <row r="178" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N178" s="22"/>
+      <c r="O178" s="22"/>
+    </row>
+    <row r="179" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N179" s="22"/>
+      <c r="O179" s="22"/>
+    </row>
+    <row r="180" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N180" s="22"/>
+      <c r="O180" s="22"/>
+    </row>
+    <row r="181" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N181" s="22"/>
+      <c r="O181" s="22"/>
+    </row>
+    <row r="182" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N182" s="22"/>
+      <c r="O182" s="22"/>
+    </row>
+    <row r="183" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N183" s="22"/>
+      <c r="O183" s="22"/>
+    </row>
+    <row r="184" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N184" s="22"/>
+      <c r="O184" s="22"/>
+    </row>
+    <row r="185" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N185" s="22"/>
+      <c r="O185" s="22"/>
+    </row>
+    <row r="186" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N186" s="22"/>
+      <c r="O186" s="22"/>
+    </row>
+    <row r="187" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N187" s="22"/>
+      <c r="O187" s="22"/>
+    </row>
+    <row r="188" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N188" s="22"/>
+      <c r="O188" s="22"/>
+    </row>
+    <row r="189" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N189" s="22"/>
+      <c r="O189" s="22"/>
+    </row>
+    <row r="190" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N190" s="22"/>
+      <c r="O190" s="22"/>
+    </row>
+    <row r="191" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N191" s="22"/>
+      <c r="O191" s="22"/>
+    </row>
+    <row r="192" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N192" s="22"/>
+      <c r="O192" s="22"/>
+    </row>
+    <row r="193" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N193" s="22"/>
+      <c r="O193" s="22"/>
+    </row>
+    <row r="194" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N194" s="22"/>
+      <c r="O194" s="22"/>
+    </row>
+    <row r="195" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N195" s="22"/>
+      <c r="O195" s="22"/>
+    </row>
+    <row r="196" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N196" s="22"/>
+      <c r="O196" s="22"/>
+    </row>
+    <row r="197" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N197" s="22"/>
+      <c r="O197" s="22"/>
+    </row>
+    <row r="198" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N198" s="22"/>
+      <c r="O198" s="22"/>
+    </row>
+    <row r="199" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N199" s="22"/>
+      <c r="O199" s="22"/>
+    </row>
+    <row r="200" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N200" s="22"/>
+      <c r="O200" s="22"/>
+    </row>
+    <row r="201" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N201" s="22"/>
+      <c r="O201" s="22"/>
+    </row>
+    <row r="202" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N202" s="22"/>
+      <c r="O202" s="22"/>
+    </row>
+    <row r="203" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N203" s="22"/>
+      <c r="O203" s="22"/>
+    </row>
+    <row r="204" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N204" s="22"/>
+      <c r="O204" s="22"/>
+    </row>
+    <row r="205" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N205" s="22"/>
+      <c r="O205" s="22"/>
+    </row>
+    <row r="206" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N206" s="22"/>
+      <c r="O206" s="22"/>
+    </row>
+    <row r="207" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N207" s="22"/>
+      <c r="O207" s="22"/>
+    </row>
+    <row r="208" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N208" s="22"/>
+      <c r="O208" s="22"/>
+    </row>
+    <row r="209" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N209" s="22"/>
+      <c r="O209" s="22"/>
+    </row>
+    <row r="210" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N210" s="22"/>
+      <c r="O210" s="22"/>
+    </row>
+    <row r="211" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N211" s="22"/>
+      <c r="O211" s="22"/>
+    </row>
+    <row r="212" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N212" s="22"/>
+      <c r="O212" s="22"/>
+    </row>
+    <row r="213" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N213" s="22"/>
+      <c r="O213" s="22"/>
+    </row>
+    <row r="214" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N214" s="22"/>
+      <c r="O214" s="22"/>
+    </row>
+    <row r="215" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N215" s="22"/>
+      <c r="O215" s="22"/>
+    </row>
+    <row r="216" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N216" s="22"/>
+      <c r="O216" s="22"/>
+    </row>
+    <row r="217" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N217" s="22"/>
+      <c r="O217" s="22"/>
+    </row>
+    <row r="218" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N218" s="22"/>
+      <c r="O218" s="22"/>
+    </row>
+    <row r="219" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N219" s="22"/>
+      <c r="O219" s="22"/>
+    </row>
+    <row r="220" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N220" s="22"/>
+      <c r="O220" s="22"/>
+    </row>
+    <row r="221" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N221" s="22"/>
+      <c r="O221" s="22"/>
+    </row>
+    <row r="222" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N222" s="22"/>
+      <c r="O222" s="22"/>
+    </row>
+    <row r="223" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N223" s="22"/>
+      <c r="O223" s="22"/>
+    </row>
+    <row r="224" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N224" s="22"/>
+      <c r="O224" s="22"/>
+    </row>
+    <row r="225" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N225" s="22"/>
+      <c r="O225" s="22"/>
+    </row>
+    <row r="226" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N226" s="22"/>
+      <c r="O226" s="22"/>
+    </row>
+    <row r="227" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N227" s="22"/>
+      <c r="O227" s="22"/>
+    </row>
+    <row r="228" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N228" s="22"/>
+      <c r="O228" s="22"/>
+    </row>
+    <row r="229" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N229" s="22"/>
+      <c r="O229" s="22"/>
+    </row>
+    <row r="230" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N230" s="22"/>
+      <c r="O230" s="22"/>
+    </row>
+    <row r="231" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N231" s="22"/>
+      <c r="O231" s="22"/>
+    </row>
+    <row r="232" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N232" s="22"/>
+      <c r="O232" s="22"/>
+    </row>
+    <row r="233" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N233" s="22"/>
+      <c r="O233" s="22"/>
+    </row>
+    <row r="234" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N234" s="22"/>
+      <c r="O234" s="22"/>
+    </row>
+    <row r="235" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N235" s="22"/>
+      <c r="O235" s="22"/>
+    </row>
+    <row r="236" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N236" s="22"/>
+      <c r="O236" s="22"/>
+    </row>
+    <row r="237" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N237" s="22"/>
+      <c r="O237" s="22"/>
+    </row>
+    <row r="238" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N238" s="22"/>
+      <c r="O238" s="22"/>
+    </row>
+    <row r="239" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N239" s="22"/>
+      <c r="O239" s="22"/>
+    </row>
+    <row r="240" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N240" s="22"/>
+      <c r="O240" s="22"/>
+    </row>
+    <row r="241" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N241" s="22"/>
+      <c r="O241" s="22"/>
+    </row>
+    <row r="242" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N242" s="22"/>
+      <c r="O242" s="22"/>
+    </row>
+    <row r="243" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N243" s="22"/>
+      <c r="O243" s="22"/>
+    </row>
+    <row r="244" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N244" s="22"/>
+      <c r="O244" s="22"/>
+    </row>
+    <row r="245" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N245" s="22"/>
+      <c r="O245" s="22"/>
+    </row>
+    <row r="246" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N246" s="22"/>
+      <c r="O246" s="22"/>
+    </row>
+    <row r="247" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N247" s="22"/>
+      <c r="O247" s="22"/>
+    </row>
+    <row r="248" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N248" s="22"/>
+      <c r="O248" s="22"/>
+    </row>
+    <row r="249" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N249" s="22"/>
+      <c r="O249" s="22"/>
+    </row>
+    <row r="250" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N250" s="22"/>
+      <c r="O250" s="22"/>
+    </row>
+    <row r="251" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N251" s="22"/>
+      <c r="O251" s="22"/>
+    </row>
+    <row r="252" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N252" s="22"/>
+      <c r="O252" s="22"/>
+    </row>
+    <row r="253" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N253" s="22"/>
+      <c r="O253" s="22"/>
+    </row>
+    <row r="254" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N254" s="22"/>
+      <c r="O254" s="22"/>
+    </row>
+    <row r="255" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N255" s="22"/>
+      <c r="O255" s="22"/>
+    </row>
+    <row r="256" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N256" s="22"/>
+      <c r="O256" s="22"/>
+    </row>
+    <row r="257" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N257" s="22"/>
+      <c r="O257" s="22"/>
+    </row>
+    <row r="258" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N258" s="22"/>
+      <c r="O258" s="22"/>
+    </row>
+    <row r="259" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N259" s="22"/>
+      <c r="O259" s="22"/>
+    </row>
+    <row r="260" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N260" s="22"/>
+      <c r="O260" s="22"/>
+    </row>
+    <row r="261" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N261" s="22"/>
+      <c r="O261" s="22"/>
+    </row>
+    <row r="262" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N262" s="22"/>
+      <c r="O262" s="22"/>
+    </row>
+    <row r="263" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N263" s="22"/>
+      <c r="O263" s="22"/>
+    </row>
+    <row r="264" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N264" s="22"/>
+      <c r="O264" s="22"/>
+    </row>
+    <row r="265" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N265" s="22"/>
+      <c r="O265" s="22"/>
+    </row>
+    <row r="266" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N266" s="22"/>
+      <c r="O266" s="22"/>
+    </row>
+    <row r="267" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N267" s="22"/>
+      <c r="O267" s="22"/>
+    </row>
+    <row r="268" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N268" s="22"/>
+      <c r="O268" s="22"/>
+    </row>
+    <row r="269" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N269" s="22"/>
+      <c r="O269" s="22"/>
+    </row>
+    <row r="270" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N270" s="22"/>
+      <c r="O270" s="22"/>
+    </row>
+    <row r="271" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N271" s="22"/>
+      <c r="O271" s="22"/>
+    </row>
+    <row r="272" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N272" s="22"/>
+      <c r="O272" s="22"/>
+    </row>
+    <row r="273" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N273" s="22"/>
+      <c r="O273" s="22"/>
+    </row>
+    <row r="274" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N274" s="22"/>
+      <c r="O274" s="22"/>
+    </row>
+    <row r="275" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N275" s="22"/>
+      <c r="O275" s="22"/>
+    </row>
+    <row r="276" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N276" s="22"/>
+      <c r="O276" s="22"/>
+    </row>
+    <row r="277" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N277" s="22"/>
+      <c r="O277" s="22"/>
+    </row>
+    <row r="278" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N278" s="22"/>
+      <c r="O278" s="22"/>
+    </row>
+    <row r="279" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N279" s="22"/>
+      <c r="O279" s="22"/>
+    </row>
+    <row r="280" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N280" s="22"/>
+      <c r="O280" s="22"/>
+    </row>
+    <row r="281" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N281" s="22"/>
+      <c r="O281" s="22"/>
+    </row>
+    <row r="282" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N282" s="22"/>
+      <c r="O282" s="22"/>
+    </row>
+    <row r="283" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N283" s="22"/>
+      <c r="O283" s="22"/>
+    </row>
+    <row r="284" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N284" s="22"/>
+      <c r="O284" s="22"/>
+    </row>
+    <row r="285" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N285" s="22"/>
+      <c r="O285" s="22"/>
+    </row>
+    <row r="286" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N286" s="22"/>
+      <c r="O286" s="22"/>
+    </row>
+    <row r="287" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N287" s="22"/>
+      <c r="O287" s="22"/>
+    </row>
+    <row r="288" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N288" s="22"/>
+      <c r="O288" s="22"/>
+    </row>
+    <row r="289" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N289" s="22"/>
+      <c r="O289" s="22"/>
+    </row>
+    <row r="290" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N290" s="22"/>
+      <c r="O290" s="22"/>
+    </row>
+    <row r="291" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N291" s="22"/>
+      <c r="O291" s="22"/>
+    </row>
+    <row r="292" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N292" s="22"/>
+      <c r="O292" s="22"/>
+    </row>
+    <row r="293" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N293" s="22"/>
+      <c r="O293" s="22"/>
+    </row>
+    <row r="294" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N294" s="22"/>
+      <c r="O294" s="22"/>
+    </row>
+    <row r="295" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N295" s="22"/>
+      <c r="O295" s="22"/>
+    </row>
+    <row r="296" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N296" s="22"/>
+      <c r="O296" s="22"/>
+    </row>
+    <row r="297" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N297" s="22"/>
+      <c r="O297" s="22"/>
+    </row>
+    <row r="298" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N298" s="22"/>
+      <c r="O298" s="22"/>
+    </row>
+    <row r="299" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N299" s="22"/>
+      <c r="O299" s="22"/>
+    </row>
+    <row r="300" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N300" s="22"/>
+      <c r="O300" s="22"/>
+    </row>
+    <row r="301" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N301" s="22"/>
+      <c r="O301" s="22"/>
+    </row>
+    <row r="302" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N302" s="22"/>
+      <c r="O302" s="22"/>
+    </row>
+    <row r="303" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N303" s="22"/>
+      <c r="O303" s="22"/>
+    </row>
+    <row r="304" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N304" s="22"/>
+      <c r="O304" s="22"/>
+    </row>
+    <row r="305" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N305" s="22"/>
+      <c r="O305" s="22"/>
+    </row>
+    <row r="306" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N306" s="22"/>
+      <c r="O306" s="22"/>
+    </row>
+    <row r="307" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N307" s="22"/>
+      <c r="O307" s="22"/>
+    </row>
+    <row r="308" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N308" s="22"/>
+      <c r="O308" s="22"/>
+    </row>
+    <row r="309" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N309" s="22"/>
+      <c r="O309" s="22"/>
+    </row>
+    <row r="310" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N310" s="22"/>
+      <c r="O310" s="22"/>
+    </row>
+    <row r="311" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N311" s="22"/>
+      <c r="O311" s="22"/>
+    </row>
+    <row r="312" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N312" s="22"/>
+      <c r="O312" s="22"/>
+    </row>
+    <row r="313" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N313" s="22"/>
+      <c r="O313" s="22"/>
+    </row>
+    <row r="314" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N314" s="22"/>
+      <c r="O314" s="22"/>
+    </row>
+    <row r="315" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N315" s="22"/>
+      <c r="O315" s="22"/>
+    </row>
+    <row r="316" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N316" s="22"/>
+      <c r="O316" s="22"/>
+    </row>
+    <row r="317" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N317" s="22"/>
+      <c r="O317" s="22"/>
+    </row>
+    <row r="318" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N318" s="22"/>
+      <c r="O318" s="22"/>
+    </row>
+    <row r="319" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N319" s="22"/>
+      <c r="O319" s="22"/>
+    </row>
+    <row r="320" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N320" s="22"/>
+      <c r="O320" s="22"/>
+    </row>
+    <row r="321" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N321" s="22"/>
+      <c r="O321" s="22"/>
+    </row>
+    <row r="322" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N322" s="22"/>
+      <c r="O322" s="22"/>
+    </row>
+    <row r="323" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N323" s="22"/>
+      <c r="O323" s="22"/>
+    </row>
+    <row r="324" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N324" s="22"/>
+      <c r="O324" s="22"/>
+    </row>
+    <row r="325" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N325" s="22"/>
+      <c r="O325" s="22"/>
+    </row>
+    <row r="326" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N326" s="22"/>
+      <c r="O326" s="22"/>
+    </row>
+    <row r="327" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N327" s="22"/>
+      <c r="O327" s="22"/>
+    </row>
+    <row r="328" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N328" s="22"/>
+      <c r="O328" s="22"/>
+    </row>
+    <row r="329" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N329" s="22"/>
+      <c r="O329" s="22"/>
+    </row>
+    <row r="330" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N330" s="22"/>
+      <c r="O330" s="22"/>
+    </row>
+    <row r="331" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N331" s="22"/>
+      <c r="O331" s="22"/>
+    </row>
+    <row r="332" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N332" s="22"/>
+      <c r="O332" s="22"/>
+    </row>
+    <row r="333" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N333" s="22"/>
+      <c r="O333" s="22"/>
+    </row>
+    <row r="334" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N334" s="22"/>
+      <c r="O334" s="22"/>
+    </row>
+    <row r="335" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N335" s="22"/>
+      <c r="O335" s="22"/>
+    </row>
+    <row r="336" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N336" s="22"/>
+      <c r="O336" s="22"/>
+    </row>
+    <row r="337" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N337" s="22"/>
+      <c r="O337" s="22"/>
+    </row>
+    <row r="338" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N338" s="22"/>
+      <c r="O338" s="22"/>
+    </row>
+    <row r="339" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N339" s="22"/>
+      <c r="O339" s="22"/>
+    </row>
+    <row r="340" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N340" s="22"/>
+      <c r="O340" s="22"/>
+    </row>
+    <row r="341" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N341" s="22"/>
+      <c r="O341" s="22"/>
+    </row>
+    <row r="342" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N342" s="22"/>
+      <c r="O342" s="22"/>
+    </row>
+    <row r="343" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N343" s="22"/>
+      <c r="O343" s="22"/>
+    </row>
+    <row r="344" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N344" s="22"/>
+      <c r="O344" s="22"/>
+    </row>
+    <row r="345" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N345" s="22"/>
+      <c r="O345" s="22"/>
+    </row>
+    <row r="346" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N346" s="22"/>
+      <c r="O346" s="22"/>
+    </row>
+    <row r="347" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N347" s="22"/>
+      <c r="O347" s="22"/>
+    </row>
+    <row r="348" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N348" s="22"/>
+      <c r="O348" s="22"/>
+    </row>
+    <row r="349" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N349" s="22"/>
+      <c r="O349" s="22"/>
+    </row>
+    <row r="350" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N350" s="22"/>
+      <c r="O350" s="22"/>
+    </row>
+    <row r="351" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N351" s="22"/>
+      <c r="O351" s="22"/>
+    </row>
+    <row r="352" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N352" s="22"/>
+      <c r="O352" s="22"/>
+    </row>
+    <row r="353" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N353" s="22"/>
+      <c r="O353" s="22"/>
+    </row>
+    <row r="354" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N354" s="22"/>
+      <c r="O354" s="22"/>
+    </row>
+    <row r="355" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N355" s="22"/>
+      <c r="O355" s="22"/>
+    </row>
+    <row r="356" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N356" s="22"/>
+      <c r="O356" s="22"/>
+    </row>
+    <row r="357" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N357" s="22"/>
+      <c r="O357" s="22"/>
+    </row>
+    <row r="358" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N358" s="22"/>
+      <c r="O358" s="22"/>
+    </row>
+    <row r="359" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N359" s="22"/>
+      <c r="O359" s="22"/>
+    </row>
+    <row r="360" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N360" s="22"/>
+      <c r="O360" s="22"/>
+    </row>
+    <row r="361" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N361" s="22"/>
+      <c r="O361" s="22"/>
+    </row>
+    <row r="362" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N362" s="22"/>
+      <c r="O362" s="22"/>
+    </row>
+    <row r="363" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N363" s="22"/>
+      <c r="O363" s="22"/>
+    </row>
+    <row r="364" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N364" s="22"/>
+      <c r="O364" s="22"/>
+    </row>
+    <row r="365" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N365" s="22"/>
+      <c r="O365" s="22"/>
+    </row>
+    <row r="366" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N366" s="22"/>
+      <c r="O366" s="22"/>
+    </row>
+    <row r="367" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N367" s="22"/>
+      <c r="O367" s="22"/>
+    </row>
+    <row r="368" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N368" s="22"/>
+      <c r="O368" s="22"/>
+    </row>
+    <row r="369" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N369" s="22"/>
+      <c r="O369" s="22"/>
+    </row>
+    <row r="370" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N370" s="22"/>
+      <c r="O370" s="22"/>
+    </row>
+    <row r="371" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N371" s="22"/>
+      <c r="O371" s="22"/>
+    </row>
+    <row r="372" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N372" s="22"/>
+      <c r="O372" s="22"/>
+    </row>
+    <row r="373" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N373" s="22"/>
+      <c r="O373" s="22"/>
+    </row>
+    <row r="374" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N374" s="22"/>
+      <c r="O374" s="22"/>
+    </row>
+    <row r="375" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N375" s="22"/>
+      <c r="O375" s="22"/>
+    </row>
+    <row r="376" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N376" s="22"/>
+      <c r="O376" s="22"/>
+    </row>
+    <row r="377" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N377" s="22"/>
+      <c r="O377" s="22"/>
+    </row>
+    <row r="378" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N378" s="22"/>
+      <c r="O378" s="22"/>
+    </row>
+    <row r="379" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N379" s="22"/>
+      <c r="O379" s="22"/>
+    </row>
+    <row r="380" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N380" s="22"/>
+      <c r="O380" s="22"/>
+    </row>
+    <row r="381" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N381" s="22"/>
+      <c r="O381" s="22"/>
+    </row>
+    <row r="382" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N382" s="22"/>
+      <c r="O382" s="22"/>
+    </row>
+    <row r="383" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N383" s="22"/>
+      <c r="O383" s="22"/>
+    </row>
+    <row r="384" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N384" s="22"/>
+      <c r="O384" s="22"/>
+    </row>
+    <row r="385" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N385" s="22"/>
+      <c r="O385" s="22"/>
+    </row>
+    <row r="386" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N386" s="22"/>
+      <c r="O386" s="22"/>
+    </row>
+    <row r="387" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N387" s="22"/>
+      <c r="O387" s="22"/>
+    </row>
+    <row r="388" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N388" s="22"/>
+      <c r="O388" s="22"/>
+    </row>
+    <row r="389" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N389" s="22"/>
+      <c r="O389" s="22"/>
+    </row>
+    <row r="390" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N390" s="22"/>
+      <c r="O390" s="22"/>
+    </row>
+    <row r="391" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N391" s="22"/>
+      <c r="O391" s="22"/>
+    </row>
+    <row r="392" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N392" s="22"/>
+      <c r="O392" s="22"/>
+    </row>
+    <row r="393" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N393" s="22"/>
+      <c r="O393" s="22"/>
+    </row>
+    <row r="394" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N394" s="22"/>
+      <c r="O394" s="22"/>
+    </row>
+    <row r="395" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N395" s="22"/>
+      <c r="O395" s="22"/>
+    </row>
+    <row r="396" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N396" s="22"/>
+      <c r="O396" s="22"/>
+    </row>
+    <row r="397" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N397" s="22"/>
+      <c r="O397" s="22"/>
+    </row>
+    <row r="398" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N398" s="22"/>
+      <c r="O398" s="22"/>
+    </row>
+    <row r="399" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N399" s="22"/>
+      <c r="O399" s="22"/>
+    </row>
+    <row r="400" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N400" s="22"/>
+      <c r="O400" s="22"/>
+    </row>
+    <row r="401" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N401" s="22"/>
+      <c r="O401" s="22"/>
+    </row>
+    <row r="402" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N402" s="22"/>
+      <c r="O402" s="22"/>
+    </row>
+    <row r="403" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N403" s="22"/>
+      <c r="O403" s="22"/>
+    </row>
+    <row r="404" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N404" s="22"/>
+      <c r="O404" s="22"/>
+    </row>
+    <row r="405" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N405" s="22"/>
+      <c r="O405" s="22"/>
+    </row>
+    <row r="406" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N406" s="22"/>
+      <c r="O406" s="22"/>
+    </row>
+    <row r="407" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N407" s="22"/>
+      <c r="O407" s="22"/>
+    </row>
+    <row r="408" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N408" s="22"/>
+      <c r="O408" s="22"/>
+    </row>
+    <row r="409" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N409" s="22"/>
+      <c r="O409" s="22"/>
+    </row>
+    <row r="410" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N410" s="22"/>
+      <c r="O410" s="22"/>
+    </row>
+    <row r="411" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N411" s="22"/>
+      <c r="O411" s="22"/>
+    </row>
+    <row r="412" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N412" s="22"/>
+      <c r="O412" s="22"/>
+    </row>
+    <row r="413" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N413" s="22"/>
+      <c r="O413" s="22"/>
+    </row>
+    <row r="414" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N414" s="22"/>
+      <c r="O414" s="22"/>
+    </row>
+    <row r="415" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N415" s="22"/>
+      <c r="O415" s="22"/>
+    </row>
+    <row r="416" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N416" s="22"/>
+      <c r="O416" s="22"/>
+    </row>
+    <row r="417" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N417" s="22"/>
+      <c r="O417" s="22"/>
+    </row>
+    <row r="418" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N418" s="22"/>
+      <c r="O418" s="22"/>
+    </row>
+    <row r="419" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N419" s="22"/>
+      <c r="O419" s="22"/>
+    </row>
+    <row r="420" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N420" s="22"/>
+      <c r="O420" s="22"/>
+    </row>
+    <row r="421" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N421" s="22"/>
+      <c r="O421" s="22"/>
+    </row>
+    <row r="422" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N422" s="22"/>
+      <c r="O422" s="22"/>
+    </row>
+    <row r="423" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N423" s="22"/>
+      <c r="O423" s="22"/>
+    </row>
+    <row r="424" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N424" s="22"/>
+      <c r="O424" s="22"/>
+    </row>
+    <row r="425" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N425" s="22"/>
+      <c r="O425" s="22"/>
+    </row>
+    <row r="426" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N426" s="22"/>
+      <c r="O426" s="22"/>
+    </row>
+    <row r="427" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N427" s="22"/>
+      <c r="O427" s="22"/>
+    </row>
+    <row r="428" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N428" s="22"/>
+      <c r="O428" s="22"/>
+    </row>
+    <row r="429" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N429" s="22"/>
+      <c r="O429" s="22"/>
+    </row>
+    <row r="430" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N430" s="22"/>
+      <c r="O430" s="22"/>
+    </row>
+    <row r="431" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N431" s="22"/>
+      <c r="O431" s="22"/>
+    </row>
+    <row r="432" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N432" s="22"/>
+      <c r="O432" s="22"/>
+    </row>
+    <row r="433" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N433" s="22"/>
+      <c r="O433" s="22"/>
+    </row>
+    <row r="434" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N434" s="22"/>
+      <c r="O434" s="22"/>
+    </row>
+    <row r="435" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N435" s="22"/>
+      <c r="O435" s="22"/>
+    </row>
+    <row r="436" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N436" s="22"/>
+      <c r="O436" s="22"/>
+    </row>
+    <row r="437" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N437" s="22"/>
+      <c r="O437" s="22"/>
+    </row>
+    <row r="438" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N438" s="22"/>
+      <c r="O438" s="22"/>
+    </row>
+    <row r="439" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N439" s="22"/>
+      <c r="O439" s="22"/>
+    </row>
+    <row r="440" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N440" s="22"/>
+      <c r="O440" s="22"/>
+    </row>
+    <row r="441" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N441" s="22"/>
+      <c r="O441" s="22"/>
+    </row>
+    <row r="442" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N442" s="22"/>
+      <c r="O442" s="22"/>
+    </row>
+    <row r="443" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N443" s="22"/>
+      <c r="O443" s="22"/>
+    </row>
+    <row r="444" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N444" s="22"/>
+      <c r="O444" s="22"/>
+    </row>
+    <row r="445" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N445" s="22"/>
+      <c r="O445" s="22"/>
+    </row>
+    <row r="446" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N446" s="22"/>
+      <c r="O446" s="22"/>
+    </row>
+    <row r="447" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N447" s="22"/>
+      <c r="O447" s="22"/>
+    </row>
+    <row r="448" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N448" s="22"/>
+      <c r="O448" s="22"/>
+    </row>
+    <row r="449" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N449" s="22"/>
+      <c r="O449" s="22"/>
+    </row>
+    <row r="450" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N450" s="22"/>
+      <c r="O450" s="22"/>
+    </row>
+    <row r="451" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N451" s="22"/>
+      <c r="O451" s="22"/>
+    </row>
+    <row r="452" spans="14:15" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="N452" s="22"/>
+      <c r="O452" s="22"/>
+    </row>
+    <row r="453" spans="14:15" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="454" spans="14:15" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="455" spans="14:15" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="456" spans="14:15" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="457" spans="14:15" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="458" spans="14:15" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="459" spans="14:15" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="460" spans="14:15" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="461" spans="14:15" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="462" spans="14:15" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="463" spans="14:15" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
+    <row r="464" spans="14:15" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="465" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="466" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
     <row r="467" s="5" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -19271,7 +20575,7 @@
           <x14:formula1>
             <xm:f>Report!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M216</xm:sqref>
+          <xm:sqref>M2:M216 N35:N216 N2:N33 O2:O33 O35:O216</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -37023,8 +38327,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84:C85"/>
+    <sheetView topLeftCell="M79" workbookViewId="0">
+      <selection activeCell="S106" sqref="S106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
investigated the failures and kept comments on failed ones
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxiang\dev\surveyor-qa\selenium-wd\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\surveyor-qa\selenium-wd\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37023,8 +37023,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84:C85"/>
+    <sheetView tabSelected="1" topLeftCell="Q45" workbookViewId="0">
+      <selection activeCell="V81" sqref="V81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41810,7 +41810,7 @@
         <v>8</v>
       </c>
       <c r="V81" s="22">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="W81" s="22"/>
       <c r="X81" s="22"/>

</xml_diff>

<commit_message>
changes to run high load test cases with different combinations of input param
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -625,7 +625,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="519">
   <si>
     <t>Enabled</t>
   </si>
@@ -2896,7 +2896,7 @@
   <dimension ref="A1:P1138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15842,8 +15842,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AA801"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R49" sqref="R49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20039,7 +20039,7 @@
   <dimension ref="A1:AB578"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37122,8 +37122,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView topLeftCell="O90" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="S107" sqref="S107:S112"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U111" sqref="U111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43711,8 +43712,8 @@
       <c r="U107" s="40">
         <v>10</v>
       </c>
-      <c r="V107" s="40" t="s">
-        <v>190</v>
+      <c r="V107" s="43">
+        <v>25</v>
       </c>
     </row>
     <row r="108" spans="1:24" s="42" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -43796,16 +43797,20 @@
         <v>22</v>
       </c>
       <c r="H109" s="40"/>
-      <c r="I109" s="40"/>
-      <c r="J109" s="40"/>
-      <c r="K109" s="40"/>
-      <c r="L109" s="40"/>
-      <c r="M109" s="40" t="s">
-        <v>185</v>
-      </c>
-      <c r="N109" s="40" t="s">
-        <v>186</v>
-      </c>
+      <c r="I109" s="43">
+        <v>29.757819448754098</v>
+      </c>
+      <c r="J109" s="43">
+        <v>-95.353906211853001</v>
+      </c>
+      <c r="K109" s="43">
+        <v>29.7362085557276</v>
+      </c>
+      <c r="L109" s="43">
+        <v>-95.381543693542397</v>
+      </c>
+      <c r="M109" s="40"/>
+      <c r="N109" s="40"/>
       <c r="O109" s="40"/>
       <c r="P109" s="40"/>
       <c r="Q109" s="40">
@@ -43932,8 +43937,8 @@
       <c r="T111" s="40">
         <v>7</v>
       </c>
-      <c r="U111" s="40">
-        <v>10</v>
+      <c r="U111" s="43">
+        <v>8</v>
       </c>
       <c r="V111" s="40" t="s">
         <v>190</v>

</xml_diff>

<commit_message>
fixes for setting correct highlight checkbox values in report view
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20136" windowHeight="8148" tabRatio="799" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20136" windowHeight="8148" tabRatio="799" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -32,6 +32,9 @@
     <sheet name="Survey" sheetId="9" r:id="rId18"/>
     <sheet name="Report" sheetId="10" r:id="rId19"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId20"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2169,7 +2172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -2424,7 +2427,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2481,7 +2484,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1 2" xfId="7"/>
@@ -2507,6 +2509,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Survey"/>
+      <sheetName val="General"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2585,23 +2602,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2637,23 +2637,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -15843,7 +15826,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[localTestCaseData.xlsx]General!#REF!</xm:f>
+            <xm:f>[1]General!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>H36 J36</xm:sqref>
         </x14:dataValidation>
@@ -15858,8 +15841,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AC800"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15869,7 +15852,7 @@
     <col min="3" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5546875" customWidth="1"/>
     <col min="9" max="9" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="10.44140625" customWidth="1"/>
@@ -15969,8 +15952,12 @@
       <c r="M2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
+      <c r="N2" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="P2" s="2" t="s">
         <v>110</v>
       </c>
@@ -16015,8 +16002,12 @@
       <c r="M3" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
+      <c r="N3" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="P3" s="29" t="s">
         <v>111</v>
       </c>
@@ -16061,8 +16052,12 @@
       <c r="M4" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
+      <c r="N4" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="22" t="s">
         <v>112</v>
       </c>
@@ -16120,8 +16115,12 @@
       <c r="M5" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
+      <c r="N5" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P5" s="22" t="s">
         <v>113</v>
       </c>
@@ -16179,8 +16178,12 @@
       <c r="M6" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
+      <c r="N6" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P6" s="22" t="s">
         <v>290</v>
       </c>
@@ -16238,8 +16241,12 @@
       <c r="M7" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
+      <c r="N7" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P7" s="22" t="s">
         <v>293</v>
       </c>
@@ -16297,8 +16304,12 @@
       <c r="M8" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
+      <c r="N8" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O8" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P8" s="22" t="s">
         <v>292</v>
       </c>
@@ -16356,8 +16367,12 @@
       <c r="M9" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
+      <c r="N9" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P9" s="22" t="s">
         <v>291</v>
       </c>
@@ -16415,8 +16430,12 @@
       <c r="M10" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
+      <c r="N10" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P10" s="22" t="s">
         <v>174</v>
       </c>
@@ -16474,8 +16493,12 @@
       <c r="M11" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
+      <c r="N11" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="P11" s="22" t="s">
         <v>187</v>
       </c>
@@ -16533,8 +16556,12 @@
       <c r="M12" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
+      <c r="N12" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P12" s="22" t="s">
         <v>188</v>
       </c>
@@ -16592,8 +16619,12 @@
       <c r="M13" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
+      <c r="N13" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="P13" s="22" t="s">
         <v>366</v>
       </c>
@@ -16651,8 +16682,12 @@
       <c r="M14" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
+      <c r="N14" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P14" s="22" t="s">
         <v>192</v>
       </c>
@@ -16710,8 +16745,12 @@
       <c r="M15" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
+      <c r="N15" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O15" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P15" s="22" t="s">
         <v>272</v>
       </c>
@@ -16769,8 +16808,12 @@
       <c r="M16" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
+      <c r="N16" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O16" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P16" s="22" t="s">
         <v>276</v>
       </c>
@@ -16828,8 +16871,12 @@
       <c r="M17" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
+      <c r="N17" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="P17" s="22" t="s">
         <v>364</v>
       </c>
@@ -16887,8 +16934,12 @@
       <c r="M18" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
+      <c r="N18" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="22" t="s">
         <v>365</v>
       </c>
@@ -16946,8 +16997,12 @@
       <c r="M19" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
+      <c r="N19" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O19" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P19" s="22" t="s">
         <v>283</v>
       </c>
@@ -17005,8 +17060,12 @@
       <c r="M20" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
+      <c r="N20" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O20" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P20" s="22" t="s">
         <v>287</v>
       </c>
@@ -17064,8 +17123,12 @@
       <c r="M21" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
+      <c r="N21" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O21" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P21" s="22" t="s">
         <v>288</v>
       </c>
@@ -17123,8 +17186,12 @@
       <c r="M22" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
+      <c r="N22" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O22" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P22" s="22" t="s">
         <v>289</v>
       </c>
@@ -17182,8 +17249,12 @@
       <c r="M23" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
+      <c r="N23" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O23" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P23" s="22" t="s">
         <v>294</v>
       </c>
@@ -17241,8 +17312,12 @@
       <c r="M24" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
+      <c r="N24" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O24" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P24" s="22" t="s">
         <v>295</v>
       </c>
@@ -17300,8 +17375,12 @@
       <c r="M25" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
+      <c r="N25" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O25" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P25" s="22" t="s">
         <v>298</v>
       </c>
@@ -17359,8 +17438,12 @@
       <c r="M26" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
+      <c r="N26" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O26" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P26" s="22" t="s">
         <v>299</v>
       </c>
@@ -17418,8 +17501,12 @@
       <c r="M27" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
+      <c r="N27" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O27" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P27" s="22" t="s">
         <v>300</v>
       </c>
@@ -17477,8 +17564,12 @@
       <c r="M28" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
+      <c r="N28" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O28" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="P28" s="22" t="s">
         <v>437</v>
       </c>
@@ -17536,8 +17627,12 @@
       <c r="M29" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
+      <c r="N29" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O29" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P29" s="22" t="s">
         <v>438</v>
       </c>
@@ -17595,8 +17690,12 @@
       <c r="M30" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
+      <c r="N30" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O30" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="P30" s="22" t="s">
         <v>302</v>
       </c>
@@ -17654,8 +17753,12 @@
       <c r="M31" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
+      <c r="N31" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O31" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P31" s="22" t="s">
         <v>310</v>
       </c>
@@ -17713,8 +17816,12 @@
       <c r="M32" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
+      <c r="N32" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O32" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P32" s="22" t="s">
         <v>314</v>
       </c>
@@ -17772,8 +17879,12 @@
       <c r="M33" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
+      <c r="N33" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O33" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="P33" s="22" t="s">
         <v>318</v>
       </c>
@@ -17831,8 +17942,8 @@
       <c r="M34" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N34" s="38" t="b">
-        <v>0</v>
+      <c r="N34" s="22" t="b">
+        <v>1</v>
       </c>
       <c r="O34" s="22" t="b">
         <v>0</v>
@@ -17894,8 +18005,12 @@
       <c r="M35" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
+      <c r="N35" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O35" s="22" t="b">
+        <v>1</v>
+      </c>
       <c r="P35" s="22" t="s">
         <v>323</v>
       </c>
@@ -17953,6 +18068,12 @@
       <c r="M36" s="22" t="s">
         <v>83</v>
       </c>
+      <c r="N36" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O36" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P36" s="22" t="s">
         <v>406</v>
       </c>
@@ -17997,6 +18118,12 @@
       <c r="M37" s="22" t="s">
         <v>84</v>
       </c>
+      <c r="N37" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O37" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P37" s="22" t="s">
         <v>444</v>
       </c>
@@ -18041,6 +18168,12 @@
       <c r="M38" s="22" t="s">
         <v>83</v>
       </c>
+      <c r="N38" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O38" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P38" s="22" t="s">
         <v>407</v>
       </c>
@@ -18085,6 +18218,12 @@
       <c r="M39" s="22" t="s">
         <v>84</v>
       </c>
+      <c r="N39" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O39" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P39" s="22" t="s">
         <v>408</v>
       </c>
@@ -18129,6 +18268,12 @@
       <c r="M40" s="22" t="s">
         <v>83</v>
       </c>
+      <c r="N40" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O40" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P40" s="22" t="s">
         <v>409</v>
       </c>
@@ -18173,6 +18318,12 @@
       <c r="M41" s="22" t="s">
         <v>83</v>
       </c>
+      <c r="N41" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O41" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P41" s="22" t="s">
         <v>301</v>
       </c>
@@ -18217,6 +18368,12 @@
       <c r="M42" s="22" t="s">
         <v>83</v>
       </c>
+      <c r="N42" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O42" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P42" s="22" t="s">
         <v>288</v>
       </c>
@@ -18261,8 +18418,12 @@
       <c r="M43" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N43" s="22"/>
-      <c r="O43" s="22"/>
+      <c r="N43" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O43" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P43" s="22" t="s">
         <v>485</v>
       </c>
@@ -18320,8 +18481,12 @@
       <c r="M44" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="N44" s="37"/>
-      <c r="O44" s="37"/>
+      <c r="N44" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="O44" s="22" t="b">
+        <v>0</v>
+      </c>
       <c r="P44" s="35" t="s">
         <v>486</v>
       </c>
@@ -20626,13 +20791,13 @@
           <x14:formula1>
             <xm:f>General!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:L218</xm:sqref>
+          <xm:sqref>C2:L218 N2:N986 O2:O1605</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Report!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M216 N35:N216 N2:N33 O2:O33 O35:O216</xm:sqref>
+          <xm:sqref>M2:M216</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -38387,31 +38552,31 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[localTestCaseData.xlsx]Survey!#REF!</xm:f>
+            <xm:f>[1]Survey!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>F52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[localTestCaseData.xlsx]Survey!#REF!</xm:f>
+            <xm:f>[1]Survey!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>C52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[localTestCaseData.xlsx]Survey!#REF!</xm:f>
+            <xm:f>[1]Survey!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[localTestCaseData.xlsx]Survey!#REF!</xm:f>
+            <xm:f>[1]Survey!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[localTestCaseData.xlsx]Survey!#REF!</xm:f>
+            <xm:f>[1]Survey!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G52</xm:sqref>
         </x14:dataValidation>
@@ -38426,7 +38591,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
pagetest6 fixes + fix unit test mode
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20136" windowHeight="8148" tabRatio="799" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20136" windowHeight="8148" tabRatio="799" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -628,7 +628,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="514">
   <si>
     <t>Enabled</t>
   </si>
@@ -1980,9 +1980,6 @@
     <t>32,26,27,30</t>
   </si>
   <si>
-    <t>29d38a22e2d14a70931d</t>
-  </si>
-  <si>
     <t>perf01</t>
   </si>
   <si>
@@ -2167,6 +2164,12 @@
   </si>
   <si>
     <t>TC210_survey</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>5ae5a88e1a6f49c29072</t>
   </si>
 </sst>
 </file>
@@ -2874,8 +2877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1138"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:K36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3040,7 +3043,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H6" s="22" t="b">
         <v>0</v>
@@ -3060,7 +3063,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="H7" s="22" t="b">
         <v>0</v>
@@ -3080,7 +3083,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H8" s="22" t="b">
         <v>0</v>
@@ -3100,7 +3103,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H9" s="22" t="b">
         <v>0</v>
@@ -3120,7 +3123,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H10" s="22" t="b">
         <v>0</v>
@@ -3140,7 +3143,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H11" s="22" t="b">
         <v>0</v>
@@ -3160,7 +3163,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H12" s="22" t="b">
         <v>0</v>
@@ -3180,7 +3183,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H13" s="22" t="b">
         <v>0</v>
@@ -3200,7 +3203,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H14" s="22" t="b">
         <v>0</v>
@@ -3641,7 +3644,7 @@
       <c r="B35" s="33"/>
       <c r="C35" s="33"/>
       <c r="D35" s="33" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E35" s="33"/>
       <c r="F35" s="33"/>
@@ -3671,7 +3674,7 @@
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
       <c r="D36" s="22" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
@@ -15841,7 +15844,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AC800"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
@@ -15903,10 +15906,10 @@
         <v>81</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>510</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>511</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>89</v>
@@ -18383,7 +18386,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C43" s="22" t="b">
         <v>0</v>
@@ -18425,7 +18428,7 @@
         <v>0</v>
       </c>
       <c r="P43" s="22" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q43" s="22"/>
       <c r="R43" s="22"/>
@@ -18488,7 +18491,7 @@
         <v>0</v>
       </c>
       <c r="P44" s="35" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="Q44" s="35"/>
       <c r="R44" s="35"/>
@@ -21334,7 +21337,7 @@
         <v>22</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -23285,10 +23288,10 @@
         <v>362</v>
       </c>
       <c r="F15" s="33" t="s">
+        <v>506</v>
+      </c>
+      <c r="G15" s="33" t="s">
         <v>507</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>508</v>
       </c>
       <c r="H15" s="33"/>
       <c r="I15" s="33" t="s">
@@ -23355,10 +23358,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23677,6 +23680,56 @@
       </c>
       <c r="P6" s="7">
         <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="C7" s="22">
+        <v>37.402092570550302</v>
+      </c>
+      <c r="D7" s="22">
+        <v>-121.98482039739901</v>
+      </c>
+      <c r="E7" s="22">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F7" s="22">
+        <v>5</v>
+      </c>
+      <c r="G7" s="22">
+        <v>5</v>
+      </c>
+      <c r="H7" s="22">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="I7" s="22">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="J7" s="22">
+        <v>-43</v>
+      </c>
+      <c r="K7" s="22">
+        <v>-40</v>
+      </c>
+      <c r="L7" s="22">
+        <v>-30</v>
+      </c>
+      <c r="M7" s="22">
+        <v>-25</v>
+      </c>
+      <c r="N7" s="22">
+        <v>2</v>
+      </c>
+      <c r="O7" s="22">
+        <v>10</v>
+      </c>
+      <c r="P7" s="22">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -33191,7 +33244,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C52" s="22" t="s">
         <v>19</v>
@@ -38591,8 +38644,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50:V50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39403,7 +39456,7 @@
         <v>11</v>
       </c>
       <c r="S13" s="22" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="T13" s="22">
         <v>7</v>
@@ -40069,7 +40122,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>177</v>
@@ -40132,7 +40185,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>177</v>
@@ -40195,7 +40248,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>177</v>
@@ -40258,7 +40311,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>177</v>
@@ -40321,7 +40374,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>177</v>
@@ -40384,7 +40437,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C30" s="22" t="s">
         <v>177</v>
@@ -40447,7 +40500,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>177</v>
@@ -40510,7 +40563,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C32" s="22" t="s">
         <v>177</v>
@@ -40573,7 +40626,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>177</v>
@@ -40636,7 +40689,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C34" s="22" t="s">
         <v>177</v>
@@ -40699,7 +40752,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C35" s="22" t="s">
         <v>177</v>
@@ -40762,7 +40815,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C36" s="22" t="s">
         <v>177</v>
@@ -40825,7 +40878,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C37" s="22" t="s">
         <v>177</v>
@@ -41647,7 +41700,7 @@
         <v>325</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>450</v>
+        <v>513</v>
       </c>
       <c r="D50" s="22">
         <v>1</v>
@@ -41683,13 +41736,13 @@
         <v>11</v>
       </c>
       <c r="S50" s="22">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="T50" s="22">
         <v>2</v>
       </c>
       <c r="U50" s="22">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="V50" s="22">
         <v>4</v>
@@ -43270,10 +43323,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="22" t="s">
+        <v>474</v>
+      </c>
+      <c r="C80" s="22" t="s">
         <v>475</v>
-      </c>
-      <c r="C80" s="22" t="s">
-        <v>476</v>
       </c>
       <c r="D80" s="22">
         <v>6</v>
@@ -43309,7 +43362,7 @@
         <v>11</v>
       </c>
       <c r="S80" s="22" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="T80" s="22">
         <v>1</v>
@@ -43326,7 +43379,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="22" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C81" s="22" t="s">
         <v>177</v>
@@ -43369,7 +43422,7 @@
         <v>11</v>
       </c>
       <c r="S81" s="22" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="T81" s="22">
         <v>1</v>
@@ -43391,7 +43444,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C82" s="22" t="s">
         <v>177</v>
@@ -43456,7 +43509,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C83" s="22" t="s">
         <v>177</v>
@@ -43499,7 +43552,7 @@
         <v>11</v>
       </c>
       <c r="S83" s="22" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="T83" s="22">
         <v>1</v>
@@ -43521,7 +43574,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="22" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C84" s="22" t="s">
         <v>177</v>
@@ -43586,7 +43639,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C85" s="22" t="s">
         <v>177</v>
@@ -43638,7 +43691,7 @@
         <v>4</v>
       </c>
       <c r="V85" s="22" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="W85" s="22"/>
       <c r="X85" s="22"/>
@@ -43651,7 +43704,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C86" s="19" t="s">
         <v>177</v>
@@ -43713,7 +43766,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="36" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C87" s="33" t="s">
         <v>177</v>
@@ -43780,7 +43833,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="36" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C88" s="33" t="s">
         <v>177</v>
@@ -43847,7 +43900,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="36" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C89" s="33" t="s">
         <v>177</v>
@@ -43914,7 +43967,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="33" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C90" s="33" t="s">
         <v>177</v>
@@ -43951,7 +44004,7 @@
         <v>11</v>
       </c>
       <c r="S90" s="33" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="T90" s="33">
         <v>1</v>
@@ -43973,7 +44026,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="36" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C91" s="33" t="s">
         <v>177</v>
@@ -44040,7 +44093,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="33" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C92" s="33" t="s">
         <v>177</v>
@@ -44077,7 +44130,7 @@
         <v>11</v>
       </c>
       <c r="S92" s="33" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="T92" s="33">
         <v>1</v>
@@ -44099,7 +44152,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="36" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C93" s="33" t="s">
         <v>177</v>
@@ -44166,7 +44219,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="36" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C94" s="33" t="s">
         <v>177</v>
@@ -44233,7 +44286,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="36" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C95" s="33" t="s">
         <v>177</v>
@@ -44300,7 +44353,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="36" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C96" s="33" t="s">
         <v>177</v>
@@ -44367,7 +44420,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="36" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C97" s="33" t="s">
         <v>177</v>
@@ -44434,7 +44487,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="36" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C98" s="33" t="s">
         <v>177</v>
@@ -44501,7 +44554,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="36" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C99" s="33" t="s">
         <v>177</v>
@@ -44568,7 +44621,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="36" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C100" s="33" t="s">
         <v>177</v>
@@ -44635,7 +44688,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="36" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C101" s="33" t="s">
         <v>177</v>
@@ -44702,7 +44755,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="36" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C102" s="33" t="s">
         <v>177</v>
@@ -44769,7 +44822,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="36" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C103" s="33" t="s">
         <v>177</v>
@@ -44836,7 +44889,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="36" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C104" s="33" t="s">
         <v>177</v>
@@ -44903,7 +44956,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="36" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C105" s="33" t="s">
         <v>177</v>
@@ -44970,7 +45023,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="36" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C106" s="33" t="s">
         <v>177</v>

</xml_diff>

<commit_message>
add file content comparison for .prj shape files
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -38645,7 +38645,7 @@
   <dimension ref="A1:AA2827"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50:V50"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41702,9 +41702,6 @@
       <c r="C50" s="22" t="s">
         <v>513</v>
       </c>
-      <c r="D50" s="22">
-        <v>1</v>
-      </c>
       <c r="E50" s="22" t="s">
         <v>354</v>
       </c>

</xml_diff>

<commit_message>
fixes for some failing driver view tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -625,7 +625,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="515">
   <si>
     <t>Enabled</t>
   </si>
@@ -2165,6 +2165,12 @@
   <si>
     <t>Highlight GAP Assets</t>
   </si>
+  <si>
+    <t>01_Surveyor-man.db3</t>
+  </si>
+  <si>
+    <t>EthaneStnd</t>
+  </si>
 </sst>
 </file>
 
@@ -2424,7 +2430,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2493,6 +2499,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1 2" xfId="7"/>
@@ -2866,10 +2874,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1138"/>
+  <dimension ref="A1:Z1138"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3600,7 +3608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A33" s="22">
         <v>32</v>
       </c>
@@ -3614,7 +3622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" s="22" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A34" s="22">
         <v>33</v>
       </c>
@@ -3628,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" s="34" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="33">
         <v>34</v>
       </c>
@@ -3658,7 +3666,7 @@
       <c r="O35" s="33"/>
       <c r="P35" s="33"/>
     </row>
-    <row r="36" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="38">
         <v>35</v>
       </c>
@@ -3688,18 +3696,45 @@
       <c r="O36" s="38"/>
       <c r="P36" s="38"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A37" s="48">
+        <v>36</v>
+      </c>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48" t="s">
+        <v>514</v>
+      </c>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48">
+        <v>2</v>
+      </c>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48">
+        <v>0</v>
+      </c>
+      <c r="L37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="49"/>
+      <c r="O37" s="49"/>
+      <c r="P37" s="49"/>
+      <c r="Q37" s="49"/>
+      <c r="R37" s="49"/>
+      <c r="S37" s="49"/>
+      <c r="T37" s="49"/>
+      <c r="U37" s="49"/>
+      <c r="V37" s="49"/>
+      <c r="W37" s="49"/>
+      <c r="X37" s="49"/>
+      <c r="Y37" s="49"/>
+      <c r="Z37" s="49"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -3710,7 +3745,7 @@
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -3721,7 +3756,7 @@
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -3732,7 +3767,7 @@
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -3743,7 +3778,7 @@
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -3754,7 +3789,7 @@
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
@@ -3765,7 +3800,7 @@
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -3776,7 +3811,7 @@
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
@@ -3787,7 +3822,7 @@
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -3798,7 +3833,7 @@
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -3809,7 +3844,7 @@
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -15834,7 +15869,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AA800"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -22720,7 +22755,7 @@
   <dimension ref="A1:AB1069"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23099,7 +23134,7 @@
         <v>126</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>267</v>
+        <v>513</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Updated constants for timezone
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\surveyor-qa\selenium-wd\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxiang\dev\surveyor-qa\selenium-wd\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="12" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -29,8 +29,9 @@
     <sheet name="Report Opt Tabular PDF Content" sheetId="12" r:id="rId15"/>
     <sheet name="Roles" sheetId="6" r:id="rId16"/>
     <sheet name="General" sheetId="7" r:id="rId17"/>
-    <sheet name="Survey" sheetId="9" r:id="rId18"/>
-    <sheet name="Report" sheetId="10" r:id="rId19"/>
+    <sheet name="Timezone" sheetId="24" r:id="rId18"/>
+    <sheet name="Survey" sheetId="9" r:id="rId19"/>
+    <sheet name="Report" sheetId="10" r:id="rId20"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -625,7 +626,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="533">
   <si>
     <t>Enabled</t>
   </si>
@@ -2174,11 +2175,62 @@
   <si>
     <t>UNIT_TEST_RUN</t>
   </si>
+  <si>
+    <t>Atlantic Standard Time</t>
+  </si>
+  <si>
+    <t>Argentina Standard Time</t>
+  </si>
+  <si>
+    <t>GMT Standard Time</t>
+  </si>
+  <si>
+    <t>Coordinated Universal Time</t>
+  </si>
+  <si>
+    <t>W. Europe Standard Time</t>
+  </si>
+  <si>
+    <t>Central European Standard Time</t>
+  </si>
+  <si>
+    <t>E. Europe Standard Time</t>
+  </si>
+  <si>
+    <t>E. Africa Standard Time</t>
+  </si>
+  <si>
+    <t>Pakistan Standard Time</t>
+  </si>
+  <si>
+    <t>Bangladesh Standard Time</t>
+  </si>
+  <si>
+    <t>SE Asia Standard Time</t>
+  </si>
+  <si>
+    <t>Tokyo Standard Time</t>
+  </si>
+  <si>
+    <t>E. Australia Standard Time</t>
+  </si>
+  <si>
+    <t>Central Pacific Standard Time</t>
+  </si>
+  <si>
+    <t>New Zealand Standard Time</t>
+  </si>
+  <si>
+    <t>Hawaiian Standard Time</t>
+  </si>
+  <si>
+    <t>Alaskan Standard Time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -2433,7 +2485,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2504,6 +2556,8 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1 2" xfId="7"/>
@@ -2607,6 +2661,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2642,6 +2713,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -20222,7 +20310,7 @@
   <dimension ref="A1:AB578"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21137,6 +21225,7 @@
     <row r="578" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -21244,6 +21333,1875 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B578"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.44140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" style="42" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="6"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="6"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="6"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="6"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="6"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="6"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="6"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="6"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="6"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="6"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="6"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="6"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="6"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="6"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="6"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="6"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="6"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="6"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="6"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="6"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="6"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="6"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="6"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="6"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="6"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="6"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="6"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="6"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="6"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="6"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="6"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="6"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="6"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="6"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="6"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="6"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="6"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="6"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="6"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="6"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="6"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="6"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" s="6"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" s="6"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" s="6"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" s="6"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" s="6"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" s="6"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="6"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" s="6"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" s="6"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" s="6"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="6"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" s="6"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="6"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="6"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" s="6"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" s="6"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" s="6"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" s="6"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" s="6"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" s="6"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" s="6"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" s="6"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" s="6"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" s="6"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" s="6"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" s="6"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" s="6"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" s="6"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" s="6"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" s="6"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" s="6"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" s="6"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" s="6"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" s="6"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" s="6"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" s="6"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" s="6"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" s="6"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="6"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" s="6"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" s="6"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" s="6"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" s="6"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" s="6"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" s="6"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" s="6"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" s="6"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" s="6"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" s="6"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" s="6"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" s="6"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" s="6"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" s="6"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" s="6"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" s="6"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" s="6"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" s="6"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" s="6"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" s="6"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" s="6"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" s="6"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" s="6"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" s="6"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" s="6"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" s="6"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" s="6"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" s="6"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" s="6"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" s="6"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" s="6"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" s="6"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" s="6"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" s="6"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164" s="6"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165" s="6"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166" s="6"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167" s="6"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168" s="6"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169" s="6"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170" s="6"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" s="6"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172" s="6"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173" s="6"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174" s="6"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175" s="6"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176" s="6"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177" s="6"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178" s="6"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179" s="6"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180" s="6"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181" s="6"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182" s="6"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183" s="6"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184" s="6"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A185" s="6"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186" s="6"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187" s="6"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A188" s="6"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189" s="6"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A190" s="6"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191" s="6"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A192" s="6"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193" s="6"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194" s="6"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195" s="6"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196" s="6"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197" s="6"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198" s="6"/>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199" s="6"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A200" s="6"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A201" s="6"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A202" s="6"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A203" s="6"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A204" s="6"/>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A205" s="6"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206" s="6"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A207" s="6"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A208" s="6"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A209" s="6"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A210" s="6"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A211" s="6"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A212" s="6"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A213" s="6"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A214" s="6"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A215" s="6"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A216" s="6"/>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A217" s="6"/>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A218" s="6"/>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A219" s="6"/>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A220" s="6"/>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A221" s="6"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A222" s="6"/>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A223" s="6"/>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A224" s="6"/>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A225" s="6"/>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A226" s="6"/>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A227" s="6"/>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A228" s="6"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A229" s="6"/>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A230" s="6"/>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A231" s="6"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A232" s="6"/>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A233" s="6"/>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A234" s="6"/>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A235" s="6"/>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A236" s="6"/>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A237" s="6"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A238" s="6"/>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A239" s="6"/>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A240" s="6"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A241" s="6"/>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A242" s="6"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A243" s="6"/>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A244" s="6"/>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A245" s="6"/>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A246" s="6"/>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A247" s="6"/>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A248" s="6"/>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A249" s="6"/>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A250" s="6"/>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A251" s="6"/>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A252" s="6"/>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A253" s="6"/>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A254" s="6"/>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A255" s="6"/>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A256" s="6"/>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A257" s="6"/>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A258" s="6"/>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A259" s="6"/>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A260" s="6"/>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A261" s="6"/>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A262" s="6"/>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A263" s="6"/>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A264" s="6"/>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A265" s="6"/>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A266" s="6"/>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A267" s="6"/>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A268" s="6"/>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A269" s="6"/>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A270" s="6"/>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A271" s="6"/>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A272" s="6"/>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A273" s="6"/>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A274" s="6"/>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A275" s="6"/>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A276" s="6"/>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A277" s="6"/>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A278" s="6"/>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A279" s="6"/>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A280" s="6"/>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A281" s="6"/>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A282" s="6"/>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A283" s="6"/>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A284" s="6"/>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A285" s="6"/>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A286" s="6"/>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A287" s="6"/>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A288" s="6"/>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A289" s="6"/>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A290" s="6"/>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A291" s="6"/>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A292" s="6"/>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A293" s="6"/>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A294" s="6"/>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A295" s="6"/>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A296" s="6"/>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A297" s="6"/>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A298" s="6"/>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A299" s="6"/>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A300" s="6"/>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A301" s="6"/>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A302" s="6"/>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A303" s="6"/>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A304" s="6"/>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A305" s="6"/>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A306" s="6"/>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A307" s="6"/>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A308" s="6"/>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A309" s="6"/>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A310" s="6"/>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A311" s="6"/>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A312" s="6"/>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A313" s="6"/>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A314" s="6"/>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A315" s="6"/>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A316" s="6"/>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A317" s="6"/>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A318" s="6"/>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A319" s="6"/>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A320" s="6"/>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A321" s="6"/>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A322" s="6"/>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A323" s="6"/>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A324" s="6"/>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A325" s="6"/>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A326" s="6"/>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A327" s="6"/>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A328" s="6"/>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A329" s="6"/>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A330" s="6"/>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A331" s="6"/>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A332" s="6"/>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A333" s="6"/>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A334" s="6"/>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A335" s="6"/>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A336" s="6"/>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A337" s="6"/>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A338" s="6"/>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A339" s="6"/>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A340" s="6"/>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A341" s="6"/>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A342" s="6"/>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A343" s="6"/>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A344" s="6"/>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A345" s="6"/>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A346" s="6"/>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A347" s="6"/>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A348" s="6"/>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A349" s="6"/>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A350" s="6"/>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A351" s="6"/>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A352" s="6"/>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A353" s="6"/>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A354" s="6"/>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A355" s="6"/>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A356" s="6"/>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A357" s="6"/>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A358" s="6"/>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A359" s="6"/>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A360" s="6"/>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A361" s="6"/>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A362" s="6"/>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A363" s="6"/>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A364" s="6"/>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A365" s="6"/>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A366" s="6"/>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A367" s="6"/>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A368" s="6"/>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A369" s="6"/>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A370" s="6"/>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A371" s="6"/>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A372" s="6"/>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A373" s="6"/>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A374" s="6"/>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A375" s="6"/>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A376" s="6"/>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A377" s="6"/>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A378" s="6"/>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A379" s="6"/>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A380" s="6"/>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A381" s="6"/>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A382" s="6"/>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A383" s="6"/>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A384" s="6"/>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A385" s="6"/>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A386" s="6"/>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A387" s="6"/>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A388" s="6"/>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A389" s="6"/>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A390" s="6"/>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A391" s="6"/>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A392" s="6"/>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A393" s="6"/>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A394" s="6"/>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A395" s="6"/>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A396" s="6"/>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A397" s="6"/>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A398" s="6"/>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A399" s="6"/>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A400" s="6"/>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A401" s="6"/>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A402" s="6"/>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A403" s="6"/>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A404" s="6"/>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A405" s="6"/>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A406" s="6"/>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A407" s="6"/>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A408" s="6"/>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A409" s="6"/>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A410" s="6"/>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A411" s="6"/>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A412" s="6"/>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A413" s="6"/>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A414" s="6"/>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A415" s="6"/>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A416" s="6"/>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A417" s="6"/>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A418" s="6"/>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A419" s="6"/>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A420" s="6"/>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A421" s="6"/>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A422" s="6"/>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A423" s="6"/>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A424" s="6"/>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A425" s="6"/>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A426" s="6"/>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A427" s="6"/>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A428" s="6"/>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A429" s="6"/>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A430" s="6"/>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A431" s="6"/>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A432" s="6"/>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A433" s="6"/>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A434" s="6"/>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A435" s="6"/>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A436" s="6"/>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A437" s="6"/>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A438" s="6"/>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A439" s="6"/>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A440" s="6"/>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A441" s="6"/>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A442" s="6"/>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A443" s="6"/>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A444" s="6"/>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A445" s="6"/>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A446" s="6"/>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A447" s="6"/>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A448" s="6"/>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A449" s="6"/>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A450" s="6"/>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A451" s="6"/>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A452" s="6"/>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A453" s="6"/>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A454" s="6"/>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A455" s="6"/>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A456" s="6"/>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A457" s="6"/>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A458" s="6"/>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A459" s="6"/>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A460" s="6"/>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A461" s="6"/>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A462" s="6"/>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A463" s="6"/>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A464" s="6"/>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A465" s="6"/>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A466" s="6"/>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A467" s="6"/>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A468" s="6"/>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A469" s="6"/>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A470" s="6"/>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A471" s="6"/>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A472" s="6"/>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A473" s="6"/>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A474" s="6"/>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A475" s="6"/>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A476" s="6"/>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A477" s="6"/>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A478" s="6"/>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A479" s="6"/>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A480" s="6"/>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A481" s="6"/>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A482" s="6"/>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A483" s="6"/>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A484" s="6"/>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A485" s="6"/>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A486" s="6"/>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A487" s="6"/>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A488" s="6"/>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A489" s="6"/>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A490" s="6"/>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A491" s="6"/>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A492" s="6"/>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A493" s="6"/>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A494" s="6"/>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A495" s="6"/>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A496" s="6"/>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A497" s="6"/>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A498" s="6"/>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A499" s="6"/>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A500" s="6"/>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A501" s="6"/>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A502" s="6"/>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A503" s="6"/>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A504" s="6"/>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A505" s="6"/>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A506" s="6"/>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A507" s="6"/>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A508" s="6"/>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A509" s="6"/>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A510" s="6"/>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A511" s="6"/>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A512" s="6"/>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A513" s="6"/>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A514" s="6"/>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A515" s="6"/>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A516" s="6"/>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A517" s="6"/>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A518" s="6"/>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A519" s="6"/>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A520" s="6"/>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A521" s="6"/>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A522" s="6"/>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A523" s="6"/>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A524" s="6"/>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A525" s="6"/>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A526" s="6"/>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A527" s="6"/>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A528" s="6"/>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A529" s="6"/>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A530" s="6"/>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A531" s="6"/>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A532" s="6"/>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A533" s="6"/>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A534" s="6"/>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A535" s="6"/>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A536" s="6"/>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A537" s="6"/>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A538" s="6"/>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A539" s="6"/>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A540" s="6"/>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A541" s="6"/>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A542" s="6"/>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A543" s="6"/>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A544" s="6"/>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A545" s="6"/>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A546" s="6"/>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A547" s="6"/>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A548" s="6"/>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A549" s="6"/>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A550" s="6"/>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A551" s="6"/>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A552" s="6"/>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A553" s="6"/>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A554" s="6"/>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A555" s="6"/>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A556" s="6"/>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A557" s="6"/>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A558" s="6"/>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A559" s="6"/>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A560" s="6"/>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A561" s="6"/>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A562" s="6"/>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A563" s="6"/>
+    </row>
+    <row r="564" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A564" s="6"/>
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A565" s="6"/>
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A566" s="6"/>
+    </row>
+    <row r="567" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A567" s="6"/>
+    </row>
+    <row r="568" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A568" s="6"/>
+    </row>
+    <row r="569" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A569" s="6"/>
+    </row>
+    <row r="570" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A570" s="6"/>
+    </row>
+    <row r="571" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A571" s="6"/>
+    </row>
+    <row r="572" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A572" s="6"/>
+    </row>
+    <row r="573" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A573" s="6"/>
+    </row>
+    <row r="574" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A574" s="6"/>
+    </row>
+    <row r="575" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A575" s="6"/>
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A576" s="6"/>
+    </row>
+    <row r="577" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A577" s="6"/>
+    </row>
+    <row r="578" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A578" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -21327,124 +23285,6 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>353</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>354</v>
-      </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>355</v>
-      </c>
-      <c r="C5" t="s">
-        <v>225</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>356</v>
-      </c>
-      <c r="C6" t="s">
-        <v>226</v>
-      </c>
       <c r="D6" t="s">
         <v>42</v>
       </c>
@@ -21514,6 +23354,124 @@
       </c>
       <c r="D3" s="7">
         <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet11"/>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>355</v>
+      </c>
+      <c r="C5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>356</v>
+      </c>
+      <c r="C6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -22757,7 +24715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1069"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -37315,7 +39273,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Enabled TC210 in complianceReportsPageTest5
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -32808,7 +32808,7 @@
   <dimension ref="A1:AB1073"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fixes for few of failing simulator based tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -149,7 +149,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Shirish Pulikkal:</t>
         </r>
@@ -158,7 +158,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Use this column for dynamically generated Analyzers.
@@ -2276,7 +2276,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2389,19 +2389,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -19276,8 +19263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39871,8 +39858,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40169,7 +40156,7 @@
         <v>3</v>
       </c>
       <c r="L8" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:26" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40201,7 +40188,7 @@
         <v>3</v>
       </c>
       <c r="L9" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:26" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -40233,7 +40220,7 @@
         <v>3</v>
       </c>
       <c r="L10" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:26" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
@@ -41102,8 +41089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1069"/>
   <sheetViews>
-    <sheetView topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -50262,7 +50249,7 @@
   <dimension ref="A1:AB1073"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
bug fixes - simulator based tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\surveyor-qa\selenium-wd\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -627,7 +627,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="551">
   <si>
     <t>Enabled</t>
   </si>
@@ -2967,7 +2967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -41513,7 +41513,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD16"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42810,8 +42810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1069"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1069"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43597,35 +43597,23 @@
       <c r="AA32" s="55"/>
       <c r="AB32" s="55"/>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+    <row r="33" spans="1:28" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="67">
+        <v>32</v>
+      </c>
+      <c r="B33" s="67" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="67" t="s">
+        <v>26</v>
+      </c>
       <c r="F33" s="70"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="21"/>
-      <c r="Q33" s="21"/>
-      <c r="R33" s="21"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
-      <c r="U33" s="21"/>
-      <c r="V33" s="21"/>
-      <c r="W33" s="21"/>
-      <c r="X33" s="21"/>
-      <c r="Y33" s="21"/>
-      <c r="Z33" s="21"/>
-      <c r="AA33" s="21"/>
-      <c r="AB33" s="21"/>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" s="21"/>
@@ -51991,8 +51979,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AB1073"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD53"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updates in test data & test case sheet post defect fixes (DE1636, DE1646, DE1852, DE1484)
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -42810,8 +42810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1069"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51979,8 +51979,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AB1073"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52500,9 +52500,11 @@
         <v>39</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="26" spans="1:8" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
@@ -52672,7 +52674,10 @@
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0.1</v>
       </c>
     </row>
     <row r="34" spans="1:28" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed fialues in ObserverViewPageTest
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -2303,7 +2303,7 @@
     <t>sqapicsu</t>
   </si>
   <si>
-    <t>Surveyor-LisaAndMain.db3</t>
+    <t>NoIndications.db3</t>
   </si>
 </sst>
 </file>
@@ -41582,7 +41582,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42993,8 +42993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1069"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
intial changes for parallel parameterized support for compliance report test
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sxiang\dev\surveyor-qa\selenium-wd\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\surveyor-qa\selenium-wd\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="12" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -626,7 +626,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="539">
   <si>
     <t>Enabled</t>
   </si>
@@ -2226,6 +2226,24 @@
   <si>
     <t>Alaskan Standard Time</t>
   </si>
+  <si>
+    <t>TC243-1</t>
+  </si>
+  <si>
+    <t>TC243-2</t>
+  </si>
+  <si>
+    <t>TC243-3</t>
+  </si>
+  <si>
+    <t>TC243-4</t>
+  </si>
+  <si>
+    <t>TC243-5</t>
+  </si>
+  <si>
+    <t>11,15,18</t>
+  </si>
 </sst>
 </file>
 
@@ -15961,7 +15979,7 @@
   <dimension ref="A1:AA800"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21335,8 +21353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B578"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39273,8 +39291,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S111" sqref="S111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45714,135 +45733,270 @@
       <c r="Z106" s="33"/>
       <c r="AA106" s="33"/>
     </row>
-    <row r="107" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A107" s="19"/>
-      <c r="B107" s="19"/>
-      <c r="C107" s="19"/>
-      <c r="D107" s="19"/>
-      <c r="E107" s="19"/>
-      <c r="F107" s="19"/>
-      <c r="G107" s="19"/>
-      <c r="H107" s="19"/>
-      <c r="I107" s="19"/>
-      <c r="J107" s="19"/>
-      <c r="K107" s="19"/>
-      <c r="L107" s="19"/>
-      <c r="M107" s="19"/>
-      <c r="N107" s="19"/>
-      <c r="O107" s="19"/>
-      <c r="P107" s="19"/>
-      <c r="Q107" s="19"/>
-      <c r="R107" s="19"/>
-      <c r="S107" s="19"/>
-      <c r="T107" s="19"/>
-      <c r="U107" s="19"/>
-      <c r="V107" s="19"/>
-      <c r="W107" s="19"/>
-      <c r="X107" s="19"/>
-    </row>
-    <row r="108" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A108" s="19"/>
-      <c r="B108" s="19"/>
-      <c r="C108" s="19"/>
-      <c r="D108" s="19"/>
-      <c r="E108" s="19"/>
-      <c r="F108" s="19"/>
-      <c r="G108" s="19"/>
-      <c r="H108" s="19"/>
-      <c r="I108" s="19"/>
-      <c r="J108" s="19"/>
-      <c r="K108" s="19"/>
-      <c r="L108" s="19"/>
-      <c r="M108" s="19"/>
-      <c r="N108" s="19"/>
-      <c r="O108" s="19"/>
-      <c r="P108" s="19"/>
-      <c r="Q108" s="19"/>
-      <c r="R108" s="19"/>
-      <c r="S108" s="19"/>
-      <c r="T108" s="19"/>
-      <c r="U108" s="19"/>
-      <c r="V108" s="19"/>
-      <c r="W108" s="19"/>
-      <c r="X108" s="19"/>
-    </row>
-    <row r="109" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A109" s="19"/>
-      <c r="B109" s="19"/>
-      <c r="C109" s="19"/>
-      <c r="D109" s="19"/>
-      <c r="E109" s="19"/>
-      <c r="F109" s="19"/>
-      <c r="G109" s="19"/>
-      <c r="H109" s="19"/>
-      <c r="I109" s="19"/>
-      <c r="J109" s="19"/>
-      <c r="K109" s="19"/>
-      <c r="L109" s="19"/>
-      <c r="M109" s="19"/>
-      <c r="N109" s="19"/>
-      <c r="O109" s="19"/>
-      <c r="P109" s="19"/>
-      <c r="Q109" s="19"/>
-      <c r="R109" s="19"/>
-      <c r="S109" s="19"/>
-      <c r="T109" s="19"/>
-      <c r="U109" s="19"/>
-      <c r="V109" s="19"/>
-      <c r="W109" s="19"/>
-      <c r="X109" s="19"/>
-    </row>
-    <row r="110" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A110" s="19"/>
-      <c r="B110" s="19"/>
-      <c r="C110" s="19"/>
-      <c r="D110" s="19"/>
-      <c r="E110" s="19"/>
-      <c r="F110" s="19"/>
-      <c r="G110" s="19"/>
-      <c r="H110" s="19"/>
-      <c r="I110" s="19"/>
-      <c r="J110" s="19"/>
-      <c r="K110" s="19"/>
-      <c r="L110" s="19"/>
-      <c r="M110" s="19"/>
-      <c r="N110" s="19"/>
-      <c r="O110" s="19"/>
-      <c r="P110" s="19"/>
-      <c r="Q110" s="19"/>
-      <c r="R110" s="19"/>
-      <c r="S110" s="19"/>
-      <c r="T110" s="19"/>
-      <c r="U110" s="19"/>
-      <c r="V110" s="19"/>
-      <c r="W110" s="19"/>
-      <c r="X110" s="19"/>
-    </row>
-    <row r="111" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A111" s="19"/>
-      <c r="B111" s="19"/>
-      <c r="C111" s="19"/>
-      <c r="D111" s="19"/>
-      <c r="E111" s="19"/>
-      <c r="F111" s="19"/>
-      <c r="G111" s="19"/>
-      <c r="H111" s="19"/>
-      <c r="I111" s="19"/>
-      <c r="J111" s="19"/>
-      <c r="K111" s="19"/>
-      <c r="L111" s="19"/>
-      <c r="M111" s="19"/>
-      <c r="N111" s="19"/>
-      <c r="O111" s="19"/>
-      <c r="P111" s="19"/>
-      <c r="Q111" s="19"/>
-      <c r="R111" s="19"/>
-      <c r="S111" s="19"/>
-      <c r="T111" s="19"/>
-      <c r="U111" s="19"/>
-      <c r="V111" s="19"/>
-      <c r="W111" s="19"/>
-      <c r="X111" s="19"/>
+    <row r="107" spans="1:27" s="46" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A107" s="46">
+        <v>106</v>
+      </c>
+      <c r="B107" s="46" t="s">
+        <v>533</v>
+      </c>
+      <c r="C107" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="D107" s="46">
+        <v>1</v>
+      </c>
+      <c r="E107" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="F107" s="46">
+        <v>0</v>
+      </c>
+      <c r="G107" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K107" s="47">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L107" s="47">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="O107" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="P107" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="Q107" s="46">
+        <v>8.5</v>
+      </c>
+      <c r="R107" s="46">
+        <v>11</v>
+      </c>
+      <c r="S107" s="46" t="s">
+        <v>538</v>
+      </c>
+      <c r="T107" s="46">
+        <v>1</v>
+      </c>
+      <c r="U107" s="46">
+        <v>1</v>
+      </c>
+      <c r="V107" s="46" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="108" spans="1:27" s="46" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A108" s="46">
+        <v>107</v>
+      </c>
+      <c r="B108" s="46" t="s">
+        <v>534</v>
+      </c>
+      <c r="C108" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="D108" s="46">
+        <v>1</v>
+      </c>
+      <c r="E108" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="F108" s="46">
+        <v>0</v>
+      </c>
+      <c r="G108" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K108" s="47">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L108" s="47">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="O108" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="P108" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="Q108" s="46">
+        <v>8.5</v>
+      </c>
+      <c r="R108" s="46">
+        <v>11</v>
+      </c>
+      <c r="S108" s="46" t="s">
+        <v>538</v>
+      </c>
+      <c r="T108" s="46">
+        <v>1</v>
+      </c>
+      <c r="U108" s="46">
+        <v>1</v>
+      </c>
+      <c r="V108" s="46" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="109" spans="1:27" s="46" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A109" s="46">
+        <v>108</v>
+      </c>
+      <c r="B109" s="46" t="s">
+        <v>535</v>
+      </c>
+      <c r="C109" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="D109" s="46">
+        <v>1</v>
+      </c>
+      <c r="E109" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="F109" s="46">
+        <v>0</v>
+      </c>
+      <c r="G109" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K109" s="47">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L109" s="47">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="O109" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="P109" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="Q109" s="46">
+        <v>8.5</v>
+      </c>
+      <c r="R109" s="46">
+        <v>11</v>
+      </c>
+      <c r="S109" s="46" t="s">
+        <v>538</v>
+      </c>
+      <c r="T109" s="46">
+        <v>1</v>
+      </c>
+      <c r="U109" s="46">
+        <v>1</v>
+      </c>
+      <c r="V109" s="46" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="110" spans="1:27" s="46" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A110" s="46">
+        <v>109</v>
+      </c>
+      <c r="B110" s="46" t="s">
+        <v>536</v>
+      </c>
+      <c r="C110" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="D110" s="46">
+        <v>1</v>
+      </c>
+      <c r="E110" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="F110" s="46">
+        <v>0</v>
+      </c>
+      <c r="G110" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K110" s="47">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L110" s="47">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="O110" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="P110" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="Q110" s="46">
+        <v>8.5</v>
+      </c>
+      <c r="R110" s="46">
+        <v>11</v>
+      </c>
+      <c r="S110" s="46" t="s">
+        <v>538</v>
+      </c>
+      <c r="T110" s="46">
+        <v>1</v>
+      </c>
+      <c r="U110" s="46">
+        <v>1</v>
+      </c>
+      <c r="V110" s="46" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="111" spans="1:27" s="46" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A111" s="46">
+        <v>110</v>
+      </c>
+      <c r="B111" s="46" t="s">
+        <v>537</v>
+      </c>
+      <c r="C111" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="D111" s="46">
+        <v>1</v>
+      </c>
+      <c r="E111" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="F111" s="46">
+        <v>0</v>
+      </c>
+      <c r="G111" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="K111" s="47">
+        <v>37.415700000000001</v>
+      </c>
+      <c r="L111" s="47">
+        <v>-121.98390000000001</v>
+      </c>
+      <c r="O111" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="P111" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="Q111" s="46">
+        <v>8.5</v>
+      </c>
+      <c r="R111" s="46">
+        <v>11</v>
+      </c>
+      <c r="S111" s="46" t="s">
+        <v>538</v>
+      </c>
+      <c r="T111" s="46">
+        <v>1</v>
+      </c>
+      <c r="U111" s="46">
+        <v>1</v>
+      </c>
+      <c r="V111" s="46" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="112" spans="1:27" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A112" s="19"/>

</xml_diff>

<commit_message>
Updated view selection for boundary checkbox
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="9" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -627,7 +627,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="564">
   <si>
     <t>Enabled</t>
   </si>
@@ -2299,6 +2299,27 @@
   <si>
     <t>sqapicsu</t>
   </si>
+  <si>
+    <t>TC175</t>
+  </si>
+  <si>
+    <t>debug_175</t>
+  </si>
+  <si>
+    <t>TC183</t>
+  </si>
+  <si>
+    <t>TC191</t>
+  </si>
+  <si>
+    <t>debug_183</t>
+  </si>
+  <si>
+    <t>debug_191</t>
+  </si>
+  <si>
+    <t>31,37</t>
+  </si>
 </sst>
 </file>
 
@@ -2587,7 +2608,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2704,6 +2725,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="11" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="11"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="20% - Accent1 2" xfId="7"/>
@@ -3029,18 +3051,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
     <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3123,6 +3145,11 @@
       <c r="F4" s="59" t="s">
         <v>330</v>
       </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="68"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3135,9 +3162,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J104" sqref="J104"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T113" sqref="T113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9977,80 +10004,182 @@
       </c>
     </row>
     <row r="113" spans="1:24" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A113" s="18"/>
-      <c r="B113" s="18"/>
-      <c r="C113" s="18"/>
-      <c r="D113" s="18"/>
-      <c r="E113" s="18"/>
-      <c r="F113" s="18"/>
-      <c r="G113" s="18"/>
-      <c r="H113" s="18"/>
-      <c r="I113" s="18"/>
-      <c r="J113" s="18"/>
-      <c r="K113" s="18"/>
-      <c r="L113" s="18"/>
-      <c r="M113" s="18"/>
-      <c r="N113" s="18"/>
-      <c r="O113" s="18"/>
-      <c r="P113" s="18"/>
-      <c r="Q113" s="18"/>
-      <c r="R113" s="18"/>
-      <c r="S113" s="18"/>
-      <c r="T113" s="18"/>
-      <c r="U113" s="18"/>
-      <c r="V113" s="18"/>
+      <c r="A113" s="18">
+        <v>112</v>
+      </c>
+      <c r="B113" s="18" t="s">
+        <v>557</v>
+      </c>
+      <c r="C113" s="18" t="s">
+        <v>558</v>
+      </c>
+      <c r="D113" s="18">
+        <v>2</v>
+      </c>
+      <c r="E113" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="F113" s="65">
+        <v>0</v>
+      </c>
+      <c r="G113" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="H113" s="65"/>
+      <c r="I113" s="65">
+        <v>29.757819448754098</v>
+      </c>
+      <c r="J113" s="65">
+        <v>-95.353906211853001</v>
+      </c>
+      <c r="K113" s="65">
+        <v>29.7362085557276</v>
+      </c>
+      <c r="L113" s="65">
+        <v>-95.381543693542397</v>
+      </c>
+      <c r="M113" s="65"/>
+      <c r="N113" s="65"/>
+      <c r="O113" s="65"/>
+      <c r="P113" s="65"/>
+      <c r="Q113" s="65">
+        <v>40</v>
+      </c>
+      <c r="R113" s="65">
+        <v>40</v>
+      </c>
+      <c r="S113" s="65">
+        <v>44</v>
+      </c>
+      <c r="T113" s="65">
+        <v>6</v>
+      </c>
+      <c r="U113" s="65">
+        <v>5</v>
+      </c>
+      <c r="V113" s="65">
+        <v>23</v>
+      </c>
       <c r="W113" s="18"/>
       <c r="X113" s="18"/>
     </row>
     <row r="114" spans="1:24" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A114" s="18"/>
-      <c r="B114" s="18"/>
-      <c r="C114" s="18"/>
-      <c r="D114" s="18"/>
-      <c r="E114" s="18"/>
-      <c r="F114" s="18"/>
-      <c r="G114" s="18"/>
-      <c r="H114" s="18"/>
-      <c r="I114" s="18"/>
-      <c r="J114" s="18"/>
-      <c r="K114" s="18"/>
-      <c r="L114" s="18"/>
-      <c r="M114" s="18"/>
-      <c r="N114" s="18"/>
-      <c r="O114" s="18"/>
-      <c r="P114" s="18"/>
-      <c r="Q114" s="18"/>
-      <c r="R114" s="18"/>
-      <c r="S114" s="18"/>
-      <c r="T114" s="18"/>
-      <c r="U114" s="18"/>
-      <c r="V114" s="18"/>
+      <c r="A114" s="18">
+        <v>113</v>
+      </c>
+      <c r="B114" s="18" t="s">
+        <v>559</v>
+      </c>
+      <c r="C114" s="67" t="s">
+        <v>561</v>
+      </c>
+      <c r="D114" s="67">
+        <v>1</v>
+      </c>
+      <c r="E114" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="F114" s="65">
+        <v>0</v>
+      </c>
+      <c r="G114" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="H114" s="65"/>
+      <c r="I114" s="65">
+        <v>29.757819448754098</v>
+      </c>
+      <c r="J114" s="65">
+        <v>-95.353906211853001</v>
+      </c>
+      <c r="K114" s="65">
+        <v>29.7362085557276</v>
+      </c>
+      <c r="L114" s="65">
+        <v>-95.381543693542397</v>
+      </c>
+      <c r="M114" s="65"/>
+      <c r="N114" s="65"/>
+      <c r="O114" s="65"/>
+      <c r="P114" s="65"/>
+      <c r="Q114" s="65">
+        <v>40</v>
+      </c>
+      <c r="R114" s="65">
+        <v>40</v>
+      </c>
+      <c r="S114" s="65">
+        <v>44</v>
+      </c>
+      <c r="T114" s="65">
+        <v>8</v>
+      </c>
+      <c r="U114" s="65">
+        <v>4</v>
+      </c>
+      <c r="V114" s="65" t="s">
+        <v>563</v>
+      </c>
       <c r="W114" s="18"/>
       <c r="X114" s="18"/>
     </row>
     <row r="115" spans="1:24" s="2" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
-      <c r="A115" s="18"/>
-      <c r="B115" s="18"/>
-      <c r="C115" s="18"/>
-      <c r="D115" s="18"/>
-      <c r="E115" s="18"/>
-      <c r="F115" s="18"/>
-      <c r="G115" s="18"/>
-      <c r="H115" s="18"/>
-      <c r="I115" s="18"/>
-      <c r="J115" s="18"/>
-      <c r="K115" s="18"/>
-      <c r="L115" s="18"/>
-      <c r="M115" s="18"/>
-      <c r="N115" s="18"/>
-      <c r="O115" s="18"/>
-      <c r="P115" s="18"/>
-      <c r="Q115" s="18"/>
-      <c r="R115" s="18"/>
-      <c r="S115" s="18"/>
-      <c r="T115" s="18"/>
-      <c r="U115" s="18"/>
-      <c r="V115" s="18"/>
+      <c r="A115" s="18">
+        <v>114</v>
+      </c>
+      <c r="B115" s="18" t="s">
+        <v>560</v>
+      </c>
+      <c r="C115" s="67" t="s">
+        <v>562</v>
+      </c>
+      <c r="D115" s="67">
+        <v>1</v>
+      </c>
+      <c r="E115" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="F115" s="65">
+        <v>0</v>
+      </c>
+      <c r="G115" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="H115" s="65"/>
+      <c r="I115" s="65">
+        <v>29.757819448754098</v>
+      </c>
+      <c r="J115" s="65">
+        <v>-95.353906211853001</v>
+      </c>
+      <c r="K115" s="65">
+        <v>29.7362085557276</v>
+      </c>
+      <c r="L115" s="65">
+        <v>-95.381543693542397</v>
+      </c>
+      <c r="M115" s="65"/>
+      <c r="N115" s="65"/>
+      <c r="O115" s="65"/>
+      <c r="P115" s="65"/>
+      <c r="Q115" s="65">
+        <v>40</v>
+      </c>
+      <c r="R115" s="65">
+        <v>40</v>
+      </c>
+      <c r="S115" s="65">
+        <v>44</v>
+      </c>
+      <c r="T115" s="65">
+        <v>8</v>
+      </c>
+      <c r="U115" s="65">
+        <v>4</v>
+      </c>
+      <c r="V115" s="65">
+        <v>38</v>
+      </c>
       <c r="W115" s="18"/>
       <c r="X115" s="18"/>
     </row>
@@ -19638,8 +19767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="B25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20456,25 +20585,47 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="67">
+        <v>37</v>
+      </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
+      <c r="D38" s="6" t="s">
+        <v>371</v>
+      </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
+      <c r="G38" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" s="6">
+        <v>1</v>
+      </c>
       <c r="J38" s="6"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="67">
+        <v>38</v>
+      </c>
       <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
+      <c r="C39" s="76" t="s">
+        <v>551</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>106</v>
+      </c>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
+      <c r="G39" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
+      <c r="I39" s="6">
+        <v>2</v>
+      </c>
       <c r="J39" s="6"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -32567,9 +32718,12 @@
       <c r="J1138" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C39" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -32590,8 +32744,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AC801"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37656,7 +37810,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37788,14 +37942,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" style="12" bestFit="1" customWidth="1"/>
@@ -38319,7 +38473,7 @@
   <dimension ref="A1:AB578"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42716,7 +42870,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52153,7 +52307,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AB1073"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixes for DriverViewTests post deployment to develop
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -627,7 +627,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="570">
   <si>
     <t>Enabled</t>
   </si>
@@ -2326,6 +2326,18 @@
   <si>
     <t>1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17</t>
   </si>
+  <si>
+    <t>SimAuto-Analyzer4</t>
+  </si>
+  <si>
+    <t>SimAuto-AnalyzerKey4</t>
+  </si>
+  <si>
+    <t>SimAuto-Analyzer5</t>
+  </si>
+  <si>
+    <t>SimAuto-AnalyzerKey5</t>
+  </si>
 </sst>
 </file>
 
@@ -2334,7 +2346,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2454,14 +2466,6 @@
       <color indexed="37"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -2600,7 +2604,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2612,9 +2616,8 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2730,9 +2733,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="11" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="11">
     <cellStyle name="20% - Accent1 2" xfId="7"/>
     <cellStyle name="20% - Accent2 2" xfId="9"/>
     <cellStyle name="20% - Accent4 2" xfId="10"/>
@@ -2741,7 +2743,6 @@
     <cellStyle name="Check Cell 2" xfId="6"/>
     <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Good 2" xfId="3"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8"/>
     <cellStyle name="Input 2" xfId="5"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
@@ -3162,8 +3163,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AA2827"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -41604,7 +41605,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:L19"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42161,11 +42162,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" s="74" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A17" s="74">
         <v>16</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="74" t="s">
         <v>548</v>
       </c>
       <c r="C17" s="74" t="s">
@@ -42183,7 +42184,6 @@
       <c r="G17" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="H17" s="74"/>
       <c r="I17" s="74" t="s">
         <v>160</v>
       </c>
@@ -42197,11 +42197,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" s="74" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A18" s="74">
         <v>17</v>
       </c>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="74" t="s">
         <v>550</v>
       </c>
       <c r="C18" s="74" t="s">
@@ -42219,7 +42219,6 @@
       <c r="G18" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="H18" s="74"/>
       <c r="I18" s="74" t="s">
         <v>160</v>
       </c>
@@ -42233,11 +42232,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" s="74" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
       <c r="A19" s="74">
         <v>18</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="74" t="s">
         <v>552</v>
       </c>
       <c r="C19" s="74" t="s">
@@ -42255,7 +42254,6 @@
       <c r="G19" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="H19" s="74"/>
       <c r="I19" s="74" t="s">
         <v>160</v>
       </c>
@@ -42743,7 +42741,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43097,10 +43095,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB1069"/>
+  <dimension ref="A1:AB1068"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43886,7 +43884,7 @@
       <c r="AA32" s="55"/>
       <c r="AB32" s="55"/>
     </row>
-    <row r="33" spans="1:28" s="57" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="67">
         <v>32</v>
       </c>
@@ -43904,67 +43902,43 @@
       </c>
       <c r="F33" s="70"/>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A34" s="21"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
+    <row r="34" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="67">
+        <v>33</v>
+      </c>
+      <c r="B34" s="67" t="s">
+        <v>566</v>
+      </c>
+      <c r="C34" s="67" t="s">
+        <v>567</v>
+      </c>
+      <c r="D34" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="67" t="s">
+        <v>26</v>
+      </c>
       <c r="F34" s="70"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21"/>
-      <c r="O34" s="21"/>
-      <c r="P34" s="21"/>
-      <c r="Q34" s="21"/>
-      <c r="R34" s="21"/>
-      <c r="S34" s="21"/>
-      <c r="T34" s="21"/>
-      <c r="U34" s="21"/>
-      <c r="V34" s="21"/>
-      <c r="W34" s="21"/>
-      <c r="X34" s="21"/>
-      <c r="Y34" s="21"/>
-      <c r="Z34" s="21"/>
-      <c r="AA34" s="21"/>
-      <c r="AB34" s="21"/>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
+    </row>
+    <row r="35" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="67">
+        <v>34</v>
+      </c>
+      <c r="B35" s="67" t="s">
+        <v>568</v>
+      </c>
+      <c r="C35" s="67" t="s">
+        <v>569</v>
+      </c>
+      <c r="D35" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" s="67" t="s">
+        <v>26</v>
+      </c>
       <c r="F35" s="70"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="21"/>
-      <c r="O35" s="21"/>
-      <c r="P35" s="21"/>
-      <c r="Q35" s="21"/>
-      <c r="R35" s="21"/>
-      <c r="S35" s="21"/>
-      <c r="T35" s="21"/>
-      <c r="U35" s="21"/>
-      <c r="V35" s="21"/>
-      <c r="W35" s="21"/>
-      <c r="X35" s="21"/>
-      <c r="Y35" s="21"/>
-      <c r="Z35" s="21"/>
-      <c r="AA35" s="21"/>
-      <c r="AB35" s="21"/>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -43972,7 +43946,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="70"/>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -43980,7 +43954,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="70"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -43988,7 +43962,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="70"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -43996,7 +43970,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="70"/>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -44004,7 +43978,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="70"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -44012,7 +43986,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="70"/>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -44020,7 +43994,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="70"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -44028,7 +44002,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="70"/>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -44036,7 +44010,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="70"/>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -44044,7 +44018,7 @@
       <c r="E45" s="2"/>
       <c r="F45" s="70"/>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -44052,7 +44026,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="70"/>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -44060,7 +44034,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="70"/>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -52181,12 +52155,12 @@
       <c r="F1062" s="70"/>
     </row>
     <row r="1063" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1063" s="2"/>
-      <c r="B1063" s="2"/>
-      <c r="C1063" s="2"/>
-      <c r="D1063" s="2"/>
-      <c r="E1063" s="2"/>
-      <c r="F1063" s="70"/>
+      <c r="A1063" s="5"/>
+      <c r="B1063" s="5"/>
+      <c r="C1063" s="5"/>
+      <c r="D1063" s="5"/>
+      <c r="E1063" s="5"/>
+      <c r="F1063" s="72"/>
     </row>
     <row r="1064" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1064" s="5"/>
@@ -52221,40 +52195,32 @@
       <c r="F1067" s="72"/>
     </row>
     <row r="1068" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1068" s="5"/>
-      <c r="B1068" s="5"/>
-      <c r="C1068" s="5"/>
-      <c r="D1068" s="5"/>
-      <c r="E1068" s="5"/>
-      <c r="F1068" s="72"/>
-    </row>
-    <row r="1069" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1069" s="24"/>
-      <c r="B1069" s="24"/>
-      <c r="C1069" s="24"/>
-      <c r="D1069" s="24"/>
-      <c r="E1069" s="23"/>
-      <c r="F1069" s="73"/>
-      <c r="G1069" s="22"/>
-      <c r="H1069" s="22"/>
-      <c r="I1069" s="22"/>
-      <c r="J1069" s="22"/>
-      <c r="K1069" s="22"/>
-      <c r="L1069" s="22"/>
-      <c r="M1069" s="22"/>
-      <c r="N1069" s="22"/>
-      <c r="O1069" s="22"/>
-      <c r="P1069" s="22"/>
-      <c r="Q1069" s="22"/>
-      <c r="R1069" s="22"/>
-      <c r="S1069" s="22"/>
-      <c r="T1069" s="22"/>
-      <c r="U1069" s="22"/>
-      <c r="V1069" s="22"/>
-      <c r="W1069" s="22"/>
-      <c r="X1069" s="22"/>
-      <c r="Y1069" s="22"/>
-      <c r="Z1069" s="22"/>
+      <c r="A1068" s="24"/>
+      <c r="B1068" s="24"/>
+      <c r="C1068" s="24"/>
+      <c r="D1068" s="24"/>
+      <c r="E1068" s="23"/>
+      <c r="F1068" s="73"/>
+      <c r="G1068" s="22"/>
+      <c r="H1068" s="22"/>
+      <c r="I1068" s="22"/>
+      <c r="J1068" s="22"/>
+      <c r="K1068" s="22"/>
+      <c r="L1068" s="22"/>
+      <c r="M1068" s="22"/>
+      <c r="N1068" s="22"/>
+      <c r="O1068" s="22"/>
+      <c r="P1068" s="22"/>
+      <c r="Q1068" s="22"/>
+      <c r="R1068" s="22"/>
+      <c r="S1068" s="22"/>
+      <c r="T1068" s="22"/>
+      <c r="U1068" s="22"/>
+      <c r="V1068" s="22"/>
+      <c r="W1068" s="22"/>
+      <c r="X1068" s="22"/>
+      <c r="Y1068" s="22"/>
+      <c r="Z1068" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test data fixes in simulator based tests
</commit_message>
<xml_diff>
--- a/selenium-wd/data/TestCaseData.xlsx
+++ b/selenium-wd/data/TestCaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="799" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzers" sheetId="22" r:id="rId1"/>
@@ -2610,7 +2610,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2729,6 +2729,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent1 2" xfId="7"/>
@@ -41597,7 +41598,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43161,8 +43162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1069"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sq